<commit_message>
Practice Leetcode on 20230827
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73336ED2-6125-074A-AC26-0C1F60DC0E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C7030D-F39B-3540-B91D-0D2CE8E384B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="290">
   <si>
     <t xml:space="preserve">
 </t>
@@ -909,6 +909,150 @@
   </si>
   <si>
     <t>save max and min value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/566/</t>
+  </si>
+  <si>
+    <t>2023.08.23</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/576/</t>
+  </si>
+  <si>
+    <t>House Robber</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>devide and conquer (use check now and +next)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>save all step value, last and now to statistic</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/98/design/670/</t>
+  </si>
+  <si>
+    <t>Shuffle an Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.24</t>
+  </si>
+  <si>
+    <t>random.shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/98/design/562/</t>
+  </si>
+  <si>
+    <t>two list which one of use to save min value sequence</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min Stack</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/743/</t>
+  </si>
+  <si>
+    <t>Fizz Buzz</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>if else</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.25</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/744/</t>
+  </si>
+  <si>
+    <t>Count Primes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>use "Sieve of Eeatosthese" method: set True for all num(with it's times) before n^0.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/745/</t>
+  </si>
+  <si>
+    <t>while to reach out</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power of Three</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/roman-to-integer/</t>
+  </si>
+  <si>
+    <t>2023.08.26</t>
+  </si>
+  <si>
+    <t>if i &lt; i+1, value-=i</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/565/</t>
+  </si>
+  <si>
+    <t>check last bit and sum all 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Roman to Integer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of 1 Bits</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/762/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hamming Distance</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin() with count('1')</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.27</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/648/</t>
+  </si>
+  <si>
+    <t>bin() with int(x, 2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/601/</t>
+  </si>
+  <si>
+    <t>Reverse Bits</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pascal's Triangle</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1464,16 +1608,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
     <col min="5" max="5" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="88.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.83203125" customWidth="1"/>
     <col min="7" max="7" width="53.5" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="2" customWidth="1"/>
   </cols>
@@ -2362,103 +2506,289 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
+      <c r="B37" s="2">
+        <v>53</v>
+      </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="7"/>
+      <c r="D37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2">
         <v>36</v>
       </c>
+      <c r="B38" s="2">
+        <v>198</v>
+      </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="7"/>
+      <c r="D38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2">
         <v>37</v>
       </c>
+      <c r="B39" s="2">
+        <v>384</v>
+      </c>
       <c r="C39" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2">
         <v>38</v>
       </c>
+      <c r="B40" s="2">
+        <v>155</v>
+      </c>
       <c r="C40" s="12"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="7"/>
+      <c r="D40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2">
         <v>39</v>
       </c>
+      <c r="B41" s="2">
+        <v>412</v>
+      </c>
       <c r="C41" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E41" s="7"/>
+      <c r="D41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2">
         <v>40</v>
       </c>
+      <c r="B42" s="2">
+        <v>204</v>
+      </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="7"/>
+      <c r="D42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2">
         <v>41</v>
       </c>
+      <c r="B43" s="2">
+        <v>326</v>
+      </c>
       <c r="C43" s="12"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="7"/>
+      <c r="D43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2">
         <v>42</v>
       </c>
+      <c r="B44" s="2">
+        <v>13</v>
+      </c>
       <c r="C44" s="12"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="D44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2">
         <v>43</v>
       </c>
+      <c r="B45" s="2">
+        <v>191</v>
+      </c>
       <c r="C45" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="7"/>
+      <c r="D45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2">
         <v>44</v>
       </c>
+      <c r="B46" s="2">
+        <v>44</v>
+      </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="7"/>
+      <c r="D46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2">
         <v>45</v>
       </c>
+      <c r="B47" s="2">
+        <v>190</v>
+      </c>
       <c r="C47" s="12"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="7"/>
+      <c r="D47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="2">
         <v>46</v>
       </c>
+      <c r="B48" s="2">
+        <v>118</v>
+      </c>
       <c r="C48" s="12"/>
-      <c r="E48" s="7"/>
+      <c r="D48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
@@ -2658,6 +2988,7 @@
     <hyperlink ref="F5" r:id="rId2" xr:uid="{330AC4A1-EE6C-DD40-B251-9FCCA7277915}"/>
     <hyperlink ref="F6" r:id="rId3" xr:uid="{9DDED772-F21E-7B48-9CB2-CB46C4DE0963}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{F57CED91-3449-574E-8615-4599E779544E}"/>
+    <hyperlink ref="F46" r:id="rId5" xr:uid="{B257738E-11CD-C047-9119-DEAD4671692E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Practice Leetcode on 20230828
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C7030D-F39B-3540-B91D-0D2CE8E384B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4297D371-68CC-CD4D-9F03-51230E53F8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="top-interview-questions-easy" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="298">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1053,6 +1053,35 @@
   </si>
   <si>
     <t>Pascal's Triangle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/721/</t>
+  </si>
+  <si>
+    <t>2023.08.28</t>
+  </si>
+  <si>
+    <t>add 0 to first and last, then run all</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/722/</t>
+  </si>
+  <si>
+    <t>Missing Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack and return len(stack) == 0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>math and find one</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1608,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2789,103 +2818,141 @@
       <c r="F48" s="7" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="2">
         <v>47</v>
       </c>
+      <c r="B49" s="2">
+        <v>20</v>
+      </c>
       <c r="C49" s="12"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="7"/>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="D49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="2">
         <v>48</v>
       </c>
+      <c r="B50" s="2">
+        <v>268</v>
+      </c>
       <c r="C50" s="12"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="D50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:8">
       <c r="A52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:8">
       <c r="A53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:8">
       <c r="A54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:8">
       <c r="A55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:8">
       <c r="A56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:8">
       <c r="A57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:8">
       <c r="A58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:8">
       <c r="A59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:8">
       <c r="A60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:8">
       <c r="A61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:8">
       <c r="A62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:8">
       <c r="A63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:8">
       <c r="A64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2998,7 +3065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[20230830] Leetcode - Blind 75 (4-6)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AF8B71-5C68-D040-B027-8B91B6D6F708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6675C50-299F-CE41-BA6F-27FCCAD5604A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="306">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1093,6 +1093,27 @@
   </si>
   <si>
     <t>new_list &amp; ptr and compare l1, l2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.30</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/invert-binary-tree/</t>
+  </si>
+  <si>
+    <t>dp[] and compare max &amp; min</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list == list[::-1] or two pointer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>if root, exchange sub</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1252,7 +1273,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1317,9 +1338,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1640,7 +1658,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3068,18 +3086,18 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55" customWidth="1"/>
     <col min="8" max="8" width="29.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
@@ -3139,14 +3157,16 @@
       <c r="B3" s="21">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="2" t="s">
         <v>161</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -3173,14 +3193,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="21"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>110</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="2" t="s">
         <v>292</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -3202,13 +3224,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="21"/>
+      <c r="C5" s="2">
+        <v>21</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="2" t="s">
         <v>206</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -3229,17 +3254,26 @@
         <v>4</v>
       </c>
       <c r="B6" s="21"/>
+      <c r="C6" s="2">
+        <v>121</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>97</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="K6" t="s">
         <v>23</v>
@@ -3250,32 +3284,56 @@
         <v>5</v>
       </c>
       <c r="B7" s="21"/>
+      <c r="C7" s="2">
+        <v>125</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="K7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" ht="16">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="21"/>
+      <c r="C8" s="2">
+        <v>226</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="K8" t="s">
         <v>24</v>
@@ -3292,9 +3350,10 @@
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="I9" s="2"/>
       <c r="K9" t="s">
         <v>25</v>
       </c>
@@ -3310,9 +3369,10 @@
       <c r="E10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="I10" s="2"/>
       <c r="K10" t="s">
         <v>25</v>
       </c>
@@ -3328,9 +3388,10 @@
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="I11" s="2"/>
       <c r="K11" t="s">
         <v>23</v>
       </c>
@@ -3346,7 +3407,7 @@
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K12" t="s">
@@ -3364,7 +3425,7 @@
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K13" t="s">
@@ -3382,7 +3443,7 @@
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K14" t="s">
@@ -3400,7 +3461,7 @@
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K15" t="s">
@@ -3420,7 +3481,7 @@
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K16" t="s">
@@ -3438,7 +3499,7 @@
       <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K17" t="s">
@@ -3456,7 +3517,7 @@
       <c r="E18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K18" t="s">
@@ -3474,7 +3535,7 @@
       <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="K19" t="s">
@@ -3492,7 +3553,7 @@
       <c r="E20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K20" t="s">
@@ -3510,7 +3571,7 @@
       <c r="E21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="2" t="s">
         <v>31</v>
       </c>
       <c r="K21" t="s">
@@ -3528,7 +3589,7 @@
       <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="2" t="s">
         <v>32</v>
       </c>
       <c r="K22" t="s">
@@ -3546,7 +3607,7 @@
       <c r="E23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K23" t="s">
@@ -3564,7 +3625,7 @@
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="K24" t="s">
@@ -3582,7 +3643,7 @@
       <c r="E25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="K25" t="s">
@@ -3600,7 +3661,7 @@
       <c r="E26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G26" s="6" t="s">
@@ -3621,7 +3682,7 @@
       <c r="E27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -3644,7 +3705,7 @@
       <c r="E28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="2" t="s">
         <v>38</v>
       </c>
       <c r="K28" t="s">
@@ -3662,7 +3723,7 @@
       <c r="E29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K29" t="s">
@@ -3680,7 +3741,7 @@
       <c r="E30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="2" t="s">
         <v>41</v>
       </c>
       <c r="K30" t="s">
@@ -3698,7 +3759,7 @@
       <c r="E31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="2" t="s">
         <v>42</v>
       </c>
       <c r="K31" t="s">
@@ -3716,7 +3777,7 @@
       <c r="E32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G32" s="6" t="s">
@@ -3737,7 +3798,7 @@
       <c r="E33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="2" t="s">
         <v>44</v>
       </c>
       <c r="K33" t="s">
@@ -3755,7 +3816,7 @@
       <c r="E34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K34" t="s">
@@ -3773,7 +3834,7 @@
       <c r="E35" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="2" t="s">
         <v>46</v>
       </c>
       <c r="K35" t="s">
@@ -3793,7 +3854,7 @@
       <c r="E36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="2" t="s">
         <v>47</v>
       </c>
       <c r="K36" t="s">
@@ -3811,7 +3872,7 @@
       <c r="E37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="2" t="s">
         <v>48</v>
       </c>
       <c r="K37" t="s">
@@ -3829,7 +3890,7 @@
       <c r="E38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="2" t="s">
         <v>49</v>
       </c>
       <c r="K38" t="s">
@@ -3847,7 +3908,7 @@
       <c r="E39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G39" s="6" t="s">
@@ -3868,7 +3929,7 @@
       <c r="E40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="2" t="s">
         <v>51</v>
       </c>
       <c r="K40" t="s">
@@ -3886,7 +3947,7 @@
       <c r="E41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F41" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K41" t="s">
@@ -3904,7 +3965,7 @@
       <c r="E42" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="F42" s="2" t="s">
         <v>53</v>
       </c>
       <c r="K42" t="s">
@@ -3922,7 +3983,7 @@
       <c r="E43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F43" s="22" t="s">
+      <c r="F43" s="2" t="s">
         <v>54</v>
       </c>
       <c r="K43" t="s">
@@ -3942,7 +4003,7 @@
       <c r="E44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F44" s="22" t="s">
+      <c r="F44" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G44" s="6" t="s">
@@ -3963,7 +4024,7 @@
       <c r="E45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F45" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K45" t="s">
@@ -3981,7 +4042,7 @@
       <c r="E46" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F46" s="22" t="s">
+      <c r="F46" s="2" t="s">
         <v>57</v>
       </c>
       <c r="K46" t="s">
@@ -3999,7 +4060,7 @@
       <c r="E47" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F47" s="2" t="s">
         <v>58</v>
       </c>
       <c r="K47" t="s">
@@ -4017,7 +4078,7 @@
       <c r="E48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F48" s="2" t="s">
         <v>59</v>
       </c>
       <c r="K48" t="s">
@@ -4035,7 +4096,7 @@
       <c r="E49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="F49" s="2" t="s">
         <v>60</v>
       </c>
       <c r="K49" t="s">
@@ -4053,7 +4114,7 @@
       <c r="E50" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="22" t="s">
+      <c r="F50" s="2" t="s">
         <v>61</v>
       </c>
       <c r="K50" t="s">
@@ -4071,7 +4132,7 @@
       <c r="E51" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F51" s="22" t="s">
+      <c r="F51" s="2" t="s">
         <v>62</v>
       </c>
       <c r="K51" t="s">
@@ -4091,7 +4152,7 @@
       <c r="E52" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F52" s="22" t="s">
+      <c r="F52" s="2" t="s">
         <v>63</v>
       </c>
       <c r="K52" t="s">
@@ -4109,7 +4170,7 @@
       <c r="E53" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F53" s="22" t="s">
+      <c r="F53" s="2" t="s">
         <v>64</v>
       </c>
       <c r="K53" t="s">
@@ -4127,7 +4188,7 @@
       <c r="E54" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F54" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K54" t="s">
@@ -4145,7 +4206,7 @@
       <c r="E55" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="F55" s="2" t="s">
         <v>66</v>
       </c>
       <c r="K55" t="s">
@@ -4163,7 +4224,7 @@
       <c r="E56" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F56" s="22" t="s">
+      <c r="F56" s="2" t="s">
         <v>67</v>
       </c>
       <c r="K56" t="s">
@@ -4181,7 +4242,7 @@
       <c r="E57" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F57" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K57" t="s">
@@ -4199,7 +4260,7 @@
       <c r="E58" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F58" s="22" t="s">
+      <c r="F58" s="2" t="s">
         <v>69</v>
       </c>
       <c r="K58" t="s">
@@ -4217,7 +4278,7 @@
       <c r="E59" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F59" s="22" t="s">
+      <c r="F59" s="2" t="s">
         <v>70</v>
       </c>
       <c r="K59" t="s">
@@ -4235,7 +4296,7 @@
       <c r="E60" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F60" s="22" t="s">
+      <c r="F60" s="2" t="s">
         <v>71</v>
       </c>
       <c r="K60" t="s">
@@ -4255,7 +4316,7 @@
       <c r="E61" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="22" t="s">
+      <c r="F61" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G61" s="6" t="s">
@@ -4276,7 +4337,7 @@
       <c r="E62" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F62" s="22" t="s">
+      <c r="F62" s="2" t="s">
         <v>73</v>
       </c>
       <c r="K62" t="s">
@@ -4294,7 +4355,7 @@
       <c r="E63" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F63" s="22" t="s">
+      <c r="F63" s="2" t="s">
         <v>74</v>
       </c>
       <c r="K63" t="s">
@@ -4312,7 +4373,7 @@
       <c r="E64" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F64" s="22" t="s">
+      <c r="F64" s="2" t="s">
         <v>75</v>
       </c>
       <c r="K64" t="s">
@@ -4330,7 +4391,7 @@
       <c r="E65" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F65" s="22" t="s">
+      <c r="F65" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K65" t="s">
@@ -4348,7 +4409,7 @@
       <c r="E66" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F66" s="22" t="s">
+      <c r="F66" s="2" t="s">
         <v>77</v>
       </c>
       <c r="K66" t="s">
@@ -4366,7 +4427,7 @@
       <c r="E67" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F67" s="22" t="s">
+      <c r="F67" s="2" t="s">
         <v>78</v>
       </c>
       <c r="K67" t="s">
@@ -4386,7 +4447,7 @@
       <c r="E68" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F68" s="22" t="s">
+      <c r="F68" s="2" t="s">
         <v>79</v>
       </c>
       <c r="K68" t="s">
@@ -4404,7 +4465,7 @@
       <c r="E69" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F69" s="22" t="s">
+      <c r="F69" s="2" t="s">
         <v>80</v>
       </c>
       <c r="K69" t="s">
@@ -4422,7 +4483,7 @@
       <c r="E70" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F70" s="22" t="s">
+      <c r="F70" s="2" t="s">
         <v>81</v>
       </c>
       <c r="K70" t="s">
@@ -4440,7 +4501,7 @@
       <c r="E71" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F71" s="22" t="s">
+      <c r="F71" s="2" t="s">
         <v>82</v>
       </c>
       <c r="K71" t="s">
@@ -4458,7 +4519,7 @@
       <c r="E72" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F72" s="22" t="s">
+      <c r="F72" s="2" t="s">
         <v>83</v>
       </c>
       <c r="K72" t="s">
@@ -4476,7 +4537,7 @@
       <c r="E73" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F73" s="22" t="s">
+      <c r="F73" s="2" t="s">
         <v>84</v>
       </c>
       <c r="K73" t="s">
@@ -4494,7 +4555,7 @@
       <c r="E74" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F74" s="22" t="s">
+      <c r="F74" s="2" t="s">
         <v>85</v>
       </c>
       <c r="K74" t="s">
@@ -4512,7 +4573,7 @@
       <c r="E75" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F75" s="22" t="s">
+      <c r="F75" s="2" t="s">
         <v>86</v>
       </c>
       <c r="K75" t="s">
@@ -4530,7 +4591,7 @@
       <c r="E76" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F76" s="22" t="s">
+      <c r="F76" s="2" t="s">
         <v>87</v>
       </c>
       <c r="K76" t="s">
@@ -4548,7 +4609,7 @@
       <c r="E77" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F77" s="22" t="s">
+      <c r="F77" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K77" t="s">
@@ -4559,7 +4620,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="F78" s="22" t="s">
+      <c r="F78" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G78" s="6" t="s">
@@ -4570,7 +4631,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="F79" s="22" t="s">
+      <c r="F79" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G79" s="6" t="s">
@@ -4578,10 +4639,10 @@
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="F80" s="22"/>
+      <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="F81" s="22"/>
+      <c r="F81" s="2"/>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="2" t="s">

</xml_diff>

<commit_message>
[20230831] Leetcode - Blind 75 (7-9)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6675C50-299F-CE41-BA6F-27FCCAD5604A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F500DE5F-4E72-AF44-9F38-FCE30DF5851E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="313">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1114,6 +1114,30 @@
   </si>
   <si>
     <t>if root, exchange sub</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.31</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-anagram/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-search/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flood-fill/</t>
+  </si>
+  <si>
+    <t>Counter faster than sorted</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>left = mid + 1; right = mid - 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new fill to extend four direction</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3086,7 +3110,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3344,6 +3368,9 @@
         <v>7</v>
       </c>
       <c r="B9" s="21"/>
+      <c r="C9" s="2">
+        <v>242</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>112</v>
       </c>
@@ -3353,7 +3380,15 @@
       <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="G9" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="K9" t="s">
         <v>25</v>
       </c>
@@ -3363,6 +3398,9 @@
         <v>8</v>
       </c>
       <c r="B10" s="21"/>
+      <c r="C10" s="2">
+        <v>704</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
@@ -3372,16 +3410,27 @@
       <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="G10" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="K10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" ht="16">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="21"/>
+      <c r="C11" s="2">
+        <v>733</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>114</v>
       </c>
@@ -3391,7 +3440,15 @@
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="G11" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="K11" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
[20230902] Leetcode - Blind 75 (12-13)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34182322-6BD8-6C47-AFC2-A4E9D3F01B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE09839-F45B-D746-885A-6116A5FD2068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="top-interview-questions-easy" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="324">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1167,6 +1167,17 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/first-bad-version/</t>
+  </si>
+  <si>
+    <t>2023.09.02</t>
+  </si>
+  <si>
+    <t>two ptr with one step and two step, or, id with table</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two stack, first for input and second for out</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3138,7 +3149,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3561,6 +3572,12 @@
       <c r="G14" t="s">
         <v>318</v>
       </c>
+      <c r="H14" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>321</v>
+      </c>
       <c r="K14" t="s">
         <v>22</v>
       </c>
@@ -3584,6 +3601,12 @@
       </c>
       <c r="G15" t="s">
         <v>319</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="K15" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
[20230903] Leetcode - Blind 75 (14-16)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE09839-F45B-D746-885A-6116A5FD2068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68EEF33-A2D6-F345-8FF6-186DC353351F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="333">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1178,6 +1178,38 @@
   <si>
     <t>two stack, first for input and second for out</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>peek()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS, right = mid, left = mid + 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.03</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ransom-note/</t>
+  </si>
+  <si>
+    <t>two Counter and &amp; is smaller one</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t>DP, cur_step = cur + last</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-palindrome/</t>
   </si>
 </sst>
 </file>
@@ -1336,7 +1368,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1401,6 +1433,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3149,7 +3184,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3210,6 +3245,9 @@
         <v>7</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="L2" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3569,7 +3607,7 @@
       <c r="F14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="6" t="s">
         <v>318</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -3582,8 +3620,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="2">
+    <row r="15" spans="1:12" ht="16">
+      <c r="A15" s="9">
         <v>13</v>
       </c>
       <c r="B15" s="21"/>
@@ -3599,7 +3637,7 @@
       <c r="F15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>319</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -3610,6 +3648,9 @@
       </c>
       <c r="K15" t="s">
         <v>22</v>
+      </c>
+      <c r="L15" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3631,18 +3672,27 @@
       <c r="F16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="6" t="s">
         <v>320</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="K16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" ht="16">
       <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" s="16"/>
+      <c r="C17" s="2">
+        <v>383</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>115</v>
       </c>
@@ -3652,15 +3702,27 @@
       <c r="F17" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="G17" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>327</v>
+      </c>
       <c r="K17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="16">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="16"/>
+      <c r="C18" s="2">
+        <v>70</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>116</v>
       </c>
@@ -3669,6 +3731,15 @@
       </c>
       <c r="F18" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="K18" t="s">
         <v>22</v>
@@ -3679,6 +3750,9 @@
         <v>17</v>
       </c>
       <c r="B19" s="16"/>
+      <c r="C19" s="2">
+        <v>409</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>111</v>
       </c>
@@ -3687,6 +3761,9 @@
       </c>
       <c r="F19" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="G19" t="s">
+        <v>332</v>
       </c>
       <c r="K19" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
[20230904] Leetcode - Blind 75 (17-19)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68EEF33-A2D6-F345-8FF6-186DC353351F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEF8D65-D966-9649-AEA2-1B997C4D3591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="339">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1210,6 +1210,27 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/longest-palindrome/</t>
+  </si>
+  <si>
+    <t>2023.09.04</t>
+  </si>
+  <si>
+    <t>count = 2*(char shows twice) + 1 (char shows once)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/</t>
+  </si>
+  <si>
+    <t>pre, cur, cur.next = pre.next , pre, cur</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/</t>
+  </si>
+  <si>
+    <t>Counter and return 1/2 nums</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1399,6 +1420,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1433,9 +1457,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1770,14 +1791,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -1819,7 +1840,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1852,7 +1873,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -1878,7 +1899,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -1902,7 +1923,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1926,7 +1947,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1950,7 +1971,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1974,7 +1995,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1998,7 +2019,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2022,7 +2043,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2046,7 +2067,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -2070,7 +2091,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -2094,7 +2115,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>126</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -2120,7 +2141,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -2144,7 +2165,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="11"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -2168,7 +2189,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2192,7 +2213,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -2216,7 +2237,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -2240,7 +2261,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -2264,7 +2285,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -2288,7 +2309,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>127</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -2314,7 +2335,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -2338,7 +2359,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -2362,7 +2383,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -2386,7 +2407,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2410,7 +2431,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -2434,7 +2455,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>128</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -2460,7 +2481,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -2484,7 +2505,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -2508,7 +2529,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -2532,7 +2553,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -2556,7 +2577,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="11" t="s">
         <v>129</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -2582,7 +2603,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="10"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -2606,7 +2627,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="11" t="s">
         <v>130</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -2632,7 +2653,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="10"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -2656,7 +2677,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="10"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -2680,7 +2701,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="10"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -2704,7 +2725,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="11" t="s">
         <v>131</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2730,7 +2751,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="10"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -2754,7 +2775,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="11" t="s">
         <v>132</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2780,7 +2801,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="10"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -2804,7 +2825,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="10"/>
+      <c r="C43" s="11"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -2828,7 +2849,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="10"/>
+      <c r="C44" s="11"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -2852,7 +2873,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="11" t="s">
         <v>133</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2878,7 +2899,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="10"/>
+      <c r="C46" s="11"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -2902,7 +2923,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="10"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -2926,7 +2947,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="10"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -2950,7 +2971,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="10"/>
+      <c r="C49" s="11"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -2974,7 +2995,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="10"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -3196,22 +3217,22 @@
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="55" customWidth="1"/>
-    <col min="8" max="8" width="39.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -3247,7 +3268,7 @@
       <c r="K2" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3255,7 +3276,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -3293,7 +3314,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -3324,7 +3345,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -3354,7 +3375,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -3384,7 +3405,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -3414,7 +3435,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -3444,7 +3465,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -3474,7 +3495,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -3504,7 +3525,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -3534,7 +3555,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -3564,7 +3585,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -3594,7 +3615,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -3624,7 +3645,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -3657,7 +3678,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="17">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -3689,7 +3710,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -3719,7 +3740,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -3749,7 +3770,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -3762,18 +3783,27 @@
       <c r="F19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="6" t="s">
         <v>332</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>333</v>
       </c>
       <c r="K19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="16">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="2">
+        <v>206</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>110</v>
       </c>
@@ -3783,15 +3813,27 @@
       <c r="F20" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="G20" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>333</v>
+      </c>
       <c r="K20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="16">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="2">
+        <v>169</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>117</v>
       </c>
@@ -3800,6 +3842,15 @@
       </c>
       <c r="F21" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>333</v>
       </c>
       <c r="K21" t="s">
         <v>22</v>
@@ -3809,7 +3860,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="D22" s="2" t="s">
         <v>118</v>
       </c>
@@ -3827,7 +3878,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="17"/>
       <c r="D23" s="2" t="s">
         <v>112</v>
       </c>
@@ -3845,7 +3896,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="17"/>
       <c r="D24" s="2" t="s">
         <v>110</v>
       </c>
@@ -3863,7 +3914,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="D25" s="2" t="s">
         <v>112</v>
       </c>
@@ -3881,7 +3932,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="17"/>
       <c r="D26" s="2" t="s">
         <v>117</v>
       </c>
@@ -3902,7 +3953,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="17"/>
       <c r="D27" s="2" t="s">
         <v>116</v>
       </c>
@@ -3923,7 +3974,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="18">
         <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -3943,7 +3994,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="18"/>
       <c r="D29" s="2" t="s">
         <v>113</v>
       </c>
@@ -3961,7 +4012,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="18"/>
       <c r="D30" s="2" t="s">
         <v>119</v>
       </c>
@@ -3979,7 +4030,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="17"/>
+      <c r="B31" s="18"/>
       <c r="D31" s="2" t="s">
         <v>111</v>
       </c>
@@ -3997,7 +4048,7 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="17"/>
+      <c r="B32" s="18"/>
       <c r="D32" s="2" t="s">
         <v>117</v>
       </c>
@@ -4018,7 +4069,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="17"/>
+      <c r="B33" s="18"/>
       <c r="D33" s="2" t="s">
         <v>112</v>
       </c>
@@ -4036,7 +4087,7 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="17"/>
+      <c r="B34" s="18"/>
       <c r="D34" s="2" t="s">
         <v>113</v>
       </c>
@@ -4054,7 +4105,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="17"/>
+      <c r="B35" s="18"/>
       <c r="D35" s="2" t="s">
         <v>109</v>
       </c>
@@ -4072,7 +4123,7 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="18">
+      <c r="B36" s="19">
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -4092,7 +4143,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="18"/>
+      <c r="B37" s="19"/>
       <c r="D37" s="2" t="s">
         <v>120</v>
       </c>
@@ -4110,7 +4161,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="18"/>
+      <c r="B38" s="19"/>
       <c r="D38" s="2" t="s">
         <v>116</v>
       </c>
@@ -4128,7 +4179,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="18"/>
+      <c r="B39" s="19"/>
       <c r="D39" s="2" t="s">
         <v>117</v>
       </c>
@@ -4149,7 +4200,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="18"/>
+      <c r="B40" s="19"/>
       <c r="D40" s="2" t="s">
         <v>109</v>
       </c>
@@ -4167,7 +4218,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="18"/>
+      <c r="B41" s="19"/>
       <c r="D41" s="2" t="s">
         <v>114</v>
       </c>
@@ -4185,7 +4236,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="18"/>
+      <c r="B42" s="19"/>
       <c r="D42" s="2" t="s">
         <v>113</v>
       </c>
@@ -4203,7 +4254,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="18"/>
+      <c r="B43" s="19"/>
       <c r="D43" s="2" t="s">
         <v>113</v>
       </c>
@@ -4221,7 +4272,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="19">
+      <c r="B44" s="20">
         <v>5</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -4244,7 +4295,7 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="19"/>
+      <c r="B45" s="20"/>
       <c r="D45" s="2" t="s">
         <v>117</v>
       </c>
@@ -4262,7 +4313,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="19"/>
+      <c r="B46" s="20"/>
       <c r="D46" s="2" t="s">
         <v>121</v>
       </c>
@@ -4280,7 +4331,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="19"/>
+      <c r="B47" s="20"/>
       <c r="D47" s="2" t="s">
         <v>117</v>
       </c>
@@ -4298,7 +4349,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="19"/>
+      <c r="B48" s="20"/>
       <c r="D48" s="2" t="s">
         <v>112</v>
       </c>
@@ -4316,7 +4367,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="19"/>
+      <c r="B49" s="20"/>
       <c r="D49" s="2" t="s">
         <v>16</v>
       </c>
@@ -4334,7 +4385,7 @@
       <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B50" s="19"/>
+      <c r="B50" s="20"/>
       <c r="D50" s="2" t="s">
         <v>113</v>
       </c>
@@ -4352,7 +4403,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="19"/>
+      <c r="B51" s="20"/>
       <c r="D51" s="2" t="s">
         <v>117</v>
       </c>
@@ -4370,7 +4421,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="20">
+      <c r="B52" s="21">
         <v>6</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -4390,7 +4441,7 @@
       <c r="A53" s="2">
         <v>51</v>
       </c>
-      <c r="B53" s="20"/>
+      <c r="B53" s="21"/>
       <c r="D53" s="2" t="s">
         <v>116</v>
       </c>
@@ -4408,7 +4459,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="20"/>
+      <c r="B54" s="21"/>
       <c r="D54" s="2" t="s">
         <v>111</v>
       </c>
@@ -4426,7 +4477,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="20"/>
+      <c r="B55" s="21"/>
       <c r="D55" s="2" t="s">
         <v>122</v>
       </c>
@@ -4444,7 +4495,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="20"/>
+      <c r="B56" s="21"/>
       <c r="D56" s="2" t="s">
         <v>121</v>
       </c>
@@ -4462,7 +4513,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="20"/>
+      <c r="B57" s="21"/>
       <c r="D57" s="2" t="s">
         <v>112</v>
       </c>
@@ -4480,7 +4531,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="20"/>
+      <c r="B58" s="21"/>
       <c r="D58" s="2" t="s">
         <v>111</v>
       </c>
@@ -4498,7 +4549,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="20"/>
+      <c r="B59" s="21"/>
       <c r="D59" s="2" t="s">
         <v>116</v>
       </c>
@@ -4516,7 +4567,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="20"/>
+      <c r="B60" s="21"/>
       <c r="D60" s="2" t="s">
         <v>112</v>
       </c>
@@ -4534,7 +4585,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="13">
+      <c r="B61" s="14">
         <v>7</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -4557,7 +4608,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="13"/>
+      <c r="B62" s="14"/>
       <c r="D62" s="2" t="s">
         <v>121</v>
       </c>
@@ -4575,7 +4626,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="13"/>
+      <c r="B63" s="14"/>
       <c r="D63" s="2" t="s">
         <v>113</v>
       </c>
@@ -4593,7 +4644,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="13"/>
+      <c r="B64" s="14"/>
       <c r="D64" s="2" t="s">
         <v>111</v>
       </c>
@@ -4611,7 +4662,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="13"/>
+      <c r="B65" s="14"/>
       <c r="D65" s="2" t="s">
         <v>113</v>
       </c>
@@ -4629,7 +4680,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="13"/>
+      <c r="B66" s="14"/>
       <c r="D66" s="2" t="s">
         <v>119</v>
       </c>
@@ -4647,7 +4698,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="13"/>
+      <c r="B67" s="14"/>
       <c r="D67" s="2" t="s">
         <v>110</v>
       </c>
@@ -4665,7 +4716,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="14">
+      <c r="B68" s="15">
         <v>8</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -4685,7 +4736,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="14"/>
+      <c r="B69" s="15"/>
       <c r="D69" s="2" t="s">
         <v>111</v>
       </c>
@@ -4703,7 +4754,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="14"/>
+      <c r="B70" s="15"/>
       <c r="D70" s="2" t="s">
         <v>112</v>
       </c>
@@ -4721,7 +4772,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="14"/>
+      <c r="B71" s="15"/>
       <c r="D71" s="2" t="s">
         <v>109</v>
       </c>
@@ -4739,7 +4790,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="14"/>
+      <c r="B72" s="15"/>
       <c r="D72" s="2" t="s">
         <v>119</v>
       </c>
@@ -4757,7 +4808,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="14"/>
+      <c r="B73" s="15"/>
       <c r="D73" s="2" t="s">
         <v>113</v>
       </c>
@@ -4775,7 +4826,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="14"/>
+      <c r="B74" s="15"/>
       <c r="D74" s="2" t="s">
         <v>109</v>
       </c>
@@ -4793,7 +4844,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="14"/>
+      <c r="B75" s="15"/>
       <c r="D75" s="2" t="s">
         <v>16</v>
       </c>
@@ -4811,7 +4862,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="14"/>
+      <c r="B76" s="15"/>
       <c r="D76" s="2" t="s">
         <v>119</v>
       </c>
@@ -4829,7 +4880,7 @@
       <c r="A77" s="2">
         <v>75</v>
       </c>
-      <c r="B77" s="14"/>
+      <c r="B77" s="15"/>
       <c r="D77" s="2" t="s">
         <v>109</v>
       </c>
@@ -4875,15 +4926,15 @@
       <c r="A85" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="15"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="15"/>
-      <c r="H85" s="15"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4979,14 +5030,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>

</xml_diff>

<commit_message>
[20230905] Leetcode - Blind 75 (20-22)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEF8D65-D966-9649-AEA2-1B997C4D3591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD369399-F63E-1D4E-BE45-B47B167D00A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="346">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1230,6 +1230,30 @@
   </si>
   <si>
     <t>Counter and return 1/2 nums</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-binary/</t>
+  </si>
+  <si>
+    <t>2023.09.05</t>
+  </si>
+  <si>
+    <t>int + bin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/diameter-of-binary-tree/solutions/</t>
+  </si>
+  <si>
+    <t>DFS to find most far distance, but save the dis from one side</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/middle-of-the-linked-list/</t>
+  </si>
+  <si>
+    <t>two ptr, one step and two steps</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3204,8 +3228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3217,7 +3241,7 @@
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="55" customWidth="1"/>
-    <col min="8" max="8" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -3861,6 +3885,9 @@
         <v>20</v>
       </c>
       <c r="B22" s="17"/>
+      <c r="C22" s="2">
+        <v>67</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>118</v>
       </c>
@@ -3870,15 +3897,27 @@
       <c r="F22" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="G22" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>340</v>
+      </c>
       <c r="K22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" ht="16">
       <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" s="17"/>
+      <c r="C23" s="2">
+        <v>543</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>112</v>
       </c>
@@ -3888,15 +3927,27 @@
       <c r="F23" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="G23" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>340</v>
+      </c>
       <c r="K23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" ht="16">
       <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24" s="17"/>
+      <c r="C24" s="2">
+        <v>876</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>110</v>
       </c>
@@ -3905,6 +3956,15 @@
       </c>
       <c r="F24" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>340</v>
       </c>
       <c r="K24" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
[20230906] Leetcode - Blind 75 (23-25)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD369399-F63E-1D4E-BE45-B47B167D00A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0270A5F2-7685-6048-AB47-B87354520CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="351">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1254,6 +1254,24 @@
   </si>
   <si>
     <t>two ptr, one step and two steps</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>2023.09.06</t>
+  </si>
+  <si>
+    <t>recurision; loop with deque, append all node</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop or sort</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>use sum_val to find all subarray, max_val to get max subarray</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1800,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3970,11 +3988,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" ht="16">
       <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" s="17"/>
+      <c r="C25" s="2">
+        <v>104</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>112</v>
       </c>
@@ -3983,6 +4004,15 @@
       </c>
       <c r="F25" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="K25" t="s">
         <v>24</v>
@@ -3993,6 +4023,9 @@
         <v>24</v>
       </c>
       <c r="B26" s="17"/>
+      <c r="C26" s="2">
+        <v>217</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>117</v>
       </c>
@@ -4004,6 +4037,12 @@
       </c>
       <c r="G26" s="6" t="s">
         <v>97</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="K26" t="s">
         <v>24</v>
@@ -4014,6 +4053,9 @@
         <v>25</v>
       </c>
       <c r="B27" s="17"/>
+      <c r="C27" s="2">
+        <v>53</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>116</v>
       </c>
@@ -4025,6 +4067,12 @@
       </c>
       <c r="G27" s="6" t="s">
         <v>99</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="K27" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
[20230907] Leetcode - Blind 75 (26-27)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0270A5F2-7685-6048-AB47-B87354520CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C17B110-4202-304D-8C08-7D187FC7F5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="356">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1272,6 +1272,23 @@
   </si>
   <si>
     <t>use sum_val to find all subarray, max_val to get max subarray</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-interval/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/01-matrix/</t>
+  </si>
+  <si>
+    <t>2023.09.07</t>
+  </si>
+  <si>
+    <t>check newList on left and right first, and compare min/max</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BFS or DP with deque, ini que, BFS Traversal four direct</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3247,7 +3264,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4085,6 +4102,9 @@
       <c r="B28" s="18">
         <v>3</v>
       </c>
+      <c r="C28" s="2">
+        <v>57</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>117</v>
       </c>
@@ -4093,6 +4113,15 @@
       </c>
       <c r="F28" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>353</v>
       </c>
       <c r="K28" t="s">
         <v>90</v>
@@ -4103,6 +4132,9 @@
         <v>27</v>
       </c>
       <c r="B29" s="18"/>
+      <c r="C29" s="2">
+        <v>542</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>113</v>
       </c>
@@ -4111,6 +4143,15 @@
       </c>
       <c r="F29" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>353</v>
       </c>
       <c r="K29" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
[20230908] Leetcode - Blind 75 (28-29)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C17B110-4202-304D-8C08-7D187FC7F5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A12BC4-7264-4F42-9739-9C4709F67B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="top-interview-questions-easy" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="361">
   <si>
     <t xml:space="preserve">
 </t>
@@ -371,924 +371,944 @@
     <t>https://leetcode.com/problems/search-in-rotated-sorted-array/</t>
   </si>
   <si>
+    <t>https://leetcode.com/problems/container-with-most-water/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer: </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.techinterviewhandbook.org/grind75</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Binary Tree</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Hash Table</t>
+  </si>
+  <si>
+    <t>Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Trie</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/727/</t>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Listed List</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tree</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sorting and Searching</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamic Programming</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Math</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Others</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/564/</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.09</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>differency</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>count</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rotate Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>move</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contains Duplicate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Single Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/646/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/578/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/549/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>set</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intersection of Two Arrays II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/674/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list or str-int</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter or two ptr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.11</t>
+  </si>
+  <si>
+    <t>Plus One</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/559/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move Zeroes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/567/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ptr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.12</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/546/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/769/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>triple with set</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rotate Image</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/770/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>col &amp; row change with reverse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.13</t>
+  </si>
+  <si>
+    <t>reverse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>border for origin/after</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reverse String</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/879/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reverse Integer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/880/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>First Unique Character in a String</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/881/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter or sorted</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.14</t>
+  </si>
+  <si>
+    <t>two ptr or [::-1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/882/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/883/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>String to Integer (atoi)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/884/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>edge case no thinking</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>find()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.15</t>
+  </si>
+  <si>
+    <t>min</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement strStr()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/885/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Longest Common Prefix</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/887/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Node in a Linked List</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/553/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>no need to access head</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two ptr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.16</t>
+  </si>
+  <si>
+    <t>pre and current to redirect</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove Nth Node From End of List</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/603/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/560/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/771/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_list and compare</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LC Num</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.17</t>
+  </si>
+  <si>
+    <t>list with [::-1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>  Palindrome Linked List</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/772/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/773/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/555/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>recurision: none/left/right/return.  Loop: dequeue and pop all</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.20</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS or Loop with Stack/List</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Validate Binary Search Tree</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/625/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS with Recursion or BFS with Loop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.21</t>
+  </si>
+  <si>
+    <t>def Mirror with left &lt;-&gt; right side</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/627/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/631/</t>
+  </si>
+  <si>
+    <t>Convert Sorted Array to Binary Search Tree</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/628/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>recurision with mid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/96/sorting-and-searching/587/</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>merge with sort or m+n-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/96/sorting-and-searching/774/</t>
+  </si>
+  <si>
+    <t>2023.08.22</t>
+  </si>
+  <si>
+    <t>binary search</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/569/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/572/</t>
+  </si>
+  <si>
+    <t>step1=step2, step2+=step1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>First Bad Version</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>save max and min value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/566/</t>
+  </si>
+  <si>
+    <t>2023.08.23</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/576/</t>
+  </si>
+  <si>
+    <t>House Robber</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>devide and conquer (use check now and +next)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>save all step value, last and now to statistic</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/98/design/670/</t>
+  </si>
+  <si>
+    <t>Shuffle an Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.24</t>
+  </si>
+  <si>
+    <t>random.shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/98/design/562/</t>
+  </si>
+  <si>
+    <t>two list which one of use to save min value sequence</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min Stack</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/743/</t>
+  </si>
+  <si>
+    <t>Fizz Buzz</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>if else</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.25</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/744/</t>
+  </si>
+  <si>
+    <t>Count Primes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>use "Sieve of Eeatosthese" method: set True for all num(with it's times) before n^0.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/745/</t>
+  </si>
+  <si>
+    <t>while to reach out</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power of Three</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/roman-to-integer/</t>
+  </si>
+  <si>
+    <t>2023.08.26</t>
+  </si>
+  <si>
+    <t>if i &lt; i+1, value-=i</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/565/</t>
+  </si>
+  <si>
+    <t>check last bit and sum all 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Roman to Integer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of 1 Bits</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/762/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hamming Distance</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin() with count('1')</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.27</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/648/</t>
+  </si>
+  <si>
+    <t>bin() with int(x, 2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/601/</t>
+  </si>
+  <si>
+    <t>Reverse Bits</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pascal's Triangle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/721/</t>
+  </si>
+  <si>
+    <t>2023.08.28</t>
+  </si>
+  <si>
+    <t>add 0 to first and last, then run all</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/722/</t>
+  </si>
+  <si>
+    <t>Missing Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack and return len(stack) == 0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>math and find one</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-parentheses/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
+  </si>
+  <si>
+    <t>2023.08.29</t>
+  </si>
+  <si>
+    <t>hash with (target - num)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack and check last one</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_list &amp; ptr and compare l1, l2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.30</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/invert-binary-tree/</t>
+  </si>
+  <si>
+    <t>dp[] and compare max &amp; min</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list == list[::-1] or two pointer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>if root, exchange sub</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.08.31</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-anagram/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-search/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flood-fill/</t>
+  </si>
+  <si>
+    <t>Counter faster than sorted</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>left = mid + 1; right = mid - 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new fill to extend four direction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>BST: left smaller, right higher, find mid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/balanced-binary-tree/</t>
+  </si>
+  <si>
+    <t>check left, right subtree, if no balanced, False</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-queue-using-stacks/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/first-bad-version/</t>
+  </si>
+  <si>
+    <t>2023.09.02</t>
+  </si>
+  <si>
+    <t>two ptr with one step and two step, or, id with table</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two stack, first for input and second for out</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>peek()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS, right = mid, left = mid + 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.03</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ransom-note/</t>
+  </si>
+  <si>
+    <t>two Counter and &amp; is smaller one</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t>DP, cur_step = cur + last</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-palindrome/</t>
+  </si>
+  <si>
+    <t>2023.09.04</t>
+  </si>
+  <si>
+    <t>count = 2*(char shows twice) + 1 (char shows once)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/</t>
+  </si>
+  <si>
+    <t>pre, cur, cur.next = pre.next , pre, cur</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/</t>
+  </si>
+  <si>
+    <t>Counter and return 1/2 nums</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-binary/</t>
+  </si>
+  <si>
+    <t>2023.09.05</t>
+  </si>
+  <si>
+    <t>int + bin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/diameter-of-binary-tree/solutions/</t>
+  </si>
+  <si>
+    <t>DFS to find most far distance, but save the dis from one side</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/middle-of-the-linked-list/</t>
+  </si>
+  <si>
+    <t>two ptr, one step and two steps</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>2023.09.06</t>
+  </si>
+  <si>
+    <t>recurision; loop with deque, append all node</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop or sort</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>use sum_val to find all subarray, max_val to get max subarray</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-interval/</t>
+  </si>
+  <si>
+    <t>2023.09.07</t>
+  </si>
+  <si>
+    <t>check newList on left and right first, and compare min/max</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BFS or DP with deque, ini que, BFS Traversal four direct</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.08</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/01-matrix/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/k-closest-points-to-origin/</t>
+  </si>
+  <si>
     <t>https://leetcode.com/problems/3sum/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/container-with-most-water/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refer: </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.techinterviewhandbook.org/grind75</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stack</t>
-  </si>
-  <si>
-    <t>Linked List</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Binary Tree</t>
-  </si>
-  <si>
-    <t>Graph</t>
-  </si>
-  <si>
-    <t>Binary Search Tree</t>
-  </si>
-  <si>
-    <t>Hash Table</t>
-  </si>
-  <si>
-    <t>Dynamic Programming</t>
-  </si>
-  <si>
-    <t>Array</t>
-  </si>
-  <si>
-    <t>Binary</t>
-  </si>
-  <si>
-    <t>Heap</t>
-  </si>
-  <si>
-    <t>Trie</t>
-  </si>
-  <si>
-    <t>Recursion</t>
-  </si>
-  <si>
-    <t>Matrix</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remove Duplicates from Sorted Array</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/727/</t>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Listed List</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tree</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sorting and Searching</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dynamic Programming</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Design</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Math</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Others</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/564/</t>
-  </si>
-  <si>
-    <t>Best Time to Buy and Sell Stock II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.09</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>differency</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>count</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rotate Array</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.10</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>move</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contains Duplicate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Single Number</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>hash</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/646/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/578/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/549/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>set</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intersection of Two Arrays II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/674/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>list or str-int</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Counter or two ptr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.11</t>
-  </si>
-  <si>
-    <t>Plus One</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/559/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Move Zeroes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/567/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ptr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.12</t>
-  </si>
-  <si>
-    <t>Two Sum</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/546/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valid Sudoku</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/769/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>triple with set</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rotate Image</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/770/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>col &amp; row change with reverse</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.13</t>
-  </si>
-  <si>
-    <t>reverse</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>border for origin/after</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reverse String</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/879/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reverse Integer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/880/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>First Unique Character in a String</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/881/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Counter</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Counter or sorted</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.14</t>
-  </si>
-  <si>
-    <t>two ptr or [::-1]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valid Anagram</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/882/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valid Palindrome</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/883/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>String to Integer (atoi)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/884/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>edge case no thinking</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>find()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.15</t>
-  </si>
-  <si>
-    <t>min</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Implement strStr()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/885/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Longest Common Prefix</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/887/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Delete Node in a Linked List</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/553/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>no need to access head</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>two ptr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.16</t>
-  </si>
-  <si>
-    <t>pre and current to redirect</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remove Nth Node From End of List</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/603/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reverse Linked List</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/560/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Merge Two Sorted Lists</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/771/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>new_list and compare</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LC Num</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.17</t>
-  </si>
-  <si>
-    <t>list with [::-1]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>  Palindrome Linked List</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/772/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Linked List Cycle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/93/linked-list/773/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maximum Depth of Binary Tree</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/555/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>recurision: none/left/right/return.  Loop: dequeue and pop all</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.20</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DFS or Loop with Stack/List</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Validate Binary Search Tree</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/625/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Binary Tree Level Order Traversal</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DFS with Recursion or BFS with Loop</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Symmetric Tree</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.21</t>
-  </si>
-  <si>
-    <t>def Mirror with left &lt;-&gt; right side</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/627/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/631/</t>
-  </si>
-  <si>
-    <t>Convert Sorted Array to Binary Search Tree</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/94/trees/628/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>recurision with mid</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/96/sorting-and-searching/587/</t>
-  </si>
-  <si>
-    <t>Merge Sorted Array</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>merge with sort or m+n-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/96/sorting-and-searching/774/</t>
-  </si>
-  <si>
-    <t>2023.08.22</t>
-  </si>
-  <si>
-    <t>binary search</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/569/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/572/</t>
-  </si>
-  <si>
-    <t>step1=step2, step2+=step1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>First Bad Version</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Climbing Stairs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Best Time to Buy and Sell Stock</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>save max and min value</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/566/</t>
-  </si>
-  <si>
-    <t>2023.08.23</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/97/dynamic-programming/576/</t>
-  </si>
-  <si>
-    <t>House Robber</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Maximum Subarray</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>devide and conquer (use check now and +next)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>save all step value, last and now to statistic</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/98/design/670/</t>
-  </si>
-  <si>
-    <t>Shuffle an Array</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.24</t>
-  </si>
-  <si>
-    <t>random.shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/98/design/562/</t>
-  </si>
-  <si>
-    <t>two list which one of use to save min value sequence</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Min Stack</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/743/</t>
-  </si>
-  <si>
-    <t>Fizz Buzz</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>if else</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.25</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/744/</t>
-  </si>
-  <si>
-    <t>Count Primes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>use "Sieve of Eeatosthese" method: set True for all num(with it's times) before n^0.5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/102/math/745/</t>
-  </si>
-  <si>
-    <t>while to reach out</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Power of Three</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/roman-to-integer/</t>
-  </si>
-  <si>
-    <t>2023.08.26</t>
-  </si>
-  <si>
-    <t>if i &lt; i+1, value-=i</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/565/</t>
-  </si>
-  <si>
-    <t>check last bit and sum all 1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Roman to Integer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of 1 Bits</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/762/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hamming Distance</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin() with count('1')</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.27</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/648/</t>
-  </si>
-  <si>
-    <t>bin() with int(x, 2)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/601/</t>
-  </si>
-  <si>
-    <t>Reverse Bits</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pascal's Triangle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/721/</t>
-  </si>
-  <si>
-    <t>2023.08.28</t>
-  </si>
-  <si>
-    <t>add 0 to first and last, then run all</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/99/others/722/</t>
-  </si>
-  <si>
-    <t>Missing Number</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stack and return len(stack) == 0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valid Parentheses</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>math and find one</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/valid-parentheses/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
-  </si>
-  <si>
-    <t>2023.08.29</t>
-  </si>
-  <si>
-    <t>hash with (target - num)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stack and check last one</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>new_list &amp; ptr and compare l1, l2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.30</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/valid-palindrome/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/invert-binary-tree/</t>
-  </si>
-  <si>
-    <t>dp[] and compare max &amp; min</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>list == list[::-1] or two pointer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>if root, exchange sub</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.08.31</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/valid-anagram/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/binary-search/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/flood-fill/</t>
-  </si>
-  <si>
-    <t>Counter faster than sorted</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>left = mid + 1; right = mid - 1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>new fill to extend four direction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/</t>
-  </si>
-  <si>
-    <t>BST: left smaller, right higher, find mid</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.09.01</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Balanced Binary Tree</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/balanced-binary-tree/</t>
-  </si>
-  <si>
-    <t>check left, right subtree, if no balanced, False</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/linked-list-cycle/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/implement-queue-using-stacks/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/first-bad-version/</t>
-  </si>
-  <si>
-    <t>2023.09.02</t>
-  </si>
-  <si>
-    <t>two ptr with one step and two step, or, id with table</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>two stack, first for input and second for out</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>peek()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>BS, right = mid, left = mid + 1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.09.03</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/ransom-note/</t>
-  </si>
-  <si>
-    <t>two Counter and &amp; is smaller one</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/climbing-stairs/</t>
-  </si>
-  <si>
-    <t>DP, cur_step = cur + last</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/longest-palindrome/</t>
-  </si>
-  <si>
-    <t>2023.09.04</t>
-  </si>
-  <si>
-    <t>count = 2*(char shows twice) + 1 (char shows once)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/reverse-linked-list/</t>
-  </si>
-  <si>
-    <t>pre, cur, cur.next = pre.next , pre, cur</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/majority-element/</t>
-  </si>
-  <si>
-    <t>Counter and return 1/2 nums</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/add-binary/</t>
-  </si>
-  <si>
-    <t>2023.09.05</t>
-  </si>
-  <si>
-    <t>int + bin</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/diameter-of-binary-tree/solutions/</t>
-  </si>
-  <si>
-    <t>DFS to find most far distance, but save the dis from one side</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/middle-of-the-linked-list/</t>
-  </si>
-  <si>
-    <t>two ptr, one step and two steps</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/</t>
-  </si>
-  <si>
-    <t>2023.09.06</t>
-  </si>
-  <si>
-    <t>recurision; loop with deque, append all node</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>loop or sort</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>use sum_val to find all subarray, max_val to get max subarray</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/insert-interval/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/01-matrix/</t>
-  </si>
-  <si>
-    <t>2023.09.07</t>
-  </si>
-  <si>
-    <t>check newList on left and right first, and compare min/max</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>BFS or DP with deque, ini que, BFS Traversal four direct</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>math with sort; use heapq with heappop and heappushpop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>set or dict with start/end point calcul</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1851,7 +1871,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1864,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>
@@ -1900,22 +1920,22 @@
         <v>26</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>125</v>
-      </c>
       <c r="G3" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
@@ -1937,16 +1957,16 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1963,16 +1983,16 @@
         <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1987,16 +2007,16 @@
         <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2011,16 +2031,16 @@
         <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2035,16 +2055,16 @@
         <v>21</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>150</v>
-      </c>
       <c r="G8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2059,16 +2079,16 @@
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2083,16 +2103,16 @@
         <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2107,16 +2127,16 @@
         <v>21</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2131,16 +2151,16 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2155,16 +2175,16 @@
         <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2175,22 +2195,22 @@
         <v>344</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>172</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2205,16 +2225,16 @@
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>174</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2229,16 +2249,16 @@
         <v>21</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="H16" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2253,16 +2273,16 @@
         <v>21</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>182</v>
-      </c>
       <c r="G17" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2277,16 +2297,16 @@
         <v>21</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>184</v>
-      </c>
       <c r="G18" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2301,16 +2321,16 @@
         <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="G19" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="H19" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2325,16 +2345,16 @@
         <v>21</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="G20" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2349,16 +2369,16 @@
         <v>21</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>194</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2369,22 +2389,22 @@
         <v>237</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="G22" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="H22" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2399,16 +2419,16 @@
         <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>202</v>
-      </c>
       <c r="G23" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2423,16 +2443,16 @@
         <v>21</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>204</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2447,16 +2467,16 @@
         <v>21</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="G25" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="H25" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2471,16 +2491,16 @@
         <v>21</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>212</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2495,16 +2515,16 @@
         <v>21</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>214</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2515,22 +2535,22 @@
         <v>104</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="G28" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="H28" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2545,16 +2565,16 @@
         <v>38</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>221</v>
-      </c>
       <c r="G29" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2569,16 +2589,16 @@
         <v>21</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2593,16 +2613,16 @@
         <v>38</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="H31" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2617,16 +2637,16 @@
         <v>21</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2637,22 +2657,22 @@
         <v>88</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="H33" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2667,16 +2687,16 @@
         <v>21</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2687,22 +2707,22 @@
         <v>70</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2717,16 +2737,16 @@
         <v>21</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2741,16 +2761,16 @@
         <v>38</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="H37" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2765,16 +2785,16 @@
         <v>38</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2785,22 +2805,22 @@
         <v>384</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2815,16 +2835,16 @@
         <v>38</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F40" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="H40" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2835,22 +2855,22 @@
         <v>412</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="H41" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2865,16 +2885,16 @@
         <v>38</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>265</v>
-      </c>
       <c r="H42" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2889,16 +2909,16 @@
         <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F43" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>267</v>
-      </c>
       <c r="H43" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2913,16 +2933,16 @@
         <v>21</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F44" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2933,22 +2953,22 @@
         <v>191</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F45" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="H45" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2963,16 +2983,16 @@
         <v>21</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2987,16 +3007,16 @@
         <v>21</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F47" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="H47" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3011,16 +3031,16 @@
         <v>21</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3035,16 +3055,16 @@
         <v>21</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F49" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3059,16 +3079,16 @@
         <v>21</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3263,8 +3283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3275,7 +3295,7 @@
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55" customWidth="1"/>
+    <col min="7" max="7" width="69.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
@@ -3284,7 +3304,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -3325,7 +3345,7 @@
         <v>7</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>8</v>
@@ -3342,22 +3362,22 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>95</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>0</v>
@@ -3378,22 +3398,22 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
@@ -3409,22 +3429,22 @@
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="K5" t="s">
         <v>22</v>
@@ -3439,7 +3459,7 @@
         <v>121</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>21</v>
@@ -3451,10 +3471,10 @@
         <v>96</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K6" t="s">
         <v>22</v>
@@ -3469,7 +3489,7 @@
         <v>125</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>21</v>
@@ -3478,13 +3498,13 @@
         <v>13</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K7" t="s">
         <v>23</v>
@@ -3499,7 +3519,7 @@
         <v>226</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>21</v>
@@ -3508,13 +3528,13 @@
         <v>14</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K8" t="s">
         <v>23</v>
@@ -3529,7 +3549,7 @@
         <v>242</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>21</v>
@@ -3538,13 +3558,13 @@
         <v>15</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K9" t="s">
         <v>24</v>
@@ -3568,13 +3588,13 @@
         <v>16</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K10" t="s">
         <v>24</v>
@@ -3589,7 +3609,7 @@
         <v>733</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>21</v>
@@ -3598,13 +3618,13 @@
         <v>17</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K11" t="s">
         <v>22</v>
@@ -3619,7 +3639,7 @@
         <v>235</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>38</v>
@@ -3628,13 +3648,13 @@
         <v>18</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>314</v>
       </c>
       <c r="K12" t="s">
         <v>22</v>
@@ -3649,22 +3669,22 @@
         <v>110</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>317</v>
-      </c>
       <c r="I13" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K13" t="s">
         <v>24</v>
@@ -3679,7 +3699,7 @@
         <v>141</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>21</v>
@@ -3688,13 +3708,13 @@
         <v>19</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K14" t="s">
         <v>22</v>
@@ -3709,7 +3729,7 @@
         <v>232</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>21</v>
@@ -3718,19 +3738,19 @@
         <v>20</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K15" t="s">
         <v>22</v>
       </c>
       <c r="L15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3753,13 +3773,13 @@
         <v>25</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="K16" t="s">
         <v>22</v>
@@ -3774,7 +3794,7 @@
         <v>383</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>21</v>
@@ -3783,13 +3803,13 @@
         <v>26</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="I17" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K17" t="s">
         <v>24</v>
@@ -3804,7 +3824,7 @@
         <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>21</v>
@@ -3813,13 +3833,13 @@
         <v>27</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="I18" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K18" t="s">
         <v>22</v>
@@ -3834,7 +3854,7 @@
         <v>409</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>21</v>
@@ -3843,13 +3863,13 @@
         <v>28</v>
       </c>
       <c r="G19" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="K19" t="s">
         <v>22</v>
@@ -3864,7 +3884,7 @@
         <v>206</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>21</v>
@@ -3873,13 +3893,13 @@
         <v>29</v>
       </c>
       <c r="G20" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="I20" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K20" t="s">
         <v>22</v>
@@ -3894,7 +3914,7 @@
         <v>169</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>21</v>
@@ -3903,13 +3923,13 @@
         <v>30</v>
       </c>
       <c r="G21" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>338</v>
-      </c>
       <c r="I21" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K21" t="s">
         <v>22</v>
@@ -3924,7 +3944,7 @@
         <v>67</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>21</v>
@@ -3933,13 +3953,13 @@
         <v>31</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>340</v>
       </c>
       <c r="K22" t="s">
         <v>24</v>
@@ -3954,7 +3974,7 @@
         <v>543</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
@@ -3963,13 +3983,13 @@
         <v>32</v>
       </c>
       <c r="G23" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="I23" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K23" t="s">
         <v>89</v>
@@ -3984,7 +4004,7 @@
         <v>876</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>21</v>
@@ -3993,13 +4013,13 @@
         <v>33</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>345</v>
-      </c>
       <c r="I24" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K24" t="s">
         <v>22</v>
@@ -4014,7 +4034,7 @@
         <v>104</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>21</v>
@@ -4023,13 +4043,13 @@
         <v>34</v>
       </c>
       <c r="G25" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="K25" t="s">
         <v>24</v>
@@ -4044,7 +4064,7 @@
         <v>217</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>21</v>
@@ -4056,10 +4076,10 @@
         <v>97</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K26" t="s">
         <v>24</v>
@@ -4074,7 +4094,7 @@
         <v>53</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>38</v>
@@ -4086,10 +4106,10 @@
         <v>99</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K27" t="s">
         <v>22</v>
@@ -4106,7 +4126,7 @@
         <v>57</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>38</v>
@@ -4115,13 +4135,13 @@
         <v>37</v>
       </c>
       <c r="G28" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="K28" t="s">
         <v>90</v>
@@ -4136,7 +4156,7 @@
         <v>542</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>38</v>
@@ -4145,13 +4165,13 @@
         <v>39</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K29" t="s">
         <v>89</v>
@@ -4162,14 +4182,26 @@
         <v>28</v>
       </c>
       <c r="B30" s="18"/>
+      <c r="C30" s="2">
+        <v>973</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="K30" t="s">
         <v>89</v>
@@ -4180,14 +4212,26 @@
         <v>29</v>
       </c>
       <c r="B31" s="18"/>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
       <c r="D31" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="K31" t="s">
         <v>89</v>
@@ -4199,7 +4243,7 @@
       </c>
       <c r="B32" s="18"/>
       <c r="D32" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>38</v>
@@ -4208,7 +4252,7 @@
         <v>42</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>105</v>
+        <v>357</v>
       </c>
       <c r="K32" t="s">
         <v>89</v>
@@ -4220,7 +4264,7 @@
       </c>
       <c r="B33" s="18"/>
       <c r="D33" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>38</v>
@@ -4238,7 +4282,7 @@
       </c>
       <c r="B34" s="18"/>
       <c r="D34" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>38</v>
@@ -4256,7 +4300,7 @@
       </c>
       <c r="B35" s="18"/>
       <c r="D35" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>38</v>
@@ -4276,7 +4320,7 @@
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>38</v>
@@ -4294,7 +4338,7 @@
       </c>
       <c r="B37" s="19"/>
       <c r="D37" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>38</v>
@@ -4312,7 +4356,7 @@
       </c>
       <c r="B38" s="19"/>
       <c r="D38" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>38</v>
@@ -4330,7 +4374,7 @@
       </c>
       <c r="B39" s="19"/>
       <c r="D39" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>38</v>
@@ -4351,7 +4395,7 @@
       </c>
       <c r="B40" s="19"/>
       <c r="D40" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>38</v>
@@ -4369,7 +4413,7 @@
       </c>
       <c r="B41" s="19"/>
       <c r="D41" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
@@ -4387,7 +4431,7 @@
       </c>
       <c r="B42" s="19"/>
       <c r="D42" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>38</v>
@@ -4405,7 +4449,7 @@
       </c>
       <c r="B43" s="19"/>
       <c r="D43" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>38</v>
@@ -4446,7 +4490,7 @@
       </c>
       <c r="B45" s="20"/>
       <c r="D45" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>38</v>
@@ -4464,7 +4508,7 @@
       </c>
       <c r="B46" s="20"/>
       <c r="D46" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>38</v>
@@ -4482,7 +4526,7 @@
       </c>
       <c r="B47" s="20"/>
       <c r="D47" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>38</v>
@@ -4500,7 +4544,7 @@
       </c>
       <c r="B48" s="20"/>
       <c r="D48" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>38</v>
@@ -4536,7 +4580,7 @@
       </c>
       <c r="B50" s="20"/>
       <c r="D50" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>38</v>
@@ -4554,7 +4598,7 @@
       </c>
       <c r="B51" s="20"/>
       <c r="D51" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>38</v>
@@ -4574,7 +4618,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>38</v>
@@ -4592,7 +4636,7 @@
       </c>
       <c r="B53" s="21"/>
       <c r="D53" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>38</v>
@@ -4610,7 +4654,7 @@
       </c>
       <c r="B54" s="21"/>
       <c r="D54" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>38</v>
@@ -4628,7 +4672,7 @@
       </c>
       <c r="B55" s="21"/>
       <c r="D55" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>38</v>
@@ -4646,7 +4690,7 @@
       </c>
       <c r="B56" s="21"/>
       <c r="D56" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>38</v>
@@ -4664,7 +4708,7 @@
       </c>
       <c r="B57" s="21"/>
       <c r="D57" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>38</v>
@@ -4682,7 +4726,7 @@
       </c>
       <c r="B58" s="21"/>
       <c r="D58" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>38</v>
@@ -4700,7 +4744,7 @@
       </c>
       <c r="B59" s="21"/>
       <c r="D59" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>38</v>
@@ -4718,7 +4762,7 @@
       </c>
       <c r="B60" s="21"/>
       <c r="D60" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>38</v>
@@ -4738,7 +4782,7 @@
         <v>7</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>38</v>
@@ -4747,7 +4791,7 @@
         <v>71</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K61" t="s">
         <v>91</v>
@@ -4759,7 +4803,7 @@
       </c>
       <c r="B62" s="14"/>
       <c r="D62" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>38</v>
@@ -4777,7 +4821,7 @@
       </c>
       <c r="B63" s="14"/>
       <c r="D63" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>38</v>
@@ -4795,7 +4839,7 @@
       </c>
       <c r="B64" s="14"/>
       <c r="D64" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>38</v>
@@ -4813,7 +4857,7 @@
       </c>
       <c r="B65" s="14"/>
       <c r="D65" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>38</v>
@@ -4831,7 +4875,7 @@
       </c>
       <c r="B66" s="14"/>
       <c r="D66" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>38</v>
@@ -4849,7 +4893,7 @@
       </c>
       <c r="B67" s="14"/>
       <c r="D67" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>38</v>
@@ -4869,7 +4913,7 @@
         <v>8</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>38</v>
@@ -4887,7 +4931,7 @@
       </c>
       <c r="B69" s="15"/>
       <c r="D69" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>88</v>
@@ -4905,7 +4949,7 @@
       </c>
       <c r="B70" s="15"/>
       <c r="D70" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>88</v>
@@ -4923,7 +4967,7 @@
       </c>
       <c r="B71" s="15"/>
       <c r="D71" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>88</v>
@@ -4941,7 +4985,7 @@
       </c>
       <c r="B72" s="15"/>
       <c r="D72" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>88</v>
@@ -4959,7 +5003,7 @@
       </c>
       <c r="B73" s="15"/>
       <c r="D73" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>88</v>
@@ -4977,7 +5021,7 @@
       </c>
       <c r="B74" s="15"/>
       <c r="D74" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>88</v>
@@ -5013,7 +5057,7 @@
       </c>
       <c r="B76" s="15"/>
       <c r="D76" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>88</v>
@@ -5031,7 +5075,7 @@
       </c>
       <c r="B77" s="15"/>
       <c r="D77" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>88</v>
@@ -5073,7 +5117,7 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B85" s="16" t="s">
         <v>94</v>
@@ -5155,9 +5199,10 @@
     <hyperlink ref="G32" r:id="rId53" xr:uid="{CA8DA924-CE20-40EC-85EC-5844F4DD1F5B}"/>
     <hyperlink ref="G61" r:id="rId54" xr:uid="{75FBD306-6E88-4541-8B52-48157A1D46CA}"/>
     <hyperlink ref="A1" r:id="rId55" xr:uid="{66549CE5-88E8-426D-9FB5-F1976BC0AFDA}"/>
+    <hyperlink ref="G29" r:id="rId56" xr:uid="{16782551-B1ED-A343-A5C0-BA361524E57A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 
@@ -5180,7 +5225,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5195,7 +5240,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
[20230909] Leetcode - Blind 75 (30-31)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A12BC4-7264-4F42-9739-9C4709F67B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF594C5-5BF5-8045-B8E1-B244C9FFDA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="top-interview-questions-easy" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="365">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1309,6 +1309,21 @@
   </si>
   <si>
     <t>set or dict with start/end point calcul</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.09</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BFS with [root] or DFS with level num</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>check step by step: all zero, one zero with +-num, two p/n with one p/n</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3296,7 +3311,7 @@
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -4238,10 +4253,13 @@
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="2">
+      <c r="A32" s="9">
         <v>30</v>
       </c>
       <c r="B32" s="18"/>
+      <c r="C32" s="2">
+        <v>15</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>116</v>
       </c>
@@ -4253,6 +4271,12 @@
       </c>
       <c r="G32" s="6" t="s">
         <v>357</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>361</v>
       </c>
       <c r="K32" t="s">
         <v>89</v>
@@ -4263,6 +4287,9 @@
         <v>31</v>
       </c>
       <c r="B33" s="18"/>
+      <c r="C33" s="2">
+        <v>102</v>
+      </c>
       <c r="D33" s="2" t="s">
         <v>111</v>
       </c>
@@ -4271,6 +4298,15 @@
       </c>
       <c r="F33" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>361</v>
       </c>
       <c r="K33" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
[20230910] Leetcode - Blind 75 (32-33)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF594C5-5BF5-8045-B8E1-B244C9FFDA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E93E1C-C801-7A4D-BE1A-F23976B8CE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -26,12 +26,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="371">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1324,6 +1334,29 @@
   </si>
   <si>
     <t>check step by step: all zero, one zero with +-num, two p/n with one p/n</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.10</t>
+  </si>
+  <si>
+    <t>BFS  with neibors</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Graph questions!!</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/clone-graph/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack with "+-*/" and need /: int(a/b)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3315,6 +3348,7 @@
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4282,7 +4316,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -4312,11 +4346,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="2">
+    <row r="34" spans="1:12">
+      <c r="A34" s="9">
         <v>32</v>
       </c>
       <c r="B34" s="18"/>
+      <c r="C34" s="2">
+        <v>133</v>
+      </c>
       <c r="D34" s="2" t="s">
         <v>112</v>
       </c>
@@ -4326,15 +4363,30 @@
       <c r="F34" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="G34" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="K34" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="2">
         <v>33</v>
       </c>
       <c r="B35" s="18"/>
+      <c r="C35" s="2">
+        <v>150</v>
+      </c>
       <c r="D35" s="2" t="s">
         <v>108</v>
       </c>
@@ -4344,11 +4396,20 @@
       <c r="F35" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="G35" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="K35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:12">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -4364,11 +4425,12 @@
       <c r="F36" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="G36" s="6"/>
       <c r="K36" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:12">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -4386,7 +4448,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -4404,7 +4466,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -4425,7 +4487,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:12">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -4443,7 +4505,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:12">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -4461,7 +4523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:12">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -4479,7 +4541,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:12">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -4497,7 +4559,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:12">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -4520,7 +4582,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:12">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -4538,7 +4600,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:12">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -4556,7 +4618,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:12">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -4574,7 +4636,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:12">
       <c r="A48" s="2">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
[20230911] Leetcode - Blind 75 (34-35)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E93E1C-C801-7A4D-BE1A-F23976B8CE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770729A7-4210-F547-9D74-23DEFA9E58D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="377">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1357,6 +1357,27 @@
   </si>
   <si>
     <t>stack with "+-*/" and need /: int(a/b)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.11</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t>DFS or deque; count how many time for course be used, record each preq; pop final</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BFS with Kahn's algorithm for Topological Sorting</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>each char of word link by dict, check each char from the word</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3331,8 +3352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3344,7 +3365,7 @@
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -4410,12 +4431,15 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="2">
+      <c r="A36" s="9">
         <v>34</v>
       </c>
       <c r="B36" s="19">
         <v>4</v>
       </c>
+      <c r="C36" s="2">
+        <v>207</v>
+      </c>
       <c r="D36" s="2" t="s">
         <v>112</v>
       </c>
@@ -4425,9 +4449,20 @@
       <c r="F36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G36" s="6"/>
+      <c r="G36" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>371</v>
+      </c>
       <c r="K36" t="s">
         <v>89</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -4435,6 +4470,9 @@
         <v>35</v>
       </c>
       <c r="B37" s="19"/>
+      <c r="C37" s="2">
+        <v>208</v>
+      </c>
       <c r="D37" s="2" t="s">
         <v>119</v>
       </c>
@@ -4443,6 +4481,15 @@
       </c>
       <c r="F37" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="K37" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
[20230912] Leetcode - Blind 75 (36-37)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770729A7-4210-F547-9D74-23DEFA9E58D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12194E40-811A-A040-B445-B066C44D7C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="381">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1378,6 +1378,21 @@
   </si>
   <si>
     <t>each char of word link by dict, check each char from the word</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.12</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/coin-change/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP to calculate each num that need how many coins (min(cur, curNum-coin+1))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>use pre, post to do left then do right</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3352,8 +3367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3369,7 +3384,7 @@
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4500,6 +4515,9 @@
         <v>36</v>
       </c>
       <c r="B38" s="19"/>
+      <c r="C38" s="2">
+        <v>322</v>
+      </c>
       <c r="D38" s="2" t="s">
         <v>115</v>
       </c>
@@ -4508,6 +4526,15 @@
       </c>
       <c r="F38" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="K38" t="s">
         <v>90</v>
@@ -4518,6 +4545,9 @@
         <v>37</v>
       </c>
       <c r="B39" s="19"/>
+      <c r="C39" s="2">
+        <v>238</v>
+      </c>
       <c r="D39" s="2" t="s">
         <v>116</v>
       </c>
@@ -4529,6 +4559,12 @@
       </c>
       <c r="G39" s="6" t="s">
         <v>98</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="K39" t="s">
         <v>89</v>
@@ -5345,9 +5381,10 @@
     <hyperlink ref="G61" r:id="rId54" xr:uid="{75FBD306-6E88-4541-8B52-48157A1D46CA}"/>
     <hyperlink ref="A1" r:id="rId55" xr:uid="{66549CE5-88E8-426D-9FB5-F1976BC0AFDA}"/>
     <hyperlink ref="G29" r:id="rId56" xr:uid="{16782551-B1ED-A343-A5C0-BA361524E57A}"/>
+    <hyperlink ref="G38" r:id="rId57" xr:uid="{7E510F02-89AE-8645-A208-3A542FD524DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[20230913] Leetcode - Blind 75 (38-39)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12194E40-811A-A040-B445-B066C44D7C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8653B3AB-058E-2344-8581-51DB0135CFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="386">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1393,6 +1393,24 @@
   </si>
   <si>
     <t>use pre, post to do left then do right</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.13</t>
+  </si>
+  <si>
+    <t>two list, one for stack, the other is for the min num when current value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/validate-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/min-stack/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS: use recurision to check left &lt; node.val &lt; right ; BFS: use two funcs to list val from min to max</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3367,8 +3385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3380,7 +3398,7 @@
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="73.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="86.5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -4584,6 +4602,15 @@
       <c r="F40" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="G40" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>381</v>
+      </c>
       <c r="K40" t="s">
         <v>22</v>
       </c>
@@ -4601,6 +4628,15 @@
       </c>
       <c r="F41" s="2" t="s">
         <v>51</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>381</v>
       </c>
       <c r="K41" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
[20230914] Leetcode - Blind 75 (40-41)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8653B3AB-058E-2344-8581-51DB0135CFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45A8356-A1ED-784E-BF46-87AE0E8C869E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="391">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1411,6 +1411,24 @@
   </si>
   <si>
     <t>DFS: use recurision to check left &lt; node.val &lt; right ; BFS: use two funcs to list val from min to max</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.14</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-islands/</t>
+  </si>
+  <si>
+    <t>DFS to run each connected neibors (set to '0') when catch grid[x][y] == '1'</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotting-oranges/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>deque to run all rotting and count fresh oranges</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3385,8 +3403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4593,6 +4611,9 @@
         <v>38</v>
       </c>
       <c r="B40" s="19"/>
+      <c r="C40" s="2">
+        <v>155</v>
+      </c>
       <c r="D40" s="2" t="s">
         <v>108</v>
       </c>
@@ -4620,6 +4641,9 @@
         <v>39</v>
       </c>
       <c r="B41" s="19"/>
+      <c r="C41" s="2">
+        <v>98</v>
+      </c>
       <c r="D41" s="2" t="s">
         <v>113</v>
       </c>
@@ -4647,6 +4671,9 @@
         <v>40</v>
       </c>
       <c r="B42" s="19"/>
+      <c r="C42" s="2">
+        <v>200</v>
+      </c>
       <c r="D42" s="2" t="s">
         <v>112</v>
       </c>
@@ -4655,6 +4682,15 @@
       </c>
       <c r="F42" s="2" t="s">
         <v>52</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>386</v>
       </c>
       <c r="K42" t="s">
         <v>90</v>
@@ -4665,6 +4701,9 @@
         <v>41</v>
       </c>
       <c r="B43" s="19"/>
+      <c r="C43" s="2">
+        <v>994</v>
+      </c>
       <c r="D43" s="2" t="s">
         <v>112</v>
       </c>
@@ -4673,6 +4712,15 @@
       </c>
       <c r="F43" s="2" t="s">
         <v>53</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>386</v>
       </c>
       <c r="K43" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
[20230915] Leetcode - Blind 75 (42-43)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45A8356-A1ED-784E-BF46-87AE0E8C869E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E136397-371B-B74E-A1D5-CE5F5B87CD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="396">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1429,6 +1429,24 @@
   </si>
   <si>
     <t>deque to run all rotting and count fresh oranges</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.15</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum/</t>
+  </si>
+  <si>
+    <t>Binary Search, but check order is forward or reverse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP to list all positive value &lt;= target and return DP[-1]; DFS with recurision to list related candidates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>review DP method and concept</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1975,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3403,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="G21" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4733,6 +4751,9 @@
       <c r="B44" s="20">
         <v>5</v>
       </c>
+      <c r="C44" s="2">
+        <v>33</v>
+      </c>
       <c r="D44" s="2" t="s">
         <v>16</v>
       </c>
@@ -4745,15 +4766,24 @@
       <c r="G44" s="6" t="s">
         <v>104</v>
       </c>
+      <c r="H44" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>391</v>
+      </c>
       <c r="K44" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="2">
+      <c r="A45" s="9">
         <v>43</v>
       </c>
       <c r="B45" s="20"/>
+      <c r="C45" s="2">
+        <v>39</v>
+      </c>
       <c r="D45" s="2" t="s">
         <v>116</v>
       </c>
@@ -4763,8 +4793,20 @@
       <c r="F45" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="G45" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>391</v>
+      </c>
       <c r="K45" t="s">
         <v>89</v>
+      </c>
+      <c r="L45" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -5460,15 +5502,14 @@
     <hyperlink ref="G27" r:id="rId49" xr:uid="{2D6DF4A8-FDD6-4EAE-8BF0-A0348B5B3AF6}"/>
     <hyperlink ref="G78" r:id="rId50" xr:uid="{4096430D-1ACD-476F-B085-7768BE9FB8BE}"/>
     <hyperlink ref="G79" r:id="rId51" xr:uid="{0978875B-409E-4344-B625-DEB2F1E366E0}"/>
-    <hyperlink ref="G44" r:id="rId52" xr:uid="{AFA5C7F8-DBD5-4E1A-AA45-803BC0671B44}"/>
-    <hyperlink ref="G32" r:id="rId53" xr:uid="{CA8DA924-CE20-40EC-85EC-5844F4DD1F5B}"/>
-    <hyperlink ref="G61" r:id="rId54" xr:uid="{75FBD306-6E88-4541-8B52-48157A1D46CA}"/>
-    <hyperlink ref="A1" r:id="rId55" xr:uid="{66549CE5-88E8-426D-9FB5-F1976BC0AFDA}"/>
-    <hyperlink ref="G29" r:id="rId56" xr:uid="{16782551-B1ED-A343-A5C0-BA361524E57A}"/>
-    <hyperlink ref="G38" r:id="rId57" xr:uid="{7E510F02-89AE-8645-A208-3A542FD524DA}"/>
+    <hyperlink ref="G32" r:id="rId52" xr:uid="{CA8DA924-CE20-40EC-85EC-5844F4DD1F5B}"/>
+    <hyperlink ref="G61" r:id="rId53" xr:uid="{75FBD306-6E88-4541-8B52-48157A1D46CA}"/>
+    <hyperlink ref="A1" r:id="rId54" xr:uid="{66549CE5-88E8-426D-9FB5-F1976BC0AFDA}"/>
+    <hyperlink ref="G29" r:id="rId55" xr:uid="{16782551-B1ED-A343-A5C0-BA361524E57A}"/>
+    <hyperlink ref="G38" r:id="rId56" xr:uid="{7E510F02-89AE-8645-A208-3A542FD524DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[20230916] Leetcode - Blind 75 (44-45)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E136397-371B-B74E-A1D5-CE5F5B87CD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C003803E-EF9A-474C-8AEC-1CE3D8CB129B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="401">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1447,6 +1447,23 @@
   </si>
   <si>
     <t>review DP method and concept</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.16</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutations/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-intervals/description/</t>
+  </si>
+  <si>
+    <t>DFS with recurison to check visited and run all</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>check [i][1] &lt; [i+1][0] or max [i][1]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3421,8 +3438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G21" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4814,6 +4831,9 @@
         <v>44</v>
       </c>
       <c r="B46" s="20"/>
+      <c r="C46" s="2">
+        <v>46</v>
+      </c>
       <c r="D46" s="2" t="s">
         <v>120</v>
       </c>
@@ -4822,6 +4842,15 @@
       </c>
       <c r="F46" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>396</v>
       </c>
       <c r="K46" t="s">
         <v>89</v>
@@ -4832,6 +4861,9 @@
         <v>45</v>
       </c>
       <c r="B47" s="20"/>
+      <c r="C47" s="2">
+        <v>56</v>
+      </c>
       <c r="D47" s="2" t="s">
         <v>116</v>
       </c>
@@ -4840,6 +4872,15 @@
       </c>
       <c r="F47" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>396</v>
       </c>
       <c r="K47" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
[20230917] Leetcode - Blind 75 (46-47)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C003803E-EF9A-474C-8AEC-1CE3D8CB129B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C6BAB-BB2D-0143-998E-F0CDC4CEA141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="406">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1464,6 +1464,25 @@
   </si>
   <si>
     <t>check [i][1] &lt; [i+1][0] or max [i][1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.17</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>check root sub includes p or q under left or right subtree, if both return root, else return not empty one</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>set: normal append([time, value]), get: use Binary Search to find key value but find from last is faster (timestamp)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/time-based-key-value-store/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3438,8 +3457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3451,7 +3470,7 @@
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="86.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="98.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -4891,6 +4910,9 @@
         <v>46</v>
       </c>
       <c r="B48" s="20"/>
+      <c r="C48" s="2">
+        <v>236</v>
+      </c>
       <c r="D48" s="2" t="s">
         <v>111</v>
       </c>
@@ -4899,6 +4921,15 @@
       </c>
       <c r="F48" s="2" t="s">
         <v>58</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="K48" t="s">
         <v>90</v>
@@ -4909,6 +4940,9 @@
         <v>47</v>
       </c>
       <c r="B49" s="20"/>
+      <c r="C49" s="2">
+        <v>981</v>
+      </c>
       <c r="D49" s="2" t="s">
         <v>16</v>
       </c>
@@ -4917,6 +4951,15 @@
       </c>
       <c r="F49" s="2" t="s">
         <v>59</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="K49" t="s">
         <v>91</v>
@@ -5548,9 +5591,10 @@
     <hyperlink ref="A1" r:id="rId54" xr:uid="{66549CE5-88E8-426D-9FB5-F1976BC0AFDA}"/>
     <hyperlink ref="G29" r:id="rId55" xr:uid="{16782551-B1ED-A343-A5C0-BA361524E57A}"/>
     <hyperlink ref="G38" r:id="rId56" xr:uid="{7E510F02-89AE-8645-A208-3A542FD524DA}"/>
+    <hyperlink ref="G48" r:id="rId57" xr:uid="{567C8113-5654-6646-97E1-E4886160795C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[20230918] Leetcode - Blind 75 (48-49)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C6BAB-BB2D-0143-998E-F0CDC4CEA141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF7C007-CC69-7644-AF8F-97C7BEA4DB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="412">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1483,6 +1483,29 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/time-based-key-value-store/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.18</t>
+  </si>
+  <si>
+    <t>create Union Find class with init, find, union, *** check unionFind method</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Union Find algorithm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/accounts-merge/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-colors/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>three ptr: left, right ,idx, if nums[idx] = 0 value of idx/left exchange, if nums[idx] == 2, idx/right exchange, or idx++</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3457,8 +3480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4935,7 +4958,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:12">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -4965,11 +4988,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="2">
+    <row r="50" spans="1:12">
+      <c r="A50" s="9">
         <v>48</v>
       </c>
       <c r="B50" s="20"/>
+      <c r="C50" s="2">
+        <v>721</v>
+      </c>
       <c r="D50" s="2" t="s">
         <v>112</v>
       </c>
@@ -4979,15 +5005,30 @@
       <c r="F50" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="G50" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="K50" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="2">
         <v>49</v>
       </c>
       <c r="B51" s="20"/>
+      <c r="C51" s="2">
+        <v>75</v>
+      </c>
       <c r="D51" s="2" t="s">
         <v>116</v>
       </c>
@@ -4997,11 +5038,20 @@
       <c r="F51" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="G51" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="K51" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:12">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -5021,7 +5071,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:12">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -5039,7 +5089,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:12">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -5057,7 +5107,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:12">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -5075,7 +5125,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:12">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -5093,7 +5143,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:12">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -5111,7 +5161,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:12">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -5129,7 +5179,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:12">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -5147,7 +5197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:12">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -5165,7 +5215,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:12">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -5188,7 +5238,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:12">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -5206,7 +5256,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:12">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -5224,7 +5274,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:12">
       <c r="A64" s="2">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
[20230919] Leetcode - Blind 75 (50-51)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF7C007-CC69-7644-AF8F-97C7BEA4DB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB932B0C-7013-3E49-B45A-6D5217120499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="417">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1506,6 +1506,25 @@
   </si>
   <si>
     <t>three ptr: left, right ,idx, if nums[idx] = 0 value of idx/left exchange, if nums[idx] == 2, idx/right exchange, or idx++</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.19</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/partition-equal-subset-sum/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-break/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP: check from 0 to sum(num) which each element can be run. Optimized is to use set replace DP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP: calcul each char step is true or false, and run to final (use max(map(x, y)) to accelerate. The other is Tre with startswith()</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3480,8 +3499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5058,6 +5077,9 @@
       <c r="B52" s="21">
         <v>6</v>
       </c>
+      <c r="C52" s="2">
+        <v>139</v>
+      </c>
       <c r="D52" s="2" t="s">
         <v>119</v>
       </c>
@@ -5067,15 +5089,27 @@
       <c r="F52" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="G52" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>412</v>
+      </c>
       <c r="K52" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="2">
+      <c r="A53" s="9">
         <v>51</v>
       </c>
       <c r="B53" s="21"/>
+      <c r="C53" s="2">
+        <v>416</v>
+      </c>
       <c r="D53" s="2" t="s">
         <v>115</v>
       </c>
@@ -5084,6 +5118,15 @@
       </c>
       <c r="F53" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>412</v>
       </c>
       <c r="K53" t="s">
         <v>89</v>
@@ -5103,6 +5146,7 @@
       <c r="F54" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="G54" s="6"/>
       <c r="K54" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
[20230920] Leetcode - Blind 75 (52)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB932B0C-7013-3E49-B45A-6D5217120499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD590D6-9566-0241-91E5-B31F50D93C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="421">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1526,6 +1526,19 @@
   <si>
     <t>DP: calcul each char step is true or false, and run to final (use max(map(x, y)) to accelerate. The other is Tre with startswith()</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/string-to-integer-atoi/</t>
+  </si>
+  <si>
+    <t>three states to check each char, 0 for first char (' ', '+-', num), 1 for num after +-, 2 for num, finally check MAX, MIN</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.20</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/spiral-matrix/</t>
   </si>
 </sst>
 </file>
@@ -3499,8 +3512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="E18" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5137,6 +5150,9 @@
         <v>52</v>
       </c>
       <c r="B54" s="21"/>
+      <c r="C54" s="2">
+        <v>8</v>
+      </c>
       <c r="D54" s="2" t="s">
         <v>110</v>
       </c>
@@ -5146,7 +5162,15 @@
       <c r="F54" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G54" s="6"/>
+      <c r="G54" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="K54" t="s">
         <v>90</v>
       </c>
@@ -5156,6 +5180,9 @@
         <v>53</v>
       </c>
       <c r="B55" s="21"/>
+      <c r="C55" s="2">
+        <v>54</v>
+      </c>
       <c r="D55" s="2" t="s">
         <v>121</v>
       </c>
@@ -5165,6 +5192,10 @@
       <c r="F55" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="G55" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="I55" s="2"/>
       <c r="K55" t="s">
         <v>90</v>
       </c>
@@ -5183,6 +5214,7 @@
       <c r="F56" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="G56" s="2"/>
       <c r="K56" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
[20230921] Leetcode - Blind 75 (53-54)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD590D6-9566-0241-91E5-B31F50D93C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA083675-4572-3245-8D37-867F5D1A5719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="top-interview-questions-easy" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="425">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1539,6 +1539,20 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/spiral-matrix/</t>
+  </si>
+  <si>
+    <t>2023.09.21</t>
+  </si>
+  <si>
+    <t>while with four loop and use (top, bottom, left, right) to limit the border</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subsets/</t>
+  </si>
+  <si>
+    <t>Recursion to run I, i+1… step by step and concate it</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3512,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5195,7 +5209,12 @@
       <c r="G55" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="I55" s="2"/>
+      <c r="H55" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>421</v>
+      </c>
       <c r="K55" t="s">
         <v>90</v>
       </c>
@@ -5205,6 +5224,9 @@
         <v>54</v>
       </c>
       <c r="B56" s="21"/>
+      <c r="C56" s="2">
+        <v>78</v>
+      </c>
       <c r="D56" s="2" t="s">
         <v>120</v>
       </c>
@@ -5214,7 +5236,15 @@
       <c r="F56" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G56" s="2"/>
+      <c r="G56" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>421</v>
+      </c>
       <c r="K56" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
[20230924] Leetcode - Blind 75 (55-56)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA083675-4572-3245-8D37-867F5D1A5719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BCA337-C6AB-A340-BAA1-5682571C0DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="top-interview-questions-easy" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="430">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1552,6 +1552,24 @@
   </si>
   <si>
     <t>Recursion to run I, i+1… step by step and concate it</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.24</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-palindromic-substring/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-right-side-view/</t>
+  </si>
+  <si>
+    <t>DP ([[]]) to record s[i:j], check upper side of diagona; or ; func to traver two side of each char</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS with recurison to traver from right to left; or; BFS with deque to append from left to right</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2098,7 +2116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -3526,8 +3544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5254,6 +5272,9 @@
         <v>55</v>
       </c>
       <c r="B57" s="21"/>
+      <c r="C57" s="2">
+        <v>199</v>
+      </c>
       <c r="D57" s="2" t="s">
         <v>111</v>
       </c>
@@ -5262,6 +5283,15 @@
       </c>
       <c r="F57" s="2" t="s">
         <v>67</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>425</v>
       </c>
       <c r="K57" t="s">
         <v>22</v>
@@ -5272,6 +5302,9 @@
         <v>56</v>
       </c>
       <c r="B58" s="21"/>
+      <c r="C58" s="2">
+        <v>5</v>
+      </c>
       <c r="D58" s="2" t="s">
         <v>110</v>
       </c>
@@ -5280,6 +5313,15 @@
       </c>
       <c r="F58" s="2" t="s">
         <v>68</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>425</v>
       </c>
       <c r="K58" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
[20230925] Leetcode - Blind 75 (57-58)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BCA337-C6AB-A340-BAA1-5682571C0DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F850A-046D-1545-BAF5-F7697A4F1A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="435">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1570,6 +1570,23 @@
   </si>
   <si>
     <t>DFS with recurison to traver from right to left; or; BFS with deque to append from left to right</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.25</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths/</t>
+  </si>
+  <si>
+    <t>dp[][] table to count from left top to right bottom, [i][j] = [i-1][j] + [i][j-1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>check by inorder and preorder characteristic, divide to left and right sidt; and; use dict to faster</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3544,8 +3561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5332,6 +5349,9 @@
         <v>57</v>
       </c>
       <c r="B59" s="21"/>
+      <c r="C59" s="2">
+        <v>62</v>
+      </c>
       <c r="D59" s="2" t="s">
         <v>115</v>
       </c>
@@ -5340,6 +5360,15 @@
       </c>
       <c r="F59" s="2" t="s">
         <v>69</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>430</v>
       </c>
       <c r="K59" t="s">
         <v>22</v>
@@ -5350,6 +5379,9 @@
         <v>58</v>
       </c>
       <c r="B60" s="21"/>
+      <c r="C60" s="2">
+        <v>105</v>
+      </c>
       <c r="D60" s="2" t="s">
         <v>111</v>
       </c>
@@ -5358,6 +5390,15 @@
       </c>
       <c r="F60" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>430</v>
       </c>
       <c r="K60" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
[20230926] Leetcode - Blind 75 (59)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F850A-046D-1545-BAF5-F7697A4F1A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5668280-5879-344C-8B72-B58D25855397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
-    <sheet name="top-interview-questions-easy" sheetId="3" r:id="rId1"/>
+    <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
     <sheet name="Blind 75" sheetId="1" r:id="rId2"/>
-    <sheet name="Meduim Collection 52" sheetId="2" r:id="rId3"/>
+    <sheet name="Top Interview Q - Meduim 52" sheetId="2" r:id="rId3"/>
     <sheet name="Dynamic Programming" sheetId="4" r:id="rId4"/>
     <sheet name="Recursion I" sheetId="5" r:id="rId5"/>
     <sheet name="Heap" sheetId="6" r:id="rId6"/>
     <sheet name="Sorting" sheetId="7" r:id="rId7"/>
+    <sheet name="Binary Search" sheetId="9" r:id="rId8"/>
+    <sheet name="Graph" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="438">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1587,6 +1589,16 @@
   </si>
   <si>
     <t>check by inorder and preorder characteristic, divide to left and right sidt; and; use dict to faster</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/letter-combinations-of-a-phone-number/</t>
+  </si>
+  <si>
+    <t>2023.09.26</t>
+  </si>
+  <si>
+    <t>two pointer: left, right, find curArea and check maxArea, if left &lt; right height, then left ++ or right--</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2133,7 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -3561,8 +3573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5411,6 +5423,9 @@
       <c r="B61" s="14">
         <v>7</v>
       </c>
+      <c r="C61" s="2">
+        <v>11</v>
+      </c>
       <c r="D61" s="2" t="s">
         <v>116</v>
       </c>
@@ -5422,6 +5437,12 @@
       </c>
       <c r="G61" s="6" t="s">
         <v>105</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>436</v>
       </c>
       <c r="K61" t="s">
         <v>91</v>
@@ -5432,6 +5453,9 @@
         <v>60</v>
       </c>
       <c r="B62" s="14"/>
+      <c r="C62" s="2">
+        <v>17</v>
+      </c>
       <c r="D62" s="2" t="s">
         <v>120</v>
       </c>
@@ -5440,6 +5464,9 @@
       </c>
       <c r="F62" s="2" t="s">
         <v>72</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>435</v>
       </c>
       <c r="K62" t="s">
         <v>89</v>
@@ -5842,7 +5869,7 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6480,4 +6507,34 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED2A95A-A5C1-7B46-B514-8AACCDB615E6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R38" sqref="R38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F6B7C9-F416-9A49-83DC-B48E6AB23806}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[20230927] Leetcode - Blind 75 (60)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5668280-5879-344C-8B72-B58D25855397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A6BCB7-0B28-1A46-981F-F91C05CBBFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="441">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1600,6 +1600,16 @@
   <si>
     <t>two pointer: left, right, find curArea and check maxArea, if left &lt; right height, then left ++ or right--</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.27</t>
+  </si>
+  <si>
+    <t>Backtracking Algorithm or Iteration, BT is a loog function ( if condition, for loop)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-search/</t>
   </si>
 </sst>
 </file>
@@ -3573,8 +3583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5468,6 +5478,12 @@
       <c r="G62" s="6" t="s">
         <v>435</v>
       </c>
+      <c r="H62" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>438</v>
+      </c>
       <c r="K62" t="s">
         <v>89</v>
       </c>
@@ -5477,6 +5493,9 @@
         <v>61</v>
       </c>
       <c r="B63" s="14"/>
+      <c r="C63" s="2">
+        <v>79</v>
+      </c>
       <c r="D63" s="2" t="s">
         <v>112</v>
       </c>
@@ -5485,6 +5504,9 @@
       </c>
       <c r="F63" s="2" t="s">
         <v>73</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>440</v>
       </c>
       <c r="K63" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
[20230928] Leetcode - Blind 75 (61)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A6BCB7-0B28-1A46-981F-F91C05CBBFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33FEF54-91C7-694A-9375-4DF6D106391B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="443">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1610,6 +1610,13 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/word-search/</t>
+  </si>
+  <si>
+    <t>2023.09.28</t>
+  </si>
+  <si>
+    <t>DFS with visited to check left, right, up, down, and optimization by counting each char of word compared to board</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3583,8 +3590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5507,6 +5514,12 @@
       </c>
       <c r="G63" s="6" t="s">
         <v>440</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>441</v>
       </c>
       <c r="K63" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
[20230929] Leetcode - Blind 75 (62)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33FEF54-91C7-694A-9375-4DF6D106391B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F6C0C4-18AA-BA44-9B0C-49A38DB3A39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="446">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1616,6 +1616,16 @@
   </si>
   <si>
     <t>DFS with visited to check left, right, up, down, and optimization by counting each char of word compared to board</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.09.29</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-all-anagrams-in-a-string/</t>
+  </si>
+  <si>
+    <t>Table to save p, moving window to check: in window then -=1, or out of window then += 1, if all table = 0: it is Anagrams</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3590,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5538,6 +5548,15 @@
       </c>
       <c r="F64" s="2" t="s">
         <v>74</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>443</v>
       </c>
       <c r="K64" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
[20231002] Leetcode - Blind 75 (63)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F6C0C4-18AA-BA44-9B0C-49A38DB3A39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BC0D5E-9CCA-F649-9CE4-0C20AA8315D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="450">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1627,6 +1627,20 @@
   <si>
     <t>Table to save p, moving window to check: in window then -=1, or out of window then += 1, if all table = 0: it is Anagrams</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-height-trees/</t>
+  </si>
+  <si>
+    <t>2023.10.02</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>leave node removal, count the leaf node (only one connection) and remove it until the last one time leaf</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/task-scheduler/</t>
   </si>
 </sst>
 </file>
@@ -3600,8 +3614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="E45" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5540,6 +5554,9 @@
         <v>62</v>
       </c>
       <c r="B64" s="14"/>
+      <c r="C64" s="2">
+        <v>438</v>
+      </c>
       <c r="D64" s="2" t="s">
         <v>110</v>
       </c>
@@ -5567,6 +5584,9 @@
         <v>63</v>
       </c>
       <c r="B65" s="14"/>
+      <c r="C65" s="2">
+        <v>310</v>
+      </c>
       <c r="D65" s="2" t="s">
         <v>112</v>
       </c>
@@ -5575,6 +5595,15 @@
       </c>
       <c r="F65" s="2" t="s">
         <v>75</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>447</v>
       </c>
       <c r="K65" t="s">
         <v>89</v>
@@ -5585,6 +5614,9 @@
         <v>64</v>
       </c>
       <c r="B66" s="14"/>
+      <c r="C66" s="2">
+        <v>621</v>
+      </c>
       <c r="D66" s="2" t="s">
         <v>118</v>
       </c>
@@ -5594,6 +5626,10 @@
       <c r="F66" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="G66" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="I66" s="2"/>
       <c r="K66" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
[20231003] Leetcode - Blind 75 (64)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BC0D5E-9CCA-F649-9CE4-0C20AA8315D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F20678-3B23-1E45-9C34-6F90C5F5A5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="452">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1641,6 +1641,13 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/task-scheduler/</t>
+  </si>
+  <si>
+    <t>2023.10.03</t>
+  </si>
+  <si>
+    <t>List the max num of Char to block and count it =&gt; (max num -1) * (n + 1) + max num</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3614,8 +3621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E45" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5629,7 +5636,12 @@
       <c r="G66" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="I66" s="2"/>
+      <c r="H66" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>450</v>
+      </c>
       <c r="K66" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
[20231004] Leetcode - Blind 75 (65)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F20678-3B23-1E45-9C34-6F90C5F5A5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8737D6E-5C6A-AF40-BCDE-32C0181ABBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="456">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1647,6 +1647,21 @@
   </si>
   <si>
     <t>List the max num of Char to block and count it =&gt; (max num -1) * (n + 1) + max num</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.04</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lru-cache/description/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-smallest-element-in-a-bst/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bidirection ListNode with table (save node); the best answer is OrderedDict with move_to_end/popitem(last=false)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2194,7 +2209,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3621,8 +3636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="G38" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5651,6 +5666,9 @@
         <v>65</v>
       </c>
       <c r="B67" s="14"/>
+      <c r="C67" s="2">
+        <v>146</v>
+      </c>
       <c r="D67" s="2" t="s">
         <v>109</v>
       </c>
@@ -5659,6 +5677,15 @@
       </c>
       <c r="F67" s="2" t="s">
         <v>77</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>452</v>
       </c>
       <c r="K67" t="s">
         <v>89</v>
@@ -5671,6 +5698,9 @@
       <c r="B68" s="15">
         <v>8</v>
       </c>
+      <c r="C68" s="2">
+        <v>230</v>
+      </c>
       <c r="D68" s="2" t="s">
         <v>113</v>
       </c>
@@ -5680,6 +5710,10 @@
       <c r="F68" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="G68" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="I68" s="2"/>
       <c r="K68" t="s">
         <v>90</v>
       </c>
@@ -5698,6 +5732,7 @@
       <c r="F69" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="G69" s="6"/>
       <c r="K69" t="s">
         <v>89</v>
       </c>
@@ -5960,9 +5995,10 @@
     <hyperlink ref="G29" r:id="rId55" xr:uid="{16782551-B1ED-A343-A5C0-BA361524E57A}"/>
     <hyperlink ref="G38" r:id="rId56" xr:uid="{7E510F02-89AE-8645-A208-3A542FD524DA}"/>
     <hyperlink ref="G48" r:id="rId57" xr:uid="{567C8113-5654-6646-97E1-E4886160795C}"/>
+    <hyperlink ref="G67" r:id="rId58" xr:uid="{30BC5404-4832-A54A-B085-52D7ADC8A82A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId59"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[20231005] Leetcode - Blind 75 (66)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8737D6E-5C6A-AF40-BCDE-32C0181ABBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7853E178-5B73-8040-9BEB-F90FBBD82DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="458">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1662,6 +1662,13 @@
   </si>
   <si>
     <t>Bidirection ListNode with table (save node); the best answer is OrderedDict with move_to_end/popitem(last=false)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.05</t>
+  </si>
+  <si>
+    <t>DFS to inorder traversal to save all value and output [-k], add early stopping when len(ans) == k; or; loop</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3636,8 +3643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G38" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5713,7 +5720,12 @@
       <c r="G68" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="I68" s="2"/>
+      <c r="H68" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>456</v>
+      </c>
       <c r="K68" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
[20231006] Leetcode - Blind 75 (67)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7853E178-5B73-8040-9BEB-F90FBBD82DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B7195-7D90-DD4F-8CDF-B1AE882DA43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="462">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1670,6 +1670,19 @@
   <si>
     <t>DFS to inorder traversal to save all value and output [-k], add early stopping when len(ans) == k; or; loop</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.06</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-window-substring/</t>
+  </si>
+  <si>
+    <t>use counter to run window, move right ptr to contain all needed chars, then move left ptr to shorten window</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/serialize-and-deserialize-binary-tree/</t>
   </si>
 </sst>
 </file>
@@ -3643,8 +3656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="F44" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5735,6 +5748,9 @@
         <v>67</v>
       </c>
       <c r="B69" s="15"/>
+      <c r="C69" s="2">
+        <v>76</v>
+      </c>
       <c r="D69" s="2" t="s">
         <v>110</v>
       </c>
@@ -5744,7 +5760,15 @@
       <c r="F69" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G69" s="6"/>
+      <c r="G69" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>458</v>
+      </c>
       <c r="K69" t="s">
         <v>89</v>
       </c>
@@ -5754,6 +5778,9 @@
         <v>68</v>
       </c>
       <c r="B70" s="15"/>
+      <c r="C70" s="2">
+        <v>297</v>
+      </c>
       <c r="D70" s="2" t="s">
         <v>111</v>
       </c>
@@ -5763,6 +5790,10 @@
       <c r="F70" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="G70" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="I70" s="2"/>
       <c r="K70" t="s">
         <v>92</v>
       </c>
@@ -5897,6 +5928,9 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
+      <c r="B78" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="F78" s="2" t="s">
         <v>101</v>
       </c>
@@ -5908,6 +5942,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
+      <c r="B79" s="11"/>
       <c r="F79" s="2" t="s">
         <v>103</v>
       </c>
@@ -5936,7 +5971,7 @@
       <c r="H85" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="B61:B67"/>
     <mergeCell ref="B68:B77"/>
     <mergeCell ref="B85:H85"/>
@@ -5947,6 +5982,7 @@
     <mergeCell ref="B44:B51"/>
     <mergeCell ref="B52:B60"/>
     <mergeCell ref="B3:B15"/>
+    <mergeCell ref="B78:B79"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231007] Leetcode - Blind 75 (68)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B7195-7D90-DD4F-8CDF-B1AE882DA43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469A88B7-729B-4B4C-A020-AC1180680713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="464">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1683,6 +1683,13 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/serialize-and-deserialize-binary-tree/</t>
+  </si>
+  <si>
+    <t>use preorder to serialize or deserialize data (str &lt;-&gt; treenode)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.07</t>
   </si>
 </sst>
 </file>
@@ -3656,8 +3663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F44" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5793,7 +5800,12 @@
       <c r="G70" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="I70" s="2"/>
+      <c r="H70" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>463</v>
+      </c>
       <c r="K70" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
[20231008] Leetcode - Blind 75 (69)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469A88B7-729B-4B4C-A020-AC1180680713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660879B4-A8DF-1B4D-9EBF-14453292821A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="467">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1690,6 +1690,16 @@
   </si>
   <si>
     <t>2023.10.07</t>
+  </si>
+  <si>
+    <t>2023.10.08</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/trapping-rain-water/</t>
+  </si>
+  <si>
+    <t>two ptr to compare left and right height, water += min(max(left max, right max)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3663,8 +3673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5815,6 +5825,9 @@
         <v>69</v>
       </c>
       <c r="B71" s="15"/>
+      <c r="C71" s="2">
+        <v>42</v>
+      </c>
       <c r="D71" s="2" t="s">
         <v>108</v>
       </c>
@@ -5823,6 +5836,15 @@
       </c>
       <c r="F71" s="2" t="s">
         <v>81</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>464</v>
       </c>
       <c r="K71" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
[20231009] Leetcode - Blind 75 (70)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660879B4-A8DF-1B4D-9EBF-14453292821A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB6E504-58E0-2846-8F9B-350AB20CC868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="470">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1699,6 +1699,16 @@
   </si>
   <si>
     <t>two ptr to compare left and right height, water += min(max(left max, right max)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-median-from-data-stream/</t>
+  </si>
+  <si>
+    <t>2023.10.09</t>
+  </si>
+  <si>
+    <t>two list (max_list, min_list) to save smallest or biggest value, and keep them balance, final out max[0] or (max+min)/2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3674,7 +3684,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5855,6 +5865,9 @@
         <v>70</v>
       </c>
       <c r="B72" s="15"/>
+      <c r="C72" s="2">
+        <v>295</v>
+      </c>
       <c r="D72" s="2" t="s">
         <v>118</v>
       </c>
@@ -5863,6 +5876,15 @@
       </c>
       <c r="F72" s="2" t="s">
         <v>82</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>468</v>
       </c>
       <c r="K72" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
[20231010] Leetcode - Blind 75 (71)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB6E504-58E0-2846-8F9B-350AB20CC868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8977FD74-ECB4-D742-8CCC-C23D5D4605C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="473">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1709,6 +1709,16 @@
   </si>
   <si>
     <t>two list (max_list, min_list) to save smallest or biggest value, and keep them balance, final out max[0] or (max+min)/2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.10</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-ladder/</t>
+  </si>
+  <si>
+    <t>defaultdict to save all values by * (e.g. h*t: hit, hot, hat...), visited to save used value, queue to run all char for each word</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3684,7 +3694,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5895,6 +5905,9 @@
         <v>71</v>
       </c>
       <c r="B73" s="15"/>
+      <c r="C73" s="2">
+        <v>127</v>
+      </c>
       <c r="D73" s="2" t="s">
         <v>112</v>
       </c>
@@ -5903,6 +5916,15 @@
       </c>
       <c r="F73" s="2" t="s">
         <v>83</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>470</v>
       </c>
       <c r="K73" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
[20231011] Leetcode - Blind 75 (72)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8977FD74-ECB4-D742-8CCC-C23D5D4605C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8CC6FC-7304-2E4C-8365-1E4D2423B465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="477">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1720,6 +1720,19 @@
   <si>
     <t>defaultdict to save all values by * (e.g. h*t: hit, hot, hat...), visited to save used value, queue to run all char for each word</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.11</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/basic-calculator/</t>
+  </si>
+  <si>
+    <t>if isdigital, '+-', '(', and ')', to calcul</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-profit-in-job-scheduling/</t>
   </si>
 </sst>
 </file>
@@ -2265,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
@@ -3693,15 +3706,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
@@ -5935,6 +5948,9 @@
         <v>72</v>
       </c>
       <c r="B74" s="15"/>
+      <c r="C74" s="2">
+        <v>224</v>
+      </c>
       <c r="D74" s="2" t="s">
         <v>108</v>
       </c>
@@ -5943,6 +5959,15 @@
       </c>
       <c r="F74" s="2" t="s">
         <v>84</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>473</v>
       </c>
       <c r="K74" t="s">
         <v>92</v>
@@ -5953,6 +5978,9 @@
         <v>73</v>
       </c>
       <c r="B75" s="15"/>
+      <c r="C75" s="2">
+        <v>1235</v>
+      </c>
       <c r="D75" s="2" t="s">
         <v>16</v>
       </c>
@@ -5961,6 +5989,9 @@
       </c>
       <c r="F75" s="2" t="s">
         <v>85</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>476</v>
       </c>
       <c r="K75" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
[20231012] Leetcode - Blind 75 (73)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8CC6FC-7304-2E4C-8365-1E4D2423B465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBF8DDE-2593-3F41-937B-A16624F2D611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="479">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1733,6 +1733,13 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/maximum-profit-in-job-scheduling/</t>
+  </si>
+  <si>
+    <t>2023.10.12</t>
+  </si>
+  <si>
+    <t>add overlop interval to heap, pop and calc max if no overlop, loop to find max pro</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3706,8 +3713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5992,6 +5999,12 @@
       </c>
       <c r="G75" s="6" t="s">
         <v>476</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>477</v>
       </c>
       <c r="K75" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
[20231013] Leetcode - Blind 75 (74)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBF8DDE-2593-3F41-937B-A16624F2D611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1F9A38-9B17-C94B-BBFC-359650AA6E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="482">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1739,6 +1739,17 @@
   </si>
   <si>
     <t>add overlop interval to heap, pop and calc max if no overlop, loop to find max pro</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-k-sorted-lists/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.13</t>
+  </si>
+  <si>
+    <t>fastest answer: add all values to list, sort, generate new link-list; or; devide and conquer to merge all list</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3713,8 +3724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+    <sheetView tabSelected="1" topLeftCell="F42" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6015,6 +6026,9 @@
         <v>74</v>
       </c>
       <c r="B76" s="15"/>
+      <c r="C76" s="2">
+        <v>23</v>
+      </c>
       <c r="D76" s="2" t="s">
         <v>118</v>
       </c>
@@ -6023,6 +6037,15 @@
       </c>
       <c r="F76" s="2" t="s">
         <v>86</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>480</v>
       </c>
       <c r="K76" t="s">
         <v>89</v>
@@ -6166,9 +6189,10 @@
     <hyperlink ref="G38" r:id="rId56" xr:uid="{7E510F02-89AE-8645-A208-3A542FD524DA}"/>
     <hyperlink ref="G48" r:id="rId57" xr:uid="{567C8113-5654-6646-97E1-E4886160795C}"/>
     <hyperlink ref="G67" r:id="rId58" xr:uid="{30BC5404-4832-A54A-B085-52D7ADC8A82A}"/>
+    <hyperlink ref="G76" r:id="rId59" xr:uid="{701F1B1F-A22B-EC45-B6B0-033E9F8E7270}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId59"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[20231015] Leetcode - Blind 75 (75)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1F9A38-9B17-C94B-BBFC-359650AA6E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76DB9DC-E50E-FA42-BCFC-3493F123BAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="486">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1750,6 +1750,22 @@
   </si>
   <si>
     <t>fastest answer: add all values to list, sort, generate new link-list; or; devide and conquer to merge all list</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/largest-rectangle-in-histogram/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>monotonic stack: if h[i] &gt; h[i-1]: [i-1] add to stack else pop stack and calc max area</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>monotonic stack</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3724,8 +3740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F42" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5689,7 +5705,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:12">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -5719,7 +5735,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:12">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -5749,7 +5765,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:12">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -5779,7 +5795,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:12">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -5811,7 +5827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:12">
       <c r="A69" s="2">
         <v>67</v>
       </c>
@@ -5841,7 +5857,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:12">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -5871,7 +5887,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:12">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -5901,7 +5917,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:12">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -5931,7 +5947,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:12">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -5961,7 +5977,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:12">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -5991,7 +6007,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:12">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -6021,7 +6037,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:12">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -6051,11 +6067,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
-      <c r="A77" s="2">
+    <row r="77" spans="1:12">
+      <c r="A77" s="9">
         <v>75</v>
       </c>
       <c r="B77" s="15"/>
+      <c r="C77" s="2">
+        <v>84</v>
+      </c>
       <c r="D77" s="2" t="s">
         <v>108</v>
       </c>
@@ -6065,11 +6084,23 @@
       <c r="F77" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="G77" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>482</v>
+      </c>
       <c r="K77" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="L77" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -6083,7 +6114,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:12">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -6095,7 +6126,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:12">
       <c r="F80" s="2"/>
     </row>
     <row r="81" spans="1:8">

</xml_diff>

<commit_message>
[20231016] Leetcode - Blind 75 (76)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76DB9DC-E50E-FA42-BCFC-3493F123BAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C766DC-0054-8345-B96B-C8D68B52E707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="510">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1767,6 +1767,86 @@
   <si>
     <t>monotonic stack</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/776/</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/777/</t>
+  </si>
+  <si>
+    <t>  Group Anagrams</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/778/</t>
+  </si>
+  <si>
+    <t>  Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/779/</t>
+  </si>
+  <si>
+    <t>  Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/780/</t>
+  </si>
+  <si>
+    <t>  Increasing Triplet Subsequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/781/</t>
+  </si>
+  <si>
+    <t>Missing Ranges</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/4153/</t>
+  </si>
+  <si>
+    <t>  Count and Say</t>
+  </si>
+  <si>
+    <t>Array and Strings</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked List</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trees and Graphs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backtracking</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.16</t>
+  </si>
+  <si>
+    <t>max, min, ans, if nums[i] &lt; 0: max &lt;-&gt; min, find max for answer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.17</t>
   </si>
 </sst>
 </file>
@@ -3740,8 +3820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6107,11 +6187,29 @@
       <c r="B78" s="11" t="s">
         <v>132</v>
       </c>
+      <c r="C78" s="2">
+        <v>152</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F78" s="2" t="s">
         <v>101</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>100</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -6119,11 +6217,23 @@
         <v>77</v>
       </c>
       <c r="B79" s="11"/>
+      <c r="C79" s="2">
+        <v>153</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F79" s="2" t="s">
         <v>103</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>102</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -6229,24 +6339,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="13" t="s">
-        <v>122</v>
+        <v>486</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -6294,10 +6405,18 @@
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>487</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
       <c r="I3" s="3" t="s">
@@ -6308,15 +6427,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="16">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>489</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="8"/>
       <c r="I4" s="3"/>
@@ -6327,10 +6452,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>491</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
@@ -6339,10 +6470,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>493</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
@@ -6351,10 +6488,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>495</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
@@ -6363,10 +6506,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>497</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -6375,10 +6524,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>499</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -6387,10 +6542,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>500</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
@@ -6399,8 +6560,12 @@
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="6"/>
       <c r="G11" s="2"/>
@@ -6411,8 +6576,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="6"/>
       <c r="G12" s="2"/>
@@ -6423,8 +6590,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="6"/>
       <c r="G13" s="2"/>
@@ -6435,8 +6604,12 @@
         <v>12</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="6"/>
       <c r="G14" s="2"/>
@@ -6447,8 +6620,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="6"/>
       <c r="G15" s="2"/>
@@ -6459,8 +6634,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="6"/>
       <c r="G16" s="2"/>
@@ -6471,8 +6648,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="6"/>
       <c r="G17" s="2"/>
@@ -6483,8 +6662,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="6"/>
       <c r="G18" s="2"/>
@@ -6495,8 +6676,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="6"/>
       <c r="G19" s="2"/>
@@ -6507,8 +6690,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="6"/>
       <c r="G20" s="2"/>
@@ -6519,8 +6704,12 @@
         <v>19</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="6"/>
       <c r="G21" s="2"/>
@@ -6531,8 +6720,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="6"/>
       <c r="G22" s="2"/>
@@ -6543,8 +6734,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="6"/>
       <c r="G23" s="2"/>
@@ -6555,8 +6748,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="6"/>
       <c r="G24" s="2"/>
@@ -6567,8 +6762,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="6"/>
       <c r="G25" s="2"/>
@@ -6578,7 +6775,12 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="C26" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="2"/>
@@ -6588,7 +6790,10 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="2"/>
@@ -6598,7 +6803,10 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E28" s="6"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -6607,7 +6815,10 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E29" s="6"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -6616,7 +6827,10 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E30" s="6"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -6625,7 +6839,10 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E31" s="6"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -6634,7 +6851,10 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="2"/>
@@ -6644,7 +6864,10 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E33" s="6"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -6653,7 +6876,10 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E34" s="6"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -6662,7 +6888,12 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="C35" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E35" s="6"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -6671,7 +6902,10 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E36" s="6"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -6680,7 +6914,10 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E37" s="6"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -6689,7 +6926,10 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E38" s="6"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -6698,7 +6938,12 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="C39" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="2"/>
@@ -6708,7 +6953,10 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E40" s="6"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -6717,6 +6965,10 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
+      <c r="C41" s="11"/>
+      <c r="D41" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E41" s="6"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -6725,7 +6977,10 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E42" s="6"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -6734,7 +6989,12 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="C43" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E43" s="6"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -6743,7 +7003,10 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="2"/>
@@ -6753,7 +7016,10 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E45" s="6"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -6762,7 +7028,10 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E46" s="6"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -6771,7 +7040,10 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E47" s="6"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -6780,6 +7052,10 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E48" s="6"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -6788,7 +7064,10 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E49" s="6"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -6797,14 +7076,64 @@
       <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="C50" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E50" s="6"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="C54" s="11"/>
+      <c r="D54" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="10">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231017] Leetcode - Blind 75 (77) and Medium (1)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C766DC-0054-8345-B96B-C8D68B52E707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B389AFDB-06A5-944B-984E-00160038C00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="515">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1847,6 +1847,26 @@
   </si>
   <si>
     <t>2023.10.17</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>binary search to find nums[left]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5min</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Sum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list all conditions: 1) all 0, 2) p &amp; n &amp; zero each one 3) two p one n 4) two n one p</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2392,8 +2412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3820,8 +3840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView topLeftCell="F49" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6221,7 +6241,7 @@
         <v>153</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>38</v>
@@ -6232,8 +6252,14 @@
       <c r="G79" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="H79" s="2" t="s">
+        <v>511</v>
+      </c>
       <c r="I79" s="2" t="s">
         <v>509</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -6341,17 +6367,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
     <col min="5" max="5" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82.33203125" customWidth="1"/>
+    <col min="7" max="7" width="72.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6400,11 +6428,13 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="32">
+    <row r="3" spans="1:11" ht="16" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>15</v>
+      </c>
       <c r="C3" s="12" t="s">
         <v>502</v>
       </c>
@@ -6412,13 +6442,17 @@
         <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>513</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
       </c>
@@ -6595,7 +6629,6 @@
         <v>38</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="6"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
@@ -6681,7 +6714,9 @@
         <v>38</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="6"/>
+      <c r="F19" s="2" t="s">
+        <v>499</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
@@ -6869,6 +6904,9 @@
         <v>38</v>
       </c>
       <c r="E33" s="6"/>
+      <c r="F33" s="2" t="s">
+        <v>499</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
@@ -6945,7 +6983,9 @@
         <v>38</v>
       </c>
       <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="F39" s="2" t="s">
+        <v>499</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
@@ -6982,6 +7022,9 @@
         <v>38</v>
       </c>
       <c r="E42" s="6"/>
+      <c r="F42" s="2" t="s">
+        <v>499</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
@@ -7112,6 +7155,9 @@
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="F53" s="2" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2">
@@ -7124,16 +7170,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231017] Leetcode - Top-Interview-Medium 52 (2-3)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B389AFDB-06A5-944B-984E-00160038C00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475D4B13-61E4-1944-B3B8-C743DBD34812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="518">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1866,6 +1866,17 @@
   </si>
   <si>
     <t>list all conditions: 1) all 0, 2) p &amp; n &amp; zero each one 3) two p one n 4) two n one p</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.18</t>
+  </si>
+  <si>
+    <t>check first row/col has zero and set 0 for (1 to end) for each col/row, finally set first row/col to 0 if it contain 0; or; best time/space; use set to record</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dic[''.join(sorted(s))] to add to list by sorted s, finally generate dic.values()</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6367,8 +6378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6379,7 +6390,7 @@
     <col min="4" max="4" width="6.1640625" customWidth="1"/>
     <col min="5" max="5" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="82.33203125" customWidth="1"/>
-    <col min="7" max="7" width="72.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="116.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6461,11 +6472,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16">
+    <row r="4" spans="1:11" ht="16" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>73</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
@@ -6476,8 +6489,12 @@
       <c r="F4" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>515</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
@@ -6485,7 +6502,9 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>49</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
@@ -6496,8 +6515,12 @@
       <c r="F5" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2">
@@ -7170,16 +7193,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231018] Leetcode - Top-Interview-Medium 52 (4-5)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475D4B13-61E4-1944-B3B8-C743DBD34812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D44809-360F-984F-A48E-F1F6A355A2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="521">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1877,6 +1877,17 @@
   </si>
   <si>
     <t>dic[''.join(sorted(s))] to add to list by sorted s, finally generate dic.values()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maintaining a sliding window approach, use dict to record right idx, if </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>func to find max left/right interval by check each char, be careful for one or two mid value; or; DP ([[]]) to record s[i:j], check upper side of diagona</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3851,8 +3862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="F49" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView topLeftCell="F36" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6378,8 +6389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="F17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6526,7 +6537,9 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
@@ -6537,14 +6550,20 @@
       <c r="F6" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
@@ -6555,8 +6574,12 @@
       <c r="F7" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2">
@@ -7193,16 +7216,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231019] Leetcode - Top-Interview-Medium 52 (6)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D44809-360F-984F-A48E-F1F6A355A2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEB1A7D-BA4D-7445-ADA5-0B0FBC29BE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="538">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1889,6 +1889,58 @@
   <si>
     <t>func to find max left/right interval by check each char, be careful for one or two mid value; or; DP ([[]]) to record s[i:j], check upper side of diagona</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.20</t>
+  </si>
+  <si>
+    <t>first, second to save i, j, so num[i] &lt; first then first = nums[i], next nums[j] &lt; second then second = nums[j], else True</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/783/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/784/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/785/</t>
+  </si>
+  <si>
+    <t>Intersection of Two Linked Lists</t>
+  </si>
+  <si>
+    <t>Odd Even Linked List</t>
+  </si>
+  <si>
+    <t> Add Two Numbers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/786/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/787/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/788/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/789/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/790/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/792/</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node</t>
+  </si>
+  <si>
+    <t>Binary Tree Zigzag Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree Inorder Traversal</t>
   </si>
 </sst>
 </file>
@@ -6390,7 +6442,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="F17:G17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6585,7 +6637,9 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>334</v>
+      </c>
       <c r="C8" s="11"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
@@ -6596,14 +6650,20 @@
       <c r="F8" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>163</v>
+      </c>
       <c r="C9" s="11"/>
       <c r="D9" s="2" t="s">
         <v>38</v>
@@ -6635,7 +6695,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="16">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -6646,8 +6706,12 @@
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>523</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -6660,8 +6724,12 @@
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>524</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
@@ -6674,7 +6742,12 @@
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>525</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
@@ -6689,8 +6762,12 @@
       <c r="D14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>529</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -6703,8 +6780,12 @@
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="6"/>
+      <c r="E15" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>530</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
@@ -6717,8 +6798,12 @@
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="6"/>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>531</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
@@ -6731,8 +6816,12 @@
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="6"/>
+      <c r="E17" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>532</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -6745,8 +6834,12 @@
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="6"/>
+      <c r="E18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>533</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
@@ -6775,8 +6868,12 @@
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="6"/>
+      <c r="E20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>534</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
@@ -7216,16 +7313,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231021] Leetcode - Top-Interview-Medium 52 (8-9)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEB1A7D-BA4D-7445-ADA5-0B0FBC29BE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342546E2-E8FE-314E-9979-E5AA4FD48EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="541">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1941,6 +1941,17 @@
   </si>
   <si>
     <t>Binary Tree Inorder Traversal</t>
+  </si>
+  <si>
+    <t>2023.10.21</t>
+  </si>
+  <si>
+    <t>recurison to root str, for loop for cur str &amp; cnt, finally answer + again</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_list to save v1 + v2 + carry from l1.val, l2.val, l1/l2 next if l1/l2 or None</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3914,8 +3925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="F36" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6442,7 +6453,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6675,13 +6686,14 @@
         <v>499</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>38</v>
+      </c>
       <c r="C10" s="11"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
@@ -6692,14 +6704,20 @@
       <c r="F10" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="16">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
       <c r="C11" s="11" t="s">
         <v>503</v>
       </c>
@@ -6712,8 +6730,12 @@
       <c r="F11" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2">
@@ -7313,16 +7335,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231022] Leetcode - Top-Interview-Medium 52 (10-11)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342546E2-E8FE-314E-9979-E5AA4FD48EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA4599E-F34E-9D43-AAF1-4E112C99214F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="544">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1951,6 +1951,17 @@
   </si>
   <si>
     <t>new_list to save v1 + v2 + carry from l1.val, l2.val, l1/l2 next if l1/l2 or None</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.22</t>
+  </si>
+  <si>
+    <t>two ptr: odd = head, even = evenHead = head.next, loop even &amp; even.next to end, concat odd.next to evenHead, return head</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two ptr to cycle: if shorter one == none then shorter = longer, longer as will (one cycle after will find interaction); or; set add/in; or; stack to pop</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6453,7 +6464,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6741,7 +6752,9 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>328</v>
+      </c>
       <c r="C12" s="11"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
@@ -6752,14 +6765,20 @@
       <c r="F12" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>160</v>
+      </c>
       <c r="C13" s="11"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
@@ -6770,8 +6789,12 @@
       <c r="F13" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2">
@@ -7335,16 +7358,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231023] Leetcode - Top-Interview-Medium 52 (12-13)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA4599E-F34E-9D43-AAF1-4E112C99214F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207EC9D0-C1C9-2445-AADD-D6DAC4D205BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="547">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1962,6 +1962,17 @@
   </si>
   <si>
     <t>two ptr to cycle: if shorter one == none then shorter = longer, longer as will (one cycle after will find interaction); or; set add/in; or; stack to pop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.23</t>
+  </si>
+  <si>
+    <t>recurison: def inorder: inorder(node.left), ans.append(node.val), inorder(node.right)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>queue to save (subroot, level), be care for level, if odd: insert(0,val) else append(val)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6464,7 +6475,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6800,7 +6811,9 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>94</v>
+      </c>
       <c r="C14" s="11" t="s">
         <v>504</v>
       </c>
@@ -6813,14 +6826,20 @@
       <c r="F14" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>103</v>
+      </c>
       <c r="C15" s="11"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
@@ -6831,8 +6850,12 @@
       <c r="F15" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2">
@@ -7358,16 +7381,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231024] Leetcode - Top-Interview-Medium 52 (14-15)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207EC9D0-C1C9-2445-AADD-D6DAC4D205BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927DEBA3-FDCE-8448-9FB4-27CE60277D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="551">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1973,6 +1973,21 @@
   </si>
   <si>
     <t>queue to save (subroot, level), be care for level, if odd: insert(0,val) else append(val)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.24</t>
+  </si>
+  <si>
+    <t>preorder to find root, inorder to find idx, recurison to traver left=[start:idx+1], right = [idx+1:end]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tree compose of inorder and preorder</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>deque with rightNode=None, while q with loop len(q), cur.next, rightNode = rightNode, cur, use extend to add cur.right/cur.left</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3947,8 +3962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6475,7 +6490,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6488,6 +6503,7 @@
     <col min="6" max="6" width="82.33203125" customWidth="1"/>
     <col min="7" max="7" width="116.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6858,10 +6874,12 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="2">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>105</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
@@ -6872,14 +6890,23 @@
       <c r="F16" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>116</v>
+      </c>
       <c r="C17" s="11"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
@@ -6890,8 +6917,12 @@
       <c r="F17" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2">
@@ -7381,16 +7412,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231025] Leetcode - Top-Interview-Medium 52 (16-18)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927DEBA3-FDCE-8448-9FB4-27CE60277D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0410760C-1425-7649-B90A-779F99FE16F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="556">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1776,218 +1776,239 @@
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/776/</t>
   </si>
   <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/777/</t>
+  </si>
+  <si>
+    <t>  Group Anagrams</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/778/</t>
+  </si>
+  <si>
+    <t>  Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/779/</t>
+  </si>
+  <si>
+    <t>  Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/780/</t>
+  </si>
+  <si>
+    <t>  Increasing Triplet Subsequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/781/</t>
+  </si>
+  <si>
+    <t>Missing Ranges</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/4153/</t>
+  </si>
+  <si>
+    <t>  Count and Say</t>
+  </si>
+  <si>
+    <t>Array and Strings</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked List</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trees and Graphs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backtracking</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.16</t>
+  </si>
+  <si>
+    <t>max, min, ans, if nums[i] &lt; 0: max &lt;-&gt; min, find max for answer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.17</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>binary search to find nums[left]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5min</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Sum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list all conditions: 1) all 0, 2) p &amp; n &amp; zero each one 3) two p one n 4) two n one p</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.18</t>
+  </si>
+  <si>
+    <t>check first row/col has zero and set 0 for (1 to end) for each col/row, finally set first row/col to 0 if it contain 0; or; best time/space; use set to record</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dic[''.join(sorted(s))] to add to list by sorted s, finally generate dic.values()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maintaining a sliding window approach, use dict to record right idx, if </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>func to find max left/right interval by check each char, be careful for one or two mid value; or; DP ([[]]) to record s[i:j], check upper side of diagona</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.20</t>
+  </si>
+  <si>
+    <t>first, second to save i, j, so num[i] &lt; first then first = nums[i], next nums[j] &lt; second then second = nums[j], else True</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/783/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/784/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/785/</t>
+  </si>
+  <si>
+    <t>Intersection of Two Linked Lists</t>
+  </si>
+  <si>
+    <t> Add Two Numbers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/786/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/787/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/788/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/789/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/790/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/792/</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node</t>
+  </si>
+  <si>
+    <t>Binary Tree Zigzag Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree Inorder Traversal</t>
+  </si>
+  <si>
+    <t>2023.10.21</t>
+  </si>
+  <si>
+    <t>recurison to root str, for loop for cur str &amp; cnt, finally answer + again</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_list to save v1 + v2 + carry from l1.val, l2.val, l1/l2 next if l1/l2 or None</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.22</t>
+  </si>
+  <si>
+    <t>two ptr: odd = head, even = evenHead = head.next, loop even &amp; even.next to end, concat odd.next to evenHead, return head</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two ptr to cycle: if shorter one == none then shorter = longer, longer as will (one cycle after will find interaction); or; set add/in; or; stack to pop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.23</t>
+  </si>
+  <si>
+    <t>recurison: def inorder: inorder(node.left), ans.append(node.val), inorder(node.right)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>queue to save (subroot, level), be care for level, if odd: insert(0,val) else append(val)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.24</t>
+  </si>
+  <si>
+    <t>preorder to find root, inorder to find idx, recurison to traver left=[start:idx+1], right = [idx+1:end]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tree compose of inorder and preorder</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>deque with rightNode=None, while q with loop len(q), cur.next, rightNode = rightNode, cur, use extend to add cur.right/cur.left</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.24</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.25</t>
+  </si>
+  <si>
+    <t>BST: left &lt; mid &lt; right, so recurison or loop (stack) to run left first, check len(answer) == k or k-1 == 0, then run right</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inorder Successor in BST</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Set Matrix Zeroes</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/777/</t>
-  </si>
-  <si>
-    <t>  Group Anagrams</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/778/</t>
-  </si>
-  <si>
-    <t>  Longest Substring Without Repeating Characters</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/779/</t>
-  </si>
-  <si>
-    <t>  Longest Palindromic Substring</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/780/</t>
-  </si>
-  <si>
-    <t>  Increasing Triplet Subsequence</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/781/</t>
-  </si>
-  <si>
-    <t>Missing Ranges</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Premium</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/4153/</t>
-  </si>
-  <si>
-    <t>  Count and Say</t>
-  </si>
-  <si>
-    <t>Array and Strings</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Linked List</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trees and Graphs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Backtracking</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Array</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.10.16</t>
-  </si>
-  <si>
-    <t>max, min, ans, if nums[i] &lt; 0: max &lt;-&gt; min, find max for answer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.10.17</t>
-  </si>
-  <si>
-    <t>Binary Search</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>binary search to find nums[left]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>5min</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>3Sum</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>list all conditions: 1) all 0, 2) p &amp; n &amp; zero each one 3) two p one n 4) two n one p</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.10.18</t>
-  </si>
-  <si>
-    <t>check first row/col has zero and set 0 for (1 to end) for each col/row, finally set first row/col to 0 if it contain 0; or; best time/space; use set to record</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>dic[''.join(sorted(s))] to add to list by sorted s, finally generate dic.values()</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.10.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maintaining a sliding window approach, use dict to record right idx, if </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>func to find max left/right interval by check each char, be careful for one or two mid value; or; DP ([[]]) to record s[i:j], check upper side of diagona</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.10.20</t>
-  </si>
-  <si>
-    <t>first, second to save i, j, so num[i] &lt; first then first = nums[i], next nums[j] &lt; second then second = nums[j], else True</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/783/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/784/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/107/linked-list/785/</t>
-  </si>
-  <si>
-    <t>Intersection of Two Linked Lists</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Odd Even Linked List</t>
-  </si>
-  <si>
-    <t> Add Two Numbers</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/786/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/787/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/788/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/789/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/790/</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/792/</t>
-  </si>
-  <si>
-    <t>Populating Next Right Pointers in Each Node</t>
-  </si>
-  <si>
-    <t>Binary Tree Zigzag Level Order Traversal</t>
-  </si>
-  <si>
-    <t>Binary Tree Inorder Traversal</t>
-  </si>
-  <si>
-    <t>2023.10.21</t>
-  </si>
-  <si>
-    <t>recurison to root str, for loop for cur str &amp; cnt, finally answer + again</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>new_list to save v1 + v2 + carry from l1.val, l2.val, l1/l2 next if l1/l2 or None</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.10.22</t>
-  </si>
-  <si>
-    <t>two ptr: odd = head, even = evenHead = head.next, loop even &amp; even.next to end, concat odd.next to evenHead, return head</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>two ptr to cycle: if shorter one == none then shorter = longer, longer as will (one cycle after will find interaction); or; set add/in; or; stack to pop</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.10.23</t>
-  </si>
-  <si>
-    <t>recurison: def inorder: inorder(node.left), ans.append(node.val), inorder(node.right)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>queue to save (subroot, level), be care for level, if odd: insert(0,val) else append(val)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023.10.24</t>
-  </si>
-  <si>
-    <t>preorder to find root, inorder to find idx, recurison to traver left=[start:idx+1], right = [idx+1:end]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tree compose of inorder and preorder</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>deque with rightNode=None, while q with loop len(q), cur.next, rightNode = rightNode, cur, use extend to add cur.right/cur.left</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS to check all cell, DFS func set cell = '0' and run to x,y +- 1 if the next cell = '1'</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6333,7 +6354,7 @@
         <v>152</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>38</v>
@@ -6345,10 +6366,10 @@
         <v>100</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>22</v>
@@ -6363,7 +6384,7 @@
         <v>153</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>38</v>
@@ -6375,13 +6396,13 @@
         <v>102</v>
       </c>
       <c r="H79" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="K79" s="2" t="s">
         <v>511</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -6490,7 +6511,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6559,22 +6580,22 @@
         <v>15</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>487</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
@@ -6596,16 +6617,16 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>489</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -6622,16 +6643,16 @@
         <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>491</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -6646,16 +6667,16 @@
         <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>493</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -6670,16 +6691,16 @@
         <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>495</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -6694,16 +6715,16 @@
         <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>497</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -6715,13 +6736,13 @@
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>499</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -6737,16 +6758,16 @@
         <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16">
@@ -6757,22 +6778,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -6787,16 +6808,16 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>527</v>
+        <v>554</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -6808,19 +6829,19 @@
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -6831,22 +6852,22 @@
         <v>94</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -6861,16 +6882,16 @@
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -6888,16 +6909,16 @@
         <v>70</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -6912,23 +6933,25 @@
         <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>230</v>
+      </c>
       <c r="C18" s="11"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
@@ -6937,23 +6960,31 @@
         <v>78</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+        <v>531</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>285</v>
+      </c>
       <c r="C19" s="11"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>552</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -6962,7 +6993,9 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>200</v>
+      </c>
       <c r="C20" s="11"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
@@ -6971,10 +7004,14 @@
         <v>52</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>534</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+        <v>532</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2">
@@ -6982,7 +7019,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="11" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>38</v>
@@ -7147,7 +7184,7 @@
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -7226,7 +7263,7 @@
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -7265,7 +7302,7 @@
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -7398,7 +7435,7 @@
         <v>38</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -7412,16 +7449,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231026] Leetcode - Top-Interview-Medium 52 (19)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0410760C-1425-7649-B90A-779F99FE16F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FD84B2-6F3F-4147-B4F1-65C5C4D86F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="567">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2009,6 +2009,44 @@
   </si>
   <si>
     <t>DFS to check all cell, DFS func set cell = '0' and run to x,y +- 1 if the next cell = '1'</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>  Generate Parentheses</t>
+  </si>
+  <si>
+    <t>Permutations</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subsets</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>  Word Search</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/109/backtracking/797/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/109/backtracking/796/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/109/backtracking/795/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/109/backtracking/794/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/109/backtracking/793/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.26</t>
+  </si>
+  <si>
+    <t>backtracking (combination, next_digits) to reach out all char</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2555,7 +2593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
@@ -3983,8 +4021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6511,7 +6549,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="H24" sqref="G24:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7017,29 +7055,45 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>17</v>
+      </c>
       <c r="C21" s="11" t="s">
         <v>504</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>22</v>
+      </c>
       <c r="C22" s="11"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="6"/>
+      <c r="E22" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>563</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
@@ -7052,8 +7106,12 @@
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="6"/>
+      <c r="E23" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>562</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
@@ -7066,8 +7124,12 @@
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="6"/>
+      <c r="E24" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>561</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
@@ -7080,8 +7142,12 @@
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="6"/>
+      <c r="E25" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>560</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
@@ -7095,7 +7161,7 @@
       <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="2"/>
       <c r="F26" s="6"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -7108,7 +7174,7 @@
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="6"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -7121,7 +7187,7 @@
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
@@ -7449,20 +7515,22 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{DAA83750-82B9-324D-9255-A9482685F25F}"/>
+    <hyperlink ref="F23" r:id="rId2" xr:uid="{75C6E6A3-A8D9-9C47-AF0A-9126415857B3}"/>
+    <hyperlink ref="F21" r:id="rId3" xr:uid="{EDE168FA-0F6F-634A-A5AA-2EC3EA3EBF66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20231027] Leetcode - Top-Interview-Medium 52 (20-21)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FD84B2-6F3F-4147-B4F1-65C5C4D86F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39612946-3D65-A34F-8823-AD6BF969166A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="570">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2047,6 +2047,17 @@
   </si>
   <si>
     <t>backtracking (combination, next_digits) to reach out all char</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.27</t>
+  </si>
+  <si>
+    <t>use left, right to count '(' or ')', if left &lt; n then add '(', if right &lt; left then add ')' to run backtracking</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>backtracking (combination, visited), for idx, v to run nums, if visited: continue, combination add, visited True, run BT, combination pop, visited False</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6549,7 +6560,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="G24:H25"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6560,7 +6571,7 @@
     <col min="4" max="4" width="6.1640625" customWidth="1"/>
     <col min="5" max="5" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="82.33203125" customWidth="1"/>
-    <col min="7" max="7" width="116.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -7094,8 +7105,12 @@
       <c r="F22" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2">
@@ -7112,8 +7127,12 @@
       <c r="F23" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2">
@@ -7515,16 +7534,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231028] Leetcode - Top-Interview-Medium 52 (22-23)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39612946-3D65-A34F-8823-AD6BF969166A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FD5FF4-842B-F841-A7DD-DA3BAF2A5D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="575">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2058,6 +2058,25 @@
   </si>
   <si>
     <t>backtracking (combination, visited), for idx, v to run nums, if visited: continue, combination add, visited True, run BT, combination pop, visited False</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.27</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.28</t>
+  </si>
+  <si>
+    <t>backtracking (combination, idx), append(com) then for I in range(idx, l) next (i+1, com + nums[i)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>backtracking(x, y, level), if level == word_len: return True, check if not x,y range or visited[x][y] or word[level] !=, visited=true, tmp(x+-1, y+-1, level+1), visit=false</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>remember, seem will test</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4032,8 +4051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6559,8 +6578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6970,7 +6989,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:10">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -6994,7 +7013,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -7018,7 +7037,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:10">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -7038,7 +7057,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:10">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -7062,7 +7081,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:10">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -7088,7 +7107,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:10">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -7112,11 +7131,13 @@
         <v>567</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:10">
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2">
+        <v>46</v>
+      </c>
       <c r="C23" s="11"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
@@ -7131,14 +7152,16 @@
         <v>569</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2">
+        <v>78</v>
+      </c>
       <c r="C24" s="11"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
@@ -7149,14 +7172,20 @@
       <c r="F24" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="2">
+      <c r="G24" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="9">
         <v>23</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>79</v>
+      </c>
       <c r="C25" s="11"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
@@ -7167,10 +7196,17 @@
       <c r="F25" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="G25" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -7185,7 +7221,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:10">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -7198,7 +7234,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:10">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -7210,7 +7246,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:10">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -7222,7 +7258,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:10">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -7234,7 +7270,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:10">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -7246,7 +7282,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:10">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -7534,16 +7570,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231029] Leetcode - Top-Interview-Medium 52 (24-25)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FD5FF4-842B-F841-A7DD-DA3BAF2A5D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FDD130-85C8-C547-BEB7-5621FC1EDA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="596">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2077,6 +2077,79 @@
   </si>
   <si>
     <t>remember, seem will test</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sort Colors</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/798/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/799/</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/800/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/802/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/803/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/806/</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix II</t>
+  </si>
+  <si>
+    <t>Meeting Rooms II</t>
+  </si>
+  <si>
+    <t>Find Peak Element</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search for a Range</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/801/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/804/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Premium</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.29</t>
+  </si>
+  <si>
+    <t>two ptr: left=0, right=len-1, while ptr &lt;= right: if ptr=0 switch ptr and left, ptr=2 switch ptr and right, ptr=1 nothing</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sorted(count.items(), key = lambda item:item[1], reverse = True)</t>
+  </si>
+  <si>
+    <t>Counter with heapq or Sorted</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2624,7 +2697,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6578,8 +6651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6588,8 +6661,8 @@
     <col min="2" max="2" width="7.1640625" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.1640625" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="82.33203125" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="6" max="6" width="85.6640625" customWidth="1"/>
     <col min="7" max="7" width="130.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.1640625" bestFit="1" customWidth="1"/>
@@ -7210,29 +7283,54 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
+      <c r="B26" s="2">
+        <v>75</v>
+      </c>
       <c r="C26" s="11" t="s">
         <v>128</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="2">
         <v>25</v>
       </c>
+      <c r="B27" s="2">
+        <v>347</v>
+      </c>
       <c r="C27" s="11"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="J27" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="2">
@@ -7242,7 +7340,12 @@
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>580</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
@@ -7254,7 +7357,12 @@
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>589</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
@@ -7266,7 +7374,12 @@
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>581</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
@@ -7278,7 +7391,12 @@
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>582</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
@@ -7290,8 +7408,12 @@
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="E32" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>590</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
@@ -7303,9 +7425,11 @@
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="2" t="s">
+        <v>585</v>
+      </c>
       <c r="F33" s="2" t="s">
-        <v>498</v>
+        <v>591</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -7318,7 +7442,12 @@
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>583</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
@@ -7332,7 +7461,8 @@
       <c r="D35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="6"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
@@ -7344,7 +7474,8 @@
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="6"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="6"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
@@ -7356,7 +7487,7 @@
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="6"/>
+      <c r="E37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
@@ -7368,7 +7499,7 @@
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
@@ -7570,22 +7701,24 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{DAA83750-82B9-324D-9255-A9482685F25F}"/>
     <hyperlink ref="F23" r:id="rId2" xr:uid="{75C6E6A3-A8D9-9C47-AF0A-9126415857B3}"/>
     <hyperlink ref="F21" r:id="rId3" xr:uid="{EDE168FA-0F6F-634A-A5AA-2EC3EA3EBF66}"/>
+    <hyperlink ref="F26" r:id="rId4" xr:uid="{5BC4F9F1-046B-0E4D-BD56-EF580A1D6AC7}"/>
+    <hyperlink ref="E33" r:id="rId5" display="https://leetcode.com/problems/meeting-rooms-ii/" xr:uid="{F37CEB58-E4BE-0244-B88A-6F88ADD52801}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20231030] Leetcode - Top-Interview-Medium 52 (26-27)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FDD130-85C8-C547-BEB7-5621FC1EDA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA2DC75-AC1A-5D4F-BF9D-4563889B18A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="600">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2150,6 +2150,21 @@
   </si>
   <si>
     <t>Counter with heapq or Sorted</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.30</t>
+  </si>
+  <si>
+    <t>Quicksort!!</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sorted; or; heapq with heapify; or; quicksort(TLE)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>binary search (refer to four template for BS)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6651,8 +6666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7336,6 +7351,9 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
+      <c r="B28" s="2">
+        <v>215</v>
+      </c>
       <c r="C28" s="11"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
@@ -7346,13 +7364,23 @@
       <c r="F28" s="6" t="s">
         <v>580</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="2">
         <v>27</v>
       </c>
+      <c r="B29" s="2">
+        <v>162</v>
+      </c>
       <c r="C29" s="11"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
@@ -7363,8 +7391,12 @@
       <c r="F29" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="2">
@@ -7701,16 +7733,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231031] Leetcode - Top-Interview-Medium 52 (28-29)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA2DC75-AC1A-5D4F-BF9D-4563889B18A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527CEFF4-E757-4E4B-A388-174A6536CE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="603">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2119,10 +2119,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Search for a Range</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Search in Rotated Sorted Array</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2165,6 +2161,22 @@
   </si>
   <si>
     <t>binary search (refer to four template for BS)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.31</t>
+  </si>
+  <si>
+    <t>Search for a Range
+Find First and Last Position of Element in Sorted Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>binary search with while to reach left/right boundary; or; BS with Boolean to run two times BS for left or right boundary</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort first, if not ans or ans[-1][1] &lt; inte[0]: append, else ans[-1][1] = max(ans[-1][1], inte[1]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2324,7 +2336,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2393,6 +2405,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6666,8 +6681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6676,7 +6691,7 @@
     <col min="2" max="2" width="7.1640625" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.1640625" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="5" max="5" width="49" customWidth="1"/>
     <col min="6" max="6" width="85.6640625" customWidth="1"/>
     <col min="7" max="7" width="130.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
@@ -7314,10 +7329,10 @@
         <v>576</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -7338,13 +7353,13 @@
         <v>578</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J27" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -7365,13 +7380,13 @@
         <v>580</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>596</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -7389,36 +7404,46 @@
         <v>586</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="32">
       <c r="A30" s="2">
         <v>28</v>
       </c>
+      <c r="B30" s="2">
+        <v>34</v>
+      </c>
       <c r="C30" s="11"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>587</v>
+      <c r="E30" s="23" t="s">
+        <v>600</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="2">
         <v>29</v>
       </c>
+      <c r="B31" s="2">
+        <v>56</v>
+      </c>
       <c r="C31" s="11"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
@@ -7429,8 +7454,12 @@
       <c r="F31" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2">
@@ -7441,10 +7470,10 @@
         <v>38</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -7461,7 +7490,7 @@
         <v>585</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -7733,16 +7762,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231101] Leetcode - Top-Interview-Medium 52 (30-32)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527CEFF4-E757-4E4B-A388-174A6536CE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C99470-1E94-4C49-AD3E-C1F55B9B109A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="606">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2177,6 +2177,18 @@
   </si>
   <si>
     <t>sort first, if not ans or ans[-1][1] &lt; inte[0]: append, else ans[-1][1] = max(ans[-1][1], inte[1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS but includes two logic: first if mid==target: return, #if left]&lt;=mid then if left &lt; =target &lt; mid: right=mid-1 else left=mid+1#, ## again for else with reverse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two methods: 1. set start from left bottom cornor: if m[i][j] &gt; tar then &gt; target: move up else move right, or; 2. scan each row and BS for col element</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2371,6 +2383,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2405,9 +2420,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2741,14 +2753,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -2790,7 +2802,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -2823,7 +2835,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -2849,7 +2861,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2873,7 +2885,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2897,7 +2909,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2921,7 +2933,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2945,7 +2957,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2969,7 +2981,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2993,7 +3005,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -3017,7 +3029,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -3041,7 +3053,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3065,7 +3077,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>125</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3091,7 +3103,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3115,7 +3127,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3139,7 +3151,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3163,7 +3175,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3187,7 +3199,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -3211,7 +3223,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3235,7 +3247,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3259,7 +3271,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -3285,7 +3297,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -3309,7 +3321,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3333,7 +3345,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3357,7 +3369,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3381,7 +3393,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3405,7 +3417,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -3431,7 +3443,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -3455,7 +3467,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="11"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3479,7 +3491,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -3503,7 +3515,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -3527,7 +3539,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>128</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -3553,7 +3565,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -3577,7 +3589,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>129</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -3603,7 +3615,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -3627,7 +3639,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="11"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -3651,7 +3663,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -3675,7 +3687,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="12" t="s">
         <v>130</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -3701,7 +3713,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -3725,7 +3737,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="12" t="s">
         <v>131</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -3751,7 +3763,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="11"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -3775,7 +3787,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="11"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -3799,7 +3811,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -3823,7 +3835,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="12" t="s">
         <v>132</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -3849,7 +3861,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="11"/>
+      <c r="C46" s="12"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -3873,7 +3885,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="C47" s="12"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -3897,7 +3909,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="11"/>
+      <c r="C48" s="12"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -3921,7 +3933,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="11"/>
+      <c r="C49" s="12"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -3945,7 +3957,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="11"/>
+      <c r="C50" s="12"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -4175,15 +4187,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -4227,7 +4239,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="23">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -4265,7 +4277,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="22"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -4296,7 +4308,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -4326,7 +4338,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -4356,7 +4368,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -4386,7 +4398,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="22"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -4416,7 +4428,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -4446,7 +4458,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="22"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -4476,7 +4488,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="22"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -4506,7 +4518,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -4536,7 +4548,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -4566,7 +4578,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -4596,7 +4608,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -4629,7 +4641,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="18">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -4661,7 +4673,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -4691,7 +4703,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -4721,7 +4733,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -4751,7 +4763,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="2">
         <v>206</v>
       </c>
@@ -4781,7 +4793,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="2">
         <v>169</v>
       </c>
@@ -4811,7 +4823,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="17"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="2">
         <v>67</v>
       </c>
@@ -4841,7 +4853,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="17"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="2">
         <v>543</v>
       </c>
@@ -4871,7 +4883,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="17"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="2">
         <v>876</v>
       </c>
@@ -4901,7 +4913,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="2">
         <v>104</v>
       </c>
@@ -4931,7 +4943,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="2">
         <v>217</v>
       </c>
@@ -4961,7 +4973,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="2">
         <v>53</v>
       </c>
@@ -4991,7 +5003,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="19">
         <v>3</v>
       </c>
       <c r="C28" s="2">
@@ -5023,7 +5035,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="18"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2">
         <v>542</v>
       </c>
@@ -5053,7 +5065,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="18"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="2">
         <v>973</v>
       </c>
@@ -5083,7 +5095,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="18"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="2">
         <v>3</v>
       </c>
@@ -5113,7 +5125,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="18"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="2">
         <v>15</v>
       </c>
@@ -5143,7 +5155,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="18"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="2">
         <v>102</v>
       </c>
@@ -5173,7 +5185,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="18"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="2">
         <v>133</v>
       </c>
@@ -5206,7 +5218,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="18"/>
+      <c r="B35" s="19"/>
       <c r="C35" s="2">
         <v>150</v>
       </c>
@@ -5236,7 +5248,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B36" s="20">
         <v>4</v>
       </c>
       <c r="C36" s="2">
@@ -5271,7 +5283,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="2">
         <v>208</v>
       </c>
@@ -5301,7 +5313,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="19"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="2">
         <v>322</v>
       </c>
@@ -5331,7 +5343,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="19"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="2">
         <v>238</v>
       </c>
@@ -5361,7 +5373,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="19"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="2">
         <v>155</v>
       </c>
@@ -5391,7 +5403,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="19"/>
+      <c r="B41" s="20"/>
       <c r="C41" s="2">
         <v>98</v>
       </c>
@@ -5421,7 +5433,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="2">
         <v>200</v>
       </c>
@@ -5451,7 +5463,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="19"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="2">
         <v>994</v>
       </c>
@@ -5481,7 +5493,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" s="21">
         <v>5</v>
       </c>
       <c r="C44" s="2">
@@ -5513,7 +5525,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="20"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="2">
         <v>39</v>
       </c>
@@ -5546,7 +5558,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="20"/>
+      <c r="B46" s="21"/>
       <c r="C46" s="2">
         <v>46</v>
       </c>
@@ -5576,7 +5588,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="20"/>
+      <c r="B47" s="21"/>
       <c r="C47" s="2">
         <v>56</v>
       </c>
@@ -5606,7 +5618,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="20"/>
+      <c r="B48" s="21"/>
       <c r="C48" s="2">
         <v>236</v>
       </c>
@@ -5636,7 +5648,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="20"/>
+      <c r="B49" s="21"/>
       <c r="C49" s="2">
         <v>981</v>
       </c>
@@ -5666,7 +5678,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="20"/>
+      <c r="B50" s="21"/>
       <c r="C50" s="2">
         <v>721</v>
       </c>
@@ -5699,7 +5711,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="20"/>
+      <c r="B51" s="21"/>
       <c r="C51" s="2">
         <v>75</v>
       </c>
@@ -5729,7 +5741,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="21">
+      <c r="B52" s="22">
         <v>6</v>
       </c>
       <c r="C52" s="2">
@@ -5761,7 +5773,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="21"/>
+      <c r="B53" s="22"/>
       <c r="C53" s="2">
         <v>416</v>
       </c>
@@ -5791,7 +5803,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="21"/>
+      <c r="B54" s="22"/>
       <c r="C54" s="2">
         <v>8</v>
       </c>
@@ -5821,7 +5833,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="21"/>
+      <c r="B55" s="22"/>
       <c r="C55" s="2">
         <v>54</v>
       </c>
@@ -5851,7 +5863,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="21"/>
+      <c r="B56" s="22"/>
       <c r="C56" s="2">
         <v>78</v>
       </c>
@@ -5881,7 +5893,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="21"/>
+      <c r="B57" s="22"/>
       <c r="C57" s="2">
         <v>199</v>
       </c>
@@ -5911,7 +5923,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="21"/>
+      <c r="B58" s="22"/>
       <c r="C58" s="2">
         <v>5</v>
       </c>
@@ -5941,7 +5953,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="21"/>
+      <c r="B59" s="22"/>
       <c r="C59" s="2">
         <v>62</v>
       </c>
@@ -5971,7 +5983,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="21"/>
+      <c r="B60" s="22"/>
       <c r="C60" s="2">
         <v>105</v>
       </c>
@@ -6001,7 +6013,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="14">
+      <c r="B61" s="15">
         <v>7</v>
       </c>
       <c r="C61" s="2">
@@ -6033,7 +6045,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="14"/>
+      <c r="B62" s="15"/>
       <c r="C62" s="2">
         <v>17</v>
       </c>
@@ -6063,7 +6075,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="14"/>
+      <c r="B63" s="15"/>
       <c r="C63" s="2">
         <v>79</v>
       </c>
@@ -6093,7 +6105,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="14"/>
+      <c r="B64" s="15"/>
       <c r="C64" s="2">
         <v>438</v>
       </c>
@@ -6123,7 +6135,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="14"/>
+      <c r="B65" s="15"/>
       <c r="C65" s="2">
         <v>310</v>
       </c>
@@ -6153,7 +6165,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="14"/>
+      <c r="B66" s="15"/>
       <c r="C66" s="2">
         <v>621</v>
       </c>
@@ -6183,7 +6195,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="14"/>
+      <c r="B67" s="15"/>
       <c r="C67" s="2">
         <v>146</v>
       </c>
@@ -6213,7 +6225,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="15">
+      <c r="B68" s="16">
         <v>8</v>
       </c>
       <c r="C68" s="2">
@@ -6245,7 +6257,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="15"/>
+      <c r="B69" s="16"/>
       <c r="C69" s="2">
         <v>76</v>
       </c>
@@ -6275,7 +6287,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="15"/>
+      <c r="B70" s="16"/>
       <c r="C70" s="2">
         <v>297</v>
       </c>
@@ -6305,7 +6317,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="15"/>
+      <c r="B71" s="16"/>
       <c r="C71" s="2">
         <v>42</v>
       </c>
@@ -6335,7 +6347,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="15"/>
+      <c r="B72" s="16"/>
       <c r="C72" s="2">
         <v>295</v>
       </c>
@@ -6365,7 +6377,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="15"/>
+      <c r="B73" s="16"/>
       <c r="C73" s="2">
         <v>127</v>
       </c>
@@ -6395,7 +6407,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="15"/>
+      <c r="B74" s="16"/>
       <c r="C74" s="2">
         <v>224</v>
       </c>
@@ -6425,7 +6437,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="15"/>
+      <c r="B75" s="16"/>
       <c r="C75" s="2">
         <v>1235</v>
       </c>
@@ -6455,7 +6467,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="15"/>
+      <c r="B76" s="16"/>
       <c r="C76" s="2">
         <v>23</v>
       </c>
@@ -6485,7 +6497,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="15"/>
+      <c r="B77" s="16"/>
       <c r="C77" s="2">
         <v>84</v>
       </c>
@@ -6518,7 +6530,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="12" t="s">
         <v>132</v>
       </c>
       <c r="C78" s="2">
@@ -6550,7 +6562,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="11"/>
+      <c r="B79" s="12"/>
       <c r="C79" s="2">
         <v>153</v>
       </c>
@@ -6586,15 +6598,15 @@
       <c r="A85" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -6681,8 +6693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6699,14 +6711,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>486</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -6750,7 +6762,7 @@
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>501</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -6783,7 +6795,7 @@
       <c r="B4" s="2">
         <v>73</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -6809,7 +6821,7 @@
       <c r="B5" s="2">
         <v>49</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -6833,7 +6845,7 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
@@ -6857,7 +6869,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
@@ -6881,7 +6893,7 @@
       <c r="B8" s="2">
         <v>334</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
@@ -6905,7 +6917,7 @@
       <c r="B9" s="2">
         <v>163</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -6924,7 +6936,7 @@
       <c r="B10" s="2">
         <v>38</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
@@ -6948,7 +6960,7 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>502</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -6974,7 +6986,7 @@
       <c r="B12" s="2">
         <v>328</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -6998,7 +7010,7 @@
       <c r="B13" s="2">
         <v>160</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
@@ -7022,7 +7034,7 @@
       <c r="B14" s="2">
         <v>94</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>503</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -7048,7 +7060,7 @@
       <c r="B15" s="2">
         <v>103</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -7072,7 +7084,7 @@
       <c r="B16" s="2">
         <v>105</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
@@ -7099,7 +7111,7 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
@@ -7123,7 +7135,7 @@
       <c r="B18" s="2">
         <v>230</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -7147,7 +7159,7 @@
       <c r="B19" s="2">
         <v>285</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -7167,7 +7179,7 @@
       <c r="B20" s="2">
         <v>200</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
@@ -7191,7 +7203,7 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>504</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -7217,7 +7229,7 @@
       <c r="B22" s="2">
         <v>22</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
@@ -7241,7 +7253,7 @@
       <c r="B23" s="2">
         <v>46</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -7265,7 +7277,7 @@
       <c r="B24" s="2">
         <v>78</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
@@ -7289,7 +7301,7 @@
       <c r="B25" s="2">
         <v>79</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
@@ -7316,7 +7328,7 @@
       <c r="B26" s="2">
         <v>75</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="12" t="s">
         <v>128</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -7342,7 +7354,7 @@
       <c r="B27" s="2">
         <v>347</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -7369,7 +7381,7 @@
       <c r="B28" s="2">
         <v>215</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -7396,7 +7408,7 @@
       <c r="B29" s="2">
         <v>162</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -7420,11 +7432,11 @@
       <c r="B30" s="2">
         <v>34</v>
       </c>
-      <c r="C30" s="11"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="11" t="s">
         <v>600</v>
       </c>
       <c r="F30" s="6" t="s">
@@ -7444,7 +7456,7 @@
       <c r="B31" s="2">
         <v>56</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -7465,7 +7477,10 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="B32" s="2">
+        <v>33</v>
+      </c>
+      <c r="C32" s="12"/>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -7475,14 +7490,21 @@
       <c r="F32" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="B33" s="2">
+        <v>253</v>
+      </c>
+      <c r="C33" s="12"/>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
@@ -7499,7 +7521,10 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="B34" s="2">
+        <v>240</v>
+      </c>
+      <c r="C34" s="12"/>
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
@@ -7509,14 +7534,18 @@
       <c r="F34" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>129</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -7531,7 +7560,7 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
@@ -7544,7 +7573,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="C37" s="11"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -7556,7 +7585,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -7568,7 +7597,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="12" t="s">
         <v>130</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -7585,7 +7614,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -7597,7 +7626,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="C41" s="11"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
@@ -7609,7 +7638,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="C42" s="11"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -7624,7 +7653,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="12" t="s">
         <v>131</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -7638,7 +7667,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
@@ -7651,7 +7680,7 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="C45" s="11"/>
+      <c r="C45" s="12"/>
       <c r="D45" s="2" t="s">
         <v>38</v>
       </c>
@@ -7663,7 +7692,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="11"/>
+      <c r="C46" s="12"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
@@ -7675,7 +7704,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="C47" s="12"/>
       <c r="D47" s="2" t="s">
         <v>38</v>
       </c>
@@ -7687,7 +7716,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="C48" s="11"/>
+      <c r="C48" s="12"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
@@ -7699,7 +7728,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="C49" s="11"/>
+      <c r="C49" s="12"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
@@ -7711,7 +7740,7 @@
       <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="12" t="s">
         <v>132</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -7725,7 +7754,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="C51" s="11"/>
+      <c r="C51" s="12"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
@@ -7734,7 +7763,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="C52" s="11"/>
+      <c r="C52" s="12"/>
       <c r="D52" s="2" t="s">
         <v>38</v>
       </c>
@@ -7743,7 +7772,7 @@
       <c r="A53" s="2">
         <v>51</v>
       </c>
-      <c r="C53" s="11"/>
+      <c r="C53" s="12"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
@@ -7755,23 +7784,23 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="C54" s="11"/>
+      <c r="C54" s="12"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231102] Leetcode - Top-Interview-Medium 52 (33-34)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C99470-1E94-4C49-AD3E-C1F55B9B109A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC6559D-9F49-004D-851D-494DE13A5593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="615">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2189,6 +2189,38 @@
   </si>
   <si>
     <t>two methods: 1. set start from left bottom cornor: if m[i][j] &gt; tar then &gt; target: move up else move right, or; 2. scan each row and BS for col element</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/111/dynamic-programming/810/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/111/dynamic-programming/809/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/111/dynamic-programming/807/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/111/dynamic-programming/808/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jump Game</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Longest Increasing Subsequence</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.02</t>
+  </si>
+  <si>
+    <t>check each nums[idx] + idx can reach destination, if so, destination set to current idx</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dp[m][n]: i=0 or j=0 then dp[i][j]=1, else dp[i][j] = dp[i-1][j]+dp[i][j-1]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6693,8 +6725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7545,29 +7577,51 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
+      <c r="B35" s="2">
+        <v>55</v>
+      </c>
       <c r="C35" s="12" t="s">
         <v>129</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2">
         <v>34</v>
       </c>
+      <c r="B36" s="2">
+        <v>62</v>
+      </c>
       <c r="C36" s="12"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2">
@@ -7577,7 +7631,12 @@
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>607</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
@@ -7589,7 +7648,12 @@
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>606</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
@@ -7603,9 +7667,9 @@
       <c r="D39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="11"/>
       <c r="F39" s="2" t="s">
-        <v>498</v>
+        <v>590</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -7618,7 +7682,7 @@
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
@@ -7644,7 +7708,7 @@
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="2" t="s">
-        <v>498</v>
+        <v>590</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -7791,16 +7855,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231103] Leetcode - Top-Interview-Medium 52 (35-36)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC6559D-9F49-004D-851D-494DE13A5593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769648E1-FB80-D94C-97B8-D53F09680324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="619">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2221,6 +2221,20 @@
   </si>
   <si>
     <t>dp[m][n]: i=0 or j=0 then dp[i][j]=1, else dp[i][j] = dp[i-1][j]+dp[i][j-1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.03</t>
+  </si>
+  <si>
+    <t>minCoin[curNum] = min(minCoin[curNum], minCoin[curNum - coin] + 1)</t>
+  </si>
+  <si>
+    <t>smaller num will replace nums[-1]: 1. use bisect_left iteration to replace, 2. DP: check how many number can be in front of dp[i], if so, max(dp[i],dp[j]+1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bisect: find the index for insert nums[i] in order</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4198,7 +4212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
@@ -6725,8 +6739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6739,7 +6753,7 @@
     <col min="6" max="6" width="85.6640625" customWidth="1"/>
     <col min="7" max="7" width="130.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="56.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -7529,7 +7543,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:10">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -7549,7 +7563,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:10">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -7573,7 +7587,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:10">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -7599,7 +7613,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:10">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -7623,10 +7637,13 @@
         <v>612</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:10">
       <c r="A37" s="2">
         <v>35</v>
       </c>
+      <c r="B37" s="2">
+        <v>322</v>
+      </c>
       <c r="C37" s="12"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
@@ -7637,13 +7654,20 @@
       <c r="F37" s="6" t="s">
         <v>607</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="G37" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="2">
         <v>36</v>
       </c>
+      <c r="B38" s="2">
+        <v>300</v>
+      </c>
       <c r="C38" s="12"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
@@ -7654,10 +7678,17 @@
       <c r="F38" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="G38" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="J38" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -7674,7 +7705,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:10">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -7686,7 +7717,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:10">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -7698,7 +7729,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:10">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -7713,7 +7744,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:10">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -7727,7 +7758,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:10">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -7740,7 +7771,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:10">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -7752,7 +7783,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:10">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -7764,7 +7795,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:10">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -7776,7 +7807,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:10">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -7855,16 +7886,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231104] Leetcode - Top-Interview-Medium 52 (38)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769648E1-FB80-D94C-97B8-D53F09680324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B3BB0E-6DB2-BB4D-A845-3DAFC0D0E74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="627">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2235,6 +2235,33 @@
   </si>
   <si>
     <t>bisect: find the index for insert nums[i] in order</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flatten 2D Vector</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/112/design/812/</t>
+  </si>
+  <si>
+    <t>Insert Delete GetRandom O(1)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/112/design/813/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design Tic-Tac-Toe</t>
+  </si>
+  <si>
+    <t>Serialize and Deserialize Binary Tree</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.04</t>
+  </si>
+  <si>
+    <t>use preOrder with ' '.join to list (serialize), deque(data.split()) with popleft to deserialize</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6739,8 +6766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7692,40 +7719,64 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
+      <c r="B39" s="2">
+        <v>251</v>
+      </c>
       <c r="C39" s="12" t="s">
         <v>130</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="11"/>
+      <c r="E39" s="2" t="s">
+        <v>619</v>
+      </c>
       <c r="F39" s="2" t="s">
         <v>590</v>
       </c>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="2">
         <v>38</v>
       </c>
+      <c r="B40" s="2">
+        <v>297</v>
+      </c>
       <c r="C40" s="12"/>
       <c r="D40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="2">
         <v>39</v>
       </c>
+      <c r="B41" s="2">
+        <v>380</v>
+      </c>
       <c r="C41" s="12"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>622</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
@@ -7733,11 +7784,16 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
+      <c r="B42" s="2">
+        <v>348</v>
+      </c>
       <c r="C42" s="12"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="6"/>
+      <c r="E42" s="2" t="s">
+        <v>623</v>
+      </c>
       <c r="F42" s="2" t="s">
         <v>590</v>
       </c>
@@ -7754,7 +7810,7 @@
       <c r="D43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
@@ -7766,7 +7822,7 @@
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E44" s="6"/>
+      <c r="E44" s="2"/>
       <c r="F44" s="6"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -7886,16 +7942,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -7904,6 +7960,9 @@
     <hyperlink ref="F21" r:id="rId3" xr:uid="{EDE168FA-0F6F-634A-A5AA-2EC3EA3EBF66}"/>
     <hyperlink ref="F26" r:id="rId4" xr:uid="{5BC4F9F1-046B-0E4D-BD56-EF580A1D6AC7}"/>
     <hyperlink ref="E33" r:id="rId5" display="https://leetcode.com/problems/meeting-rooms-ii/" xr:uid="{F37CEB58-E4BE-0244-B88A-6F88ADD52801}"/>
+    <hyperlink ref="E39" r:id="rId6" display="https://leetcode.com/problems/flatten-2d-vector/" xr:uid="{6E932F6C-C5CF-6F40-85DE-B544500B10B6}"/>
+    <hyperlink ref="F41" r:id="rId7" xr:uid="{44B3F707-1C15-9349-AAAF-736092E1CF37}"/>
+    <hyperlink ref="E42" r:id="rId8" display="https://leetcode.com/problems/design-tic-tac-toe/" xr:uid="{60846593-E208-244C-9E3C-68800E4AFEA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20231105] Leetcode - Top-Interview-Medium 52 (39)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B3BB0E-6DB2-BB4D-A845-3DAFC0D0E74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEDC620-DDD6-D745-B0AB-429B185C0B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="630">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2262,6 +2262,16 @@
   </si>
   <si>
     <t>use preOrder with ' '.join to list (serialize), deque(data.split()) with popleft to deserialize</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.05</t>
+  </si>
+  <si>
+    <t>random.choice(self.data)</t>
+  </si>
+  <si>
+    <t>use dict &amp; list to save idx, remove need switch [-1] &lt;-&gt; [val] in dict, data then del and pop()</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6766,8 +6776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7777,8 +7787,15 @@
       <c r="F41" s="6" t="s">
         <v>622</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="J41" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="2">
@@ -7942,16 +7959,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231106] Leetcode - Top-Interview-Medium 52 (41-42)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEDC620-DDD6-D745-B0AB-429B185C0B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90D5DC6-DECE-8645-82B2-993E9356D7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="646">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2272,6 +2272,66 @@
   </si>
   <si>
     <t>use dict &amp; list to save idx, remove need switch [-1] &lt;-&gt; [val] in dict, data then del and pop()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Happy Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/113/math/815/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Factorial Trailing Zeroes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/113/math/817/</t>
+  </si>
+  <si>
+    <t>Excel Sheet Column Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pow(x, n)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/113/math/819/</t>
+  </si>
+  <si>
+    <t>Sqrt(x)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Divide Two Integers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/113/math/821/</t>
+  </si>
+  <si>
+    <t>Fraction to Recurring Decimal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/113/math/818/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.06</t>
+  </si>
+  <si>
+    <t>while n != 1: with set(), if in set will false, else cnt again</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/113/math/816/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pattern = 5, 5! -&gt; one 0, 25! -&gt; six 0, count how many 5! Times</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6776,8 +6836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7815,34 +7875,56 @@
         <v>590</v>
       </c>
       <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="2">
         <v>41</v>
       </c>
+      <c r="B43" s="2">
+        <v>202</v>
+      </c>
       <c r="C43" s="12" t="s">
         <v>131</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="2">
         <v>42</v>
       </c>
+      <c r="B44" s="2">
+        <v>172</v>
+      </c>
       <c r="C44" s="12"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="2">
@@ -7852,7 +7934,12 @@
       <c r="D45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="6"/>
+      <c r="E45" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>633</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
@@ -7864,7 +7951,12 @@
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="6"/>
+      <c r="E46" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>641</v>
+      </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
@@ -7876,7 +7968,12 @@
       <c r="D47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>636</v>
+      </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
@@ -7888,7 +7985,12 @@
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="6"/>
+      <c r="E48" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>590</v>
+      </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
@@ -7900,7 +8002,12 @@
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>639</v>
+      </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
@@ -7914,7 +8021,7 @@
       <c r="D50" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E50" s="6"/>
+      <c r="E50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
@@ -7959,16 +8066,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -7980,6 +8087,8 @@
     <hyperlink ref="E39" r:id="rId6" display="https://leetcode.com/problems/flatten-2d-vector/" xr:uid="{6E932F6C-C5CF-6F40-85DE-B544500B10B6}"/>
     <hyperlink ref="F41" r:id="rId7" xr:uid="{44B3F707-1C15-9349-AAAF-736092E1CF37}"/>
     <hyperlink ref="E42" r:id="rId8" display="https://leetcode.com/problems/design-tic-tac-toe/" xr:uid="{60846593-E208-244C-9E3C-68800E4AFEA2}"/>
+    <hyperlink ref="F43" r:id="rId9" xr:uid="{5932DEC8-20C8-C649-9D15-FC22C096FE7F}"/>
+    <hyperlink ref="F44" r:id="rId10" xr:uid="{6DD4110D-7061-1C46-A430-79DA813250EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20231107] Leetcode - Top-Interview-Medium 52 (43-44)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90D5DC6-DECE-8645-82B2-993E9356D7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859B7FFC-96D2-BF46-A204-DA118EF391B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="651">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2332,6 +2332,25 @@
   </si>
   <si>
     <t>pattern = 5, 5! -&gt; one 0, 25! -&gt; six 0, count how many 5! Times</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.07</t>
+  </si>
+  <si>
+    <t>char to ascii - A: 26 * answer + (ord(c) - a) + 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ord() -&gt; char to ascii</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>x ** n; or; recurision: n=0,1 return 1 or x, tmp = recur(x, n//2) if n % 2 == 0: tmp*tmp, else x * tmp*tmp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>math for pow()</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6836,8 +6855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6850,7 +6869,7 @@
     <col min="6" max="6" width="85.6640625" customWidth="1"/>
     <col min="7" max="7" width="130.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="56.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6926,7 +6945,7 @@
       <c r="I3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="7"/>
       <c r="K3" t="s">
         <v>0</v>
       </c>
@@ -6955,7 +6974,7 @@
         <v>514</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2">
@@ -7513,7 +7532,7 @@
       <c r="H27" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="2" t="s">
         <v>593</v>
       </c>
     </row>
@@ -7781,7 +7800,7 @@
       <c r="H38" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="2" t="s">
         <v>618</v>
       </c>
     </row>
@@ -7853,7 +7872,7 @@
       <c r="H41" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="2" t="s">
         <v>628</v>
       </c>
     </row>
@@ -7930,9 +7949,12 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
+      <c r="B45" s="2">
+        <v>171</v>
+      </c>
       <c r="C45" s="12"/>
       <c r="D45" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>634</v>
@@ -7940,13 +7962,23 @@
       <c r="F45" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
+      <c r="G45" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="2">
         <v>44</v>
       </c>
+      <c r="B46" s="2">
+        <v>50</v>
+      </c>
       <c r="C46" s="12"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
@@ -7957,8 +7989,15 @@
       <c r="F46" s="6" t="s">
         <v>641</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+      <c r="G46" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="2">
@@ -8066,16 +8105,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231108] Leetcode - Top-Interview-Medium 52 (45-47)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859B7FFC-96D2-BF46-A204-DA118EF391B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F1C1DA-63F3-8C40-B734-2333F5E7A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="656">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2351,6 +2351,25 @@
   </si>
   <si>
     <t>math for pow()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.08</t>
+  </si>
+  <si>
+    <t>while t,p * tmp &lt; x: tmp = (tmp + x // tmp) // 2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sqrt -&gt; tmp = (tmp + x // tmp) // 2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.08</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>numerator/denominator: first part for Integer by //, else for after '.' by using dict to save position of remainder with while to remainder * 10 // demo…loop</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6855,8 +6874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8003,9 +8022,12 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
+      <c r="B47" s="2">
+        <v>69</v>
+      </c>
       <c r="C47" s="12"/>
       <c r="D47" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>637</v>
@@ -8013,13 +8035,23 @@
       <c r="F47" s="6" t="s">
         <v>636</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
+      <c r="G47" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="2">
         <v>46</v>
       </c>
+      <c r="B48" s="2">
+        <v>29</v>
+      </c>
       <c r="C48" s="12"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
@@ -8037,6 +8069,9 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
+      <c r="B49" s="2">
+        <v>166</v>
+      </c>
       <c r="C49" s="12"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
@@ -8047,8 +8082,12 @@
       <c r="F49" s="6" t="s">
         <v>639</v>
       </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="G49" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2">
@@ -8105,16 +8144,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231109] Leetcode - Top-Interview-Medium 52 (48-49)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F1C1DA-63F3-8C40-B734-2333F5E7A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7BA5AB-A531-4B4C-A052-A50E1E9F1757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="669">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2370,6 +2370,54 @@
   </si>
   <si>
     <t>numerator/denominator: first part for Integer by //, else for after '.' by using dict to save position of remainder with while to remainder * 10 // demo…loop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.09</t>
+  </si>
+  <si>
+    <t>Sum of Two Integers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Evaluate Reverse Polish Notation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Majority Element</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task Scheduler</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find the Celebrity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/114/others/826/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/114/others/824/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/114/others/822/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/114/others/823/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>use XOR and AND withmask (0xffffffff) to cal, mask to confirm sign for b, carry = (a&amp;b) &lt;&lt; 1, a = a ^ b</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> use stack to if not  '+-*/': append else pop and check if '+-*/' and  append(pop '+-*/' pop), return stack[0]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6874,8 +6922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8093,23 +8141,50 @@
       <c r="A50" s="2">
         <v>48</v>
       </c>
+      <c r="B50" s="2">
+        <v>371</v>
+      </c>
       <c r="C50" s="12" t="s">
         <v>132</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>664</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2">
         <v>49</v>
       </c>
+      <c r="B51" s="2">
+        <v>150</v>
+      </c>
       <c r="C51" s="12"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -8120,6 +8195,12 @@
       <c r="D52" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="E52" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="2">
@@ -8129,6 +8210,9 @@
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="E53" s="2" t="s">
+        <v>661</v>
+      </c>
       <c r="F53" s="2" t="s">
         <v>498</v>
       </c>
@@ -8141,19 +8225,25 @@
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="E54" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>662</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231110] Leetcode - Top-Interview-Medium 52 (50-52)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7BA5AB-A531-4B4C-A052-A50E1E9F1757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E775066C-475F-9D41-BCAB-DB8E4DAF9C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="672">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2418,6 +2418,18 @@
   </si>
   <si>
     <t xml:space="preserve"> use stack to if not  '+-*/': append else pop and check if '+-*/' and  append(pop '+-*/' pop), return stack[0]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter and check key-value; or; Moore Voting Algorithm (for loop nums: if char==cnt: cnt ++ else cnt --, finally, char is answer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_len = max(table.values())</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>e.g. ACCCEEE 2 ==&gt; CE_CE_CE =&gt; (max num - 1) * (n + 1) + count of (max num), finally, max(count, len(tasks))</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6922,8 +6934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8113,7 +8125,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:10">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -8137,7 +8149,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:10">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -8163,7 +8175,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:10">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -8184,16 +8196,19 @@
         <v>668</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="2">
         <v>50</v>
       </c>
+      <c r="B52" s="2">
+        <v>169</v>
+      </c>
       <c r="C52" s="12"/>
       <c r="D52" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>659</v>
@@ -8201,11 +8216,20 @@
       <c r="F52" s="6" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="G52" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="2">
         <v>51</v>
       </c>
+      <c r="B53" s="2">
+        <v>645</v>
+      </c>
       <c r="C53" s="12"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
@@ -8217,10 +8241,13 @@
         <v>498</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:10">
       <c r="A54" s="2">
         <v>52</v>
       </c>
+      <c r="B54" s="2">
+        <v>621</v>
+      </c>
       <c r="C54" s="12"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
@@ -8231,19 +8258,28 @@
       <c r="F54" s="6" t="s">
         <v>662</v>
       </c>
+      <c r="G54" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>670</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231113] Leetcode - review 1
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E775066C-475F-9D41-BCAB-DB8E4DAF9C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934220C7-0C6B-8141-87B3-24CEEC18C76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="680">
   <si>
     <t xml:space="preserve">
 </t>
@@ -444,9 +444,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/727/</t>
-  </si>
-  <si>
     <t>String</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -490,14 +487,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>differency</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>count</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Rotate Array</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -506,10 +495,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>move</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Contains Duplicate</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -518,10 +503,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>hash</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/646/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -534,10 +515,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>set</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Intersection of Two Arrays II</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -546,14 +523,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>list or str-int</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Counter or two ptr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>2023.08.11</t>
   </si>
   <si>
@@ -573,10 +542,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>ptr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>2023.08.12</t>
   </si>
   <si>
@@ -588,18 +553,10 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Valid Sudoku</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/769/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>triple with set</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Rotate Image</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -619,10 +576,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>border for origin/after</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Reverse String</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -647,33 +600,13 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Counter</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Counter or sorted</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>2023.08.14</t>
   </si>
   <si>
-    <t>two ptr or [::-1]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Valid Anagram</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/882/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Valid Palindrome</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/883/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -695,10 +628,6 @@
   </si>
   <si>
     <t>2023.08.15</t>
-  </si>
-  <si>
-    <t>min</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Implement strStr()</t>
@@ -2430,6 +2359,109 @@
   </si>
   <si>
     <t>e.g. ACCCEEE 2 ==&gt; CE_CE_CE =&gt; (max num - 1) * (n + 1) + count of (max num), finally, max(count, len(tasks))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/dynamic-programming/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/727/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>for loop with a ptr to switch</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>total of each differency</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>move: [:k], [k:] = [len-k:], [:len]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash table; or; sort and compare</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>set: sum(set(nums)) * 2 - sum(nums)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast answer: list((collections.Counter(nums1) &amp; collections.Counter(nums2)).elements())</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter for one num and check element; or; sort and two ptr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list with insert or str-int</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop with a ptr to switch</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash: (target - num) in table</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>triple with set; or; row/col/block to set() then add value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast answer: res += [(i, board[i][j]), (board[i][j], j), (i // 3, j // 3, board[i][j])] and return len(res) == len(set(res))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reverse()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>border ((-(2**31) &lt;= x &lt;= (2**31-1))) for origin/after and int(str[::-1])</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter and loop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Sudoku (數獨)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter or sorted equal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Anagram (字謎)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Palindrome (回文)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.lower()</t>
+  </si>
+  <si>
+    <t>lower() with two ptr or [::-1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>run all prefix by len(min(str))</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2979,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2989,8 +3021,9 @@
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="5" max="5" width="39.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="83.83203125" customWidth="1"/>
-    <col min="7" max="7" width="53.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="96.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3008,7 +3041,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>
@@ -3029,7 +3062,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>7</v>
+        <v>656</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>8</v>
@@ -3053,16 +3086,16 @@
         <v>123</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>124</v>
+        <v>655</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>137</v>
+        <v>658</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>0</v>
+        <v>134</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>657</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" t="s">
@@ -3081,21 +3114,23 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="8" t="s">
+        <v>657</v>
+      </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="16">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -3107,19 +3142,22 @@
         <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>140</v>
+        <v>660</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>136</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3131,19 +3169,22 @@
         <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>143</v>
+        <v>661</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>136</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -3155,19 +3196,22 @@
         <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>147</v>
+        <v>662</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>136</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -3179,19 +3223,25 @@
         <v>21</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>151</v>
+        <v>664</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>144</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -3203,19 +3253,22 @@
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>150</v>
+        <v>665</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>144</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -3227,19 +3280,22 @@
         <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>157</v>
+        <v>666</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>144</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3251,20 +3307,23 @@
         <v>21</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>143</v>
+        <v>667</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="2">
+        <v>149</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12" s="2">
@@ -3275,19 +3334,25 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>161</v>
+        <v>673</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>163</v>
+        <v>668</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>149</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3299,19 +3364,22 @@
         <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>149</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3319,25 +3387,31 @@
         <v>344</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>156</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3349,19 +3423,22 @@
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>169</v>
+        <v>671</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>156</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3373,19 +3450,22 @@
         <v>21</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>176</v>
+        <v>672</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>156</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -3397,19 +3477,22 @@
         <v>21</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>180</v>
+        <v>675</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>177</v>
+        <v>674</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>164</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="16">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3421,19 +3504,25 @@
         <v>21</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>182</v>
+        <v>676</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>179</v>
+        <v>678</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>164</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -3445,19 +3534,19 @@
         <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="16">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3469,19 +3558,22 @@
         <v>21</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>171</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="16">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -3493,19 +3585,22 @@
         <v>21</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>189</v>
+        <v>679</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>171</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3513,25 +3608,25 @@
         <v>237</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3543,19 +3638,19 @@
         <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3567,19 +3662,19 @@
         <v>21</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3591,19 +3686,19 @@
         <v>21</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3615,19 +3710,19 @@
         <v>21</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3639,19 +3734,19 @@
         <v>21</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3659,25 +3754,25 @@
         <v>104</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -3689,19 +3784,19 @@
         <v>38</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -3713,19 +3808,19 @@
         <v>21</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -3737,19 +3832,19 @@
         <v>38</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -3761,16 +3856,16 @@
         <v>21</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -3781,22 +3876,22 @@
         <v>88</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -3811,16 +3906,16 @@
         <v>21</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -3831,22 +3926,22 @@
         <v>70</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -3861,16 +3956,16 @@
         <v>21</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -3885,16 +3980,16 @@
         <v>38</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -3909,16 +4004,16 @@
         <v>38</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -3929,22 +4024,22 @@
         <v>384</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -3959,16 +4054,16 @@
         <v>38</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -3979,22 +4074,22 @@
         <v>412</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -4009,16 +4104,16 @@
         <v>38</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -4033,16 +4128,16 @@
         <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -4057,16 +4152,16 @@
         <v>21</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -4077,22 +4172,22 @@
         <v>191</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -4107,16 +4202,16 @@
         <v>21</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -4131,16 +4226,16 @@
         <v>21</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -4155,16 +4250,16 @@
         <v>21</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -4179,16 +4274,16 @@
         <v>21</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -4203,16 +4298,16 @@
         <v>21</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -4398,6 +4493,7 @@
     <hyperlink ref="F6" r:id="rId3" xr:uid="{9DDED772-F21E-7B48-9CB2-CB46C4DE0963}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{F57CED91-3449-574E-8615-4599E779544E}"/>
     <hyperlink ref="F46" r:id="rId5" xr:uid="{B257738E-11CD-C047-9119-DEAD4671692E}"/>
+    <hyperlink ref="F3" r:id="rId6" xr:uid="{0D9C7814-359E-3C4E-9D41-31A80D0FBD6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4407,7 +4503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
@@ -4470,7 +4566,7 @@
         <v>7</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>8</v>
@@ -4493,16 +4589,16 @@
         <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>95</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>0</v>
@@ -4529,16 +4625,16 @@
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
@@ -4560,16 +4656,16 @@
         <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="K5" t="s">
         <v>22</v>
@@ -4596,10 +4692,10 @@
         <v>96</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="K6" t="s">
         <v>22</v>
@@ -4623,13 +4719,13 @@
         <v>13</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="K7" t="s">
         <v>23</v>
@@ -4653,13 +4749,13 @@
         <v>14</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="K8" t="s">
         <v>23</v>
@@ -4683,13 +4779,13 @@
         <v>15</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="K9" t="s">
         <v>24</v>
@@ -4713,13 +4809,13 @@
         <v>16</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="K10" t="s">
         <v>24</v>
@@ -4743,13 +4839,13 @@
         <v>17</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="K11" t="s">
         <v>22</v>
@@ -4773,13 +4869,13 @@
         <v>18</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="K12" t="s">
         <v>22</v>
@@ -4800,16 +4896,16 @@
         <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="K13" t="s">
         <v>24</v>
@@ -4833,13 +4929,13 @@
         <v>19</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="K14" t="s">
         <v>22</v>
@@ -4863,19 +4959,19 @@
         <v>20</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="K15" t="s">
         <v>22</v>
       </c>
       <c r="L15" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -4898,13 +4994,13 @@
         <v>25</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="K16" t="s">
         <v>22</v>
@@ -4928,13 +5024,13 @@
         <v>26</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="K17" t="s">
         <v>24</v>
@@ -4958,13 +5054,13 @@
         <v>27</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="K18" t="s">
         <v>22</v>
@@ -4988,13 +5084,13 @@
         <v>28</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="K19" t="s">
         <v>22</v>
@@ -5018,13 +5114,13 @@
         <v>29</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="K20" t="s">
         <v>22</v>
@@ -5048,13 +5144,13 @@
         <v>30</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="K21" t="s">
         <v>22</v>
@@ -5078,13 +5174,13 @@
         <v>31</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="K22" t="s">
         <v>24</v>
@@ -5108,13 +5204,13 @@
         <v>32</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="K23" t="s">
         <v>89</v>
@@ -5138,13 +5234,13 @@
         <v>33</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="K24" t="s">
         <v>22</v>
@@ -5168,13 +5264,13 @@
         <v>34</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="K25" t="s">
         <v>24</v>
@@ -5201,10 +5297,10 @@
         <v>97</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="K26" t="s">
         <v>24</v>
@@ -5231,10 +5327,10 @@
         <v>99</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="K27" t="s">
         <v>22</v>
@@ -5260,13 +5356,13 @@
         <v>37</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
       <c r="K28" t="s">
         <v>90</v>
@@ -5290,13 +5386,13 @@
         <v>39</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
       <c r="K29" t="s">
         <v>89</v>
@@ -5320,13 +5416,13 @@
         <v>40</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="K30" t="s">
         <v>89</v>
@@ -5350,13 +5446,13 @@
         <v>41</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="K31" t="s">
         <v>89</v>
@@ -5380,13 +5476,13 @@
         <v>42</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="K32" t="s">
         <v>89</v>
@@ -5410,13 +5506,13 @@
         <v>43</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="K33" t="s">
         <v>22</v>
@@ -5440,19 +5536,19 @@
         <v>44</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="K34" t="s">
         <v>90</v>
       </c>
       <c r="L34" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -5473,13 +5569,13 @@
         <v>45</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="K35" t="s">
         <v>89</v>
@@ -5505,19 +5601,19 @@
         <v>46</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="K36" t="s">
         <v>89</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -5538,13 +5634,13 @@
         <v>47</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="K37" t="s">
         <v>91</v>
@@ -5568,13 +5664,13 @@
         <v>48</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="K38" t="s">
         <v>90</v>
@@ -5601,10 +5697,10 @@
         <v>98</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="K39" t="s">
         <v>89</v>
@@ -5628,13 +5724,13 @@
         <v>50</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="K40" t="s">
         <v>22</v>
@@ -5658,13 +5754,13 @@
         <v>51</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="K41" t="s">
         <v>22</v>
@@ -5688,13 +5784,13 @@
         <v>52</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="K42" t="s">
         <v>90</v>
@@ -5718,13 +5814,13 @@
         <v>53</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="K43" t="s">
         <v>89</v>
@@ -5753,10 +5849,10 @@
         <v>104</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="K44" t="s">
         <v>89</v>
@@ -5780,19 +5876,19 @@
         <v>55</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="K45" t="s">
         <v>89</v>
       </c>
       <c r="L45" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -5813,13 +5909,13 @@
         <v>56</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="K46" t="s">
         <v>89</v>
@@ -5843,13 +5939,13 @@
         <v>57</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="K47" t="s">
         <v>89</v>
@@ -5873,13 +5969,13 @@
         <v>58</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="K48" t="s">
         <v>90</v>
@@ -5903,13 +5999,13 @@
         <v>59</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="K49" t="s">
         <v>91</v>
@@ -5933,19 +6029,19 @@
         <v>60</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="K50" t="s">
         <v>89</v>
       </c>
       <c r="L50" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -5966,13 +6062,13 @@
         <v>61</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="K51" t="s">
         <v>90</v>
@@ -5998,13 +6094,13 @@
         <v>62</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="K52" t="s">
         <v>89</v>
@@ -6028,13 +6124,13 @@
         <v>63</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="K53" t="s">
         <v>89</v>
@@ -6058,13 +6154,13 @@
         <v>64</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="K54" t="s">
         <v>90</v>
@@ -6088,13 +6184,13 @@
         <v>65</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="K55" t="s">
         <v>90</v>
@@ -6118,13 +6214,13 @@
         <v>66</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="K56" t="s">
         <v>89</v>
@@ -6148,13 +6244,13 @@
         <v>67</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="K57" t="s">
         <v>22</v>
@@ -6178,13 +6274,13 @@
         <v>68</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="K58" t="s">
         <v>90</v>
@@ -6208,13 +6304,13 @@
         <v>69</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="K59" t="s">
         <v>22</v>
@@ -6238,13 +6334,13 @@
         <v>70</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="K60" t="s">
         <v>90</v>
@@ -6273,10 +6369,10 @@
         <v>105</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="K61" t="s">
         <v>91</v>
@@ -6300,13 +6396,13 @@
         <v>72</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="K62" t="s">
         <v>89</v>
@@ -6330,13 +6426,13 @@
         <v>73</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
       <c r="K63" t="s">
         <v>89</v>
@@ -6360,13 +6456,13 @@
         <v>74</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="K64" t="s">
         <v>89</v>
@@ -6390,13 +6486,13 @@
         <v>75</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="K65" t="s">
         <v>89</v>
@@ -6420,13 +6516,13 @@
         <v>76</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="K66" t="s">
         <v>91</v>
@@ -6450,13 +6546,13 @@
         <v>77</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="K67" t="s">
         <v>89</v>
@@ -6482,13 +6578,13 @@
         <v>78</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="K68" t="s">
         <v>90</v>
@@ -6512,13 +6608,13 @@
         <v>79</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="K69" t="s">
         <v>89</v>
@@ -6542,13 +6638,13 @@
         <v>80</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
       <c r="K70" t="s">
         <v>92</v>
@@ -6572,13 +6668,13 @@
         <v>81</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="K71" t="s">
         <v>91</v>
@@ -6602,13 +6698,13 @@
         <v>82</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="K72" t="s">
         <v>89</v>
@@ -6632,13 +6728,13 @@
         <v>83</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="K73" t="s">
         <v>93</v>
@@ -6662,13 +6758,13 @@
         <v>84</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="K74" t="s">
         <v>92</v>
@@ -6692,13 +6788,13 @@
         <v>85</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="K75" t="s">
         <v>93</v>
@@ -6722,13 +6818,13 @@
         <v>86</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
       <c r="K76" t="s">
         <v>89</v>
@@ -6752,19 +6848,19 @@
         <v>87</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>483</v>
+        <v>465</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>484</v>
+        <v>466</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="K77" t="s">
         <v>91</v>
       </c>
       <c r="L77" t="s">
-        <v>485</v>
+        <v>467</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -6772,13 +6868,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C78" s="2">
         <v>152</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>38</v>
@@ -6790,10 +6886,10 @@
         <v>100</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>22</v>
@@ -6808,7 +6904,7 @@
         <v>153</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>38</v>
@@ -6820,13 +6916,13 @@
         <v>102</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -6934,8 +7030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6953,7 +7049,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="14" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -6968,7 +7064,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>
@@ -7004,22 +7100,22 @@
         <v>15</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>512</v>
+        <v>494</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>513</v>
+        <v>495</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
@@ -7041,16 +7137,16 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>553</v>
+        <v>535</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="7"/>
@@ -7067,16 +7163,16 @@
         <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>489</v>
+        <v>471</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -7091,16 +7187,16 @@
         <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -7115,16 +7211,16 @@
         <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -7139,16 +7235,16 @@
         <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>495</v>
+        <v>477</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -7163,10 +7259,10 @@
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -7182,16 +7278,16 @@
         <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>537</v>
+        <v>519</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>536</v>
+        <v>518</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16">
@@ -7202,22 +7298,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>526</v>
+        <v>508</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>538</v>
+        <v>520</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>536</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -7232,16 +7328,16 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>554</v>
+        <v>536</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>523</v>
+        <v>505</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>540</v>
+        <v>522</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -7256,16 +7352,16 @@
         <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>525</v>
+        <v>507</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -7276,22 +7372,22 @@
         <v>94</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>535</v>
+        <v>517</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>527</v>
+        <v>509</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>543</v>
+        <v>525</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -7306,16 +7402,16 @@
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>534</v>
+        <v>516</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>544</v>
+        <v>526</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -7333,16 +7429,16 @@
         <v>70</v>
       </c>
       <c r="F16" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>529</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -7357,16 +7453,16 @@
         <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>533</v>
+        <v>515</v>
       </c>
       <c r="F17" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>548</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>549</v>
+        <v>531</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -7384,13 +7480,13 @@
         <v>78</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>531</v>
+        <v>513</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>551</v>
+        <v>533</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>550</v>
+        <v>532</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7405,10 +7501,10 @@
         <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -7428,13 +7524,13 @@
         <v>52</v>
       </c>
       <c r="F20" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7445,7 +7541,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>38</v>
@@ -7454,13 +7550,13 @@
         <v>72</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>564</v>
+        <v>546</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>566</v>
+        <v>548</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>565</v>
+        <v>547</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -7475,16 +7571,16 @@
         <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>556</v>
+        <v>538</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>563</v>
+        <v>545</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>568</v>
+        <v>550</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -7499,16 +7595,16 @@
         <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>570</v>
+        <v>552</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -7523,16 +7619,16 @@
         <v>38</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>558</v>
+        <v>540</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>572</v>
+        <v>554</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>571</v>
+        <v>553</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -7547,19 +7643,19 @@
         <v>38</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>559</v>
+        <v>541</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>560</v>
+        <v>542</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>573</v>
+        <v>555</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>571</v>
+        <v>553</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>574</v>
+        <v>556</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -7570,22 +7666,22 @@
         <v>75</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>576</v>
+        <v>558</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>591</v>
+        <v>573</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -7600,19 +7696,19 @@
         <v>38</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>577</v>
+        <v>559</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>578</v>
+        <v>560</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>594</v>
+        <v>576</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>591</v>
+        <v>573</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>593</v>
+        <v>575</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -7627,19 +7723,19 @@
         <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>580</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>597</v>
-      </c>
       <c r="H28" s="2" t="s">
-        <v>595</v>
+        <v>577</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>596</v>
+        <v>578</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -7654,16 +7750,16 @@
         <v>38</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>586</v>
+        <v>568</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>588</v>
+        <v>570</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>598</v>
+        <v>580</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>595</v>
+        <v>577</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="32">
@@ -7678,16 +7774,16 @@
         <v>38</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>600</v>
+        <v>582</v>
       </c>
       <c r="F30" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -7705,13 +7801,13 @@
         <v>57</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>582</v>
+        <v>564</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>602</v>
+        <v>584</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>599</v>
+        <v>581</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -7726,16 +7822,16 @@
         <v>38</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>587</v>
+        <v>569</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>589</v>
+        <v>571</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>604</v>
+        <v>586</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -7750,10 +7846,10 @@
         <v>38</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>585</v>
+        <v>567</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -7770,16 +7866,16 @@
         <v>38</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>584</v>
+        <v>566</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>583</v>
+        <v>565</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>605</v>
+        <v>587</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -7790,22 +7886,22 @@
         <v>55</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>610</v>
+        <v>592</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>608</v>
+        <v>590</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>612</v>
+        <v>594</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -7823,13 +7919,13 @@
         <v>69</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>609</v>
+        <v>591</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>614</v>
+        <v>596</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>612</v>
+        <v>594</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -7847,13 +7943,13 @@
         <v>48</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -7868,19 +7964,19 @@
         <v>38</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>611</v>
+        <v>593</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>606</v>
+        <v>588</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>617</v>
+        <v>599</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>618</v>
+        <v>600</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -7891,16 +7987,16 @@
         <v>251</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>619</v>
+        <v>601</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="G39" s="2"/>
     </row>
@@ -7916,16 +8012,16 @@
         <v>88</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>624</v>
+        <v>606</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>620</v>
+        <v>602</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>626</v>
+        <v>608</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>625</v>
+        <v>607</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -7940,19 +8036,19 @@
         <v>38</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>621</v>
+        <v>603</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>622</v>
+        <v>604</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>629</v>
+        <v>611</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>627</v>
+        <v>609</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>628</v>
+        <v>610</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -7967,10 +8063,10 @@
         <v>38</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>623</v>
+        <v>605</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="G42" s="2"/>
     </row>
@@ -7982,22 +8078,22 @@
         <v>202</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>630</v>
+        <v>612</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>631</v>
+        <v>613</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>643</v>
+        <v>625</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>642</v>
+        <v>624</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -8012,16 +8108,16 @@
         <v>38</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>632</v>
+        <v>614</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>644</v>
+        <v>626</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>645</v>
+        <v>627</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>642</v>
+        <v>624</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -8036,19 +8132,19 @@
         <v>21</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>634</v>
+        <v>616</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>633</v>
+        <v>615</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>647</v>
+        <v>629</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>646</v>
+        <v>628</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>648</v>
+        <v>630</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -8063,19 +8159,19 @@
         <v>38</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>635</v>
+        <v>617</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>641</v>
+        <v>623</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>649</v>
+        <v>631</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>646</v>
+        <v>628</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>650</v>
+        <v>632</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -8090,19 +8186,19 @@
         <v>21</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>637</v>
+        <v>619</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>636</v>
+        <v>618</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>652</v>
+        <v>634</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>651</v>
+        <v>633</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>653</v>
+        <v>635</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -8117,10 +8213,10 @@
         <v>38</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>638</v>
+        <v>620</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -8137,16 +8233,16 @@
         <v>38</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>640</v>
+        <v>622</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>639</v>
+        <v>621</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>655</v>
+        <v>637</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>654</v>
+        <v>636</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -8157,22 +8253,22 @@
         <v>371</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>657</v>
+        <v>639</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>664</v>
+        <v>646</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>666</v>
+        <v>648</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>656</v>
+        <v>638</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -8187,16 +8283,16 @@
         <v>38</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>658</v>
+        <v>640</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>665</v>
+        <v>647</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>668</v>
+        <v>650</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>656</v>
+        <v>638</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -8211,16 +8307,16 @@
         <v>21</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>659</v>
+        <v>641</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>663</v>
+        <v>645</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>669</v>
+        <v>651</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>667</v>
+        <v>649</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -8235,10 +8331,10 @@
         <v>38</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>661</v>
+        <v>643</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -8253,33 +8349,33 @@
         <v>38</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>660</v>
+        <v>642</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>662</v>
+        <v>644</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>671</v>
+        <v>653</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>667</v>
+        <v>649</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>670</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -8300,15 +8396,67 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F80E9F-AC4D-B74C-865E-81CF884A25E9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{6F009178-C59D-C84E-A361-966EC8C47EA7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[20231114] Leetcode - review 1
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934220C7-0C6B-8141-87B3-24CEEC18C76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15701549-D29C-9C43-8BAA-1118C2287279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="684">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2462,6 +2462,20 @@
   </si>
   <si>
     <t>run all prefix by len(min(str))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.14</t>
+  </si>
+  <si>
+    <t>while (ptr2 and ptr2.next)</t>
+  </si>
+  <si>
+    <t>if not root:    return 0, l = self.maxDepth(root.left), r = self.maxDepth(root.right), return max(l, r) + 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>self.isMirror(left.left, right.right) and self.isMirror(left.right, right.left)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3011,8 +3025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3600,7 +3614,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" ht="16">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3625,8 +3639,11 @@
       <c r="H22" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="I22" s="8" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3649,8 +3666,11 @@
       <c r="H23" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="I23" s="8" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="16">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3673,8 +3693,11 @@
       <c r="H24" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="I24" s="8" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3697,8 +3720,11 @@
       <c r="H25" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="I25" s="8" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3721,8 +3747,11 @@
       <c r="H26" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="I26" s="8" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="16">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3745,8 +3774,14 @@
       <c r="H27" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="I27" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="16">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3771,9 +3806,15 @@
       <c r="H28" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="I28" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="2">
+      <c r="A29" s="9">
         <v>27</v>
       </c>
       <c r="B29" s="2">
@@ -3796,7 +3837,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" ht="16">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -3818,6 +3859,12 @@
       </c>
       <c r="H30" s="2" t="s">
         <v>206</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -7030,7 +7077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
@@ -8366,16 +8413,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231130] Leetcode - add premium 1
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15701549-D29C-9C43-8BAA-1118C2287279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C51F31-F560-9846-96CE-472115111413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="687">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1732,10 +1732,6 @@
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/781/</t>
   </si>
   <si>
-    <t>Missing Ranges</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Premium</t>
   </si>
   <si>
@@ -1925,10 +1921,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Inorder Successor in BST</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Set Matrix Zeroes</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2039,9 +2031,6 @@
   </si>
   <si>
     <t>Search a 2D Matrix II</t>
-  </si>
-  <si>
-    <t>Meeting Rooms II</t>
   </si>
   <si>
     <t>Find Peak Element</t>
@@ -2167,9 +2156,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Flatten 2D Vector</t>
-  </si>
-  <si>
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/112/design/812/</t>
   </si>
   <si>
@@ -2180,9 +2166,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Design Tic-Tac-Toe</t>
-  </si>
-  <si>
     <t>Serialize and Deserialize Binary Tree</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2234,10 +2217,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Divide Two Integers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/113/math/821/</t>
   </si>
   <si>
@@ -2321,10 +2300,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Find the Celebrity</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/114/others/826/</t>
   </si>
   <si>
@@ -2476,6 +2451,46 @@
   </si>
   <si>
     <t>self.isMirror(left.left, right.right) and self.isMirror(left.right, right.left)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/782/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing Ranges (Premium)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inorder Successor in BST (Premium)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meeting Rooms II (Premium)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flatten 2D Vector (Premium)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design Tic-Tac-Toe (Premium)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Divide Two Integers (Premium)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find the Celebrity (Premium)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>check none: [lower, upper], check lower to nums[0] and nums[-1] + 1 to upper, nums[i+1] - nums[i] &lt;= 1: skip or [nums[i] + 1, nums[i+1] - 1]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2635,7 +2650,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2707,6 +2722,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3025,7 +3043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="125" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -3076,7 +3094,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>8</v>
@@ -3100,16 +3118,16 @@
         <v>123</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>134</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" t="s">
@@ -3134,13 +3152,13 @@
         <v>132</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>134</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="J4" s="3"/>
     </row>
@@ -3162,13 +3180,13 @@
         <v>139</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>136</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16">
@@ -3189,13 +3207,13 @@
         <v>140</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>136</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16">
@@ -3216,13 +3234,13 @@
         <v>141</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>136</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16">
@@ -3243,16 +3261,16 @@
         <v>143</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>144</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16">
@@ -3273,13 +3291,13 @@
         <v>146</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>144</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16">
@@ -3300,13 +3318,13 @@
         <v>148</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>144</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16">
@@ -3327,13 +3345,13 @@
         <v>151</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>149</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16">
@@ -3348,22 +3366,22 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>152</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>149</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16">
@@ -3390,7 +3408,7 @@
         <v>149</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16">
@@ -3419,10 +3437,10 @@
         <v>156</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16">
@@ -3443,13 +3461,13 @@
         <v>161</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16">
@@ -3470,13 +3488,13 @@
         <v>163</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>156</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16">
@@ -3491,19 +3509,19 @@
         <v>21</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>165</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16">
@@ -3518,22 +3536,22 @@
         <v>21</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>166</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3584,7 +3602,7 @@
         <v>171</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16">
@@ -3605,13 +3623,13 @@
         <v>175</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16">
@@ -3640,7 +3658,7 @@
         <v>171</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16">
@@ -3667,7 +3685,7 @@
         <v>180</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16">
@@ -3694,7 +3712,7 @@
         <v>180</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16">
@@ -3721,7 +3739,7 @@
         <v>180</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16">
@@ -3748,7 +3766,7 @@
         <v>190</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16">
@@ -3775,10 +3793,10 @@
         <v>190</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16">
@@ -3807,10 +3825,10 @@
         <v>190</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -3861,10 +3879,10 @@
         <v>206</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -4550,7 +4568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
@@ -6921,7 +6939,7 @@
         <v>152</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>38</v>
@@ -6933,10 +6951,10 @@
         <v>100</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>22</v>
@@ -6951,7 +6969,7 @@
         <v>153</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>38</v>
@@ -6963,13 +6981,13 @@
         <v>102</v>
       </c>
       <c r="H79" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="K79" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -7077,8 +7095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection sqref="A1:J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7147,22 +7165,22 @@
         <v>15</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>469</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
@@ -7184,16 +7202,16 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>470</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="7"/>
@@ -7216,10 +7234,10 @@
         <v>472</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -7240,10 +7258,10 @@
         <v>474</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -7264,10 +7282,10 @@
         <v>476</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -7288,10 +7306,10 @@
         <v>478</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -7306,12 +7324,17 @@
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>678</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>677</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2">
@@ -7325,16 +7348,16 @@
         <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16">
@@ -7345,22 +7368,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -7375,16 +7398,16 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -7399,16 +7422,16 @@
         <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -7419,22 +7442,22 @@
         <v>94</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -7449,16 +7472,16 @@
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -7476,16 +7499,16 @@
         <v>70</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>528</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -7500,16 +7523,16 @@
         <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>530</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -7527,13 +7550,13 @@
         <v>78</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7548,10 +7571,10 @@
         <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>534</v>
+        <v>679</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>480</v>
+        <v>569</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -7571,13 +7594,13 @@
         <v>52</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7588,7 +7611,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>38</v>
@@ -7597,13 +7620,13 @@
         <v>72</v>
       </c>
       <c r="F21" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>548</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -7618,16 +7641,16 @@
         <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -7642,16 +7665,16 @@
         <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -7666,16 +7689,16 @@
         <v>38</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -7690,19 +7713,19 @@
         <v>38</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -7719,16 +7742,16 @@
         <v>38</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -7743,19 +7766,19 @@
         <v>38</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -7770,19 +7793,19 @@
         <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -7797,16 +7820,16 @@
         <v>38</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="32">
@@ -7821,16 +7844,16 @@
         <v>38</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -7848,13 +7871,13 @@
         <v>57</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -7869,16 +7892,16 @@
         <v>38</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -7893,10 +7916,10 @@
         <v>38</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>567</v>
+        <v>680</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -7913,16 +7936,16 @@
         <v>38</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -7939,16 +7962,16 @@
         <v>38</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>587</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>590</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>595</v>
-      </c>
       <c r="H35" s="2" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -7966,13 +7989,13 @@
         <v>69</v>
       </c>
       <c r="F36" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>591</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -7990,13 +8013,13 @@
         <v>48</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -8011,19 +8034,19 @@
         <v>38</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H38" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>597</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -8040,10 +8063,10 @@
         <v>38</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>601</v>
+        <v>681</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="G39" s="2"/>
     </row>
@@ -8059,16 +8082,16 @@
         <v>88</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="F40" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>602</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -8083,19 +8106,19 @@
         <v>38</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F41" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>609</v>
-      </c>
       <c r="J41" s="2" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -8110,10 +8133,10 @@
         <v>38</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>605</v>
+        <v>682</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="G42" s="2"/>
     </row>
@@ -8131,16 +8154,16 @@
         <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -8155,16 +8178,16 @@
         <v>38</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -8179,19 +8202,19 @@
         <v>21</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -8206,19 +8229,19 @@
         <v>38</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>623</v>
-      </c>
       <c r="G46" s="2" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -8233,19 +8256,19 @@
         <v>21</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -8260,10 +8283,10 @@
         <v>38</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>620</v>
+        <v>683</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -8280,16 +8303,16 @@
         <v>38</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -8306,16 +8329,16 @@
         <v>38</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>639</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>646</v>
-      </c>
       <c r="G50" s="2" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -8330,16 +8353,16 @@
         <v>38</v>
       </c>
       <c r="E51" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>640</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>647</v>
-      </c>
       <c r="G51" s="2" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -8354,16 +8377,16 @@
         <v>21</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -8378,10 +8401,10 @@
         <v>38</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>643</v>
+        <v>684</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -8396,33 +8419,33 @@
         <v>38</v>
       </c>
       <c r="E54" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="F54" s="6" t="s">
-        <v>644</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>649</v>
-      </c>
       <c r="J54" s="2" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -8436,6 +8459,7 @@
     <hyperlink ref="E42" r:id="rId8" display="https://leetcode.com/problems/design-tic-tac-toe/" xr:uid="{60846593-E208-244C-9E3C-68800E4AFEA2}"/>
     <hyperlink ref="F43" r:id="rId9" xr:uid="{5932DEC8-20C8-C649-9D15-FC22C096FE7F}"/>
     <hyperlink ref="F44" r:id="rId10" xr:uid="{6DD4110D-7061-1C46-A430-79DA813250EC}"/>
+    <hyperlink ref="F9" r:id="rId11" xr:uid="{23F1AAC4-D72B-1641-A82D-D83601CBB88E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8453,7 +8477,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="14" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>

</xml_diff>

<commit_message>
[20231219] Leetcode - add premium - (17)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C51F31-F560-9846-96CE-472115111413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E1DEB6-DEB3-0440-A94F-F83915D9231D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="691">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2491,6 +2491,22 @@
   </si>
   <si>
     <t>check none: [lower, upper], check lower to nums[0] and nums[-1] + 1 to upper, nums[i+1] - nums[i] &lt;= 1: skip or [nums[i] + 1, nums[i+1] - 1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/108/trees-and-graphs/791/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>successor (後面一位) and predecessor (前面一位)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.19</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>find BST next node, recursion with root.val &lt;= p.val</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2650,7 +2666,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2686,6 +2702,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2724,7 +2743,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3059,14 +3078,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -3108,7 +3127,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3141,7 +3160,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -3169,7 +3188,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3196,7 +3215,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -3223,7 +3242,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -3250,7 +3269,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -3280,7 +3299,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -3307,7 +3326,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -3334,7 +3353,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -3361,7 +3380,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -3391,7 +3410,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3418,7 +3437,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>124</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3450,7 +3469,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3477,7 +3496,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3504,7 +3523,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3531,7 +3550,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3561,7 +3580,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -3585,7 +3604,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3612,7 +3631,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3639,7 +3658,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>125</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -3668,7 +3687,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -3695,7 +3714,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3722,7 +3741,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3749,7 +3768,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3776,7 +3795,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3806,7 +3825,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>126</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -3838,7 +3857,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -3862,7 +3881,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3892,7 +3911,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -3916,7 +3935,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -3940,7 +3959,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -3966,7 +3985,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -3990,7 +4009,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -4016,7 +4035,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -4040,7 +4059,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -4064,7 +4083,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -4088,7 +4107,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="13" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -4114,7 +4133,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="12"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -4138,7 +4157,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="13" t="s">
         <v>130</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -4164,7 +4183,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -4188,7 +4207,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="12"/>
+      <c r="C43" s="13"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -4212,7 +4231,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -4236,7 +4255,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="13" t="s">
         <v>131</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -4262,7 +4281,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -4286,7 +4305,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -4310,7 +4329,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="12"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -4334,7 +4353,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="12"/>
+      <c r="C49" s="13"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -4358,7 +4377,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="12"/>
+      <c r="C50" s="13"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -4589,15 +4608,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -4641,7 +4660,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -4679,7 +4698,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -4710,7 +4729,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -4740,7 +4759,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -4770,7 +4789,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -4800,7 +4819,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -4830,7 +4849,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -4860,7 +4879,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -4890,7 +4909,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -4920,7 +4939,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -4950,7 +4969,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -4980,7 +4999,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -5010,7 +5029,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -5043,7 +5062,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="19">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -5075,7 +5094,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -5105,7 +5124,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="18"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -5135,7 +5154,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="18"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -5165,7 +5184,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="18"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="2">
         <v>206</v>
       </c>
@@ -5195,7 +5214,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="18"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="2">
         <v>169</v>
       </c>
@@ -5225,7 +5244,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="18"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="2">
         <v>67</v>
       </c>
@@ -5255,7 +5274,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="18"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="2">
         <v>543</v>
       </c>
@@ -5285,7 +5304,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="18"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="2">
         <v>876</v>
       </c>
@@ -5315,7 +5334,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="18"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="2">
         <v>104</v>
       </c>
@@ -5345,7 +5364,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="18"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="2">
         <v>217</v>
       </c>
@@ -5375,7 +5394,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="2">
         <v>53</v>
       </c>
@@ -5405,7 +5424,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="20">
         <v>3</v>
       </c>
       <c r="C28" s="2">
@@ -5437,7 +5456,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="19"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="2">
         <v>542</v>
       </c>
@@ -5467,7 +5486,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="19"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="2">
         <v>973</v>
       </c>
@@ -5497,7 +5516,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="19"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="2">
         <v>3</v>
       </c>
@@ -5527,7 +5546,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="2">
         <v>15</v>
       </c>
@@ -5557,7 +5576,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="19"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="2">
         <v>102</v>
       </c>
@@ -5587,7 +5606,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="2">
         <v>133</v>
       </c>
@@ -5620,7 +5639,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="20"/>
       <c r="C35" s="2">
         <v>150</v>
       </c>
@@ -5650,7 +5669,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" s="21">
         <v>4</v>
       </c>
       <c r="C36" s="2">
@@ -5685,7 +5704,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="2">
         <v>208</v>
       </c>
@@ -5715,7 +5734,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="20"/>
+      <c r="B38" s="21"/>
       <c r="C38" s="2">
         <v>322</v>
       </c>
@@ -5745,7 +5764,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="20"/>
+      <c r="B39" s="21"/>
       <c r="C39" s="2">
         <v>238</v>
       </c>
@@ -5775,7 +5794,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="20"/>
+      <c r="B40" s="21"/>
       <c r="C40" s="2">
         <v>155</v>
       </c>
@@ -5805,7 +5824,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="21"/>
       <c r="C41" s="2">
         <v>98</v>
       </c>
@@ -5835,7 +5854,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="2">
         <v>200</v>
       </c>
@@ -5865,7 +5884,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="20"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="2">
         <v>994</v>
       </c>
@@ -5895,7 +5914,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="21">
+      <c r="B44" s="22">
         <v>5</v>
       </c>
       <c r="C44" s="2">
@@ -5927,7 +5946,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="21"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="2">
         <v>39</v>
       </c>
@@ -5960,7 +5979,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="21"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="2">
         <v>46</v>
       </c>
@@ -5990,7 +6009,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="21"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="2">
         <v>56</v>
       </c>
@@ -6020,7 +6039,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="21"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="2">
         <v>236</v>
       </c>
@@ -6050,7 +6069,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="21"/>
+      <c r="B49" s="22"/>
       <c r="C49" s="2">
         <v>981</v>
       </c>
@@ -6080,7 +6099,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="21"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="2">
         <v>721</v>
       </c>
@@ -6113,7 +6132,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="21"/>
+      <c r="B51" s="22"/>
       <c r="C51" s="2">
         <v>75</v>
       </c>
@@ -6143,7 +6162,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="22">
+      <c r="B52" s="23">
         <v>6</v>
       </c>
       <c r="C52" s="2">
@@ -6175,7 +6194,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="22"/>
+      <c r="B53" s="23"/>
       <c r="C53" s="2">
         <v>416</v>
       </c>
@@ -6205,7 +6224,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="22"/>
+      <c r="B54" s="23"/>
       <c r="C54" s="2">
         <v>8</v>
       </c>
@@ -6235,7 +6254,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="22"/>
+      <c r="B55" s="23"/>
       <c r="C55" s="2">
         <v>54</v>
       </c>
@@ -6265,7 +6284,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="22"/>
+      <c r="B56" s="23"/>
       <c r="C56" s="2">
         <v>78</v>
       </c>
@@ -6295,7 +6314,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="22"/>
+      <c r="B57" s="23"/>
       <c r="C57" s="2">
         <v>199</v>
       </c>
@@ -6325,7 +6344,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="22"/>
+      <c r="B58" s="23"/>
       <c r="C58" s="2">
         <v>5</v>
       </c>
@@ -6355,7 +6374,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="22"/>
+      <c r="B59" s="23"/>
       <c r="C59" s="2">
         <v>62</v>
       </c>
@@ -6385,7 +6404,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="22"/>
+      <c r="B60" s="23"/>
       <c r="C60" s="2">
         <v>105</v>
       </c>
@@ -6415,7 +6434,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="16">
         <v>7</v>
       </c>
       <c r="C61" s="2">
@@ -6447,7 +6466,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="15"/>
+      <c r="B62" s="16"/>
       <c r="C62" s="2">
         <v>17</v>
       </c>
@@ -6477,7 +6496,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="15"/>
+      <c r="B63" s="16"/>
       <c r="C63" s="2">
         <v>79</v>
       </c>
@@ -6507,7 +6526,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="15"/>
+      <c r="B64" s="16"/>
       <c r="C64" s="2">
         <v>438</v>
       </c>
@@ -6537,7 +6556,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="15"/>
+      <c r="B65" s="16"/>
       <c r="C65" s="2">
         <v>310</v>
       </c>
@@ -6567,7 +6586,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="15"/>
+      <c r="B66" s="16"/>
       <c r="C66" s="2">
         <v>621</v>
       </c>
@@ -6597,7 +6616,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="15"/>
+      <c r="B67" s="16"/>
       <c r="C67" s="2">
         <v>146</v>
       </c>
@@ -6627,7 +6646,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="16">
+      <c r="B68" s="17">
         <v>8</v>
       </c>
       <c r="C68" s="2">
@@ -6659,7 +6678,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="16"/>
+      <c r="B69" s="17"/>
       <c r="C69" s="2">
         <v>76</v>
       </c>
@@ -6689,7 +6708,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="16"/>
+      <c r="B70" s="17"/>
       <c r="C70" s="2">
         <v>297</v>
       </c>
@@ -6719,7 +6738,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="16"/>
+      <c r="B71" s="17"/>
       <c r="C71" s="2">
         <v>42</v>
       </c>
@@ -6749,7 +6768,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="16"/>
+      <c r="B72" s="17"/>
       <c r="C72" s="2">
         <v>295</v>
       </c>
@@ -6779,7 +6798,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="16"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="2">
         <v>127</v>
       </c>
@@ -6809,7 +6828,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="16"/>
+      <c r="B74" s="17"/>
       <c r="C74" s="2">
         <v>224</v>
       </c>
@@ -6839,7 +6858,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="16"/>
+      <c r="B75" s="17"/>
       <c r="C75" s="2">
         <v>1235</v>
       </c>
@@ -6869,7 +6888,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="16"/>
+      <c r="B76" s="17"/>
       <c r="C76" s="2">
         <v>23</v>
       </c>
@@ -6899,7 +6918,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="16"/>
+      <c r="B77" s="17"/>
       <c r="C77" s="2">
         <v>84</v>
       </c>
@@ -6932,7 +6951,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="13" t="s">
         <v>131</v>
       </c>
       <c r="C78" s="2">
@@ -6964,7 +6983,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="12"/>
+      <c r="B79" s="13"/>
       <c r="C79" s="2">
         <v>153</v>
       </c>
@@ -7000,15 +7019,15 @@
       <c r="A85" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B85" s="17" t="s">
+      <c r="B85" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7095,8 +7114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7113,14 +7132,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>468</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -7164,7 +7183,7 @@
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>482</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -7197,7 +7216,7 @@
       <c r="B4" s="2">
         <v>73</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -7223,7 +7242,7 @@
       <c r="B5" s="2">
         <v>49</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -7247,7 +7266,7 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
@@ -7271,7 +7290,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
@@ -7295,7 +7314,7 @@
       <c r="B8" s="2">
         <v>334</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
@@ -7319,14 +7338,14 @@
       <c r="B9" s="2">
         <v>163</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="12" t="s">
         <v>677</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -7343,7 +7362,7 @@
       <c r="B10" s="2">
         <v>38</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
@@ -7367,7 +7386,7 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>483</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -7393,7 +7412,7 @@
       <c r="B12" s="2">
         <v>328</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -7417,7 +7436,7 @@
       <c r="B13" s="2">
         <v>160</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
@@ -7441,7 +7460,7 @@
       <c r="B14" s="2">
         <v>94</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>484</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -7467,7 +7486,7 @@
       <c r="B15" s="2">
         <v>103</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -7491,7 +7510,7 @@
       <c r="B16" s="2">
         <v>105</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
@@ -7518,7 +7537,7 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
@@ -7542,7 +7561,7 @@
       <c r="B18" s="2">
         <v>230</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -7566,18 +7585,25 @@
       <c r="B19" s="2">
         <v>285</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="F19" s="25" t="s">
+        <v>687</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2">
@@ -7586,7 +7612,7 @@
       <c r="B20" s="2">
         <v>200</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
@@ -7610,7 +7636,7 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>485</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -7636,7 +7662,7 @@
       <c r="B22" s="2">
         <v>22</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
@@ -7660,7 +7686,7 @@
       <c r="B23" s="2">
         <v>46</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -7684,7 +7710,7 @@
       <c r="B24" s="2">
         <v>78</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
@@ -7708,7 +7734,7 @@
       <c r="B25" s="2">
         <v>79</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
@@ -7735,7 +7761,7 @@
       <c r="B26" s="2">
         <v>75</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -7761,7 +7787,7 @@
       <c r="B27" s="2">
         <v>347</v>
       </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -7788,7 +7814,7 @@
       <c r="B28" s="2">
         <v>215</v>
       </c>
-      <c r="C28" s="12"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -7815,7 +7841,7 @@
       <c r="B29" s="2">
         <v>162</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -7839,7 +7865,7 @@
       <c r="B30" s="2">
         <v>34</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
@@ -7863,7 +7889,7 @@
       <c r="B31" s="2">
         <v>56</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -7887,7 +7913,7 @@
       <c r="B32" s="2">
         <v>33</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -7911,7 +7937,7 @@
       <c r="B33" s="2">
         <v>253</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
@@ -7931,7 +7957,7 @@
       <c r="B34" s="2">
         <v>240</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
@@ -7955,7 +7981,7 @@
       <c r="B35" s="2">
         <v>55</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -7981,7 +8007,7 @@
       <c r="B36" s="2">
         <v>62</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
@@ -8005,7 +8031,7 @@
       <c r="B37" s="2">
         <v>322</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -8029,7 +8055,7 @@
       <c r="B38" s="2">
         <v>300</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -8056,7 +8082,7 @@
       <c r="B39" s="2">
         <v>251</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="13" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -8077,7 +8103,7 @@
       <c r="B40" s="2">
         <v>297</v>
       </c>
-      <c r="C40" s="12"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="2" t="s">
         <v>88</v>
       </c>
@@ -8101,7 +8127,7 @@
       <c r="B41" s="2">
         <v>380</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
@@ -8128,7 +8154,7 @@
       <c r="B42" s="2">
         <v>348</v>
       </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -8147,7 +8173,7 @@
       <c r="B43" s="2">
         <v>202</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="13" t="s">
         <v>130</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -8173,7 +8199,7 @@
       <c r="B44" s="2">
         <v>172</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
@@ -8197,7 +8223,7 @@
       <c r="B45" s="2">
         <v>171</v>
       </c>
-      <c r="C45" s="12"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
@@ -8224,7 +8250,7 @@
       <c r="B46" s="2">
         <v>50</v>
       </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
@@ -8251,7 +8277,7 @@
       <c r="B47" s="2">
         <v>69</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -8278,7 +8304,7 @@
       <c r="B48" s="2">
         <v>29</v>
       </c>
-      <c r="C48" s="12"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
@@ -8298,7 +8324,7 @@
       <c r="B49" s="2">
         <v>166</v>
       </c>
-      <c r="C49" s="12"/>
+      <c r="C49" s="13"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
@@ -8322,7 +8348,7 @@
       <c r="B50" s="2">
         <v>371</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="13" t="s">
         <v>131</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -8348,7 +8374,7 @@
       <c r="B51" s="2">
         <v>150</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" s="13"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
@@ -8372,7 +8398,7 @@
       <c r="B52" s="2">
         <v>169</v>
       </c>
-      <c r="C52" s="12"/>
+      <c r="C52" s="13"/>
       <c r="D52" s="2" t="s">
         <v>21</v>
       </c>
@@ -8396,7 +8422,7 @@
       <c r="B53" s="2">
         <v>645</v>
       </c>
-      <c r="C53" s="12"/>
+      <c r="C53" s="13"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
@@ -8414,7 +8440,7 @@
       <c r="B54" s="2">
         <v>621</v>
       </c>
-      <c r="C54" s="12"/>
+      <c r="C54" s="13"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
@@ -8436,16 +8462,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -8460,6 +8486,7 @@
     <hyperlink ref="F43" r:id="rId9" xr:uid="{5932DEC8-20C8-C649-9D15-FC22C096FE7F}"/>
     <hyperlink ref="F44" r:id="rId10" xr:uid="{6DD4110D-7061-1C46-A430-79DA813250EC}"/>
     <hyperlink ref="F9" r:id="rId11" xr:uid="{23F1AAC4-D72B-1641-A82D-D83601CBB88E}"/>
+    <hyperlink ref="F19" r:id="rId12" xr:uid="{7F6C4157-86B4-D143-AD01-622EF31612B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8476,14 +8503,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>647</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>

</xml_diff>

<commit_message>
[20231221] Leetcode - add premium - (31,37)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E1DEB6-DEB3-0440-A94F-F83915D9231D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E64962-D179-EC43-8E48-03369937B5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="696">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2507,6 +2507,26 @@
   </si>
   <si>
     <t>find BST next node, recursion with root.val &lt;= p.val</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/805/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.21</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort first, heap to check start time &gt; miniTime of heap: heapreplace or heappush</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/112/design/811/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>table = add all vec row, next: return ptr, hasNest: (self.ptr+1)  &gt;= len(self.table)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2706,6 +2726,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2740,9 +2763,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3063,7 +3083,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3078,14 +3098,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -3127,7 +3147,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3160,7 +3180,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -3188,7 +3208,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3215,7 +3235,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="13"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -3242,7 +3262,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -3269,7 +3289,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="13"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -3299,7 +3319,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -3326,7 +3346,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -3353,7 +3373,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -3380,7 +3400,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -3410,7 +3430,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="13"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3437,7 +3457,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3469,7 +3489,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="13"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3496,7 +3516,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="13"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3523,7 +3543,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3550,7 +3570,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3580,7 +3600,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -3604,7 +3624,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3631,7 +3651,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="13"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3658,7 +3678,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="14" t="s">
         <v>125</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -3687,7 +3707,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="13"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -3714,7 +3734,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="13"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3741,7 +3761,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3768,7 +3788,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3795,7 +3815,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3825,7 +3845,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="14" t="s">
         <v>126</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -3857,7 +3877,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="13"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -3881,7 +3901,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="13"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3911,7 +3931,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="13"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -3935,7 +3955,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="13"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -3959,7 +3979,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="14" t="s">
         <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -3985,7 +4005,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="13"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -4009,7 +4029,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -4035,7 +4055,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="13"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -4059,7 +4079,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="13"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -4083,7 +4103,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="13"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -4107,7 +4127,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="14" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -4133,7 +4153,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="13"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -4157,7 +4177,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="14" t="s">
         <v>130</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -4183,7 +4203,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="13"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -4207,7 +4227,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="13"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -4231,7 +4251,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="13"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -4255,7 +4275,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="14" t="s">
         <v>131</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -4281,7 +4301,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="13"/>
+      <c r="C46" s="14"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -4305,7 +4325,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="13"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -4329,7 +4349,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="13"/>
+      <c r="C48" s="14"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -4353,7 +4373,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="13"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -4377,7 +4397,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="13"/>
+      <c r="C50" s="14"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -4588,7 +4608,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4608,15 +4628,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -4660,7 +4680,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="25">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -4698,7 +4718,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -4729,7 +4749,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -4759,7 +4779,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -4789,7 +4809,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -4819,7 +4839,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -4849,7 +4869,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -4879,7 +4899,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="24"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -4909,7 +4929,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -4939,7 +4959,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="24"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -4969,7 +4989,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -4999,7 +5019,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -5029,7 +5049,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="24"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -5062,7 +5082,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="20">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -5094,7 +5114,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -5124,7 +5144,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -5154,7 +5174,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -5184,7 +5204,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="2">
         <v>206</v>
       </c>
@@ -5214,7 +5234,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="2">
         <v>169</v>
       </c>
@@ -5244,7 +5264,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="19"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="2">
         <v>67</v>
       </c>
@@ -5274,7 +5294,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="19"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="2">
         <v>543</v>
       </c>
@@ -5304,7 +5324,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="19"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="2">
         <v>876</v>
       </c>
@@ -5334,7 +5354,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="19"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="2">
         <v>104</v>
       </c>
@@ -5364,7 +5384,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="2">
         <v>217</v>
       </c>
@@ -5394,7 +5414,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="19"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="2">
         <v>53</v>
       </c>
@@ -5424,7 +5444,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="21">
         <v>3</v>
       </c>
       <c r="C28" s="2">
@@ -5456,7 +5476,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="20"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="2">
         <v>542</v>
       </c>
@@ -5486,7 +5506,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="20"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="2">
         <v>973</v>
       </c>
@@ -5516,7 +5536,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="20"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="2">
         <v>3</v>
       </c>
@@ -5546,7 +5566,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="20"/>
+      <c r="B32" s="21"/>
       <c r="C32" s="2">
         <v>15</v>
       </c>
@@ -5576,7 +5596,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="20"/>
+      <c r="B33" s="21"/>
       <c r="C33" s="2">
         <v>102</v>
       </c>
@@ -5606,7 +5626,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="20"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="2">
         <v>133</v>
       </c>
@@ -5639,7 +5659,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="2">
         <v>150</v>
       </c>
@@ -5669,7 +5689,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="22">
         <v>4</v>
       </c>
       <c r="C36" s="2">
@@ -5704,7 +5724,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="21"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="2">
         <v>208</v>
       </c>
@@ -5734,7 +5754,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="21"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="2">
         <v>322</v>
       </c>
@@ -5764,7 +5784,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="21"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="2">
         <v>238</v>
       </c>
@@ -5794,7 +5814,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="21"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="2">
         <v>155</v>
       </c>
@@ -5824,7 +5844,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="21"/>
+      <c r="B41" s="22"/>
       <c r="C41" s="2">
         <v>98</v>
       </c>
@@ -5854,7 +5874,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="2">
         <v>200</v>
       </c>
@@ -5884,7 +5904,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="2">
         <v>994</v>
       </c>
@@ -5914,7 +5934,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="22">
+      <c r="B44" s="23">
         <v>5</v>
       </c>
       <c r="C44" s="2">
@@ -5946,7 +5966,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="2">
         <v>39</v>
       </c>
@@ -5979,7 +5999,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="22"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="2">
         <v>46</v>
       </c>
@@ -6009,7 +6029,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="22"/>
+      <c r="B47" s="23"/>
       <c r="C47" s="2">
         <v>56</v>
       </c>
@@ -6039,7 +6059,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="22"/>
+      <c r="B48" s="23"/>
       <c r="C48" s="2">
         <v>236</v>
       </c>
@@ -6069,7 +6089,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="22"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="2">
         <v>981</v>
       </c>
@@ -6099,7 +6119,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="22"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="2">
         <v>721</v>
       </c>
@@ -6132,7 +6152,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="22"/>
+      <c r="B51" s="23"/>
       <c r="C51" s="2">
         <v>75</v>
       </c>
@@ -6162,7 +6182,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="23">
+      <c r="B52" s="24">
         <v>6</v>
       </c>
       <c r="C52" s="2">
@@ -6194,7 +6214,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="23"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="2">
         <v>416</v>
       </c>
@@ -6224,7 +6244,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="23"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="2">
         <v>8</v>
       </c>
@@ -6254,7 +6274,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="23"/>
+      <c r="B55" s="24"/>
       <c r="C55" s="2">
         <v>54</v>
       </c>
@@ -6284,7 +6304,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="23"/>
+      <c r="B56" s="24"/>
       <c r="C56" s="2">
         <v>78</v>
       </c>
@@ -6314,7 +6334,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="23"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="2">
         <v>199</v>
       </c>
@@ -6344,7 +6364,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="23"/>
+      <c r="B58" s="24"/>
       <c r="C58" s="2">
         <v>5</v>
       </c>
@@ -6374,7 +6394,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="23"/>
+      <c r="B59" s="24"/>
       <c r="C59" s="2">
         <v>62</v>
       </c>
@@ -6404,7 +6424,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="23"/>
+      <c r="B60" s="24"/>
       <c r="C60" s="2">
         <v>105</v>
       </c>
@@ -6434,7 +6454,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="16">
+      <c r="B61" s="17">
         <v>7</v>
       </c>
       <c r="C61" s="2">
@@ -6466,7 +6486,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="16"/>
+      <c r="B62" s="17"/>
       <c r="C62" s="2">
         <v>17</v>
       </c>
@@ -6496,7 +6516,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="16"/>
+      <c r="B63" s="17"/>
       <c r="C63" s="2">
         <v>79</v>
       </c>
@@ -6526,7 +6546,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="16"/>
+      <c r="B64" s="17"/>
       <c r="C64" s="2">
         <v>438</v>
       </c>
@@ -6556,7 +6576,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="16"/>
+      <c r="B65" s="17"/>
       <c r="C65" s="2">
         <v>310</v>
       </c>
@@ -6586,7 +6606,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="16"/>
+      <c r="B66" s="17"/>
       <c r="C66" s="2">
         <v>621</v>
       </c>
@@ -6616,7 +6636,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="16"/>
+      <c r="B67" s="17"/>
       <c r="C67" s="2">
         <v>146</v>
       </c>
@@ -6646,7 +6666,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="17">
+      <c r="B68" s="18">
         <v>8</v>
       </c>
       <c r="C68" s="2">
@@ -6678,7 +6698,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="17"/>
+      <c r="B69" s="18"/>
       <c r="C69" s="2">
         <v>76</v>
       </c>
@@ -6708,7 +6728,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="17"/>
+      <c r="B70" s="18"/>
       <c r="C70" s="2">
         <v>297</v>
       </c>
@@ -6738,7 +6758,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="17"/>
+      <c r="B71" s="18"/>
       <c r="C71" s="2">
         <v>42</v>
       </c>
@@ -6768,7 +6788,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="17"/>
+      <c r="B72" s="18"/>
       <c r="C72" s="2">
         <v>295</v>
       </c>
@@ -6798,7 +6818,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="17"/>
+      <c r="B73" s="18"/>
       <c r="C73" s="2">
         <v>127</v>
       </c>
@@ -6828,7 +6848,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="17"/>
+      <c r="B74" s="18"/>
       <c r="C74" s="2">
         <v>224</v>
       </c>
@@ -6858,7 +6878,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="17"/>
+      <c r="B75" s="18"/>
       <c r="C75" s="2">
         <v>1235</v>
       </c>
@@ -6888,7 +6908,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="17"/>
+      <c r="B76" s="18"/>
       <c r="C76" s="2">
         <v>23</v>
       </c>
@@ -6918,7 +6938,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="17"/>
+      <c r="B77" s="18"/>
       <c r="C77" s="2">
         <v>84</v>
       </c>
@@ -6951,7 +6971,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="14" t="s">
         <v>131</v>
       </c>
       <c r="C78" s="2">
@@ -6983,7 +7003,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="13"/>
+      <c r="B79" s="14"/>
       <c r="C79" s="2">
         <v>153</v>
       </c>
@@ -7019,15 +7039,15 @@
       <c r="A85" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
-      <c r="H85" s="18"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7114,8 +7134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7132,14 +7152,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>468</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -7183,7 +7203,7 @@
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>482</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -7216,7 +7236,7 @@
       <c r="B4" s="2">
         <v>73</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -7242,7 +7262,7 @@
       <c r="B5" s="2">
         <v>49</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -7266,7 +7286,7 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="13"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
@@ -7290,7 +7310,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
@@ -7314,7 +7334,7 @@
       <c r="B8" s="2">
         <v>334</v>
       </c>
-      <c r="C8" s="13"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
@@ -7338,7 +7358,7 @@
       <c r="B9" s="2">
         <v>163</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -7362,7 +7382,7 @@
       <c r="B10" s="2">
         <v>38</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
@@ -7386,7 +7406,7 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>483</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -7412,7 +7432,7 @@
       <c r="B12" s="2">
         <v>328</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -7436,7 +7456,7 @@
       <c r="B13" s="2">
         <v>160</v>
       </c>
-      <c r="C13" s="13"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
@@ -7460,7 +7480,7 @@
       <c r="B14" s="2">
         <v>94</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>484</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -7486,7 +7506,7 @@
       <c r="B15" s="2">
         <v>103</v>
       </c>
-      <c r="C15" s="13"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -7510,7 +7530,7 @@
       <c r="B16" s="2">
         <v>105</v>
       </c>
-      <c r="C16" s="13"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
@@ -7537,7 +7557,7 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
@@ -7561,7 +7581,7 @@
       <c r="B18" s="2">
         <v>230</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -7585,14 +7605,14 @@
       <c r="B19" s="2">
         <v>285</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="13" t="s">
         <v>687</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -7612,7 +7632,7 @@
       <c r="B20" s="2">
         <v>200</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
@@ -7636,7 +7656,7 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="14" t="s">
         <v>485</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -7662,7 +7682,7 @@
       <c r="B22" s="2">
         <v>22</v>
       </c>
-      <c r="C22" s="13"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
@@ -7686,7 +7706,7 @@
       <c r="B23" s="2">
         <v>46</v>
       </c>
-      <c r="C23" s="13"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -7710,7 +7730,7 @@
       <c r="B24" s="2">
         <v>78</v>
       </c>
-      <c r="C24" s="13"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
@@ -7734,7 +7754,7 @@
       <c r="B25" s="2">
         <v>79</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
@@ -7761,7 +7781,7 @@
       <c r="B26" s="2">
         <v>75</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="14" t="s">
         <v>127</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -7787,7 +7807,7 @@
       <c r="B27" s="2">
         <v>347</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -7814,7 +7834,7 @@
       <c r="B28" s="2">
         <v>215</v>
       </c>
-      <c r="C28" s="13"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -7841,7 +7861,7 @@
       <c r="B29" s="2">
         <v>162</v>
       </c>
-      <c r="C29" s="13"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -7865,7 +7885,7 @@
       <c r="B30" s="2">
         <v>34</v>
       </c>
-      <c r="C30" s="13"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
@@ -7889,7 +7909,7 @@
       <c r="B31" s="2">
         <v>56</v>
       </c>
-      <c r="C31" s="13"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -7913,7 +7933,7 @@
       <c r="B32" s="2">
         <v>33</v>
       </c>
-      <c r="C32" s="13"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -7937,18 +7957,22 @@
       <c r="B33" s="2">
         <v>253</v>
       </c>
-      <c r="C33" s="13"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="F33" s="13" t="s">
+        <v>691</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="2">
@@ -7957,7 +7981,7 @@
       <c r="B34" s="2">
         <v>240</v>
       </c>
-      <c r="C34" s="13"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
@@ -7981,7 +8005,7 @@
       <c r="B35" s="2">
         <v>55</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -8007,7 +8031,7 @@
       <c r="B36" s="2">
         <v>62</v>
       </c>
-      <c r="C36" s="13"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
@@ -8031,7 +8055,7 @@
       <c r="B37" s="2">
         <v>322</v>
       </c>
-      <c r="C37" s="13"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -8055,7 +8079,7 @@
       <c r="B38" s="2">
         <v>300</v>
       </c>
-      <c r="C38" s="13"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -8082,7 +8106,7 @@
       <c r="B39" s="2">
         <v>251</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="14" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -8091,10 +8115,15 @@
       <c r="E39" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="G39" s="2"/>
+      <c r="F39" s="13" t="s">
+        <v>694</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="2">
@@ -8103,7 +8132,7 @@
       <c r="B40" s="2">
         <v>297</v>
       </c>
-      <c r="C40" s="13"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="2" t="s">
         <v>88</v>
       </c>
@@ -8127,7 +8156,7 @@
       <c r="B41" s="2">
         <v>380</v>
       </c>
-      <c r="C41" s="13"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
@@ -8154,7 +8183,7 @@
       <c r="B42" s="2">
         <v>348</v>
       </c>
-      <c r="C42" s="13"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -8173,7 +8202,7 @@
       <c r="B43" s="2">
         <v>202</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="14" t="s">
         <v>130</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -8199,7 +8228,7 @@
       <c r="B44" s="2">
         <v>172</v>
       </c>
-      <c r="C44" s="13"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
@@ -8223,7 +8252,7 @@
       <c r="B45" s="2">
         <v>171</v>
       </c>
-      <c r="C45" s="13"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
@@ -8250,7 +8279,7 @@
       <c r="B46" s="2">
         <v>50</v>
       </c>
-      <c r="C46" s="13"/>
+      <c r="C46" s="14"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
@@ -8277,7 +8306,7 @@
       <c r="B47" s="2">
         <v>69</v>
       </c>
-      <c r="C47" s="13"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -8304,7 +8333,7 @@
       <c r="B48" s="2">
         <v>29</v>
       </c>
-      <c r="C48" s="13"/>
+      <c r="C48" s="14"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
@@ -8324,7 +8353,7 @@
       <c r="B49" s="2">
         <v>166</v>
       </c>
-      <c r="C49" s="13"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
@@ -8348,7 +8377,7 @@
       <c r="B50" s="2">
         <v>371</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="14" t="s">
         <v>131</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -8374,7 +8403,7 @@
       <c r="B51" s="2">
         <v>150</v>
       </c>
-      <c r="C51" s="13"/>
+      <c r="C51" s="14"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
@@ -8398,7 +8427,7 @@
       <c r="B52" s="2">
         <v>169</v>
       </c>
-      <c r="C52" s="13"/>
+      <c r="C52" s="14"/>
       <c r="D52" s="2" t="s">
         <v>21</v>
       </c>
@@ -8422,7 +8451,7 @@
       <c r="B53" s="2">
         <v>645</v>
       </c>
-      <c r="C53" s="13"/>
+      <c r="C53" s="14"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
@@ -8440,7 +8469,7 @@
       <c r="B54" s="2">
         <v>621</v>
       </c>
-      <c r="C54" s="13"/>
+      <c r="C54" s="14"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
@@ -8462,16 +8491,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -8487,6 +8516,8 @@
     <hyperlink ref="F44" r:id="rId10" xr:uid="{6DD4110D-7061-1C46-A430-79DA813250EC}"/>
     <hyperlink ref="F9" r:id="rId11" xr:uid="{23F1AAC4-D72B-1641-A82D-D83601CBB88E}"/>
     <hyperlink ref="F19" r:id="rId12" xr:uid="{7F6C4157-86B4-D143-AD01-622EF31612B0}"/>
+    <hyperlink ref="F33" r:id="rId13" xr:uid="{C9DFB491-9A65-254C-B502-2623E9A23D98}"/>
+    <hyperlink ref="F39" r:id="rId14" xr:uid="{A3455078-22B9-5045-AEB3-A71E06D50133}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8503,14 +8534,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>647</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>

</xml_diff>

<commit_message>
[20231222] Leetcode - add premium - (40)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E64962-D179-EC43-8E48-03369937B5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706D13C-A90F-DC40-86D4-62EA0D546A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="699">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2527,6 +2527,18 @@
   </si>
   <si>
     <t>table = add all vec row, next: return ptr, hasNest: (self.ptr+1)  &gt;= len(self.table)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.22</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/112/design/814/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OOXX, Brute Force to check four status, but optimized is that uses [n] for Row,  [n] for Col, dia antiDia to count (O: +1, X: -1), check 3 or -3</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -7134,8 +7146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8190,10 +8202,15 @@
       <c r="E42" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="G42" s="2"/>
+      <c r="F42" s="13" t="s">
+        <v>697</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="2">
@@ -8491,16 +8508,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -8518,6 +8535,7 @@
     <hyperlink ref="F19" r:id="rId12" xr:uid="{7F6C4157-86B4-D143-AD01-622EF31612B0}"/>
     <hyperlink ref="F33" r:id="rId13" xr:uid="{C9DFB491-9A65-254C-B502-2623E9A23D98}"/>
     <hyperlink ref="F39" r:id="rId14" xr:uid="{A3455078-22B9-5045-AEB3-A71E06D50133}"/>
+    <hyperlink ref="F42" r:id="rId15" xr:uid="{B731FD5C-FBF3-574A-A2E6-5EFED1F6AECE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20231223] Leetcode - add premium - (46)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0706D13C-A90F-DC40-86D4-62EA0D546A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7236A052-EF10-9542-B71D-5A0D895EF7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="701">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1732,9 +1732,6 @@
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/781/</t>
   </si>
   <si>
-    <t>Premium</t>
-  </si>
-  <si>
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/103/array-and-strings/4153/</t>
   </si>
   <si>
@@ -2046,10 +2043,6 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/110/sorting-and-searching/804/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Premium</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -2539,6 +2532,22 @@
   </si>
   <si>
     <t>OOXX, Brute Force to check four status, but optimized is that uses [n] for Row,  [n] for Col, dia antiDia to count (O: +1, X: -1), check 3 or -3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/113/math/820/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.23</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>determine sign first, then abs(dividend and divisor) and loop (31, -1, -1) to (if (dividend &gt;&gt; i) &gt;= divisor: dividend -= (divisor &lt;&lt; i), answer += (1 &lt;&lt; i))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/114/others/825/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3145,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>8</v>
@@ -3169,16 +3178,16 @@
         <v>123</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>134</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" t="s">
@@ -3203,13 +3212,13 @@
         <v>132</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>134</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J4" s="3"/>
     </row>
@@ -3231,13 +3240,13 @@
         <v>139</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>136</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16">
@@ -3258,13 +3267,13 @@
         <v>140</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>136</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16">
@@ -3285,13 +3294,13 @@
         <v>141</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>136</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16">
@@ -3312,16 +3321,16 @@
         <v>143</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>144</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16">
@@ -3342,13 +3351,13 @@
         <v>146</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>144</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16">
@@ -3369,13 +3378,13 @@
         <v>148</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>144</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16">
@@ -3396,13 +3405,13 @@
         <v>151</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>149</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16">
@@ -3417,22 +3426,22 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>152</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>149</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16">
@@ -3459,7 +3468,7 @@
         <v>149</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16">
@@ -3488,10 +3497,10 @@
         <v>156</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16">
@@ -3512,13 +3521,13 @@
         <v>161</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>156</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16">
@@ -3539,13 +3548,13 @@
         <v>163</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>156</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16">
@@ -3560,19 +3569,19 @@
         <v>21</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>165</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16">
@@ -3587,22 +3596,22 @@
         <v>21</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>166</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>164</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3653,7 +3662,7 @@
         <v>171</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16">
@@ -3674,13 +3683,13 @@
         <v>175</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16">
@@ -3709,7 +3718,7 @@
         <v>171</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16">
@@ -3736,7 +3745,7 @@
         <v>180</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16">
@@ -3763,7 +3772,7 @@
         <v>180</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16">
@@ -3790,7 +3799,7 @@
         <v>180</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16">
@@ -3817,7 +3826,7 @@
         <v>190</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16">
@@ -3844,10 +3853,10 @@
         <v>190</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16">
@@ -3876,10 +3885,10 @@
         <v>190</v>
       </c>
       <c r="I28" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>673</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -3930,10 +3939,10 @@
         <v>206</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -6990,7 +6999,7 @@
         <v>152</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>38</v>
@@ -7002,10 +7011,10 @@
         <v>100</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>22</v>
@@ -7020,7 +7029,7 @@
         <v>153</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>38</v>
@@ -7032,13 +7041,13 @@
         <v>102</v>
       </c>
       <c r="H79" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="K79" s="2" t="s">
         <v>491</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -7146,8 +7155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="F14" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7216,22 +7225,22 @@
         <v>15</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>469</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
@@ -7253,16 +7262,16 @@
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>470</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="7"/>
@@ -7285,10 +7294,10 @@
         <v>472</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -7309,10 +7318,10 @@
         <v>474</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -7333,10 +7342,10 @@
         <v>476</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -7357,10 +7366,10 @@
         <v>478</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -7375,16 +7384,16 @@
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -7399,16 +7408,16 @@
         <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16">
@@ -7419,22 +7428,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -7449,16 +7458,16 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -7473,16 +7482,16 @@
         <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -7493,22 +7502,22 @@
         <v>94</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -7523,16 +7532,16 @@
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -7550,16 +7559,16 @@
         <v>70</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -7574,16 +7583,16 @@
         <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>529</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -7601,13 +7610,13 @@
         <v>78</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -7622,19 +7631,19 @@
         <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F19" s="13" t="s">
+        <v>685</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>690</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>689</v>
-      </c>
       <c r="J19" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -7652,13 +7661,13 @@
         <v>52</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -7669,7 +7678,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>38</v>
@@ -7678,13 +7687,13 @@
         <v>72</v>
       </c>
       <c r="F21" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>544</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -7699,16 +7708,16 @@
         <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -7723,16 +7732,16 @@
         <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>549</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -7747,16 +7756,16 @@
         <v>38</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -7771,19 +7780,19 @@
         <v>38</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>539</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>540</v>
-      </c>
       <c r="G25" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>553</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -7800,16 +7809,16 @@
         <v>38</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>555</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>556</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -7824,19 +7833,19 @@
         <v>38</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>558</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H27" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -7851,19 +7860,19 @@
         <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>560</v>
-      </c>
       <c r="G28" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -7878,16 +7887,16 @@
         <v>38</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="32">
@@ -7902,16 +7911,16 @@
         <v>38</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -7929,13 +7938,13 @@
         <v>57</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -7950,16 +7959,16 @@
         <v>38</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -7974,16 +7983,16 @@
         <v>38</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="F33" s="13" t="s">
+        <v>689</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>693</v>
-      </c>
       <c r="H33" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -7998,16 +8007,16 @@
         <v>38</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -8024,16 +8033,16 @@
         <v>38</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>585</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>589</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>587</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -8051,13 +8060,13 @@
         <v>69</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -8075,13 +8084,13 @@
         <v>48</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -8096,19 +8105,19 @@
         <v>38</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -8125,16 +8134,16 @@
         <v>38</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -8149,16 +8158,16 @@
         <v>88</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>598</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>603</v>
-      </c>
       <c r="H40" s="2" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -8173,19 +8182,19 @@
         <v>38</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -8200,16 +8209,16 @@
         <v>38</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -8226,16 +8235,16 @@
         <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -8250,16 +8259,16 @@
         <v>38</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -8274,19 +8283,19 @@
         <v>21</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="H45" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>622</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -8301,19 +8310,19 @@
         <v>38</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -8328,19 +8337,19 @@
         <v>21</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H47" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>627</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -8355,13 +8364,17 @@
         <v>38</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>683</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
+        <v>681</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>697</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="2">
@@ -8375,16 +8388,16 @@
         <v>38</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -8401,16 +8414,16 @@
         <v>38</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F50" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>641</v>
-      </c>
       <c r="H50" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -8425,16 +8438,16 @@
         <v>38</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -8449,16 +8462,16 @@
         <v>21</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -8473,10 +8486,10 @@
         <v>38</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>479</v>
+        <v>682</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -8491,19 +8504,19 @@
         <v>38</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -8536,6 +8549,8 @@
     <hyperlink ref="F33" r:id="rId13" xr:uid="{C9DFB491-9A65-254C-B502-2623E9A23D98}"/>
     <hyperlink ref="F39" r:id="rId14" xr:uid="{A3455078-22B9-5045-AEB3-A71E06D50133}"/>
     <hyperlink ref="F42" r:id="rId15" xr:uid="{B731FD5C-FBF3-574A-A2E6-5EFED1F6AECE}"/>
+    <hyperlink ref="F48" r:id="rId16" xr:uid="{EC97054E-ED9E-AA43-B78B-73CB2FAEFEE3}"/>
+    <hyperlink ref="F53" r:id="rId17" xr:uid="{DC792956-B501-C94A-BC19-FF9F56FA6880}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8553,7 +8568,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="16" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>

</xml_diff>

<commit_message>
[20231224] Leetcode - add premium - (51) & Code Preparson
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7236A052-EF10-9542-B71D-5A0D895EF7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7677750-4E54-5347-ADFD-FB7D991E5FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="703">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2548,6 +2548,14 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/interview/card/top-interview-questions-medium/114/others/825/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.24</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>knows(candidate, i): candidate = i, then check is_celebrity (if knows(i, j) or not knows(j, i): return False) else True</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2707,7 +2715,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2747,8 +2755,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2785,6 +2793,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7153,10 +7164,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F14" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7233,7 +7244,7 @@
       <c r="E3" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="12" t="s">
         <v>469</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -7264,7 +7275,7 @@
       <c r="E4" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="26" t="s">
         <v>470</v>
       </c>
       <c r="G4" s="7" t="s">
@@ -7290,7 +7301,7 @@
       <c r="E5" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="12" t="s">
         <v>472</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -7314,7 +7325,7 @@
       <c r="E6" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="12" t="s">
         <v>474</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -7338,7 +7349,7 @@
       <c r="E7" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="12" t="s">
         <v>476</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -7362,7 +7373,7 @@
       <c r="E8" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="12" t="s">
         <v>478</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -7410,7 +7421,7 @@
       <c r="E10" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="12" t="s">
         <v>479</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -7436,7 +7447,7 @@
       <c r="E11" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="26" t="s">
         <v>502</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -7460,7 +7471,7 @@
       <c r="E12" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="12" t="s">
         <v>503</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -7484,7 +7495,7 @@
       <c r="E13" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="12" t="s">
         <v>504</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -7510,7 +7521,7 @@
       <c r="E14" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="12" t="s">
         <v>507</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -7534,7 +7545,7 @@
       <c r="E15" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="12" t="s">
         <v>508</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -7558,7 +7569,7 @@
       <c r="E16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="12" t="s">
         <v>509</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -7585,7 +7596,7 @@
       <c r="E17" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="12" t="s">
         <v>510</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -7609,7 +7620,7 @@
       <c r="E18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="12" t="s">
         <v>511</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -7633,7 +7644,7 @@
       <c r="E19" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="12" t="s">
         <v>685</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -7660,7 +7671,7 @@
       <c r="E20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="12" t="s">
         <v>512</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -7686,7 +7697,7 @@
       <c r="E21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="12" t="s">
         <v>543</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -7710,7 +7721,7 @@
       <c r="E22" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="12" t="s">
         <v>542</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -7734,7 +7745,7 @@
       <c r="E23" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="12" t="s">
         <v>541</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -7758,7 +7769,7 @@
       <c r="E24" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="12" t="s">
         <v>540</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -7782,7 +7793,7 @@
       <c r="E25" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="12" t="s">
         <v>539</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -7811,7 +7822,7 @@
       <c r="E26" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="12" t="s">
         <v>555</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -7835,7 +7846,7 @@
       <c r="E27" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="12" t="s">
         <v>557</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -7862,7 +7873,7 @@
       <c r="E28" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="12" t="s">
         <v>559</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -7889,7 +7900,7 @@
       <c r="E29" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="12" t="s">
         <v>566</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -7913,7 +7924,7 @@
       <c r="E30" s="11" t="s">
         <v>577</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="12" t="s">
         <v>560</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -7937,7 +7948,7 @@
       <c r="E31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="12" t="s">
         <v>561</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -7961,7 +7972,7 @@
       <c r="E32" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="12" t="s">
         <v>567</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -7985,7 +7996,7 @@
       <c r="E33" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F33" s="12" t="s">
         <v>689</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -8009,7 +8020,7 @@
       <c r="E34" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="12" t="s">
         <v>562</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -8035,7 +8046,7 @@
       <c r="E35" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="12" t="s">
         <v>585</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -8059,7 +8070,7 @@
       <c r="E36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="12" t="s">
         <v>586</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -8083,7 +8094,7 @@
       <c r="E37" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="12" t="s">
         <v>584</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -8107,7 +8118,7 @@
       <c r="E38" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="12" t="s">
         <v>583</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -8136,7 +8147,7 @@
       <c r="E39" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="12" t="s">
         <v>692</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -8160,7 +8171,7 @@
       <c r="E40" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="12" t="s">
         <v>596</v>
       </c>
       <c r="G40" s="2" t="s">
@@ -8184,7 +8195,7 @@
       <c r="E41" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="12" t="s">
         <v>598</v>
       </c>
       <c r="G41" s="2" t="s">
@@ -8211,7 +8222,7 @@
       <c r="E42" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="12" t="s">
         <v>695</v>
       </c>
       <c r="G42" s="2" t="s">
@@ -8237,7 +8248,7 @@
       <c r="E43" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="12" t="s">
         <v>606</v>
       </c>
       <c r="G43" s="2" t="s">
@@ -8261,7 +8272,7 @@
       <c r="E44" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F44" s="12" t="s">
         <v>618</v>
       </c>
       <c r="G44" s="2" t="s">
@@ -8285,7 +8296,7 @@
       <c r="E45" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="12" t="s">
         <v>608</v>
       </c>
       <c r="G45" s="2" t="s">
@@ -8312,7 +8323,7 @@
       <c r="E46" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" s="12" t="s">
         <v>615</v>
       </c>
       <c r="G46" s="2" t="s">
@@ -8339,7 +8350,7 @@
       <c r="E47" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" s="12" t="s">
         <v>611</v>
       </c>
       <c r="G47" s="2" t="s">
@@ -8366,7 +8377,7 @@
       <c r="E48" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="12" t="s">
         <v>697</v>
       </c>
       <c r="G48" s="2" t="s">
@@ -8390,7 +8401,7 @@
       <c r="E49" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F49" s="12" t="s">
         <v>613</v>
       </c>
       <c r="G49" s="2" t="s">
@@ -8416,7 +8427,7 @@
       <c r="E50" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F50" s="12" t="s">
         <v>637</v>
       </c>
       <c r="G50" s="2" t="s">
@@ -8440,7 +8451,7 @@
       <c r="E51" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F51" s="12" t="s">
         <v>638</v>
       </c>
       <c r="G51" s="2" t="s">
@@ -8464,7 +8475,7 @@
       <c r="E52" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F52" s="12" t="s">
         <v>636</v>
       </c>
       <c r="G52" s="2" t="s">
@@ -8488,8 +8499,14 @@
       <c r="E53" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="F53" s="13" t="s">
+      <c r="F53" s="12" t="s">
         <v>700</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -8506,7 +8523,7 @@
       <c r="E54" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="F54" s="12" t="s">
         <v>635</v>
       </c>
       <c r="G54" s="2" t="s">
@@ -8519,18 +8536,726 @@
         <v>643</v>
       </c>
     </row>
+    <row r="55" spans="1:10">
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="F57" s="13"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="F58" s="13"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="F59" s="13"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="F60" s="13"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="F61" s="13"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="F62" s="13"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="F63" s="13"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="F64" s="13"/>
+    </row>
+    <row r="65" spans="6:6">
+      <c r="F65" s="13"/>
+    </row>
+    <row r="66" spans="6:6">
+      <c r="F66" s="13"/>
+    </row>
+    <row r="67" spans="6:6">
+      <c r="F67" s="13"/>
+    </row>
+    <row r="68" spans="6:6">
+      <c r="F68" s="13"/>
+    </row>
+    <row r="69" spans="6:6">
+      <c r="F69" s="13"/>
+    </row>
+    <row r="70" spans="6:6">
+      <c r="F70" s="13"/>
+    </row>
+    <row r="71" spans="6:6">
+      <c r="F71" s="13"/>
+    </row>
+    <row r="72" spans="6:6">
+      <c r="F72" s="13"/>
+    </row>
+    <row r="73" spans="6:6">
+      <c r="F73" s="13"/>
+    </row>
+    <row r="74" spans="6:6">
+      <c r="F74" s="13"/>
+    </row>
+    <row r="75" spans="6:6">
+      <c r="F75" s="13"/>
+    </row>
+    <row r="76" spans="6:6">
+      <c r="F76" s="13"/>
+    </row>
+    <row r="77" spans="6:6">
+      <c r="F77" s="13"/>
+    </row>
+    <row r="78" spans="6:6">
+      <c r="F78" s="13"/>
+    </row>
+    <row r="79" spans="6:6">
+      <c r="F79" s="13"/>
+    </row>
+    <row r="80" spans="6:6">
+      <c r="F80" s="13"/>
+    </row>
+    <row r="81" spans="6:6">
+      <c r="F81" s="13"/>
+    </row>
+    <row r="82" spans="6:6">
+      <c r="F82" s="13"/>
+    </row>
+    <row r="83" spans="6:6">
+      <c r="F83" s="13"/>
+    </row>
+    <row r="84" spans="6:6">
+      <c r="F84" s="13"/>
+    </row>
+    <row r="85" spans="6:6">
+      <c r="F85" s="13"/>
+    </row>
+    <row r="86" spans="6:6">
+      <c r="F86" s="13"/>
+    </row>
+    <row r="87" spans="6:6">
+      <c r="F87" s="13"/>
+    </row>
+    <row r="88" spans="6:6">
+      <c r="F88" s="13"/>
+    </row>
+    <row r="89" spans="6:6">
+      <c r="F89" s="13"/>
+    </row>
+    <row r="90" spans="6:6">
+      <c r="F90" s="13"/>
+    </row>
+    <row r="91" spans="6:6">
+      <c r="F91" s="13"/>
+    </row>
+    <row r="92" spans="6:6">
+      <c r="F92" s="13"/>
+    </row>
+    <row r="93" spans="6:6">
+      <c r="F93" s="13"/>
+    </row>
+    <row r="94" spans="6:6">
+      <c r="F94" s="13"/>
+    </row>
+    <row r="95" spans="6:6">
+      <c r="F95" s="13"/>
+    </row>
+    <row r="96" spans="6:6">
+      <c r="F96" s="13"/>
+    </row>
+    <row r="97" spans="6:6">
+      <c r="F97" s="13"/>
+    </row>
+    <row r="98" spans="6:6">
+      <c r="F98" s="13"/>
+    </row>
+    <row r="99" spans="6:6">
+      <c r="F99" s="13"/>
+    </row>
+    <row r="100" spans="6:6">
+      <c r="F100" s="13"/>
+    </row>
+    <row r="101" spans="6:6">
+      <c r="F101" s="13"/>
+    </row>
+    <row r="102" spans="6:6">
+      <c r="F102" s="13"/>
+    </row>
+    <row r="103" spans="6:6">
+      <c r="F103" s="13"/>
+    </row>
+    <row r="104" spans="6:6">
+      <c r="F104" s="13"/>
+    </row>
+    <row r="105" spans="6:6">
+      <c r="F105" s="13"/>
+    </row>
+    <row r="106" spans="6:6">
+      <c r="F106" s="13"/>
+    </row>
+    <row r="107" spans="6:6">
+      <c r="F107" s="13"/>
+    </row>
+    <row r="108" spans="6:6">
+      <c r="F108" s="13"/>
+    </row>
+    <row r="109" spans="6:6">
+      <c r="F109" s="13"/>
+    </row>
+    <row r="110" spans="6:6">
+      <c r="F110" s="13"/>
+    </row>
+    <row r="111" spans="6:6">
+      <c r="F111" s="13"/>
+    </row>
+    <row r="112" spans="6:6">
+      <c r="F112" s="13"/>
+    </row>
+    <row r="113" spans="6:6">
+      <c r="F113" s="13"/>
+    </row>
+    <row r="114" spans="6:6">
+      <c r="F114" s="13"/>
+    </row>
+    <row r="115" spans="6:6">
+      <c r="F115" s="13"/>
+    </row>
+    <row r="116" spans="6:6">
+      <c r="F116" s="13"/>
+    </row>
+    <row r="117" spans="6:6">
+      <c r="F117" s="13"/>
+    </row>
+    <row r="118" spans="6:6">
+      <c r="F118" s="13"/>
+    </row>
+    <row r="119" spans="6:6">
+      <c r="F119" s="13"/>
+    </row>
+    <row r="120" spans="6:6">
+      <c r="F120" s="13"/>
+    </row>
+    <row r="121" spans="6:6">
+      <c r="F121" s="13"/>
+    </row>
+    <row r="122" spans="6:6">
+      <c r="F122" s="13"/>
+    </row>
+    <row r="123" spans="6:6">
+      <c r="F123" s="13"/>
+    </row>
+    <row r="124" spans="6:6">
+      <c r="F124" s="13"/>
+    </row>
+    <row r="125" spans="6:6">
+      <c r="F125" s="13"/>
+    </row>
+    <row r="126" spans="6:6">
+      <c r="F126" s="13"/>
+    </row>
+    <row r="127" spans="6:6">
+      <c r="F127" s="13"/>
+    </row>
+    <row r="128" spans="6:6">
+      <c r="F128" s="13"/>
+    </row>
+    <row r="129" spans="6:6">
+      <c r="F129" s="13"/>
+    </row>
+    <row r="130" spans="6:6">
+      <c r="F130" s="13"/>
+    </row>
+    <row r="131" spans="6:6">
+      <c r="F131" s="13"/>
+    </row>
+    <row r="132" spans="6:6">
+      <c r="F132" s="13"/>
+    </row>
+    <row r="133" spans="6:6">
+      <c r="F133" s="13"/>
+    </row>
+    <row r="134" spans="6:6">
+      <c r="F134" s="13"/>
+    </row>
+    <row r="135" spans="6:6">
+      <c r="F135" s="13"/>
+    </row>
+    <row r="136" spans="6:6">
+      <c r="F136" s="13"/>
+    </row>
+    <row r="137" spans="6:6">
+      <c r="F137" s="13"/>
+    </row>
+    <row r="138" spans="6:6">
+      <c r="F138" s="13"/>
+    </row>
+    <row r="139" spans="6:6">
+      <c r="F139" s="13"/>
+    </row>
+    <row r="140" spans="6:6">
+      <c r="F140" s="13"/>
+    </row>
+    <row r="141" spans="6:6">
+      <c r="F141" s="13"/>
+    </row>
+    <row r="142" spans="6:6">
+      <c r="F142" s="13"/>
+    </row>
+    <row r="143" spans="6:6">
+      <c r="F143" s="13"/>
+    </row>
+    <row r="144" spans="6:6">
+      <c r="F144" s="13"/>
+    </row>
+    <row r="145" spans="6:6">
+      <c r="F145" s="13"/>
+    </row>
+    <row r="146" spans="6:6">
+      <c r="F146" s="13"/>
+    </row>
+    <row r="147" spans="6:6">
+      <c r="F147" s="13"/>
+    </row>
+    <row r="148" spans="6:6">
+      <c r="F148" s="13"/>
+    </row>
+    <row r="149" spans="6:6">
+      <c r="F149" s="13"/>
+    </row>
+    <row r="150" spans="6:6">
+      <c r="F150" s="13"/>
+    </row>
+    <row r="151" spans="6:6">
+      <c r="F151" s="13"/>
+    </row>
+    <row r="152" spans="6:6">
+      <c r="F152" s="13"/>
+    </row>
+    <row r="153" spans="6:6">
+      <c r="F153" s="13"/>
+    </row>
+    <row r="154" spans="6:6">
+      <c r="F154" s="13"/>
+    </row>
+    <row r="155" spans="6:6">
+      <c r="F155" s="13"/>
+    </row>
+    <row r="156" spans="6:6">
+      <c r="F156" s="13"/>
+    </row>
+    <row r="157" spans="6:6">
+      <c r="F157" s="13"/>
+    </row>
+    <row r="158" spans="6:6">
+      <c r="F158" s="13"/>
+    </row>
+    <row r="159" spans="6:6">
+      <c r="F159" s="13"/>
+    </row>
+    <row r="160" spans="6:6">
+      <c r="F160" s="13"/>
+    </row>
+    <row r="161" spans="6:6">
+      <c r="F161" s="13"/>
+    </row>
+    <row r="162" spans="6:6">
+      <c r="F162" s="13"/>
+    </row>
+    <row r="163" spans="6:6">
+      <c r="F163" s="13"/>
+    </row>
+    <row r="164" spans="6:6">
+      <c r="F164" s="13"/>
+    </row>
+    <row r="165" spans="6:6">
+      <c r="F165" s="13"/>
+    </row>
+    <row r="166" spans="6:6">
+      <c r="F166" s="13"/>
+    </row>
+    <row r="167" spans="6:6">
+      <c r="F167" s="13"/>
+    </row>
+    <row r="168" spans="6:6">
+      <c r="F168" s="13"/>
+    </row>
+    <row r="169" spans="6:6">
+      <c r="F169" s="13"/>
+    </row>
+    <row r="170" spans="6:6">
+      <c r="F170" s="13"/>
+    </row>
+    <row r="171" spans="6:6">
+      <c r="F171" s="13"/>
+    </row>
+    <row r="172" spans="6:6">
+      <c r="F172" s="13"/>
+    </row>
+    <row r="173" spans="6:6">
+      <c r="F173" s="13"/>
+    </row>
+    <row r="174" spans="6:6">
+      <c r="F174" s="13"/>
+    </row>
+    <row r="175" spans="6:6">
+      <c r="F175" s="13"/>
+    </row>
+    <row r="176" spans="6:6">
+      <c r="F176" s="13"/>
+    </row>
+    <row r="177" spans="6:6">
+      <c r="F177" s="13"/>
+    </row>
+    <row r="178" spans="6:6">
+      <c r="F178" s="13"/>
+    </row>
+    <row r="179" spans="6:6">
+      <c r="F179" s="13"/>
+    </row>
+    <row r="180" spans="6:6">
+      <c r="F180" s="13"/>
+    </row>
+    <row r="181" spans="6:6">
+      <c r="F181" s="13"/>
+    </row>
+    <row r="182" spans="6:6">
+      <c r="F182" s="13"/>
+    </row>
+    <row r="183" spans="6:6">
+      <c r="F183" s="13"/>
+    </row>
+    <row r="184" spans="6:6">
+      <c r="F184" s="13"/>
+    </row>
+    <row r="185" spans="6:6">
+      <c r="F185" s="13"/>
+    </row>
+    <row r="186" spans="6:6">
+      <c r="F186" s="13"/>
+    </row>
+    <row r="187" spans="6:6">
+      <c r="F187" s="13"/>
+    </row>
+    <row r="188" spans="6:6">
+      <c r="F188" s="13"/>
+    </row>
+    <row r="189" spans="6:6">
+      <c r="F189" s="13"/>
+    </row>
+    <row r="190" spans="6:6">
+      <c r="F190" s="13"/>
+    </row>
+    <row r="191" spans="6:6">
+      <c r="F191" s="13"/>
+    </row>
+    <row r="192" spans="6:6">
+      <c r="F192" s="13"/>
+    </row>
+    <row r="193" spans="6:6">
+      <c r="F193" s="13"/>
+    </row>
+    <row r="194" spans="6:6">
+      <c r="F194" s="13"/>
+    </row>
+    <row r="195" spans="6:6">
+      <c r="F195" s="13"/>
+    </row>
+    <row r="196" spans="6:6">
+      <c r="F196" s="13"/>
+    </row>
+    <row r="197" spans="6:6">
+      <c r="F197" s="13"/>
+    </row>
+    <row r="198" spans="6:6">
+      <c r="F198" s="13"/>
+    </row>
+    <row r="199" spans="6:6">
+      <c r="F199" s="13"/>
+    </row>
+    <row r="200" spans="6:6">
+      <c r="F200" s="13"/>
+    </row>
+    <row r="201" spans="6:6">
+      <c r="F201" s="13"/>
+    </row>
+    <row r="202" spans="6:6">
+      <c r="F202" s="13"/>
+    </row>
+    <row r="203" spans="6:6">
+      <c r="F203" s="13"/>
+    </row>
+    <row r="204" spans="6:6">
+      <c r="F204" s="13"/>
+    </row>
+    <row r="205" spans="6:6">
+      <c r="F205" s="13"/>
+    </row>
+    <row r="206" spans="6:6">
+      <c r="F206" s="13"/>
+    </row>
+    <row r="207" spans="6:6">
+      <c r="F207" s="13"/>
+    </row>
+    <row r="208" spans="6:6">
+      <c r="F208" s="13"/>
+    </row>
+    <row r="209" spans="6:6">
+      <c r="F209" s="13"/>
+    </row>
+    <row r="210" spans="6:6">
+      <c r="F210" s="13"/>
+    </row>
+    <row r="211" spans="6:6">
+      <c r="F211" s="13"/>
+    </row>
+    <row r="212" spans="6:6">
+      <c r="F212" s="13"/>
+    </row>
+    <row r="213" spans="6:6">
+      <c r="F213" s="13"/>
+    </row>
+    <row r="214" spans="6:6">
+      <c r="F214" s="13"/>
+    </row>
+    <row r="215" spans="6:6">
+      <c r="F215" s="13"/>
+    </row>
+    <row r="216" spans="6:6">
+      <c r="F216" s="13"/>
+    </row>
+    <row r="217" spans="6:6">
+      <c r="F217" s="13"/>
+    </row>
+    <row r="218" spans="6:6">
+      <c r="F218" s="13"/>
+    </row>
+    <row r="219" spans="6:6">
+      <c r="F219" s="13"/>
+    </row>
+    <row r="220" spans="6:6">
+      <c r="F220" s="13"/>
+    </row>
+    <row r="221" spans="6:6">
+      <c r="F221" s="13"/>
+    </row>
+    <row r="222" spans="6:6">
+      <c r="F222" s="13"/>
+    </row>
+    <row r="223" spans="6:6">
+      <c r="F223" s="13"/>
+    </row>
+    <row r="224" spans="6:6">
+      <c r="F224" s="13"/>
+    </row>
+    <row r="225" spans="6:6">
+      <c r="F225" s="13"/>
+    </row>
+    <row r="226" spans="6:6">
+      <c r="F226" s="13"/>
+    </row>
+    <row r="227" spans="6:6">
+      <c r="F227" s="13"/>
+    </row>
+    <row r="228" spans="6:6">
+      <c r="F228" s="13"/>
+    </row>
+    <row r="229" spans="6:6">
+      <c r="F229" s="13"/>
+    </row>
+    <row r="230" spans="6:6">
+      <c r="F230" s="13"/>
+    </row>
+    <row r="231" spans="6:6">
+      <c r="F231" s="13"/>
+    </row>
+    <row r="232" spans="6:6">
+      <c r="F232" s="13"/>
+    </row>
+    <row r="233" spans="6:6">
+      <c r="F233" s="13"/>
+    </row>
+    <row r="234" spans="6:6">
+      <c r="F234" s="13"/>
+    </row>
+    <row r="235" spans="6:6">
+      <c r="F235" s="13"/>
+    </row>
+    <row r="236" spans="6:6">
+      <c r="F236" s="13"/>
+    </row>
+    <row r="237" spans="6:6">
+      <c r="F237" s="13"/>
+    </row>
+    <row r="238" spans="6:6">
+      <c r="F238" s="13"/>
+    </row>
+    <row r="239" spans="6:6">
+      <c r="F239" s="13"/>
+    </row>
+    <row r="240" spans="6:6">
+      <c r="F240" s="13"/>
+    </row>
+    <row r="241" spans="6:6">
+      <c r="F241" s="13"/>
+    </row>
+    <row r="242" spans="6:6">
+      <c r="F242" s="13"/>
+    </row>
+    <row r="243" spans="6:6">
+      <c r="F243" s="13"/>
+    </row>
+    <row r="244" spans="6:6">
+      <c r="F244" s="13"/>
+    </row>
+    <row r="245" spans="6:6">
+      <c r="F245" s="13"/>
+    </row>
+    <row r="246" spans="6:6">
+      <c r="F246" s="13"/>
+    </row>
+    <row r="247" spans="6:6">
+      <c r="F247" s="13"/>
+    </row>
+    <row r="248" spans="6:6">
+      <c r="F248" s="13"/>
+    </row>
+    <row r="249" spans="6:6">
+      <c r="F249" s="13"/>
+    </row>
+    <row r="250" spans="6:6">
+      <c r="F250" s="13"/>
+    </row>
+    <row r="251" spans="6:6">
+      <c r="F251" s="13"/>
+    </row>
+    <row r="252" spans="6:6">
+      <c r="F252" s="13"/>
+    </row>
+    <row r="253" spans="6:6">
+      <c r="F253" s="13"/>
+    </row>
+    <row r="254" spans="6:6">
+      <c r="F254" s="13"/>
+    </row>
+    <row r="255" spans="6:6">
+      <c r="F255" s="13"/>
+    </row>
+    <row r="256" spans="6:6">
+      <c r="F256" s="13"/>
+    </row>
+    <row r="257" spans="6:6">
+      <c r="F257" s="13"/>
+    </row>
+    <row r="258" spans="6:6">
+      <c r="F258" s="13"/>
+    </row>
+    <row r="259" spans="6:6">
+      <c r="F259" s="13"/>
+    </row>
+    <row r="260" spans="6:6">
+      <c r="F260" s="13"/>
+    </row>
+    <row r="261" spans="6:6">
+      <c r="F261" s="13"/>
+    </row>
+    <row r="262" spans="6:6">
+      <c r="F262" s="13"/>
+    </row>
+    <row r="263" spans="6:6">
+      <c r="F263" s="13"/>
+    </row>
+    <row r="264" spans="6:6">
+      <c r="F264" s="13"/>
+    </row>
+    <row r="265" spans="6:6">
+      <c r="F265" s="13"/>
+    </row>
+    <row r="266" spans="6:6">
+      <c r="F266" s="13"/>
+    </row>
+    <row r="267" spans="6:6">
+      <c r="F267" s="13"/>
+    </row>
+    <row r="268" spans="6:6">
+      <c r="F268" s="13"/>
+    </row>
+    <row r="269" spans="6:6">
+      <c r="F269" s="13"/>
+    </row>
+    <row r="270" spans="6:6">
+      <c r="F270" s="13"/>
+    </row>
+    <row r="271" spans="6:6">
+      <c r="F271" s="13"/>
+    </row>
+    <row r="272" spans="6:6">
+      <c r="F272" s="13"/>
+    </row>
+    <row r="273" spans="6:6">
+      <c r="F273" s="13"/>
+    </row>
+    <row r="274" spans="6:6">
+      <c r="F274" s="13"/>
+    </row>
+    <row r="275" spans="6:6">
+      <c r="F275" s="13"/>
+    </row>
+    <row r="276" spans="6:6">
+      <c r="F276" s="13"/>
+    </row>
+    <row r="277" spans="6:6">
+      <c r="F277" s="13"/>
+    </row>
+    <row r="278" spans="6:6">
+      <c r="F278" s="13"/>
+    </row>
+    <row r="279" spans="6:6">
+      <c r="F279" s="13"/>
+    </row>
+    <row r="280" spans="6:6">
+      <c r="F280" s="13"/>
+    </row>
+    <row r="281" spans="6:6">
+      <c r="F281" s="13"/>
+    </row>
+    <row r="282" spans="6:6">
+      <c r="F282" s="13"/>
+    </row>
+    <row r="283" spans="6:6">
+      <c r="F283" s="13"/>
+    </row>
+    <row r="284" spans="6:6">
+      <c r="F284" s="13"/>
+    </row>
+    <row r="285" spans="6:6">
+      <c r="F285" s="13"/>
+    </row>
+    <row r="286" spans="6:6">
+      <c r="F286" s="13"/>
+    </row>
+    <row r="287" spans="6:6">
+      <c r="F287" s="13"/>
+    </row>
+    <row r="288" spans="6:6">
+      <c r="F288" s="13"/>
+    </row>
+    <row r="289" spans="6:6">
+      <c r="F289" s="13"/>
+    </row>
+    <row r="290" spans="6:6">
+      <c r="F290" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
[20231225] Code Preparson & Google Interview 85 (1-2)
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7677750-4E54-5347-ADFD-FB7D991E5FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F43D4B5-8C41-8146-9FFB-6C747C870279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
     <sheet name="Blind 75" sheetId="1" r:id="rId2"/>
     <sheet name="Top Interview Q - Meduim 52" sheetId="2" r:id="rId3"/>
-    <sheet name="Dynamic Programming" sheetId="4" r:id="rId4"/>
-    <sheet name="Recursion I" sheetId="5" r:id="rId5"/>
-    <sheet name="Heap" sheetId="6" r:id="rId6"/>
-    <sheet name="Sorting" sheetId="7" r:id="rId7"/>
-    <sheet name="Binary Search" sheetId="9" r:id="rId8"/>
-    <sheet name="Graph" sheetId="8" r:id="rId9"/>
+    <sheet name="Google Interview" sheetId="10" r:id="rId4"/>
+    <sheet name="Dynamic Programming" sheetId="4" r:id="rId5"/>
+    <sheet name="Recursion I" sheetId="5" r:id="rId6"/>
+    <sheet name="Heap" sheetId="6" r:id="rId7"/>
+    <sheet name="Sorting" sheetId="7" r:id="rId8"/>
+    <sheet name="Binary Search" sheetId="9" r:id="rId9"/>
+    <sheet name="Graph" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="720">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2556,6 +2557,76 @@
   </si>
   <si>
     <t>knows(candidate, i): candidate = i, then check is_celebrity (if knows(i, j) or not knows(j, i): return False) else True</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/3044/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique Email Addresses</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/3045/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Odd Even Jump</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array
+and
+String</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hard</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.25</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>set() to save and loop for split('@') then localName.split('+')[0].replace('.', '')</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>License Key Formatting</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/472/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> split('@') , remove char: replace('.', '')</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(s.upper()).replace("-","")[::-1] and then for loop (0, len(s), k): answer += s[i:i+k] + "-" return answer[::-1][1:]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>for i in reversed(range(n)): start from last index</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fruit Into Baskets</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/3046/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2715,7 +2786,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2758,6 +2829,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2794,8 +2868,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3114,7 +3200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -3130,14 +3216,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -3179,7 +3265,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3212,7 +3298,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -3240,7 +3326,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3267,7 +3353,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -3294,7 +3380,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -3321,7 +3407,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -3351,7 +3437,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -3378,7 +3464,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -3405,7 +3491,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -3432,7 +3518,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -3462,7 +3548,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3489,7 +3575,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>124</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3521,7 +3607,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3548,7 +3634,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3575,7 +3661,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3602,7 +3688,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3632,7 +3718,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -3656,7 +3742,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3683,7 +3769,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="14"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3710,7 +3796,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="15" t="s">
         <v>125</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -3739,7 +3825,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="14"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -3766,7 +3852,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3793,7 +3879,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3820,7 +3906,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="14"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3847,7 +3933,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="14"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3877,7 +3963,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="15" t="s">
         <v>126</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -3909,7 +3995,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="14"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -3933,7 +4019,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="14"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3963,7 +4049,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="14"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -3987,7 +4073,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="14"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4011,7 +4097,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="15" t="s">
         <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -4037,7 +4123,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="14"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -4061,7 +4147,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="15" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -4087,7 +4173,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="14"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -4111,7 +4197,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="14"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -4135,7 +4221,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="14"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -4159,7 +4245,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="15" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -4185,7 +4271,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="14"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -4209,7 +4295,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="15" t="s">
         <v>130</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -4235,7 +4321,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="14"/>
+      <c r="C42" s="15"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -4259,7 +4345,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="14"/>
+      <c r="C43" s="15"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -4283,7 +4369,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="14"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -4307,7 +4393,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="15" t="s">
         <v>131</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -4333,7 +4419,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="14"/>
+      <c r="C46" s="15"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -4357,7 +4443,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="14"/>
+      <c r="C47" s="15"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -4381,7 +4467,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="14"/>
+      <c r="C48" s="15"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -4405,7 +4491,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="14"/>
+      <c r="C49" s="15"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -4429,7 +4515,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="14"/>
+      <c r="C50" s="15"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -4631,6 +4717,21 @@
     <hyperlink ref="F46" r:id="rId5" xr:uid="{B257738E-11CD-C047-9119-DEAD4671692E}"/>
     <hyperlink ref="F3" r:id="rId6" xr:uid="{0D9C7814-359E-3C4E-9D41-31A80D0FBD6B}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F6B7C9-F416-9A49-83DC-B48E6AB23806}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4660,15 +4761,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -4712,7 +4813,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="26">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -4750,7 +4851,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -4781,7 +4882,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="25"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -4811,7 +4912,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -4841,7 +4942,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -4871,7 +4972,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -4901,7 +5002,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="25"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -4931,7 +5032,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -4961,7 +5062,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -4991,7 +5092,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="25"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -5021,7 +5122,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -5051,7 +5152,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="25"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -5081,7 +5182,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="25"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -5114,7 +5215,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="21">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -5146,7 +5247,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="20"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -5176,7 +5277,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="20"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -5206,7 +5307,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="20"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -5236,7 +5337,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="2">
         <v>206</v>
       </c>
@@ -5266,7 +5367,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="2">
         <v>169</v>
       </c>
@@ -5296,7 +5397,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="2">
         <v>67</v>
       </c>
@@ -5326,7 +5427,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="20"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="2">
         <v>543</v>
       </c>
@@ -5356,7 +5457,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="20"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="2">
         <v>876</v>
       </c>
@@ -5386,7 +5487,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="20"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="2">
         <v>104</v>
       </c>
@@ -5416,7 +5517,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="20"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="2">
         <v>217</v>
       </c>
@@ -5446,7 +5547,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="20"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="2">
         <v>53</v>
       </c>
@@ -5476,7 +5577,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="22">
         <v>3</v>
       </c>
       <c r="C28" s="2">
@@ -5508,7 +5609,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="21"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="2">
         <v>542</v>
       </c>
@@ -5538,7 +5639,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="21"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="2">
         <v>973</v>
       </c>
@@ -5568,7 +5669,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="21"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="2">
         <v>3</v>
       </c>
@@ -5598,7 +5699,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="21"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="2">
         <v>15</v>
       </c>
@@ -5628,7 +5729,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="21"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="2">
         <v>102</v>
       </c>
@@ -5658,7 +5759,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="21"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="2">
         <v>133</v>
       </c>
@@ -5691,7 +5792,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="21"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="2">
         <v>150</v>
       </c>
@@ -5721,7 +5822,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="23">
         <v>4</v>
       </c>
       <c r="C36" s="2">
@@ -5756,7 +5857,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="22"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="2">
         <v>208</v>
       </c>
@@ -5786,7 +5887,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="22"/>
+      <c r="B38" s="23"/>
       <c r="C38" s="2">
         <v>322</v>
       </c>
@@ -5816,7 +5917,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="22"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="2">
         <v>238</v>
       </c>
@@ -5846,7 +5947,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="22"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="2">
         <v>155</v>
       </c>
@@ -5876,7 +5977,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="22"/>
+      <c r="B41" s="23"/>
       <c r="C41" s="2">
         <v>98</v>
       </c>
@@ -5906,7 +6007,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="22"/>
+      <c r="B42" s="23"/>
       <c r="C42" s="2">
         <v>200</v>
       </c>
@@ -5936,7 +6037,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="22"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="2">
         <v>994</v>
       </c>
@@ -5966,7 +6067,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="23">
+      <c r="B44" s="24">
         <v>5</v>
       </c>
       <c r="C44" s="2">
@@ -5998,7 +6099,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="2">
         <v>39</v>
       </c>
@@ -6031,7 +6132,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="23"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="2">
         <v>46</v>
       </c>
@@ -6061,7 +6162,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="23"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="2">
         <v>56</v>
       </c>
@@ -6091,7 +6192,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="23"/>
+      <c r="B48" s="24"/>
       <c r="C48" s="2">
         <v>236</v>
       </c>
@@ -6121,7 +6222,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="23"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="2">
         <v>981</v>
       </c>
@@ -6151,7 +6252,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="23"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="2">
         <v>721</v>
       </c>
@@ -6184,7 +6285,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="23"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="2">
         <v>75</v>
       </c>
@@ -6214,7 +6315,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="24">
+      <c r="B52" s="25">
         <v>6</v>
       </c>
       <c r="C52" s="2">
@@ -6246,7 +6347,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="24"/>
+      <c r="B53" s="25"/>
       <c r="C53" s="2">
         <v>416</v>
       </c>
@@ -6276,7 +6377,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="24"/>
+      <c r="B54" s="25"/>
       <c r="C54" s="2">
         <v>8</v>
       </c>
@@ -6306,7 +6407,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="24"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="2">
         <v>54</v>
       </c>
@@ -6336,7 +6437,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="24"/>
+      <c r="B56" s="25"/>
       <c r="C56" s="2">
         <v>78</v>
       </c>
@@ -6366,7 +6467,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="24"/>
+      <c r="B57" s="25"/>
       <c r="C57" s="2">
         <v>199</v>
       </c>
@@ -6396,7 +6497,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="24"/>
+      <c r="B58" s="25"/>
       <c r="C58" s="2">
         <v>5</v>
       </c>
@@ -6426,7 +6527,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="24"/>
+      <c r="B59" s="25"/>
       <c r="C59" s="2">
         <v>62</v>
       </c>
@@ -6456,7 +6557,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="24"/>
+      <c r="B60" s="25"/>
       <c r="C60" s="2">
         <v>105</v>
       </c>
@@ -6486,7 +6587,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="17">
+      <c r="B61" s="18">
         <v>7</v>
       </c>
       <c r="C61" s="2">
@@ -6518,7 +6619,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="17"/>
+      <c r="B62" s="18"/>
       <c r="C62" s="2">
         <v>17</v>
       </c>
@@ -6548,7 +6649,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="17"/>
+      <c r="B63" s="18"/>
       <c r="C63" s="2">
         <v>79</v>
       </c>
@@ -6578,7 +6679,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="17"/>
+      <c r="B64" s="18"/>
       <c r="C64" s="2">
         <v>438</v>
       </c>
@@ -6608,7 +6709,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="17"/>
+      <c r="B65" s="18"/>
       <c r="C65" s="2">
         <v>310</v>
       </c>
@@ -6638,7 +6739,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="17"/>
+      <c r="B66" s="18"/>
       <c r="C66" s="2">
         <v>621</v>
       </c>
@@ -6668,7 +6769,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="17"/>
+      <c r="B67" s="18"/>
       <c r="C67" s="2">
         <v>146</v>
       </c>
@@ -6698,7 +6799,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="18">
+      <c r="B68" s="19">
         <v>8</v>
       </c>
       <c r="C68" s="2">
@@ -6730,7 +6831,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="18"/>
+      <c r="B69" s="19"/>
       <c r="C69" s="2">
         <v>76</v>
       </c>
@@ -6760,7 +6861,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="18"/>
+      <c r="B70" s="19"/>
       <c r="C70" s="2">
         <v>297</v>
       </c>
@@ -6790,7 +6891,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="18"/>
+      <c r="B71" s="19"/>
       <c r="C71" s="2">
         <v>42</v>
       </c>
@@ -6820,7 +6921,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="18"/>
+      <c r="B72" s="19"/>
       <c r="C72" s="2">
         <v>295</v>
       </c>
@@ -6850,7 +6951,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="18"/>
+      <c r="B73" s="19"/>
       <c r="C73" s="2">
         <v>127</v>
       </c>
@@ -6880,7 +6981,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="18"/>
+      <c r="B74" s="19"/>
       <c r="C74" s="2">
         <v>224</v>
       </c>
@@ -6910,7 +7011,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="18"/>
+      <c r="B75" s="19"/>
       <c r="C75" s="2">
         <v>1235</v>
       </c>
@@ -6940,7 +7041,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="18"/>
+      <c r="B76" s="19"/>
       <c r="C76" s="2">
         <v>23</v>
       </c>
@@ -6970,7 +7071,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="18"/>
+      <c r="B77" s="19"/>
       <c r="C77" s="2">
         <v>84</v>
       </c>
@@ -7003,7 +7104,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="15" t="s">
         <v>131</v>
       </c>
       <c r="C78" s="2">
@@ -7035,7 +7136,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="14"/>
+      <c r="B79" s="15"/>
       <c r="C79" s="2">
         <v>153</v>
       </c>
@@ -7071,15 +7172,15 @@
       <c r="A85" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B85" s="19" t="s">
+      <c r="B85" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="19"/>
-      <c r="G85" s="19"/>
-      <c r="H85" s="19"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7166,8 +7267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7184,14 +7285,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>468</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -7235,7 +7336,7 @@
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>481</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -7268,14 +7369,14 @@
       <c r="B4" s="2">
         <v>73</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="14" t="s">
         <v>470</v>
       </c>
       <c r="G4" s="7" t="s">
@@ -7294,7 +7395,7 @@
       <c r="B5" s="2">
         <v>49</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -7318,7 +7419,7 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
@@ -7342,7 +7443,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
@@ -7366,7 +7467,7 @@
       <c r="B8" s="2">
         <v>334</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
@@ -7390,7 +7491,7 @@
       <c r="B9" s="2">
         <v>163</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -7414,7 +7515,7 @@
       <c r="B10" s="2">
         <v>38</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
@@ -7438,7 +7539,7 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>482</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -7447,7 +7548,7 @@
       <c r="E11" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="14" t="s">
         <v>502</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -7464,7 +7565,7 @@
       <c r="B12" s="2">
         <v>328</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -7488,7 +7589,7 @@
       <c r="B13" s="2">
         <v>160</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
@@ -7512,7 +7613,7 @@
       <c r="B14" s="2">
         <v>94</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>483</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -7538,7 +7639,7 @@
       <c r="B15" s="2">
         <v>103</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -7562,7 +7663,7 @@
       <c r="B16" s="2">
         <v>105</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
@@ -7589,7 +7690,7 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
@@ -7613,7 +7714,7 @@
       <c r="B18" s="2">
         <v>230</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -7637,7 +7738,7 @@
       <c r="B19" s="2">
         <v>285</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -7664,7 +7765,7 @@
       <c r="B20" s="2">
         <v>200</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
@@ -7688,7 +7789,7 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>484</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -7714,7 +7815,7 @@
       <c r="B22" s="2">
         <v>22</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
@@ -7738,7 +7839,7 @@
       <c r="B23" s="2">
         <v>46</v>
       </c>
-      <c r="C23" s="14"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -7762,7 +7863,7 @@
       <c r="B24" s="2">
         <v>78</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
@@ -7786,7 +7887,7 @@
       <c r="B25" s="2">
         <v>79</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
@@ -7813,7 +7914,7 @@
       <c r="B26" s="2">
         <v>75</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="15" t="s">
         <v>127</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -7839,7 +7940,7 @@
       <c r="B27" s="2">
         <v>347</v>
       </c>
-      <c r="C27" s="14"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -7866,7 +7967,7 @@
       <c r="B28" s="2">
         <v>215</v>
       </c>
-      <c r="C28" s="14"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -7893,7 +7994,7 @@
       <c r="B29" s="2">
         <v>162</v>
       </c>
-      <c r="C29" s="14"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -7917,7 +8018,7 @@
       <c r="B30" s="2">
         <v>34</v>
       </c>
-      <c r="C30" s="14"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
@@ -7941,7 +8042,7 @@
       <c r="B31" s="2">
         <v>56</v>
       </c>
-      <c r="C31" s="14"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -7965,7 +8066,7 @@
       <c r="B32" s="2">
         <v>33</v>
       </c>
-      <c r="C32" s="14"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -7989,7 +8090,7 @@
       <c r="B33" s="2">
         <v>253</v>
       </c>
-      <c r="C33" s="14"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
@@ -8013,7 +8114,7 @@
       <c r="B34" s="2">
         <v>240</v>
       </c>
-      <c r="C34" s="14"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
@@ -8037,7 +8138,7 @@
       <c r="B35" s="2">
         <v>55</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="15" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -8063,7 +8164,7 @@
       <c r="B36" s="2">
         <v>62</v>
       </c>
-      <c r="C36" s="14"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
@@ -8087,7 +8188,7 @@
       <c r="B37" s="2">
         <v>322</v>
       </c>
-      <c r="C37" s="14"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -8111,7 +8212,7 @@
       <c r="B38" s="2">
         <v>300</v>
       </c>
-      <c r="C38" s="14"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -8138,7 +8239,7 @@
       <c r="B39" s="2">
         <v>251</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="15" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -8164,7 +8265,7 @@
       <c r="B40" s="2">
         <v>297</v>
       </c>
-      <c r="C40" s="14"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="2" t="s">
         <v>88</v>
       </c>
@@ -8188,7 +8289,7 @@
       <c r="B41" s="2">
         <v>380</v>
       </c>
-      <c r="C41" s="14"/>
+      <c r="C41" s="15"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
@@ -8215,7 +8316,7 @@
       <c r="B42" s="2">
         <v>348</v>
       </c>
-      <c r="C42" s="14"/>
+      <c r="C42" s="15"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -8239,7 +8340,7 @@
       <c r="B43" s="2">
         <v>202</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="15" t="s">
         <v>130</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -8265,7 +8366,7 @@
       <c r="B44" s="2">
         <v>172</v>
       </c>
-      <c r="C44" s="14"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
@@ -8289,7 +8390,7 @@
       <c r="B45" s="2">
         <v>171</v>
       </c>
-      <c r="C45" s="14"/>
+      <c r="C45" s="15"/>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
@@ -8316,7 +8417,7 @@
       <c r="B46" s="2">
         <v>50</v>
       </c>
-      <c r="C46" s="14"/>
+      <c r="C46" s="15"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
@@ -8343,7 +8444,7 @@
       <c r="B47" s="2">
         <v>69</v>
       </c>
-      <c r="C47" s="14"/>
+      <c r="C47" s="15"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -8370,7 +8471,7 @@
       <c r="B48" s="2">
         <v>29</v>
       </c>
-      <c r="C48" s="14"/>
+      <c r="C48" s="15"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
@@ -8394,7 +8495,7 @@
       <c r="B49" s="2">
         <v>166</v>
       </c>
-      <c r="C49" s="14"/>
+      <c r="C49" s="15"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
@@ -8418,7 +8519,7 @@
       <c r="B50" s="2">
         <v>371</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="15" t="s">
         <v>131</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -8444,7 +8545,7 @@
       <c r="B51" s="2">
         <v>150</v>
       </c>
-      <c r="C51" s="14"/>
+      <c r="C51" s="15"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
@@ -8468,7 +8569,7 @@
       <c r="B52" s="2">
         <v>169</v>
       </c>
-      <c r="C52" s="14"/>
+      <c r="C52" s="15"/>
       <c r="D52" s="2" t="s">
         <v>21</v>
       </c>
@@ -8492,7 +8593,7 @@
       <c r="B53" s="2">
         <v>645</v>
       </c>
-      <c r="C53" s="14"/>
+      <c r="C53" s="15"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
@@ -8516,7 +8617,7 @@
       <c r="B54" s="2">
         <v>621</v>
       </c>
-      <c r="C54" s="14"/>
+      <c r="C54" s="15"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
@@ -9246,16 +9347,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9282,6 +9383,1114 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
+  <dimension ref="A1:J87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="96" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>708</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1">
+      <c r="A3" s="27">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>704</v>
+      </c>
+      <c r="C3" s="2">
+        <v>929</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>703</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1">
+      <c r="A4" s="27">
+        <v>2</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="2">
+        <v>975</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>706</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1">
+      <c r="A5" s="27">
+        <v>3</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="2">
+        <v>482</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1">
+      <c r="A6" s="27">
+        <v>4</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="2">
+        <v>904</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1">
+      <c r="A7" s="27">
+        <v>5</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1">
+      <c r="A8" s="27">
+        <v>6</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1">
+      <c r="A9" s="27">
+        <v>7</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1">
+      <c r="A10" s="27">
+        <v>8</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1">
+      <c r="A11" s="27">
+        <v>9</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>709</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1">
+      <c r="A12" s="27">
+        <v>10</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1">
+      <c r="A13" s="27">
+        <v>11</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1">
+      <c r="A14" s="27">
+        <v>12</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1">
+      <c r="A15" s="27">
+        <v>13</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1">
+      <c r="A16" s="27">
+        <v>14</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1">
+      <c r="A17" s="27">
+        <v>15</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1">
+      <c r="A18" s="27">
+        <v>16</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1">
+      <c r="A19" s="27">
+        <v>17</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1">
+      <c r="A20" s="27">
+        <v>18</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1">
+      <c r="A21" s="27">
+        <v>19</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1">
+      <c r="A22" s="27">
+        <v>20</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="A23" s="27">
+        <v>21</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1">
+      <c r="A24" s="27">
+        <v>22</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1">
+      <c r="A25" s="27">
+        <v>23</v>
+      </c>
+      <c r="B25" s="28"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1">
+      <c r="A26" s="27">
+        <v>24</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1">
+      <c r="A27" s="27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1">
+      <c r="A28" s="27">
+        <v>26</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1">
+      <c r="A29" s="27">
+        <v>27</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1">
+      <c r="A30" s="27">
+        <v>28</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1">
+      <c r="A31" s="27">
+        <v>29</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1">
+      <c r="A32" s="27">
+        <v>30</v>
+      </c>
+      <c r="B32" s="28"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" customHeight="1">
+      <c r="A33" s="27">
+        <v>31</v>
+      </c>
+      <c r="B33" s="28"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" ht="15" customHeight="1">
+      <c r="A34" s="27">
+        <v>32</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" ht="15" customHeight="1">
+      <c r="A35" s="27">
+        <v>33</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" customHeight="1">
+      <c r="A36" s="27">
+        <v>34</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" ht="15" customHeight="1">
+      <c r="A37" s="27">
+        <v>35</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" ht="15" customHeight="1">
+      <c r="A38" s="27">
+        <v>36</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1">
+      <c r="A39" s="27">
+        <v>37</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" ht="15" customHeight="1">
+      <c r="A40" s="27">
+        <v>38</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:10" ht="15" customHeight="1">
+      <c r="A41" s="27">
+        <v>39</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" ht="15" customHeight="1">
+      <c r="A42" s="27">
+        <v>40</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" ht="15" customHeight="1">
+      <c r="A43" s="27">
+        <v>41</v>
+      </c>
+      <c r="B43" s="27"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:10" ht="15" customHeight="1">
+      <c r="A44" s="27">
+        <v>42</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:10" ht="15" customHeight="1">
+      <c r="A45" s="27">
+        <v>43</v>
+      </c>
+      <c r="B45" s="27"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" ht="15" customHeight="1">
+      <c r="A46" s="27">
+        <v>44</v>
+      </c>
+      <c r="B46" s="27"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" ht="15" customHeight="1">
+      <c r="A47" s="27">
+        <v>45</v>
+      </c>
+      <c r="B47" s="27"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" ht="15" customHeight="1">
+      <c r="A48" s="27">
+        <v>46</v>
+      </c>
+      <c r="B48" s="27"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" ht="15" customHeight="1">
+      <c r="A49" s="27">
+        <v>47</v>
+      </c>
+      <c r="B49" s="27"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" ht="15" customHeight="1">
+      <c r="A50" s="27">
+        <v>48</v>
+      </c>
+      <c r="B50" s="27"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" ht="15" customHeight="1">
+      <c r="A51" s="27">
+        <v>49</v>
+      </c>
+      <c r="B51" s="27"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" ht="15" customHeight="1">
+      <c r="A52" s="27">
+        <v>50</v>
+      </c>
+      <c r="B52" s="27"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="15" customHeight="1">
+      <c r="A53" s="27">
+        <v>51</v>
+      </c>
+      <c r="B53" s="27"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" ht="15" customHeight="1">
+      <c r="A54" s="27">
+        <v>52</v>
+      </c>
+      <c r="B54" s="27"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" ht="15" customHeight="1">
+      <c r="A55" s="27">
+        <v>53</v>
+      </c>
+      <c r="B55" s="27"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" ht="15" customHeight="1">
+      <c r="A56" s="27">
+        <v>54</v>
+      </c>
+      <c r="B56" s="27"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" ht="15" customHeight="1">
+      <c r="A57" s="27">
+        <v>55</v>
+      </c>
+      <c r="B57" s="27"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" ht="15" customHeight="1">
+      <c r="A58" s="27">
+        <v>56</v>
+      </c>
+      <c r="B58" s="27"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" ht="15" customHeight="1">
+      <c r="A59" s="27">
+        <v>57</v>
+      </c>
+      <c r="B59" s="27"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" ht="15" customHeight="1">
+      <c r="A60" s="27">
+        <v>58</v>
+      </c>
+      <c r="B60" s="27"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" ht="15" customHeight="1">
+      <c r="A61" s="27">
+        <v>59</v>
+      </c>
+      <c r="B61" s="27"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" ht="15" customHeight="1">
+      <c r="A62" s="27">
+        <v>60</v>
+      </c>
+      <c r="B62" s="27"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" ht="15" customHeight="1">
+      <c r="A63" s="27">
+        <v>61</v>
+      </c>
+      <c r="B63" s="27"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" ht="15" customHeight="1">
+      <c r="A64" s="27">
+        <v>62</v>
+      </c>
+      <c r="B64" s="27"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" ht="15" customHeight="1">
+      <c r="A65" s="27">
+        <v>63</v>
+      </c>
+      <c r="B65" s="27"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" ht="15" customHeight="1">
+      <c r="A66" s="27">
+        <v>64</v>
+      </c>
+      <c r="B66" s="27"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" ht="15" customHeight="1">
+      <c r="A67" s="27">
+        <v>65</v>
+      </c>
+      <c r="B67" s="27"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" ht="15" customHeight="1">
+      <c r="A68" s="27">
+        <v>66</v>
+      </c>
+      <c r="B68" s="27"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" ht="15" customHeight="1">
+      <c r="A69" s="27">
+        <v>67</v>
+      </c>
+      <c r="B69" s="27"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" ht="15" customHeight="1">
+      <c r="A70" s="27">
+        <v>68</v>
+      </c>
+      <c r="B70" s="27"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" ht="15" customHeight="1">
+      <c r="A71" s="27">
+        <v>69</v>
+      </c>
+      <c r="B71" s="27"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" ht="15" customHeight="1">
+      <c r="A72" s="27">
+        <v>70</v>
+      </c>
+      <c r="B72" s="27"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" ht="15" customHeight="1">
+      <c r="A73" s="27">
+        <v>71</v>
+      </c>
+      <c r="B73" s="27"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" ht="15" customHeight="1">
+      <c r="A74" s="27">
+        <v>72</v>
+      </c>
+      <c r="B74" s="27"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" ht="15" customHeight="1">
+      <c r="A75" s="27">
+        <v>73</v>
+      </c>
+      <c r="B75" s="27"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" ht="15" customHeight="1">
+      <c r="A76" s="27">
+        <v>74</v>
+      </c>
+      <c r="B76" s="27"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8" ht="15" customHeight="1">
+      <c r="A77" s="27">
+        <v>75</v>
+      </c>
+      <c r="B77" s="27"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="1:8" ht="15" customHeight="1">
+      <c r="A78" s="27">
+        <v>76</v>
+      </c>
+      <c r="B78" s="27"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8" ht="15" customHeight="1">
+      <c r="A79" s="27">
+        <v>77</v>
+      </c>
+      <c r="B79" s="27"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="27">
+        <v>78</v>
+      </c>
+      <c r="B80" s="27"/>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="27">
+        <v>79</v>
+      </c>
+      <c r="B81" s="27"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="27">
+        <v>80</v>
+      </c>
+      <c r="B82" s="27"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="27">
+        <v>81</v>
+      </c>
+      <c r="B83" s="27"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="27">
+        <v>82</v>
+      </c>
+      <c r="B84" s="27"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="27">
+        <v>83</v>
+      </c>
+      <c r="B85" s="27"/>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="27">
+        <v>84</v>
+      </c>
+      <c r="B86" s="27"/>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="27">
+        <v>85</v>
+      </c>
+      <c r="B87" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{9DF6453F-4C5C-F54A-8796-90F83CF65981}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{7DC4C275-2445-8A49-B4AF-FD0F1FB8620B}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{3D8F3E8A-65F8-1947-9319-9A6D3C038568}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{45091034-383D-3D41-BB94-FEDC2A783DAD}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{F83A99E0-BEA8-5F4B-9316-55278A6B2525}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F80E9F-AC4D-B74C-865E-81CF884A25E9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -9292,14 +10501,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>645</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>
@@ -9348,7 +10557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F34D86-1608-9344-891E-7915A575FAB2}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9363,7 +10572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C48A37-262A-DE49-8582-3B78371E9BE0}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9376,7 +10585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24F8B26-181E-FA45-9F6A-F1DE45F8E2D2}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9391,7 +10600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED2A95A-A5C1-7B46-B514-8AACCDB615E6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9404,19 +10613,4 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F6B7C9-F416-9A49-83DC-B48E6AB23806}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[20231226] Google Interview (85) 3-4
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F43D4B5-8C41-8146-9FFB-6C747C870279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E95A6F-B74C-7448-BD14-1BBC8DBBEF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="733">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2627,6 +2627,58 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/interview/card/google/67/sql-2/3046/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google Phone Interview</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google Onsite Interview</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google Hiring Committee</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google Offer Review</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3047/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3048/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Review</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">slide window with dict, for loop run all and if len(table) &gt; 2: table[fruits[left]] -= 1and  if table== 0: del table[fruits[left]] </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two ptr left, right to scan curArea and calc maxArea, and move ptr by smaller for left or right</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slide window: left, dict, for right</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dict/set with left and for loop run right, if not in dict or idx less than left idx, calc max, else left+1, replace idx of right</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2786,7 +2838,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2832,6 +2884,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2868,19 +2923,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3216,14 +3259,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -3265,7 +3308,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3298,7 +3341,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -3326,7 +3369,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3353,7 +3396,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -3380,7 +3423,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -3407,7 +3450,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -3437,7 +3480,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -3464,7 +3507,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -3491,7 +3534,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -3518,7 +3561,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -3548,7 +3591,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3575,7 +3618,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="16" t="s">
         <v>124</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3607,7 +3650,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3634,7 +3677,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3661,7 +3704,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3688,7 +3731,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3718,7 +3761,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -3742,7 +3785,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3769,7 +3812,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3796,7 +3839,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>125</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -3825,7 +3868,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -3852,7 +3895,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3879,7 +3922,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3906,7 +3949,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="15"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3933,7 +3976,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3963,7 +4006,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>126</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -3995,7 +4038,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -4019,7 +4062,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -4049,7 +4092,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -4073,7 +4116,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4097,7 +4140,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="16" t="s">
         <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -4123,7 +4166,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -4147,7 +4190,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="16" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -4173,7 +4216,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="15"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -4197,7 +4240,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="15"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -4221,7 +4264,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="15"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -4245,7 +4288,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="16" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -4271,7 +4314,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="15"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -4295,7 +4338,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="16" t="s">
         <v>130</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -4321,7 +4364,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="15"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -4345,7 +4388,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="15"/>
+      <c r="C43" s="16"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -4369,7 +4412,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -4393,7 +4436,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="16" t="s">
         <v>131</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -4419,7 +4462,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="15"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -4443,7 +4486,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="15"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -4467,7 +4510,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="15"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -4491,7 +4534,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="15"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -4515,7 +4558,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="15"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -4761,15 +4804,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -4813,7 +4856,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -4851,7 +4894,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -4882,7 +4925,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -4912,7 +4955,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -4942,7 +4985,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -4972,7 +5015,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -5002,7 +5045,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -5032,7 +5075,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -5062,7 +5105,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -5092,7 +5135,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="26"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -5122,7 +5165,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -5152,7 +5195,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="26"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -5182,7 +5225,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -5215,7 +5258,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="22">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -5247,7 +5290,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -5277,7 +5320,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -5307,7 +5350,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -5337,7 +5380,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="2">
         <v>206</v>
       </c>
@@ -5367,7 +5410,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="21"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="2">
         <v>169</v>
       </c>
@@ -5397,7 +5440,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="21"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="2">
         <v>67</v>
       </c>
@@ -5427,7 +5470,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="21"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="2">
         <v>543</v>
       </c>
@@ -5457,7 +5500,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="21"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="2">
         <v>876</v>
       </c>
@@ -5487,7 +5530,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="21"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="2">
         <v>104</v>
       </c>
@@ -5517,7 +5560,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="21"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="2">
         <v>217</v>
       </c>
@@ -5547,7 +5590,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="2">
         <v>53</v>
       </c>
@@ -5577,7 +5620,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="23">
         <v>3</v>
       </c>
       <c r="C28" s="2">
@@ -5609,7 +5652,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="22"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="2">
         <v>542</v>
       </c>
@@ -5639,7 +5682,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="22"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="2">
         <v>973</v>
       </c>
@@ -5669,7 +5712,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="22"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="2">
         <v>3</v>
       </c>
@@ -5699,7 +5742,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="22"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="2">
         <v>15</v>
       </c>
@@ -5729,7 +5772,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="22"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="2">
         <v>102</v>
       </c>
@@ -5759,7 +5802,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="22"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="2">
         <v>133</v>
       </c>
@@ -5792,7 +5835,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="22"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="2">
         <v>150</v>
       </c>
@@ -5822,7 +5865,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="23">
+      <c r="B36" s="24">
         <v>4</v>
       </c>
       <c r="C36" s="2">
@@ -5857,7 +5900,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="23"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="2">
         <v>208</v>
       </c>
@@ -5887,7 +5930,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="23"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="2">
         <v>322</v>
       </c>
@@ -5917,7 +5960,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="23"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="2">
         <v>238</v>
       </c>
@@ -5947,7 +5990,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="23"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="2">
         <v>155</v>
       </c>
@@ -5977,7 +6020,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="23"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="2">
         <v>98</v>
       </c>
@@ -6007,7 +6050,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="23"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="2">
         <v>200</v>
       </c>
@@ -6037,7 +6080,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="23"/>
+      <c r="B43" s="24"/>
       <c r="C43" s="2">
         <v>994</v>
       </c>
@@ -6067,7 +6110,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="24">
+      <c r="B44" s="25">
         <v>5</v>
       </c>
       <c r="C44" s="2">
@@ -6099,7 +6142,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="24"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="2">
         <v>39</v>
       </c>
@@ -6132,7 +6175,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="24"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="2">
         <v>46</v>
       </c>
@@ -6162,7 +6205,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="24"/>
+      <c r="B47" s="25"/>
       <c r="C47" s="2">
         <v>56</v>
       </c>
@@ -6192,7 +6235,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="24"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="2">
         <v>236</v>
       </c>
@@ -6222,7 +6265,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="24"/>
+      <c r="B49" s="25"/>
       <c r="C49" s="2">
         <v>981</v>
       </c>
@@ -6252,7 +6295,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="24"/>
+      <c r="B50" s="25"/>
       <c r="C50" s="2">
         <v>721</v>
       </c>
@@ -6285,7 +6328,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="24"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="2">
         <v>75</v>
       </c>
@@ -6315,7 +6358,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="25">
+      <c r="B52" s="26">
         <v>6</v>
       </c>
       <c r="C52" s="2">
@@ -6347,7 +6390,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="25"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="2">
         <v>416</v>
       </c>
@@ -6377,7 +6420,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="25"/>
+      <c r="B54" s="26"/>
       <c r="C54" s="2">
         <v>8</v>
       </c>
@@ -6407,7 +6450,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="25"/>
+      <c r="B55" s="26"/>
       <c r="C55" s="2">
         <v>54</v>
       </c>
@@ -6437,7 +6480,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="25"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="2">
         <v>78</v>
       </c>
@@ -6467,7 +6510,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="2">
         <v>199</v>
       </c>
@@ -6497,7 +6540,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="25"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="2">
         <v>5</v>
       </c>
@@ -6527,7 +6570,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="25"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="2">
         <v>62</v>
       </c>
@@ -6557,7 +6600,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="25"/>
+      <c r="B60" s="26"/>
       <c r="C60" s="2">
         <v>105</v>
       </c>
@@ -6587,7 +6630,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="18">
+      <c r="B61" s="19">
         <v>7</v>
       </c>
       <c r="C61" s="2">
@@ -6619,7 +6662,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="18"/>
+      <c r="B62" s="19"/>
       <c r="C62" s="2">
         <v>17</v>
       </c>
@@ -6649,7 +6692,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="18"/>
+      <c r="B63" s="19"/>
       <c r="C63" s="2">
         <v>79</v>
       </c>
@@ -6679,7 +6722,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="18"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="2">
         <v>438</v>
       </c>
@@ -6709,7 +6752,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="18"/>
+      <c r="B65" s="19"/>
       <c r="C65" s="2">
         <v>310</v>
       </c>
@@ -6739,7 +6782,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="18"/>
+      <c r="B66" s="19"/>
       <c r="C66" s="2">
         <v>621</v>
       </c>
@@ -6769,7 +6812,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="18"/>
+      <c r="B67" s="19"/>
       <c r="C67" s="2">
         <v>146</v>
       </c>
@@ -6799,7 +6842,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="19">
+      <c r="B68" s="20">
         <v>8</v>
       </c>
       <c r="C68" s="2">
@@ -6831,7 +6874,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="19"/>
+      <c r="B69" s="20"/>
       <c r="C69" s="2">
         <v>76</v>
       </c>
@@ -6861,7 +6904,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="19"/>
+      <c r="B70" s="20"/>
       <c r="C70" s="2">
         <v>297</v>
       </c>
@@ -6891,7 +6934,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="19"/>
+      <c r="B71" s="20"/>
       <c r="C71" s="2">
         <v>42</v>
       </c>
@@ -6921,7 +6964,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="19"/>
+      <c r="B72" s="20"/>
       <c r="C72" s="2">
         <v>295</v>
       </c>
@@ -6951,7 +6994,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="19"/>
+      <c r="B73" s="20"/>
       <c r="C73" s="2">
         <v>127</v>
       </c>
@@ -6981,7 +7024,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="19"/>
+      <c r="B74" s="20"/>
       <c r="C74" s="2">
         <v>224</v>
       </c>
@@ -7011,7 +7054,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="19"/>
+      <c r="B75" s="20"/>
       <c r="C75" s="2">
         <v>1235</v>
       </c>
@@ -7041,7 +7084,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="19"/>
+      <c r="B76" s="20"/>
       <c r="C76" s="2">
         <v>23</v>
       </c>
@@ -7071,7 +7114,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="19"/>
+      <c r="B77" s="20"/>
       <c r="C77" s="2">
         <v>84</v>
       </c>
@@ -7104,7 +7147,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="16" t="s">
         <v>131</v>
       </c>
       <c r="C78" s="2">
@@ -7136,7 +7179,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="15"/>
+      <c r="B79" s="16"/>
       <c r="C79" s="2">
         <v>153</v>
       </c>
@@ -7172,15 +7215,15 @@
       <c r="A85" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="B85" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
-      <c r="G85" s="20"/>
-      <c r="H85" s="20"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7285,14 +7328,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>468</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -7336,7 +7379,7 @@
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>481</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -7369,7 +7412,7 @@
       <c r="B4" s="2">
         <v>73</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -7395,7 +7438,7 @@
       <c r="B5" s="2">
         <v>49</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -7419,7 +7462,7 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
@@ -7443,7 +7486,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
@@ -7467,7 +7510,7 @@
       <c r="B8" s="2">
         <v>334</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
@@ -7491,7 +7534,7 @@
       <c r="B9" s="2">
         <v>163</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -7515,7 +7558,7 @@
       <c r="B10" s="2">
         <v>38</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
@@ -7539,7 +7582,7 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="16" t="s">
         <v>482</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -7565,7 +7608,7 @@
       <c r="B12" s="2">
         <v>328</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -7589,7 +7632,7 @@
       <c r="B13" s="2">
         <v>160</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
@@ -7613,7 +7656,7 @@
       <c r="B14" s="2">
         <v>94</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="16" t="s">
         <v>483</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -7639,7 +7682,7 @@
       <c r="B15" s="2">
         <v>103</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -7663,7 +7706,7 @@
       <c r="B16" s="2">
         <v>105</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
@@ -7690,7 +7733,7 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
@@ -7714,7 +7757,7 @@
       <c r="B18" s="2">
         <v>230</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -7738,7 +7781,7 @@
       <c r="B19" s="2">
         <v>285</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -7765,7 +7808,7 @@
       <c r="B20" s="2">
         <v>200</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
@@ -7789,7 +7832,7 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="16" t="s">
         <v>484</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -7815,7 +7858,7 @@
       <c r="B22" s="2">
         <v>22</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
@@ -7839,7 +7882,7 @@
       <c r="B23" s="2">
         <v>46</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -7863,7 +7906,7 @@
       <c r="B24" s="2">
         <v>78</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
@@ -7887,7 +7930,7 @@
       <c r="B25" s="2">
         <v>79</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
@@ -7914,7 +7957,7 @@
       <c r="B26" s="2">
         <v>75</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="16" t="s">
         <v>127</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -7940,7 +7983,7 @@
       <c r="B27" s="2">
         <v>347</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -7967,7 +8010,7 @@
       <c r="B28" s="2">
         <v>215</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -7994,7 +8037,7 @@
       <c r="B29" s="2">
         <v>162</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -8018,7 +8061,7 @@
       <c r="B30" s="2">
         <v>34</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
@@ -8042,7 +8085,7 @@
       <c r="B31" s="2">
         <v>56</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -8066,7 +8109,7 @@
       <c r="B32" s="2">
         <v>33</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -8090,7 +8133,7 @@
       <c r="B33" s="2">
         <v>253</v>
       </c>
-      <c r="C33" s="15"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
@@ -8114,7 +8157,7 @@
       <c r="B34" s="2">
         <v>240</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
@@ -8138,7 +8181,7 @@
       <c r="B35" s="2">
         <v>55</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="16" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -8164,7 +8207,7 @@
       <c r="B36" s="2">
         <v>62</v>
       </c>
-      <c r="C36" s="15"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
@@ -8188,7 +8231,7 @@
       <c r="B37" s="2">
         <v>322</v>
       </c>
-      <c r="C37" s="15"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -8212,7 +8255,7 @@
       <c r="B38" s="2">
         <v>300</v>
       </c>
-      <c r="C38" s="15"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -8239,7 +8282,7 @@
       <c r="B39" s="2">
         <v>251</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="16" t="s">
         <v>129</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -8265,7 +8308,7 @@
       <c r="B40" s="2">
         <v>297</v>
       </c>
-      <c r="C40" s="15"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="2" t="s">
         <v>88</v>
       </c>
@@ -8289,7 +8332,7 @@
       <c r="B41" s="2">
         <v>380</v>
       </c>
-      <c r="C41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
@@ -8316,7 +8359,7 @@
       <c r="B42" s="2">
         <v>348</v>
       </c>
-      <c r="C42" s="15"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -8340,7 +8383,7 @@
       <c r="B43" s="2">
         <v>202</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="16" t="s">
         <v>130</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -8366,7 +8409,7 @@
       <c r="B44" s="2">
         <v>172</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
@@ -8390,7 +8433,7 @@
       <c r="B45" s="2">
         <v>171</v>
       </c>
-      <c r="C45" s="15"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
@@ -8417,7 +8460,7 @@
       <c r="B46" s="2">
         <v>50</v>
       </c>
-      <c r="C46" s="15"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
@@ -8444,7 +8487,7 @@
       <c r="B47" s="2">
         <v>69</v>
       </c>
-      <c r="C47" s="15"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -8471,7 +8514,7 @@
       <c r="B48" s="2">
         <v>29</v>
       </c>
-      <c r="C48" s="15"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
@@ -8495,7 +8538,7 @@
       <c r="B49" s="2">
         <v>166</v>
       </c>
-      <c r="C49" s="15"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
@@ -8519,7 +8562,7 @@
       <c r="B50" s="2">
         <v>371</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="16" t="s">
         <v>131</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -8545,7 +8588,7 @@
       <c r="B51" s="2">
         <v>150</v>
       </c>
-      <c r="C51" s="15"/>
+      <c r="C51" s="16"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
@@ -8569,7 +8612,7 @@
       <c r="B52" s="2">
         <v>169</v>
       </c>
-      <c r="C52" s="15"/>
+      <c r="C52" s="16"/>
       <c r="D52" s="2" t="s">
         <v>21</v>
       </c>
@@ -8593,7 +8636,7 @@
       <c r="B53" s="2">
         <v>645</v>
       </c>
-      <c r="C53" s="15"/>
+      <c r="C53" s="16"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
@@ -8617,7 +8660,7 @@
       <c r="B54" s="2">
         <v>621</v>
       </c>
-      <c r="C54" s="15"/>
+      <c r="C54" s="16"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
@@ -9347,16 +9390,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9387,7 +9430,7 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9396,21 +9439,21 @@
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="96" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>708</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
@@ -9439,17 +9482,17 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>7</v>
+        <v>728</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
-      <c r="A3" s="27">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="17" t="s">
         <v>704</v>
       </c>
       <c r="C3" s="2">
@@ -9478,10 +9521,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1">
-      <c r="A4" s="27">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="2">
         <v>975</v>
       </c>
@@ -9491,7 +9534,7 @@
       <c r="E4" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="15" t="s">
         <v>706</v>
       </c>
       <c r="G4" s="7"/>
@@ -9499,10 +9542,10 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="27">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="2">
         <v>482</v>
       </c>
@@ -9526,10 +9569,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1">
-      <c r="A6" s="27">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="2">
         <v>904</v>
       </c>
@@ -9542,100 +9585,140 @@
       <c r="F6" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
-      <c r="A7" s="27">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>720</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="27">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>721</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1">
-      <c r="A9" s="27">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>722</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1">
-      <c r="A10" s="27">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>723</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1">
-      <c r="A11" s="27">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="28" t="s">
         <v>709</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2"/>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>725</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>732</v>
+      </c>
       <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1">
-      <c r="A12" s="27">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="2"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="2">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>730</v>
+      </c>
       <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
-      <c r="A13" s="27">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1">
-      <c r="A14" s="27">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -9644,10 +9727,10 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="27">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -9656,10 +9739,10 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1">
-      <c r="A16" s="27">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -9668,10 +9751,10 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="27">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -9680,10 +9763,10 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="27">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -9692,10 +9775,10 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1">
-      <c r="A19" s="27">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="28"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -9704,10 +9787,10 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
-      <c r="A20" s="27">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="28"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -9716,10 +9799,10 @@
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1">
-      <c r="A21" s="27">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="28"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -9728,10 +9811,10 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
-      <c r="A22" s="27">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="28"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -9740,10 +9823,10 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="27">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="28"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -9752,10 +9835,10 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="27">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="28"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -9764,10 +9847,10 @@
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="27">
+      <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="28"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -9776,10 +9859,10 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="27">
+      <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -9788,10 +9871,10 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="27">
+      <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="28"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -9800,10 +9883,10 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1">
-      <c r="A28" s="27">
+      <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="28"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -9812,10 +9895,10 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29" s="27">
+      <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="28"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -9824,10 +9907,10 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="27">
+      <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="28"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -9836,10 +9919,10 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1">
-      <c r="A31" s="27">
+      <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="28"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -9848,10 +9931,10 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32" s="27">
+      <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="28"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -9860,10 +9943,10 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1">
-      <c r="A33" s="27">
+      <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="28"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -9872,10 +9955,10 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1">
-      <c r="A34" s="27">
+      <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="28"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -9884,10 +9967,10 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
-      <c r="A35" s="27">
+      <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="27"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -9896,10 +9979,10 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
-      <c r="A36" s="27">
+      <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="27"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -9909,10 +9992,10 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
-      <c r="A37" s="27">
+      <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="27"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -9921,10 +10004,10 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
-      <c r="A38" s="27">
+      <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -9933,10 +10016,10 @@
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1">
-      <c r="A39" s="27">
+      <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="27"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -9945,10 +10028,10 @@
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1">
-      <c r="A40" s="27">
-        <v>38</v>
-      </c>
-      <c r="B40" s="27"/>
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -9957,10 +10040,10 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1">
-      <c r="A41" s="27">
+      <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="27"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -9969,10 +10052,10 @@
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1">
-      <c r="A42" s="27">
+      <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="27"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -9981,10 +10064,10 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1">
-      <c r="A43" s="27">
+      <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="27"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -9993,10 +10076,10 @@
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1">
-      <c r="A44" s="27">
+      <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -10005,10 +10088,10 @@
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1">
-      <c r="A45" s="27">
+      <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="27"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -10017,10 +10100,10 @@
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1">
-      <c r="A46" s="27">
+      <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="27"/>
+      <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -10029,10 +10112,10 @@
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1">
-      <c r="A47" s="27">
+      <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="27"/>
+      <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -10041,10 +10124,10 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1">
-      <c r="A48" s="27">
+      <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="27"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -10053,10 +10136,10 @@
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1">
-      <c r="A49" s="27">
+      <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="27"/>
+      <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -10065,10 +10148,10 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1">
-      <c r="A50" s="27">
+      <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B50" s="27"/>
+      <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -10077,10 +10160,10 @@
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1">
-      <c r="A51" s="27">
+      <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="27"/>
+      <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -10089,10 +10172,10 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1">
-      <c r="A52" s="27">
+      <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="27"/>
+      <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -10101,10 +10184,10 @@
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1">
-      <c r="A53" s="27">
+      <c r="A53" s="2">
         <v>51</v>
       </c>
-      <c r="B53" s="27"/>
+      <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -10113,10 +10196,10 @@
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" ht="15" customHeight="1">
-      <c r="A54" s="27">
+      <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="27"/>
+      <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -10125,10 +10208,10 @@
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8" ht="15" customHeight="1">
-      <c r="A55" s="27">
+      <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="27"/>
+      <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -10137,10 +10220,10 @@
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1">
-      <c r="A56" s="27">
+      <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="27"/>
+      <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -10149,10 +10232,10 @@
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1">
-      <c r="A57" s="27">
+      <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="27"/>
+      <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -10161,10 +10244,10 @@
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" ht="15" customHeight="1">
-      <c r="A58" s="27">
+      <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="27"/>
+      <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -10173,10 +10256,10 @@
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" ht="15" customHeight="1">
-      <c r="A59" s="27">
+      <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="27"/>
+      <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -10185,10 +10268,10 @@
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" ht="15" customHeight="1">
-      <c r="A60" s="27">
+      <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="27"/>
+      <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -10197,10 +10280,10 @@
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" ht="15" customHeight="1">
-      <c r="A61" s="27">
+      <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="27"/>
+      <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -10209,10 +10292,10 @@
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" ht="15" customHeight="1">
-      <c r="A62" s="27">
+      <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="27"/>
+      <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -10221,10 +10304,10 @@
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" ht="15" customHeight="1">
-      <c r="A63" s="27">
+      <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="27"/>
+      <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -10233,10 +10316,10 @@
       <c r="H63" s="2"/>
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1">
-      <c r="A64" s="27">
+      <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="27"/>
+      <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -10245,10 +10328,10 @@
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1">
-      <c r="A65" s="27">
+      <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="27"/>
+      <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -10257,10 +10340,10 @@
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1">
-      <c r="A66" s="27">
+      <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="27"/>
+      <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -10269,10 +10352,10 @@
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1">
-      <c r="A67" s="27">
+      <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="27"/>
+      <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -10281,10 +10364,10 @@
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:8" ht="15" customHeight="1">
-      <c r="A68" s="27">
+      <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="27"/>
+      <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -10293,10 +10376,10 @@
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8" ht="15" customHeight="1">
-      <c r="A69" s="27">
+      <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="27"/>
+      <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -10305,10 +10388,10 @@
       <c r="H69" s="2"/>
     </row>
     <row r="70" spans="1:8" ht="15" customHeight="1">
-      <c r="A70" s="27">
+      <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="27"/>
+      <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -10317,10 +10400,10 @@
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" ht="15" customHeight="1">
-      <c r="A71" s="27">
+      <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="27"/>
+      <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -10329,10 +10412,10 @@
       <c r="H71" s="2"/>
     </row>
     <row r="72" spans="1:8" ht="15" customHeight="1">
-      <c r="A72" s="27">
+      <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="27"/>
+      <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -10341,10 +10424,10 @@
       <c r="H72" s="2"/>
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1">
-      <c r="A73" s="27">
+      <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="27"/>
+      <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -10353,10 +10436,10 @@
       <c r="H73" s="2"/>
     </row>
     <row r="74" spans="1:8" ht="15" customHeight="1">
-      <c r="A74" s="27">
+      <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="27"/>
+      <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -10365,10 +10448,10 @@
       <c r="H74" s="2"/>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1">
-      <c r="A75" s="27">
+      <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="27"/>
+      <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -10377,10 +10460,10 @@
       <c r="H75" s="2"/>
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1">
-      <c r="A76" s="27">
+      <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="27"/>
+      <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -10389,10 +10472,10 @@
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1">
-      <c r="A77" s="27">
+      <c r="A77" s="2">
         <v>75</v>
       </c>
-      <c r="B77" s="27"/>
+      <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -10401,10 +10484,10 @@
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1">
-      <c r="A78" s="27">
+      <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="27"/>
+      <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -10413,10 +10496,10 @@
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:8" ht="15" customHeight="1">
-      <c r="A79" s="27">
+      <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="27"/>
+      <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -10425,52 +10508,52 @@
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="27">
+      <c r="A80" s="2">
         <v>78</v>
       </c>
-      <c r="B80" s="27"/>
+      <c r="B80" s="2"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="27">
+      <c r="A81" s="2">
         <v>79</v>
       </c>
-      <c r="B81" s="27"/>
+      <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="27">
+      <c r="A82" s="2">
         <v>80</v>
       </c>
-      <c r="B82" s="27"/>
+      <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="27">
+      <c r="A83" s="2">
         <v>81</v>
       </c>
-      <c r="B83" s="27"/>
+      <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="27">
+      <c r="A84" s="2">
         <v>82</v>
       </c>
-      <c r="B84" s="27"/>
+      <c r="B84" s="2"/>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="27">
+      <c r="A85" s="2">
         <v>83</v>
       </c>
-      <c r="B85" s="27"/>
+      <c r="B85" s="2"/>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="27">
+      <c r="A86" s="2">
         <v>84</v>
       </c>
-      <c r="B86" s="27"/>
+      <c r="B86" s="2"/>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="27">
+      <c r="A87" s="2">
         <v>85</v>
       </c>
-      <c r="B87" s="27"/>
+      <c r="B87" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10485,6 +10568,8 @@
     <hyperlink ref="F4" r:id="rId3" xr:uid="{3D8F3E8A-65F8-1947-9319-9A6D3C038568}"/>
     <hyperlink ref="F5" r:id="rId4" xr:uid="{45091034-383D-3D41-BB94-FEDC2A783DAD}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{F83A99E0-BEA8-5F4B-9316-55278A6B2525}"/>
+    <hyperlink ref="F11" r:id="rId6" xr:uid="{8C9C80DF-DFC1-4B49-9FE1-3096DBEEE857}"/>
+    <hyperlink ref="F12" r:id="rId7" xr:uid="{511C8751-7627-D848-A2FF-61D234B86D54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10501,14 +10586,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>645</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>

</xml_diff>

<commit_message>
[20231228] Google Interview (85) 7
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D3D839-0740-EE46-8023-4684835C0B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E115F3C-165B-214D-933A-361DDE7BB57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="760">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2583,10 +2583,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Hard</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>2023.12.25</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2731,6 +2727,61 @@
   </si>
   <si>
     <t>2023.12.26</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3052/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3053/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/339/</t>
+  </si>
+  <si>
+    <t>2023.12.28</t>
+  </si>
+  <si>
+    <t>switch transpose then switch reflect: for i in range(w) with for j in range(i): switch [i][j] = [j][i], and then switch h for matrix[i].reverse()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. comfirm cur step + idx &gt;= destination (dis=len(num)-1, for loop dis,-1,-1:  if i + nums[i] &gt;= dis, dis=i). 2. keey jump max steps: for loop to check max(max_step - 1, nums[i])</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>flag to check all digits[i], if need: digits.insert(0, 1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum Window Substring</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/345/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read N Characters Given Read4 II - Call multiple times</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/436/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Longest Substring with At Most Two Distinct Characters</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3054/</t>
+  </si>
+  <si>
+    <t>same soluion as "Fruit Into Baskets"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing Ranges</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2946,6 +2997,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2984,9 +3038,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3321,14 +3372,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -3370,7 +3421,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3403,7 +3454,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -3431,7 +3482,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3458,7 +3509,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -3485,7 +3536,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -3512,7 +3563,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -3542,7 +3593,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -3569,7 +3620,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -3596,7 +3647,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -3623,7 +3674,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -3653,7 +3704,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3680,7 +3731,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>123</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3712,7 +3763,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3739,7 +3790,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3766,7 +3817,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3793,7 +3844,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3823,7 +3874,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -3847,7 +3898,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3874,7 +3925,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="16"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3901,7 +3952,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="17" t="s">
         <v>124</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -3930,7 +3981,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -3957,7 +4008,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3984,7 +4035,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="16"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -4011,7 +4062,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -4038,7 +4089,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="16"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -4068,7 +4119,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="17" t="s">
         <v>125</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -4100,7 +4151,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -4124,7 +4175,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -4154,7 +4205,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="16"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -4178,7 +4229,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="16"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4202,7 +4253,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="17" t="s">
         <v>126</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -4228,7 +4279,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -4252,7 +4303,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="17" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -4278,7 +4329,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="16"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -4302,7 +4353,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="16"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -4326,7 +4377,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="16"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -4350,7 +4401,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="17" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -4376,7 +4427,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="16"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -4400,7 +4451,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="17" t="s">
         <v>129</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -4426,7 +4477,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="16"/>
+      <c r="C42" s="17"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -4450,7 +4501,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="16"/>
+      <c r="C43" s="17"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -4474,7 +4525,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="16"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -4498,7 +4549,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="17" t="s">
         <v>130</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -4524,7 +4575,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="16"/>
+      <c r="C46" s="17"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -4548,7 +4599,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="16"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -4572,7 +4623,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="16"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -4596,7 +4647,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="16"/>
+      <c r="C49" s="17"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -4620,7 +4671,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="16"/>
+      <c r="C50" s="17"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -4866,15 +4917,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -4918,7 +4969,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="28">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -4956,7 +5007,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -4987,7 +5038,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -5017,7 +5068,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -5047,7 +5098,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -5077,7 +5128,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="27"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -5107,7 +5158,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="27"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -5137,7 +5188,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="27"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -5167,7 +5218,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="27"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -5197,7 +5248,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -5227,7 +5278,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="27"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -5257,7 +5308,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -5287,7 +5338,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -5320,7 +5371,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="23">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -5352,7 +5403,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="22"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -5382,7 +5433,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -5412,7 +5463,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -5442,7 +5493,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="2">
         <v>206</v>
       </c>
@@ -5472,7 +5523,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="2">
         <v>169</v>
       </c>
@@ -5502,7 +5553,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="22"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="2">
         <v>67</v>
       </c>
@@ -5532,7 +5583,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="2">
         <v>543</v>
       </c>
@@ -5562,7 +5613,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="22"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="2">
         <v>876</v>
       </c>
@@ -5592,7 +5643,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="22"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="2">
         <v>104</v>
       </c>
@@ -5622,7 +5673,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="22"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="2">
         <v>217</v>
       </c>
@@ -5652,7 +5703,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="22"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="2">
         <v>53</v>
       </c>
@@ -5682,7 +5733,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="24">
         <v>3</v>
       </c>
       <c r="C28" s="2">
@@ -5714,7 +5765,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="23"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="2">
         <v>542</v>
       </c>
@@ -5744,7 +5795,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="23"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="2">
         <v>973</v>
       </c>
@@ -5774,7 +5825,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="23"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="2">
         <v>3</v>
       </c>
@@ -5804,7 +5855,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="23"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="2">
         <v>15</v>
       </c>
@@ -5834,7 +5885,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="23"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="2">
         <v>102</v>
       </c>
@@ -5864,7 +5915,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="23"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="2">
         <v>133</v>
       </c>
@@ -5897,7 +5948,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="23"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="2">
         <v>150</v>
       </c>
@@ -5927,7 +5978,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="24">
+      <c r="B36" s="25">
         <v>4</v>
       </c>
       <c r="C36" s="2">
@@ -5962,7 +6013,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="2">
         <v>208</v>
       </c>
@@ -5992,7 +6043,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="24"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="2">
         <v>322</v>
       </c>
@@ -6022,7 +6073,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="24"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="2">
         <v>238</v>
       </c>
@@ -6052,7 +6103,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="24"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="2">
         <v>155</v>
       </c>
@@ -6082,7 +6133,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="24"/>
+      <c r="B41" s="25"/>
       <c r="C41" s="2">
         <v>98</v>
       </c>
@@ -6112,7 +6163,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="2">
         <v>200</v>
       </c>
@@ -6142,7 +6193,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="24"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="2">
         <v>994</v>
       </c>
@@ -6172,7 +6223,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44" s="26">
         <v>5</v>
       </c>
       <c r="C44" s="2">
@@ -6204,7 +6255,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="25"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="2">
         <v>39</v>
       </c>
@@ -6237,7 +6288,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="25"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="2">
         <v>46</v>
       </c>
@@ -6248,7 +6299,7 @@
         <v>38</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>378</v>
@@ -6267,7 +6318,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="25"/>
+      <c r="B47" s="26"/>
       <c r="C47" s="2">
         <v>56</v>
       </c>
@@ -6297,7 +6348,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="25"/>
+      <c r="B48" s="26"/>
       <c r="C48" s="2">
         <v>236</v>
       </c>
@@ -6327,7 +6378,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="25"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="2">
         <v>981</v>
       </c>
@@ -6357,7 +6408,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="25"/>
+      <c r="B50" s="26"/>
       <c r="C50" s="2">
         <v>721</v>
       </c>
@@ -6390,7 +6441,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="25"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="2">
         <v>75</v>
       </c>
@@ -6420,7 +6471,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="26">
+      <c r="B52" s="27">
         <v>6</v>
       </c>
       <c r="C52" s="2">
@@ -6452,7 +6503,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="26"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="2">
         <v>416</v>
       </c>
@@ -6482,7 +6533,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="26"/>
+      <c r="B54" s="27"/>
       <c r="C54" s="2">
         <v>8</v>
       </c>
@@ -6512,7 +6563,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="26"/>
+      <c r="B55" s="27"/>
       <c r="C55" s="2">
         <v>54</v>
       </c>
@@ -6542,7 +6593,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="26"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="2">
         <v>78</v>
       </c>
@@ -6572,7 +6623,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="26"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="2">
         <v>199</v>
       </c>
@@ -6602,7 +6653,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="26"/>
+      <c r="B58" s="27"/>
       <c r="C58" s="2">
         <v>5</v>
       </c>
@@ -6632,7 +6683,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="26"/>
+      <c r="B59" s="27"/>
       <c r="C59" s="2">
         <v>62</v>
       </c>
@@ -6662,7 +6713,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="26"/>
+      <c r="B60" s="27"/>
       <c r="C60" s="2">
         <v>105</v>
       </c>
@@ -6692,7 +6743,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="19">
+      <c r="B61" s="20">
         <v>7</v>
       </c>
       <c r="C61" s="2">
@@ -6724,7 +6775,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="19"/>
+      <c r="B62" s="20"/>
       <c r="C62" s="2">
         <v>17</v>
       </c>
@@ -6754,7 +6805,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="19"/>
+      <c r="B63" s="20"/>
       <c r="C63" s="2">
         <v>79</v>
       </c>
@@ -6784,7 +6835,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="19"/>
+      <c r="B64" s="20"/>
       <c r="C64" s="2">
         <v>438</v>
       </c>
@@ -6814,7 +6865,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="19"/>
+      <c r="B65" s="20"/>
       <c r="C65" s="2">
         <v>310</v>
       </c>
@@ -6844,7 +6895,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="19"/>
+      <c r="B66" s="20"/>
       <c r="C66" s="2">
         <v>621</v>
       </c>
@@ -6874,7 +6925,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="19"/>
+      <c r="B67" s="20"/>
       <c r="C67" s="2">
         <v>146</v>
       </c>
@@ -6904,7 +6955,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="20">
+      <c r="B68" s="21">
         <v>8</v>
       </c>
       <c r="C68" s="2">
@@ -6936,7 +6987,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="20"/>
+      <c r="B69" s="21"/>
       <c r="C69" s="2">
         <v>76</v>
       </c>
@@ -6966,7 +7017,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="20"/>
+      <c r="B70" s="21"/>
       <c r="C70" s="2">
         <v>297</v>
       </c>
@@ -6996,7 +7047,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="20"/>
+      <c r="B71" s="21"/>
       <c r="C71" s="2">
         <v>42</v>
       </c>
@@ -7026,7 +7077,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="20"/>
+      <c r="B72" s="21"/>
       <c r="C72" s="2">
         <v>295</v>
       </c>
@@ -7056,7 +7107,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="20"/>
+      <c r="B73" s="21"/>
       <c r="C73" s="2">
         <v>127</v>
       </c>
@@ -7086,7 +7137,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="20"/>
+      <c r="B74" s="21"/>
       <c r="C74" s="2">
         <v>224</v>
       </c>
@@ -7116,7 +7167,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="20"/>
+      <c r="B75" s="21"/>
       <c r="C75" s="2">
         <v>1235</v>
       </c>
@@ -7146,7 +7197,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="20"/>
+      <c r="B76" s="21"/>
       <c r="C76" s="2">
         <v>23</v>
       </c>
@@ -7176,7 +7227,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="20"/>
+      <c r="B77" s="21"/>
       <c r="C77" s="2">
         <v>84</v>
       </c>
@@ -7209,7 +7260,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="17" t="s">
         <v>130</v>
       </c>
       <c r="C78" s="2">
@@ -7241,7 +7292,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="16"/>
+      <c r="B79" s="17"/>
       <c r="C79" s="2">
         <v>153</v>
       </c>
@@ -7277,15 +7328,15 @@
       <c r="A85" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
-      <c r="H85" s="21"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7390,14 +7441,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -7441,7 +7492,7 @@
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>480</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -7474,7 +7525,7 @@
       <c r="B4" s="2">
         <v>73</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -7500,7 +7551,7 @@
       <c r="B5" s="2">
         <v>49</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -7524,7 +7575,7 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
@@ -7548,7 +7599,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
@@ -7572,7 +7623,7 @@
       <c r="B8" s="2">
         <v>334</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
@@ -7596,7 +7647,7 @@
       <c r="B9" s="2">
         <v>163</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -7620,7 +7671,7 @@
       <c r="B10" s="2">
         <v>38</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
@@ -7644,7 +7695,7 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>481</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -7670,7 +7721,7 @@
       <c r="B12" s="2">
         <v>328</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -7694,7 +7745,7 @@
       <c r="B13" s="2">
         <v>160</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
@@ -7718,7 +7769,7 @@
       <c r="B14" s="2">
         <v>94</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>482</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -7744,7 +7795,7 @@
       <c r="B15" s="2">
         <v>103</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -7768,7 +7819,7 @@
       <c r="B16" s="2">
         <v>105</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
@@ -7795,7 +7846,7 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
@@ -7819,7 +7870,7 @@
       <c r="B18" s="2">
         <v>230</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -7843,7 +7894,7 @@
       <c r="B19" s="2">
         <v>285</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -7870,7 +7921,7 @@
       <c r="B20" s="2">
         <v>200</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
@@ -7894,7 +7945,7 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="17" t="s">
         <v>483</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -7920,7 +7971,7 @@
       <c r="B22" s="2">
         <v>22</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
@@ -7944,12 +7995,12 @@
       <c r="B23" s="2">
         <v>46</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>539</v>
@@ -7968,7 +8019,7 @@
       <c r="B24" s="2">
         <v>78</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
@@ -7992,7 +8043,7 @@
       <c r="B25" s="2">
         <v>79</v>
       </c>
-      <c r="C25" s="16"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
@@ -8019,7 +8070,7 @@
       <c r="B26" s="2">
         <v>75</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="17" t="s">
         <v>126</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -8045,7 +8096,7 @@
       <c r="B27" s="2">
         <v>347</v>
       </c>
-      <c r="C27" s="16"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -8072,7 +8123,7 @@
       <c r="B28" s="2">
         <v>215</v>
       </c>
-      <c r="C28" s="16"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -8099,7 +8150,7 @@
       <c r="B29" s="2">
         <v>162</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -8123,7 +8174,7 @@
       <c r="B30" s="2">
         <v>34</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
@@ -8147,7 +8198,7 @@
       <c r="B31" s="2">
         <v>56</v>
       </c>
-      <c r="C31" s="16"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -8171,7 +8222,7 @@
       <c r="B32" s="2">
         <v>33</v>
       </c>
-      <c r="C32" s="16"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -8195,7 +8246,7 @@
       <c r="B33" s="2">
         <v>253</v>
       </c>
-      <c r="C33" s="16"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
@@ -8219,7 +8270,7 @@
       <c r="B34" s="2">
         <v>240</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
@@ -8243,7 +8294,7 @@
       <c r="B35" s="2">
         <v>55</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="17" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -8269,7 +8320,7 @@
       <c r="B36" s="2">
         <v>62</v>
       </c>
-      <c r="C36" s="16"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
@@ -8293,7 +8344,7 @@
       <c r="B37" s="2">
         <v>322</v>
       </c>
-      <c r="C37" s="16"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -8317,7 +8368,7 @@
       <c r="B38" s="2">
         <v>300</v>
       </c>
-      <c r="C38" s="16"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -8344,7 +8395,7 @@
       <c r="B39" s="2">
         <v>251</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="17" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -8370,7 +8421,7 @@
       <c r="B40" s="2">
         <v>297</v>
       </c>
-      <c r="C40" s="16"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="2" t="s">
         <v>87</v>
       </c>
@@ -8394,7 +8445,7 @@
       <c r="B41" s="2">
         <v>380</v>
       </c>
-      <c r="C41" s="16"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
@@ -8421,7 +8472,7 @@
       <c r="B42" s="2">
         <v>348</v>
       </c>
-      <c r="C42" s="16"/>
+      <c r="C42" s="17"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -8445,7 +8496,7 @@
       <c r="B43" s="2">
         <v>202</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="17" t="s">
         <v>129</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -8471,7 +8522,7 @@
       <c r="B44" s="2">
         <v>172</v>
       </c>
-      <c r="C44" s="16"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
@@ -8495,7 +8546,7 @@
       <c r="B45" s="2">
         <v>171</v>
       </c>
-      <c r="C45" s="16"/>
+      <c r="C45" s="17"/>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
@@ -8522,7 +8573,7 @@
       <c r="B46" s="2">
         <v>50</v>
       </c>
-      <c r="C46" s="16"/>
+      <c r="C46" s="17"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
@@ -8549,7 +8600,7 @@
       <c r="B47" s="2">
         <v>69</v>
       </c>
-      <c r="C47" s="16"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -8576,7 +8627,7 @@
       <c r="B48" s="2">
         <v>29</v>
       </c>
-      <c r="C48" s="16"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
@@ -8600,7 +8651,7 @@
       <c r="B49" s="2">
         <v>166</v>
       </c>
-      <c r="C49" s="16"/>
+      <c r="C49" s="17"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
@@ -8624,7 +8675,7 @@
       <c r="B50" s="2">
         <v>371</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="17" t="s">
         <v>130</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -8650,7 +8701,7 @@
       <c r="B51" s="2">
         <v>150</v>
       </c>
-      <c r="C51" s="16"/>
+      <c r="C51" s="17"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
@@ -8674,7 +8725,7 @@
       <c r="B52" s="2">
         <v>169</v>
       </c>
-      <c r="C52" s="16"/>
+      <c r="C52" s="17"/>
       <c r="D52" s="2" t="s">
         <v>21</v>
       </c>
@@ -8698,7 +8749,7 @@
       <c r="B53" s="2">
         <v>645</v>
       </c>
-      <c r="C53" s="16"/>
+      <c r="C53" s="17"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
@@ -8722,7 +8773,7 @@
       <c r="B54" s="2">
         <v>621</v>
       </c>
-      <c r="C54" s="16"/>
+      <c r="C54" s="17"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
@@ -9452,16 +9503,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9491,8 +9542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9501,21 +9552,21 @@
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="138.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="55.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>706</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
@@ -9544,7 +9595,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>8</v>
@@ -9554,7 +9605,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>702</v>
       </c>
       <c r="C3" s="2">
@@ -9570,28 +9621,28 @@
         <v>701</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="2">
         <v>975</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>708</v>
+        <v>87</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>705</v>
@@ -9607,7 +9658,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="2">
         <v>482</v>
       </c>
@@ -9615,26 +9666,26 @@
         <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>711</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>712</v>
-      </c>
       <c r="G5" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>714</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>709</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="2">
         <v>904</v>
       </c>
@@ -9642,30 +9693,30 @@
         <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>716</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>717</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>745</v>
+        <v>726</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>744</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="2"/>
@@ -9675,11 +9726,11 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="2"/>
@@ -9689,11 +9740,11 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="2"/>
@@ -9703,11 +9754,11 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="2"/>
@@ -9717,7 +9768,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="29" t="s">
         <v>707</v>
       </c>
       <c r="C11" s="2">
@@ -9727,24 +9778,24 @@
         <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>722</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>723</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="2">
         <v>11</v>
       </c>
@@ -9752,24 +9803,24 @@
         <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>724</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>725</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="2">
         <v>15</v>
       </c>
@@ -9780,23 +9831,23 @@
         <v>491</v>
       </c>
       <c r="F13" s="15" t="s">
+        <v>730</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="I13" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>732</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1">
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="2">
         <v>31</v>
       </c>
@@ -9804,26 +9855,26 @@
         <v>38</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>735</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>736</v>
-      </c>
       <c r="G14" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>738</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="2">
         <v>43</v>
       </c>
@@ -9831,109 +9882,182 @@
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>740</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="G15" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>742</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="6"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="2">
+        <v>48</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>749</v>
+      </c>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1">
+      <c r="I16" s="2" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="2"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="2">
+        <v>55</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>746</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>750</v>
+      </c>
       <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
+      <c r="I17" s="2" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="2"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="2">
+        <v>66</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>751</v>
+      </c>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
+      <c r="I18" s="2" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="6"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="2">
+        <v>76</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>753</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
+    <row r="20" spans="1:10" ht="15" customHeight="1">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="4"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="2">
+        <v>158</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>755</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
+    <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1">
+      <c r="B21" s="17"/>
+      <c r="C21" s="2">
+        <v>159</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>759</v>
+      </c>
       <c r="F22" s="6"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
+    <row r="23" spans="1:10" ht="15" customHeight="1">
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -9941,11 +10065,11 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
+    <row r="24" spans="1:10" ht="15" customHeight="1">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -9953,11 +10077,11 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
+    <row r="25" spans="1:10" ht="15" customHeight="1">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -9965,11 +10089,11 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
+    <row r="26" spans="1:10" ht="15" customHeight="1">
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -9977,11 +10101,11 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
+    <row r="27" spans="1:10" ht="15" customHeight="1">
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -9989,11 +10113,11 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
+    <row r="28" spans="1:10" ht="15" customHeight="1">
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="16"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -10001,11 +10125,11 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
+    <row r="29" spans="1:10" ht="15" customHeight="1">
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -10013,11 +10137,11 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
+    <row r="30" spans="1:10" ht="15" customHeight="1">
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="16"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -10025,11 +10149,11 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
+    <row r="31" spans="1:10" ht="15" customHeight="1">
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="16"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -10037,11 +10161,11 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
+    <row r="32" spans="1:10" ht="15" customHeight="1">
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="16"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -10053,7 +10177,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="16"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -10065,7 +10189,7 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="16"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -10679,6 +10803,8 @@
     <hyperlink ref="F12" r:id="rId7" xr:uid="{511C8751-7627-D848-A2FF-61D234B86D54}"/>
     <hyperlink ref="F13" r:id="rId8" xr:uid="{40298935-AE32-0247-9D82-7E997B96B4EF}"/>
     <hyperlink ref="F15" r:id="rId9" xr:uid="{B5C25FA9-48F0-6D48-AEC8-2A5F2A3CA88F}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{AEE9005D-FF5B-664C-8C0C-3C13C8EC79F0}"/>
+    <hyperlink ref="F19" r:id="rId11" xr:uid="{2FDED7C9-8AC7-FA48-87DD-245B7476360E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10695,14 +10821,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>643</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>

</xml_diff>

<commit_message>
[20231229] Google Interview (85) 8-9
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E115F3C-165B-214D-933A-361DDE7BB57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031E2FF4-8B19-B344-A4CC-7A78057F86F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="769">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2781,6 +2781,41 @@
   </si>
   <si>
     <t>Missing Ranges</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3055/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.29</t>
+  </si>
+  <si>
+    <t>Check for missing numbers btw the lower bound and nums[0], nums[-1] + 1 and upper bound, and btw nums (skip if nums[i+1] - nums[i] &lt;= 1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Next Closest Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/471/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3056/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expressive Words</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>split to HH, MM, sorted to set all digits, list all posible 2 digits value (a total of 16), check cur MM or then carry to check cur HH, or return [0][0]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>generateTable: save all chars order and num of char, then compare s Table to words Table, if w_nums[i] = s_nums[i] or w_nums[i] &lt; s_nums[i] and s_nums[i] &gt;= 3: cnt++</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -9503,16 +9538,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9543,7 +9578,7 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10044,38 +10079,72 @@
         <v>20</v>
       </c>
       <c r="B22" s="17"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2">
+        <v>163</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="F22" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1">
       <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" s="17"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="C23" s="2">
+        <v>681</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>764</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1">
       <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24" s="17"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="C24" s="2">
+        <v>809</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>765</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1">
       <c r="A25" s="2">
@@ -10805,6 +10874,9 @@
     <hyperlink ref="F15" r:id="rId9" xr:uid="{B5C25FA9-48F0-6D48-AEC8-2A5F2A3CA88F}"/>
     <hyperlink ref="F17" r:id="rId10" xr:uid="{AEE9005D-FF5B-664C-8C0C-3C13C8EC79F0}"/>
     <hyperlink ref="F19" r:id="rId11" xr:uid="{2FDED7C9-8AC7-FA48-87DD-245B7476360E}"/>
+    <hyperlink ref="F22" r:id="rId12" xr:uid="{E9F02547-3142-B141-89DD-AA5119FB1FD4}"/>
+    <hyperlink ref="F23" r:id="rId13" xr:uid="{94A31DA5-28D4-EF43-A9C1-C28E3DD49C08}"/>
+    <hyperlink ref="F24" r:id="rId14" xr:uid="{045B7815-64D0-D143-9F24-51F522BB93DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20231230] Google Interview (85) 19-20
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031E2FF4-8B19-B344-A4CC-7A78057F86F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE06144-6713-F14F-854F-A9C652A4F2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="779">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2816,6 +2816,45 @@
   </si>
   <si>
     <t>generateTable: save all chars order and num of char, then compare s Table to words Table, if w_nums[i] = s_nums[i] or w_nums[i] &lt; s_nums[i] and s_nums[i] &gt;= 3: cnt++</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find And Replace in String</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3057/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.30</t>
+  </si>
+  <si>
+    <t>Maximize Distance to Closest Person</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3058/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list(s) frist, for idx, src, tgt in zip(indices, sources, targets) loop to check s[idx: idx + lengthOfSrc] == src: set idx to tgt, and loop set idx+1 ~ idx+n to ''</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>a = [1,2,3]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>b = [4,5,6]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>zip to iterable list, e.g.: zip(a,b): [(1, 4), (2, 5), (3, 6)], or *zip</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>check left side, right side, and middle of left+1 to right+1, return max(left, len-right-1, (interval+1)//2)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -9538,16 +9577,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9575,10 +9614,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="G33" sqref="G33:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9957,7 +9996,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1">
+    <row r="17" spans="1:12" ht="15" customHeight="1">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -9982,7 +10021,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1">
+    <row r="18" spans="1:12" ht="15" customHeight="1">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -10007,7 +10046,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1">
+    <row r="19" spans="1:12" ht="15" customHeight="1">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -10027,7 +10066,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1">
+    <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -10047,7 +10086,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1">
+    <row r="21" spans="1:12" ht="15" customHeight="1">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -10074,7 +10113,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1">
+    <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -10098,7 +10137,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1">
+    <row r="23" spans="1:12" ht="15" customHeight="1">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -10122,7 +10161,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1">
+    <row r="24" spans="1:12" ht="15" customHeight="1">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -10146,31 +10185,64 @@
         <v>761</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1">
+    <row r="25" spans="1:12" ht="15" customHeight="1">
       <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" s="17"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1">
+      <c r="C25" s="2">
+        <v>833</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>770</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" customHeight="1">
       <c r="A26" s="2">
         <v>24</v>
       </c>
       <c r="B26" s="17"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1">
+      <c r="C26" s="2">
+        <v>849</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -10182,7 +10254,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1">
+    <row r="28" spans="1:12" ht="15" customHeight="1">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -10194,7 +10266,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1">
+    <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -10206,7 +10278,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1">
+    <row r="30" spans="1:12" ht="15" customHeight="1">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -10218,7 +10290,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="15" customHeight="1">
+    <row r="31" spans="1:12" ht="15" customHeight="1">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -10230,7 +10302,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1">
+    <row r="32" spans="1:12" ht="15" customHeight="1">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -10877,6 +10949,8 @@
     <hyperlink ref="F22" r:id="rId12" xr:uid="{E9F02547-3142-B141-89DD-AA5119FB1FD4}"/>
     <hyperlink ref="F23" r:id="rId13" xr:uid="{94A31DA5-28D4-EF43-A9C1-C28E3DD49C08}"/>
     <hyperlink ref="F24" r:id="rId14" xr:uid="{045B7815-64D0-D143-9F24-51F522BB93DE}"/>
+    <hyperlink ref="F25" r:id="rId15" xr:uid="{429F086E-CF6D-1842-B44E-CA383051A3BC}"/>
+    <hyperlink ref="F26" r:id="rId16" xr:uid="{AF788CE6-B278-424F-BFDE-B1AFFC7225A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240101] Google Interview (85) 21-26
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE06144-6713-F14F-854F-A9C652A4F2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425B360F-167F-5042-B2F7-93027757DCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="797">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2855,6 +2855,76 @@
   </si>
   <si>
     <t>check left side, right side, and middle of left+1 to right+1, return max(left, len-right-1, (interval+1)//2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/467/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dict to }:{…, use list to check if not in table: append, elif stack: if last of stack not in table: False else pop, finally, check len of stack is zeor</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merge k Sorted Lists</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/342/</t>
+  </si>
+  <si>
+    <t>Trapping Rain Water</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/341/</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/361/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>heapq.heappush or heappop to select kth, or, quick select: random select pivot if less: append to left, elif more: to right, else to mid, repeat the condition to find mid pivot</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>random.choice(nums), refer: https://en.wikipedia.org/wiki/Quickselect</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meeting Rooms II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3059/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort list firstm use heapq to push if not heap or heap[0] &gt; interval[0] else pushpop interval[1], return len(heap)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>heapq: heappush or heappushpop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backspace String Compare</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3060/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack to append/push if # and compare</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -9577,16 +9647,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9617,7 +9687,7 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33:G34"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10247,22 +10317,43 @@
         <v>25</v>
       </c>
       <c r="B27" s="17"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="2"/>
+      <c r="C27" s="2">
+        <v>20</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>781</v>
+      </c>
       <c r="H27" s="2"/>
+      <c r="I27" s="2" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1">
       <c r="A28" s="2">
         <v>26</v>
       </c>
       <c r="B28" s="17"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="6"/>
+      <c r="C28" s="2">
+        <v>23</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>783</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
@@ -10271,10 +10362,18 @@
         <v>27</v>
       </c>
       <c r="B29" s="17"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="6"/>
+      <c r="C29" s="2">
+        <v>42</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>785</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
@@ -10283,36 +10382,80 @@
         <v>28</v>
       </c>
       <c r="B30" s="17"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="2"/>
+      <c r="C30" s="2">
+        <v>215</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>788</v>
+      </c>
       <c r="H30" s="2"/>
+      <c r="I30" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1">
       <c r="A31" s="2">
         <v>29</v>
       </c>
       <c r="B31" s="17"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="2"/>
+      <c r="C31" s="2">
+        <v>253</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>791</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>792</v>
+      </c>
       <c r="H31" s="2"/>
+      <c r="I31" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1">
       <c r="A32" s="2">
         <v>30</v>
       </c>
       <c r="B32" s="17"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="C32" s="2">
+        <v>844</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>795</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1">
       <c r="A33" s="2">
@@ -10951,6 +11094,10 @@
     <hyperlink ref="F24" r:id="rId14" xr:uid="{045B7815-64D0-D143-9F24-51F522BB93DE}"/>
     <hyperlink ref="F25" r:id="rId15" xr:uid="{429F086E-CF6D-1842-B44E-CA383051A3BC}"/>
     <hyperlink ref="F26" r:id="rId16" xr:uid="{AF788CE6-B278-424F-BFDE-B1AFFC7225A4}"/>
+    <hyperlink ref="F27" r:id="rId17" xr:uid="{C15FF1BC-29B5-A54A-9ED1-86AAFF8EE833}"/>
+    <hyperlink ref="F30" r:id="rId18" xr:uid="{C05C6DC9-8350-8647-9F97-9AC563863272}"/>
+    <hyperlink ref="F31" r:id="rId19" xr:uid="{70CC2376-A3BC-624B-9913-4BE0A28B24FB}"/>
+    <hyperlink ref="F32" r:id="rId20" xr:uid="{3241DC58-93C9-D44A-9970-FCD432C41448}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240102] Google Interview (85) 27-31
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425B360F-167F-5042-B2F7-93027757DCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D8404D-E775-E64D-A10C-7CE7FCA5696C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="814">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2925,6 +2925,74 @@
   </si>
   <si>
     <t>stack to append/push if # and compare</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum Cost to Hire K Workers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3061/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>K Closest Points to Origin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/59/array-and-strings/3062/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.02</t>
+  </si>
+  <si>
+    <t>Linked
+Lists</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/60/linked-list-5/3063/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/60/linked-list-5/3064/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>calc with sort, or, best to use heap: sq= -(x*x+y*y), if len &lt; k: heappush(heap, (sq,x,y)) else heappushpop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>heapq.heappushpop(heap, (sq, x, y))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1,2 = l1.val if l1 else 0, v1+v2+add, nextList.next=ListNode(sum%10), add=sum//10, newList.next, l1,l2.next else None</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two ptr, fast run next n steps, check null, while fast.next to null, slow.next=slow.next.next, return head</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/60/linked-list-5/3065/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_list = ptr = ListNode(0), while l1, l2: compare l1.val and l2.val, new_list.next=(l1 or l2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/60/linked-list-5/3066/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -9647,16 +9715,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9687,7 +9755,7 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10462,71 +10530,143 @@
         <v>31</v>
       </c>
       <c r="B33" s="17"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="6"/>
+      <c r="C33" s="2">
+        <v>857</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>798</v>
+      </c>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1">
       <c r="A34" s="2">
         <v>32</v>
       </c>
       <c r="B34" s="17"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="2"/>
+      <c r="C34" s="2">
+        <v>973</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>800</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>806</v>
+      </c>
       <c r="H34" s="2"/>
+      <c r="I34" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="2"/>
+      <c r="B35" s="29" t="s">
+        <v>802</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>804</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>808</v>
+      </c>
       <c r="H35" s="2"/>
+      <c r="I35" s="2" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="2"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="2">
+        <v>19</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>805</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>809</v>
+      </c>
       <c r="H36" s="2"/>
+      <c r="I36" s="2" t="s">
+        <v>801</v>
+      </c>
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="2"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="2">
+        <v>21</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>811</v>
+      </c>
       <c r="H37" s="2"/>
+      <c r="I37" s="2" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="6"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="2">
+        <v>138</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>813</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
@@ -11071,10 +11211,11 @@
       <c r="B87" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -11098,6 +11239,12 @@
     <hyperlink ref="F30" r:id="rId18" xr:uid="{C05C6DC9-8350-8647-9F97-9AC563863272}"/>
     <hyperlink ref="F31" r:id="rId19" xr:uid="{70CC2376-A3BC-624B-9913-4BE0A28B24FB}"/>
     <hyperlink ref="F32" r:id="rId20" xr:uid="{3241DC58-93C9-D44A-9970-FCD432C41448}"/>
+    <hyperlink ref="F33" r:id="rId21" xr:uid="{241F443A-C747-E243-91A6-18B9E790E763}"/>
+    <hyperlink ref="F34" r:id="rId22" xr:uid="{2761ED04-F0F0-714A-A9E3-F0A8874E40C3}"/>
+    <hyperlink ref="F35" r:id="rId23" xr:uid="{3C5790E7-5315-AC41-A9BA-7C020BA3F41B}"/>
+    <hyperlink ref="F36" r:id="rId24" xr:uid="{9A48843A-A465-3746-9E93-4623A5D5473F}"/>
+    <hyperlink ref="F37" r:id="rId25" xr:uid="{4079E697-6E39-EE43-8DD7-14D744A525BC}"/>
+    <hyperlink ref="F38" r:id="rId26" xr:uid="{C83C353B-80BC-D645-9DC5-B7DB622EB54D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240104] Google Interview (85) 32-35
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D8404D-E775-E64D-A10C-7CE7FCA5696C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E7B770-FEB9-D241-AB76-E7EB6583CC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -17,12 +17,13 @@
     <sheet name="Blind 75" sheetId="1" r:id="rId2"/>
     <sheet name="Top Interview Q - Meduim 52" sheetId="2" r:id="rId3"/>
     <sheet name="Google Interview" sheetId="10" r:id="rId4"/>
-    <sheet name="Dynamic Programming" sheetId="4" r:id="rId5"/>
-    <sheet name="Recursion I" sheetId="5" r:id="rId6"/>
-    <sheet name="Heap" sheetId="6" r:id="rId7"/>
-    <sheet name="Sorting" sheetId="7" r:id="rId8"/>
-    <sheet name="Binary Search" sheetId="9" r:id="rId9"/>
-    <sheet name="Graph" sheetId="8" r:id="rId10"/>
+    <sheet name="Amazon Interview" sheetId="11" r:id="rId5"/>
+    <sheet name="Dynamic Programming" sheetId="4" r:id="rId6"/>
+    <sheet name="Recursion I" sheetId="5" r:id="rId7"/>
+    <sheet name="Heap" sheetId="6" r:id="rId8"/>
+    <sheet name="Sorting" sheetId="7" r:id="rId9"/>
+    <sheet name="Binary Search" sheetId="9" r:id="rId10"/>
+    <sheet name="Graph" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="828">
   <si>
     <t xml:space="preserve">
 </t>
@@ -2993,6 +2994,63 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/interview/card/google/60/linked-list-5/3066/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tree
+and
+Graphs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.04</t>
+  </si>
+  <si>
+    <t>three solution: recursion with table, loop with table, and interweaving node</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>interweaving node logic</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3067/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Ladder</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3068/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3069/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop run each cell, if '1' call DFS, DFS func to set '0' and check top, down, left, right side if '1'</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Course Schedule II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3070/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3160,7 +3218,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3250,6 +3308,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5090,6 +5151,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED2A95A-A5C1-7B46-B514-8AACCDB615E6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R38" sqref="R38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F6B7C9-F416-9A49-83DC-B48E6AB23806}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5108,7 +5184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
@@ -9715,16 +9791,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9754,8 +9830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10651,7 +10727,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
-      <c r="A38" s="2">
+      <c r="A38" s="9">
         <v>36</v>
       </c>
       <c r="B38" s="17"/>
@@ -10667,30 +10743,54 @@
       <c r="F38" s="6" t="s">
         <v>813</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1">
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="6"/>
+      <c r="B39" s="29" t="s">
+        <v>814</v>
+      </c>
+      <c r="C39" s="2">
+        <v>124</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>819</v>
+      </c>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1">
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="6"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="2">
+        <v>127</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>821</v>
+      </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
@@ -10698,31 +10798,51 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="2"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="2">
+        <v>200</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>824</v>
+      </c>
       <c r="H41" s="2"/>
+      <c r="I41" s="2" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1">
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="2"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="2">
+        <v>210</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>826</v>
+      </c>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1">
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="17"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -10734,7 +10854,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -10746,7 +10866,7 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -10758,7 +10878,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -10770,7 +10890,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="17"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -10782,7 +10902,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -10794,7 +10914,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -10806,7 +10926,7 @@
       <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -10818,7 +10938,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -11211,11 +11331,12 @@
       <c r="B87" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -11245,12 +11366,1045 @@
     <hyperlink ref="F36" r:id="rId24" xr:uid="{9A48843A-A465-3746-9E93-4623A5D5473F}"/>
     <hyperlink ref="F37" r:id="rId25" xr:uid="{4079E697-6E39-EE43-8DD7-14D744A525BC}"/>
     <hyperlink ref="F38" r:id="rId26" xr:uid="{C83C353B-80BC-D645-9DC5-B7DB622EB54D}"/>
+    <hyperlink ref="F39" r:id="rId27" xr:uid="{2C9D86AB-5F50-A648-92D6-88451EFD9CDD}"/>
+    <hyperlink ref="F40" r:id="rId28" xr:uid="{96AE63CF-137D-D14C-92A3-04A9C5A242AC}"/>
+    <hyperlink ref="F41" r:id="rId29" xr:uid="{88CBF58D-796A-4E4A-BE8E-9EEF9C4EFB39}"/>
+    <hyperlink ref="F42" r:id="rId30" xr:uid="{BF122794-37E4-DE45-81B3-BC48BD347011}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA7C0AF-7D3E-B64D-B4A5-6DFBB1424920}">
+  <dimension ref="A1:L87"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="16"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="30">
+        <v>12</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="30">
+        <v>36</v>
+      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="6"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F80E9F-AC4D-B74C-865E-81CF884A25E9}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -11317,7 +12471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F34D86-1608-9344-891E-7915A575FAB2}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11332,7 +12486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C48A37-262A-DE49-8582-3B78371E9BE0}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11345,7 +12499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24F8B26-181E-FA45-9F6A-F1DE45F8E2D2}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11358,19 +12512,4 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED2A95A-A5C1-7B46-B514-8AACCDB615E6}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[20240105] Google Interview (85) 36-39
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E7B770-FEB9-D241-AB76-E7EB6583CC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFDF99F-2B22-8F48-BBCD-AC7F1562F53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="838">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3051,6 +3051,44 @@
   </si>
   <si>
     <t>Task</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.05</t>
+  </si>
+  <si>
+    <t>table to save each course is whoes preq, list save number of  each course's preq, use deque to save all 0's pre course and append to answer, then downcount the num of each course's pre</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count Complete Tree Nodes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3071/</t>
+  </si>
+  <si>
+    <t>find left and right side level, if same: return max BF node num, else 1+going to sub node(left + right)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  Longest Increasing Path in a Matrix</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3072/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3073/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decode String</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack with check if c.isdigit =&gt; multiple 10 + num,  or '[' =&gt; append,  or ']' =&gt; pop and count,  else s+=char</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3218,7 +3256,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3308,9 +3346,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9791,16 +9826,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9830,8 +9865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9842,7 +9877,7 @@
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="138.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="159.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="55.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10836,43 +10871,79 @@
       <c r="F42" s="6" t="s">
         <v>826</v>
       </c>
-      <c r="H42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1">
       <c r="A43" s="2">
         <v>41</v>
       </c>
       <c r="B43" s="17"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
+      <c r="C43" s="2">
+        <v>222</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>831</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1">
       <c r="A44" s="2">
         <v>42</v>
       </c>
       <c r="B44" s="17"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="6"/>
+      <c r="C44" s="2">
+        <v>329</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>834</v>
+      </c>
       <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1">
       <c r="A45" s="2">
         <v>43</v>
       </c>
       <c r="B45" s="17"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
+      <c r="C45" s="2">
+        <v>394</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>835</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1">
       <c r="A46" s="2">
@@ -11370,6 +11441,8 @@
     <hyperlink ref="F40" r:id="rId28" xr:uid="{96AE63CF-137D-D14C-92A3-04A9C5A242AC}"/>
     <hyperlink ref="F41" r:id="rId29" xr:uid="{88CBF58D-796A-4E4A-BE8E-9EEF9C4EFB39}"/>
     <hyperlink ref="F42" r:id="rId30" xr:uid="{BF122794-37E4-DE45-81B3-BC48BD347011}"/>
+    <hyperlink ref="F44" r:id="rId31" xr:uid="{7359047E-1359-F349-B06F-468F40B64B1F}"/>
+    <hyperlink ref="F45" r:id="rId32" xr:uid="{68B01568-8EC5-B748-8FCB-0C27CA362810}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11577,10 +11650,10 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="30">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -11884,10 +11957,10 @@
       <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="30">
+      <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="30"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>

</xml_diff>

<commit_message>
[20240106] Google Interview (85) 40-43
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFDF99F-2B22-8F48-BBCD-AC7F1562F53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C70F69-E240-0440-8399-47A9F11D4AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="852">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3089,6 +3089,61 @@
   </si>
   <si>
     <t>stack with check if c.isdigit =&gt; multiple 10 + num,  or '[' =&gt; append,  or ']' =&gt; pop and count,  else s+=char</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Evaluate Division</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/331/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diameter of Binary Tree</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3074/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.06</t>
+  </si>
+  <si>
+    <t>Cracking the Safe</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3075/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>build graph to check path, dict in dict to save [dividend][divisor]=value, run all query and dfs to check the path from ori to dst with set() and neighbor</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.06</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dfs to check left and right node, if l+r &gt; dia, dia=l+r, return max(l, r) +1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robot Room Cleaner</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/1340/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Most Stones Removed with Same Row or Column</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3076/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -9826,16 +9881,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9865,8 +9920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10946,50 +11001,89 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1">
-      <c r="A46" s="2">
+      <c r="A46" s="9">
         <v>44</v>
       </c>
       <c r="B46" s="17"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+      <c r="C46" s="2">
+        <v>399</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>839</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1">
       <c r="A47" s="2">
         <v>45</v>
       </c>
       <c r="B47" s="17"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
+      <c r="C47" s="2">
+        <v>543</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1">
       <c r="A48" s="2">
         <v>46</v>
       </c>
       <c r="B48" s="17"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="6"/>
+      <c r="C48" s="2">
+        <v>753</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>844</v>
+      </c>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1">
       <c r="A49" s="2">
         <v>47</v>
       </c>
       <c r="B49" s="17"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="6"/>
+      <c r="C49" s="2">
+        <v>489</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>849</v>
+      </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
@@ -10998,11 +11092,18 @@
         <v>48</v>
       </c>
       <c r="B50" s="17"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="2"/>
+      <c r="C50" s="2">
+        <v>947</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>851</v>
+      </c>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1">
@@ -11443,6 +11544,11 @@
     <hyperlink ref="F42" r:id="rId30" xr:uid="{BF122794-37E4-DE45-81B3-BC48BD347011}"/>
     <hyperlink ref="F44" r:id="rId31" xr:uid="{7359047E-1359-F349-B06F-468F40B64B1F}"/>
     <hyperlink ref="F45" r:id="rId32" xr:uid="{68B01568-8EC5-B748-8FCB-0C27CA362810}"/>
+    <hyperlink ref="F46" r:id="rId33" xr:uid="{AA0077CD-0361-6249-A070-B1769D3D2F48}"/>
+    <hyperlink ref="F47" r:id="rId34" xr:uid="{C3660F6F-CDDF-C644-B301-A8AF4B68C863}"/>
+    <hyperlink ref="F48" r:id="rId35" xr:uid="{5E2324B8-B9BD-034F-A842-947B11D7E934}"/>
+    <hyperlink ref="F49" r:id="rId36" xr:uid="{8DE94AC9-94A2-D643-9960-A856BAEB8D3E}"/>
+    <hyperlink ref="F50" r:id="rId37" xr:uid="{21B9AE4E-5F52-A748-B048-F52947EDA17F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240108] Google Interview (85) 44-45
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C70F69-E240-0440-8399-47A9F11D4AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3682BA-F974-B946-80BC-C52ABEA16E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="858">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3144,6 +3144,28 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3076/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.08</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Union-Find, DFS, BFS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flip Equivalent Binary Trees</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/61/trees-and-graphs/3077/</t>
+  </si>
+  <si>
+    <t>Union-Find</t>
+  </si>
+  <si>
+    <t>Recursion to check, if root1 is root2: return True, if no 1 or 2 or val different: return False, then return (left=left and right=right or left=right and right=left)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -9881,16 +9903,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9920,8 +9942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11067,7 +11089,7 @@
       </c>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1">
+    <row r="49" spans="1:10" ht="15" customHeight="1">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -11087,8 +11109,8 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1">
-      <c r="A50" s="2">
+    <row r="50" spans="1:10" ht="15" customHeight="1">
+      <c r="A50" s="9">
         <v>48</v>
       </c>
       <c r="B50" s="17"/>
@@ -11104,21 +11126,41 @@
       <c r="F50" s="6" t="s">
         <v>851</v>
       </c>
-      <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1">
+      <c r="G50" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="J50" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15" customHeight="1">
       <c r="A51" s="2">
         <v>49</v>
       </c>
       <c r="B51" s="17"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1">
+      <c r="C51" s="2">
+        <v>951</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>855</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15" customHeight="1">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -11130,7 +11172,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1">
+    <row r="53" spans="1:10" ht="15" customHeight="1">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -11142,7 +11184,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15" customHeight="1">
+    <row r="54" spans="1:10" ht="15" customHeight="1">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -11154,7 +11196,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1">
+    <row r="55" spans="1:10" ht="15" customHeight="1">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -11166,7 +11208,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1">
+    <row r="56" spans="1:10" ht="15" customHeight="1">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -11178,7 +11220,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15" customHeight="1">
+    <row r="57" spans="1:10" ht="15" customHeight="1">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -11190,7 +11232,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1">
+    <row r="58" spans="1:10" ht="15" customHeight="1">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -11202,7 +11244,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1">
+    <row r="59" spans="1:10" ht="15" customHeight="1">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -11214,7 +11256,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15" customHeight="1">
+    <row r="60" spans="1:10" ht="15" customHeight="1">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -11226,7 +11268,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15" customHeight="1">
+    <row r="61" spans="1:10" ht="15" customHeight="1">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -11238,7 +11280,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1">
+    <row r="62" spans="1:10" ht="15" customHeight="1">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -11250,7 +11292,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15" customHeight="1">
+    <row r="63" spans="1:10" ht="15" customHeight="1">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -11262,7 +11304,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15" customHeight="1">
+    <row r="64" spans="1:10" ht="15" customHeight="1">
       <c r="A64" s="2">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
[20240109] Google Interview (85) 46-48
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3682BA-F974-B946-80BC-C52ABEA16E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AAC9B7-6CEB-764B-BB17-4E9ACBBF1870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="869">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3166,6 +3166,48 @@
   </si>
   <si>
     <t>Recursion to check, if root1 is root2: return True, if no 1 or 2 or val different: return False, then return (left=left and right=right or left=right and right=left)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recursion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Squares</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/62/recursion-4/370/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/62/recursion-4/399/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.09</t>
+  </si>
+  <si>
+    <t>Word Search II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/62/recursion-4/462/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strobogrammatic Number II (頻閃數字)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>table pair [0, 1, 6, 8, 9], func to backtracking: if n=0: add '', n=1: add 018, recursion n-2 and lenNum then loop n-2 returned &amp; table to add (pair[0] + stro + pair[1])</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/62/recursion-4/484/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android Unlock Patterns</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3176,7 +3218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3230,6 +3272,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -3333,7 +3391,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3423,6 +3481,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9903,16 +9967,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -9942,20 +10006,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="159.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
@@ -10029,7 +10093,7 @@
       <c r="I3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>712</v>
       </c>
     </row>
@@ -10041,7 +10105,7 @@
       <c r="C4" s="2">
         <v>975</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="30" t="s">
         <v>87</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -10380,7 +10444,7 @@
       <c r="C19" s="2">
         <v>76</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="30" t="s">
         <v>87</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -10400,7 +10464,7 @@
       <c r="C20" s="2">
         <v>158</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="31" t="s">
         <v>87</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -10601,7 +10665,7 @@
       <c r="C28" s="2">
         <v>23</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="30" t="s">
         <v>87</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -10621,7 +10685,7 @@
       <c r="C29" s="2">
         <v>42</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="31" t="s">
         <v>87</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -10721,7 +10785,7 @@
       <c r="C33" s="2">
         <v>857</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="30" t="s">
         <v>87</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -10811,7 +10875,6 @@
       <c r="I36" s="2" t="s">
         <v>801</v>
       </c>
-      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
       <c r="A37" s="2">
@@ -10875,7 +10938,7 @@
       <c r="C39" s="2">
         <v>124</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="30" t="s">
         <v>87</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -10894,7 +10957,7 @@
       <c r="C40" s="2">
         <v>127</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="31" t="s">
         <v>87</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -10987,7 +11050,7 @@
       <c r="C44" s="2">
         <v>329</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="30" t="s">
         <v>87</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -11078,7 +11141,7 @@
       <c r="C48" s="2">
         <v>753</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="30" t="s">
         <v>87</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -11097,7 +11160,7 @@
       <c r="C49" s="2">
         <v>489</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="31" t="s">
         <v>87</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -11132,7 +11195,7 @@
       <c r="H50" s="2" t="s">
         <v>852</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="2" t="s">
         <v>856</v>
       </c>
     </row>
@@ -11164,35 +11227,67 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="6"/>
+      <c r="B52" s="17" t="s">
+        <v>858</v>
+      </c>
+      <c r="C52" s="2">
+        <v>425</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>860</v>
+      </c>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1">
-      <c r="A53" s="2">
+      <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="2">
+        <v>247</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>861</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1">
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="6"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="2">
+        <v>212</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>864</v>
+      </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
@@ -11200,11 +11295,19 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="6"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="2">
+        <v>351</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>867</v>
+      </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
@@ -11212,7 +11315,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="17"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -11224,7 +11327,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="17"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -11545,7 +11648,8 @@
       <c r="B87" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
@@ -11591,6 +11695,9 @@
     <hyperlink ref="F48" r:id="rId35" xr:uid="{5E2324B8-B9BD-034F-A842-947B11D7E934}"/>
     <hyperlink ref="F49" r:id="rId36" xr:uid="{8DE94AC9-94A2-D643-9960-A856BAEB8D3E}"/>
     <hyperlink ref="F50" r:id="rId37" xr:uid="{21B9AE4E-5F52-A748-B048-F52947EDA17F}"/>
+    <hyperlink ref="F53" r:id="rId38" xr:uid="{15C1B4AD-D07E-4248-8A2A-7C2A2E0783A0}"/>
+    <hyperlink ref="F54" r:id="rId39" xr:uid="{E36AE3CD-BB80-5048-8C5E-6D3119DE81CC}"/>
+    <hyperlink ref="F55" r:id="rId40" xr:uid="{CF93A748-115E-4A48-ABCE-7B4D0955A1F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240110] Google Interview (85) 49-51
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AAC9B7-6CEB-764B-BB17-4E9ACBBF1870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C466FE01-906A-024E-AFF8-E12D2372AC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="878">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3208,6 +3208,43 @@
   </si>
   <si>
     <t>Android Unlock Patterns</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Letter Combinations of a Phone Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dict to skip num (e.g. (1,3):2, (3,1):2…), backtracking(cur, path, visited) to check from num 1 to 9, if not visited and (((cur, i) not in invalid) or visited[invalid[(cur, i)]]), append and next</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.10</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/62/recursion-4/3078/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dict to list num: chars, backtracking(combination, next_digits) to check len(next) else for s in digits</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generate Parentheses</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/62/recursion-4/3079/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>backtrack(combination, left, right) to check len(comb) == n*2: append, if left&lt;n: call BT(com+'(', left+1,right), if right &lt; left: call BT(com+')', left, right+1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sorting
+and 
+Searching</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3443,6 +3480,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3481,12 +3524,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3821,14 +3858,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -3870,7 +3907,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3903,7 +3940,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -3931,7 +3968,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -3958,7 +3995,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -3985,7 +4022,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4012,7 +4049,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -4042,7 +4079,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -4069,7 +4106,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -4096,7 +4133,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -4123,7 +4160,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -4153,7 +4190,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -4180,7 +4217,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="19" t="s">
         <v>123</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -4212,7 +4249,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -4239,7 +4276,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -4266,7 +4303,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -4293,7 +4330,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -4323,7 +4360,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -4347,7 +4384,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -4374,7 +4411,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -4401,7 +4438,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="19" t="s">
         <v>124</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -4430,7 +4467,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -4457,7 +4494,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -4484,7 +4521,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -4511,7 +4548,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -4538,7 +4575,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -4568,7 +4605,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="19" t="s">
         <v>125</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -4600,7 +4637,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -4624,7 +4661,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -4654,7 +4691,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -4678,7 +4715,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4702,7 +4739,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="19" t="s">
         <v>126</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -4728,7 +4765,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -4752,7 +4789,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="19" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -4778,7 +4815,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -4802,7 +4839,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="17"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -4826,7 +4863,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -4850,7 +4887,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="19" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -4876,7 +4913,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="17"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -4900,7 +4937,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="19" t="s">
         <v>129</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -4926,7 +4963,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="17"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -4950,7 +4987,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -4974,7 +5011,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -4998,7 +5035,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="19" t="s">
         <v>130</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -5024,7 +5061,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -5048,7 +5085,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="17"/>
+      <c r="C47" s="19"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -5072,7 +5109,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -5096,7 +5133,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="17"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -5120,7 +5157,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="17"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -5381,15 +5418,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -5433,7 +5470,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="30">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -5471,7 +5508,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -5502,7 +5539,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -5532,7 +5569,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -5562,7 +5599,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -5592,7 +5629,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -5622,7 +5659,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -5652,7 +5689,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -5682,7 +5719,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="28"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -5712,7 +5749,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -5742,7 +5779,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -5772,7 +5809,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -5802,7 +5839,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -5835,7 +5872,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="25">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -5867,7 +5904,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -5897,7 +5934,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -5927,7 +5964,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -5957,7 +5994,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="2">
         <v>206</v>
       </c>
@@ -5987,7 +6024,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="2">
         <v>169</v>
       </c>
@@ -6017,7 +6054,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="2">
         <v>67</v>
       </c>
@@ -6047,7 +6084,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="23"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="2">
         <v>543</v>
       </c>
@@ -6077,7 +6114,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="2">
         <v>876</v>
       </c>
@@ -6107,7 +6144,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="2">
         <v>104</v>
       </c>
@@ -6137,7 +6174,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="2">
         <v>217</v>
       </c>
@@ -6167,7 +6204,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="2">
         <v>53</v>
       </c>
@@ -6197,7 +6234,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="24">
+      <c r="B28" s="26">
         <v>3</v>
       </c>
       <c r="C28" s="2">
@@ -6229,7 +6266,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="24"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="2">
         <v>542</v>
       </c>
@@ -6259,7 +6296,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="24"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="2">
         <v>973</v>
       </c>
@@ -6289,7 +6326,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="24"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="2">
         <v>3</v>
       </c>
@@ -6319,7 +6356,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="24"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="2">
         <v>15</v>
       </c>
@@ -6349,7 +6386,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="2">
         <v>102</v>
       </c>
@@ -6379,7 +6416,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="24"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="2">
         <v>133</v>
       </c>
@@ -6412,7 +6449,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="24"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="2">
         <v>150</v>
       </c>
@@ -6442,7 +6479,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="27">
         <v>4</v>
       </c>
       <c r="C36" s="2">
@@ -6477,7 +6514,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="25"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="2">
         <v>208</v>
       </c>
@@ -6507,7 +6544,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="25"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="2">
         <v>322</v>
       </c>
@@ -6537,7 +6574,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="25"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="2">
         <v>238</v>
       </c>
@@ -6567,7 +6604,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="25"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="2">
         <v>155</v>
       </c>
@@ -6597,7 +6634,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="25"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="2">
         <v>98</v>
       </c>
@@ -6627,7 +6664,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="2">
         <v>200</v>
       </c>
@@ -6657,7 +6694,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="2">
         <v>994</v>
       </c>
@@ -6687,7 +6724,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="26">
+      <c r="B44" s="28">
         <v>5</v>
       </c>
       <c r="C44" s="2">
@@ -6719,7 +6756,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="26"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="2">
         <v>39</v>
       </c>
@@ -6752,7 +6789,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="26"/>
+      <c r="B46" s="28"/>
       <c r="C46" s="2">
         <v>46</v>
       </c>
@@ -6782,7 +6819,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="26"/>
+      <c r="B47" s="28"/>
       <c r="C47" s="2">
         <v>56</v>
       </c>
@@ -6812,7 +6849,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="26"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="2">
         <v>236</v>
       </c>
@@ -6842,7 +6879,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="26"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="2">
         <v>981</v>
       </c>
@@ -6872,7 +6909,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="26"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="2">
         <v>721</v>
       </c>
@@ -6905,7 +6942,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="26"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="2">
         <v>75</v>
       </c>
@@ -6935,7 +6972,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="27">
+      <c r="B52" s="29">
         <v>6</v>
       </c>
       <c r="C52" s="2">
@@ -6967,7 +7004,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="27"/>
+      <c r="B53" s="29"/>
       <c r="C53" s="2">
         <v>416</v>
       </c>
@@ -6997,7 +7034,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="27"/>
+      <c r="B54" s="29"/>
       <c r="C54" s="2">
         <v>8</v>
       </c>
@@ -7027,7 +7064,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="27"/>
+      <c r="B55" s="29"/>
       <c r="C55" s="2">
         <v>54</v>
       </c>
@@ -7057,7 +7094,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="27"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="2">
         <v>78</v>
       </c>
@@ -7087,7 +7124,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="27"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="2">
         <v>199</v>
       </c>
@@ -7117,7 +7154,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="27"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="2">
         <v>5</v>
       </c>
@@ -7147,7 +7184,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="27"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="2">
         <v>62</v>
       </c>
@@ -7177,7 +7214,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="27"/>
+      <c r="B60" s="29"/>
       <c r="C60" s="2">
         <v>105</v>
       </c>
@@ -7207,7 +7244,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B61" s="22">
         <v>7</v>
       </c>
       <c r="C61" s="2">
@@ -7239,7 +7276,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="20"/>
+      <c r="B62" s="22"/>
       <c r="C62" s="2">
         <v>17</v>
       </c>
@@ -7269,7 +7306,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="20"/>
+      <c r="B63" s="22"/>
       <c r="C63" s="2">
         <v>79</v>
       </c>
@@ -7299,7 +7336,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="20"/>
+      <c r="B64" s="22"/>
       <c r="C64" s="2">
         <v>438</v>
       </c>
@@ -7329,7 +7366,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="20"/>
+      <c r="B65" s="22"/>
       <c r="C65" s="2">
         <v>310</v>
       </c>
@@ -7359,7 +7396,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="20"/>
+      <c r="B66" s="22"/>
       <c r="C66" s="2">
         <v>621</v>
       </c>
@@ -7389,7 +7426,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="20"/>
+      <c r="B67" s="22"/>
       <c r="C67" s="2">
         <v>146</v>
       </c>
@@ -7419,7 +7456,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="21">
+      <c r="B68" s="23">
         <v>8</v>
       </c>
       <c r="C68" s="2">
@@ -7451,7 +7488,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="21"/>
+      <c r="B69" s="23"/>
       <c r="C69" s="2">
         <v>76</v>
       </c>
@@ -7481,7 +7518,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="21"/>
+      <c r="B70" s="23"/>
       <c r="C70" s="2">
         <v>297</v>
       </c>
@@ -7511,7 +7548,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="21"/>
+      <c r="B71" s="23"/>
       <c r="C71" s="2">
         <v>42</v>
       </c>
@@ -7541,7 +7578,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="21"/>
+      <c r="B72" s="23"/>
       <c r="C72" s="2">
         <v>295</v>
       </c>
@@ -7571,7 +7608,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="21"/>
+      <c r="B73" s="23"/>
       <c r="C73" s="2">
         <v>127</v>
       </c>
@@ -7601,7 +7638,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="21"/>
+      <c r="B74" s="23"/>
       <c r="C74" s="2">
         <v>224</v>
       </c>
@@ -7631,7 +7668,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="21"/>
+      <c r="B75" s="23"/>
       <c r="C75" s="2">
         <v>1235</v>
       </c>
@@ -7661,7 +7698,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="21"/>
+      <c r="B76" s="23"/>
       <c r="C76" s="2">
         <v>23</v>
       </c>
@@ -7691,7 +7728,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="21"/>
+      <c r="B77" s="23"/>
       <c r="C77" s="2">
         <v>84</v>
       </c>
@@ -7724,7 +7761,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="19" t="s">
         <v>130</v>
       </c>
       <c r="C78" s="2">
@@ -7756,7 +7793,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="17"/>
+      <c r="B79" s="19"/>
       <c r="C79" s="2">
         <v>153</v>
       </c>
@@ -7792,15 +7829,15 @@
       <c r="A85" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="22"/>
-      <c r="H85" s="22"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7905,14 +7942,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>467</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -7956,7 +7993,7 @@
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>480</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -7989,7 +8026,7 @@
       <c r="B4" s="2">
         <v>73</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -8015,7 +8052,7 @@
       <c r="B5" s="2">
         <v>49</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -8039,7 +8076,7 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
@@ -8063,7 +8100,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
@@ -8087,7 +8124,7 @@
       <c r="B8" s="2">
         <v>334</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
@@ -8111,7 +8148,7 @@
       <c r="B9" s="2">
         <v>163</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -8135,7 +8172,7 @@
       <c r="B10" s="2">
         <v>38</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
@@ -8159,7 +8196,7 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="19" t="s">
         <v>481</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -8185,7 +8222,7 @@
       <c r="B12" s="2">
         <v>328</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -8209,7 +8246,7 @@
       <c r="B13" s="2">
         <v>160</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
@@ -8233,7 +8270,7 @@
       <c r="B14" s="2">
         <v>94</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="19" t="s">
         <v>482</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -8259,7 +8296,7 @@
       <c r="B15" s="2">
         <v>103</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -8283,7 +8320,7 @@
       <c r="B16" s="2">
         <v>105</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
@@ -8310,7 +8347,7 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
@@ -8334,7 +8371,7 @@
       <c r="B18" s="2">
         <v>230</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -8358,7 +8395,7 @@
       <c r="B19" s="2">
         <v>285</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -8385,7 +8422,7 @@
       <c r="B20" s="2">
         <v>200</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
@@ -8409,7 +8446,7 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="19" t="s">
         <v>483</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -8435,7 +8472,7 @@
       <c r="B22" s="2">
         <v>22</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
@@ -8459,7 +8496,7 @@
       <c r="B23" s="2">
         <v>46</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -8483,7 +8520,7 @@
       <c r="B24" s="2">
         <v>78</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
@@ -8507,7 +8544,7 @@
       <c r="B25" s="2">
         <v>79</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
@@ -8534,7 +8571,7 @@
       <c r="B26" s="2">
         <v>75</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="19" t="s">
         <v>126</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -8560,7 +8597,7 @@
       <c r="B27" s="2">
         <v>347</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -8587,7 +8624,7 @@
       <c r="B28" s="2">
         <v>215</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -8614,7 +8651,7 @@
       <c r="B29" s="2">
         <v>162</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -8638,7 +8675,7 @@
       <c r="B30" s="2">
         <v>34</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
@@ -8662,7 +8699,7 @@
       <c r="B31" s="2">
         <v>56</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -8686,7 +8723,7 @@
       <c r="B32" s="2">
         <v>33</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -8710,7 +8747,7 @@
       <c r="B33" s="2">
         <v>253</v>
       </c>
-      <c r="C33" s="17"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
@@ -8734,7 +8771,7 @@
       <c r="B34" s="2">
         <v>240</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
@@ -8758,7 +8795,7 @@
       <c r="B35" s="2">
         <v>55</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="19" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -8784,7 +8821,7 @@
       <c r="B36" s="2">
         <v>62</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
@@ -8808,7 +8845,7 @@
       <c r="B37" s="2">
         <v>322</v>
       </c>
-      <c r="C37" s="17"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -8832,7 +8869,7 @@
       <c r="B38" s="2">
         <v>300</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -8859,7 +8896,7 @@
       <c r="B39" s="2">
         <v>251</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="19" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -8885,7 +8922,7 @@
       <c r="B40" s="2">
         <v>297</v>
       </c>
-      <c r="C40" s="17"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="2" t="s">
         <v>87</v>
       </c>
@@ -8909,7 +8946,7 @@
       <c r="B41" s="2">
         <v>380</v>
       </c>
-      <c r="C41" s="17"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
@@ -8936,7 +8973,7 @@
       <c r="B42" s="2">
         <v>348</v>
       </c>
-      <c r="C42" s="17"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -8960,7 +8997,7 @@
       <c r="B43" s="2">
         <v>202</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="19" t="s">
         <v>129</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -8986,7 +9023,7 @@
       <c r="B44" s="2">
         <v>172</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
@@ -9010,7 +9047,7 @@
       <c r="B45" s="2">
         <v>171</v>
       </c>
-      <c r="C45" s="17"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
@@ -9037,7 +9074,7 @@
       <c r="B46" s="2">
         <v>50</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
@@ -9064,7 +9101,7 @@
       <c r="B47" s="2">
         <v>69</v>
       </c>
-      <c r="C47" s="17"/>
+      <c r="C47" s="19"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -9091,7 +9128,7 @@
       <c r="B48" s="2">
         <v>29</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
@@ -9115,7 +9152,7 @@
       <c r="B49" s="2">
         <v>166</v>
       </c>
-      <c r="C49" s="17"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
@@ -9139,7 +9176,7 @@
       <c r="B50" s="2">
         <v>371</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="19" t="s">
         <v>130</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -9165,7 +9202,7 @@
       <c r="B51" s="2">
         <v>150</v>
       </c>
-      <c r="C51" s="17"/>
+      <c r="C51" s="19"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
@@ -9189,7 +9226,7 @@
       <c r="B52" s="2">
         <v>169</v>
       </c>
-      <c r="C52" s="17"/>
+      <c r="C52" s="19"/>
       <c r="D52" s="2" t="s">
         <v>21</v>
       </c>
@@ -9213,7 +9250,7 @@
       <c r="B53" s="2">
         <v>645</v>
       </c>
-      <c r="C53" s="17"/>
+      <c r="C53" s="19"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
@@ -9237,7 +9274,7 @@
       <c r="B54" s="2">
         <v>621</v>
       </c>
-      <c r="C54" s="17"/>
+      <c r="C54" s="19"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
@@ -9967,16 +10004,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10006,14 +10043,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
@@ -10023,14 +10060,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>706</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
@@ -10069,7 +10106,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>702</v>
       </c>
       <c r="C3" s="2">
@@ -10101,11 +10138,11 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="2">
         <v>975</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -10122,7 +10159,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="2">
         <v>482</v>
       </c>
@@ -10149,7 +10186,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="2">
         <v>904</v>
       </c>
@@ -10176,7 +10213,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
@@ -10190,7 +10227,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
@@ -10204,7 +10241,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
@@ -10218,7 +10255,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
@@ -10232,7 +10269,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="31" t="s">
         <v>707</v>
       </c>
       <c r="C11" s="2">
@@ -10259,7 +10296,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="2">
         <v>11</v>
       </c>
@@ -10284,7 +10321,7 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="2">
         <v>15</v>
       </c>
@@ -10311,7 +10348,7 @@
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="2">
         <v>31</v>
       </c>
@@ -10338,7 +10375,7 @@
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="2">
         <v>43</v>
       </c>
@@ -10365,7 +10402,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="2">
         <v>48</v>
       </c>
@@ -10390,7 +10427,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="2">
         <v>55</v>
       </c>
@@ -10415,7 +10452,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="2">
         <v>66</v>
       </c>
@@ -10440,11 +10477,11 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="2">
         <v>76</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -10460,11 +10497,11 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="2">
         <v>158</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -10480,7 +10517,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="2">
         <v>159</v>
       </c>
@@ -10507,7 +10544,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="17"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="2">
         <v>163</v>
       </c>
@@ -10531,7 +10568,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="17"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="2">
         <v>681</v>
       </c>
@@ -10555,7 +10592,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="17"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="2">
         <v>809</v>
       </c>
@@ -10579,7 +10616,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="2">
         <v>833</v>
       </c>
@@ -10612,7 +10649,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="2">
         <v>849</v>
       </c>
@@ -10636,7 +10673,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="2">
         <v>20</v>
       </c>
@@ -10661,11 +10698,11 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="2">
         <v>23</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -10681,11 +10718,11 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2">
         <v>42</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -10701,7 +10738,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="2">
         <v>215</v>
       </c>
@@ -10729,7 +10766,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="17"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="2">
         <v>253</v>
       </c>
@@ -10757,7 +10794,7 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="17"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="2">
         <v>844</v>
       </c>
@@ -10781,11 +10818,11 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="17"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="2">
         <v>857</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -10800,7 +10837,7 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="17"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="2">
         <v>973</v>
       </c>
@@ -10828,7 +10865,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="31" t="s">
         <v>802</v>
       </c>
       <c r="C35" s="2">
@@ -10855,7 +10892,7 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="17"/>
+      <c r="B36" s="19"/>
       <c r="C36" s="2">
         <v>19</v>
       </c>
@@ -10880,7 +10917,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="17"/>
+      <c r="B37" s="19"/>
       <c r="C37" s="2">
         <v>21</v>
       </c>
@@ -10905,7 +10942,7 @@
       <c r="A38" s="9">
         <v>36</v>
       </c>
-      <c r="B38" s="17"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="2">
         <v>138</v>
       </c>
@@ -10932,13 +10969,13 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="31" t="s">
         <v>814</v>
       </c>
       <c r="C39" s="2">
         <v>124</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -10953,11 +10990,11 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="17"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="2">
         <v>127</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -10973,7 +11010,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="17"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="2">
         <v>200</v>
       </c>
@@ -10998,7 +11035,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="17"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="2">
         <v>210</v>
       </c>
@@ -11022,7 +11059,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="17"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="2">
         <v>222</v>
       </c>
@@ -11046,11 +11083,11 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="17"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="2">
         <v>329</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D44" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -11065,7 +11102,7 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="17"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="2">
         <v>394</v>
       </c>
@@ -11089,7 +11126,7 @@
       <c r="A46" s="9">
         <v>44</v>
       </c>
-      <c r="B46" s="17"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="2">
         <v>399</v>
       </c>
@@ -11113,7 +11150,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="17"/>
+      <c r="B47" s="19"/>
       <c r="C47" s="2">
         <v>543</v>
       </c>
@@ -11137,11 +11174,11 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="17"/>
+      <c r="B48" s="19"/>
       <c r="C48" s="2">
         <v>753</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -11156,11 +11193,11 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="17"/>
+      <c r="B49" s="19"/>
       <c r="C49" s="2">
         <v>489</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -11176,7 +11213,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="17"/>
+      <c r="B50" s="19"/>
       <c r="C50" s="2">
         <v>947</v>
       </c>
@@ -11203,7 +11240,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="17"/>
+      <c r="B51" s="19"/>
       <c r="C51" s="2">
         <v>951</v>
       </c>
@@ -11227,13 +11264,13 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="19" t="s">
         <v>858</v>
       </c>
       <c r="C52" s="2">
         <v>425</v>
       </c>
-      <c r="D52" s="30" t="s">
+      <c r="D52" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -11248,7 +11285,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="17"/>
+      <c r="B53" s="19"/>
       <c r="C53" s="2">
         <v>247</v>
       </c>
@@ -11275,11 +11312,11 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="17"/>
+      <c r="B54" s="19"/>
       <c r="C54" s="2">
         <v>212</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="D54" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -11289,13 +11326,12 @@
         <v>864</v>
       </c>
       <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1">
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="17"/>
+      <c r="B55" s="19"/>
       <c r="C55" s="2">
         <v>351</v>
       </c>
@@ -11308,38 +11344,79 @@
       <c r="F55" s="6" t="s">
         <v>867</v>
       </c>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
+      <c r="G55" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="56" spans="1:10" ht="15" customHeight="1">
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="2"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="2">
+        <v>17</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>872</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>873</v>
+      </c>
       <c r="H56" s="2"/>
+      <c r="I56" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1">
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="2"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="2">
+        <v>22</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>875</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>876</v>
+      </c>
       <c r="H57" s="2"/>
+      <c r="I57" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1">
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="31" t="s">
+        <v>877</v>
+      </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -11351,7 +11428,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="19"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -11363,7 +11440,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="2"/>
+      <c r="B60" s="19"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -11375,7 +11452,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="2"/>
+      <c r="B61" s="19"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -11387,7 +11464,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="2"/>
+      <c r="B62" s="19"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -11399,7 +11476,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="19"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -11411,7 +11488,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="2"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -11648,7 +11725,8 @@
       <c r="B87" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
@@ -11698,6 +11776,8 @@
     <hyperlink ref="F53" r:id="rId38" xr:uid="{15C1B4AD-D07E-4248-8A2A-7C2A2E0783A0}"/>
     <hyperlink ref="F54" r:id="rId39" xr:uid="{E36AE3CD-BB80-5048-8C5E-6D3119DE81CC}"/>
     <hyperlink ref="F55" r:id="rId40" xr:uid="{CF93A748-115E-4A48-ABCE-7B4D0955A1F8}"/>
+    <hyperlink ref="F56" r:id="rId41" xr:uid="{5E24FF08-E138-4045-A9A3-5DCF4400154E}"/>
+    <hyperlink ref="F57" r:id="rId42" xr:uid="{E81214BD-229B-3744-9EF2-421F7DC8E233}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11725,12 +11805,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10">
@@ -12743,14 +12823,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>643</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>

</xml_diff>

<commit_message>
[20240111] Google Interview (85) 52-57
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C466FE01-906A-024E-AFF8-E12D2372AC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826E2A62-DD69-3A49-B6EC-0578C1567AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="897">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3245,6 +3245,83 @@
     <t>Sorting
 and 
 Searching</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Median of Two Sorted Arrays</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/63/sorting-and-searching-4/3080/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Sorted Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.11</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/63/sorting-and-searching-4/3081/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>optimized ans: not only left, right to binary search, but also use first, last to reach most left, right border if nums[mid]==target</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merge Intervals</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/63/sorting-and-searching-4/450/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort(key = lambda x : x[0])</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort list first, for loop intervals, if not answer or answer[-1][1] &lt; interval[0]: append, else: answer[-1][-1] = max([-1][-1], interval[1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insert Interval</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/63/sorting-and-searching-4/445/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two list (left, right) to save the left side and right side of NEW_LIST, NEW_START, NEW_END = newInterval[0], newInterval[1], return left+[[NEW L, R]] + right</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/63/sorting-and-searching-4/3082/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>return Counter(s) == Counter(t)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count of Smaller Numbers After Self</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/63/sorting-and-searching-4/3083/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamic
+Programming</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peak Index in a Mountain Array</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3843,7 +3920,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7925,7 +8002,7 @@
   <dimension ref="A1:K290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10004,16 +10081,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10043,14 +10120,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
@@ -11417,10 +11494,18 @@
       <c r="B58" s="31" t="s">
         <v>877</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="6"/>
+      <c r="C58" s="2">
+        <v>4</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>879</v>
+      </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
@@ -11429,58 +11514,121 @@
         <v>57</v>
       </c>
       <c r="B59" s="19"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="2"/>
+      <c r="C59" s="2">
+        <v>34</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>882</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>883</v>
+      </c>
       <c r="H59" s="2"/>
+      <c r="I59" s="2" t="s">
+        <v>881</v>
+      </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1">
       <c r="A60" s="2">
         <v>58</v>
       </c>
       <c r="B60" s="19"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="2"/>
+      <c r="C60" s="2">
+        <v>56</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>885</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>887</v>
+      </c>
       <c r="H60" s="2"/>
+      <c r="I60" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1">
       <c r="A61" s="2">
         <v>59</v>
       </c>
       <c r="B61" s="19"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="2"/>
+      <c r="C61" s="2">
+        <v>57</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>889</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>890</v>
+      </c>
       <c r="H61" s="2"/>
+      <c r="I61" s="2" t="s">
+        <v>881</v>
+      </c>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1">
       <c r="A62" s="2">
         <v>60</v>
       </c>
       <c r="B62" s="19"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="2"/>
+      <c r="C62" s="2">
+        <v>242</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>891</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>892</v>
+      </c>
       <c r="H62" s="2"/>
+      <c r="I62" s="2" t="s">
+        <v>881</v>
+      </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1">
       <c r="A63" s="2">
         <v>61</v>
       </c>
       <c r="B63" s="19"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="6"/>
+      <c r="C63" s="2">
+        <v>315</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>894</v>
+      </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
@@ -11491,7 +11639,9 @@
       <c r="B64" s="19"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>896</v>
+      </c>
       <c r="F64" s="6"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -11500,7 +11650,9 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="2"/>
+      <c r="B65" s="31" t="s">
+        <v>895</v>
+      </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -11512,7 +11664,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="2"/>
+      <c r="B66" s="19"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -11524,7 +11676,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="2"/>
+      <c r="B67" s="19"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -11536,7 +11688,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="2"/>
+      <c r="B68" s="19"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -11548,7 +11700,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="2"/>
+      <c r="B69" s="19"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -11560,7 +11712,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="2"/>
+      <c r="B70" s="19"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -11572,7 +11724,9 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="2"/>
+      <c r="B71" s="19" t="s">
+        <v>128</v>
+      </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -11584,7 +11738,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="2"/>
+      <c r="B72" s="19"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -11596,7 +11750,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="2"/>
+      <c r="B73" s="19"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -11608,7 +11762,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="2"/>
+      <c r="B74" s="19"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -11620,7 +11774,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="2"/>
+      <c r="B75" s="19"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -11632,7 +11786,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="2"/>
+      <c r="B76" s="19"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -11644,7 +11798,9 @@
       <c r="A77" s="2">
         <v>75</v>
       </c>
-      <c r="B77" s="2"/>
+      <c r="B77" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -11656,7 +11812,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="2"/>
+      <c r="B78" s="19"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -11668,7 +11824,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="2"/>
+      <c r="B79" s="19"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -11680,52 +11836,55 @@
       <c r="A80" s="2">
         <v>78</v>
       </c>
-      <c r="B80" s="2"/>
+      <c r="B80" s="19"/>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
         <v>79</v>
       </c>
-      <c r="B81" s="2"/>
+      <c r="B81" s="19"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
         <v>80</v>
       </c>
-      <c r="B82" s="2"/>
+      <c r="B82" s="19"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
         <v>81</v>
       </c>
-      <c r="B83" s="2"/>
+      <c r="B83" s="19"/>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
         <v>82</v>
       </c>
-      <c r="B84" s="2"/>
+      <c r="B84" s="19"/>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
         <v>83</v>
       </c>
-      <c r="B85" s="2"/>
+      <c r="B85" s="19"/>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
         <v>84</v>
       </c>
-      <c r="B86" s="2"/>
+      <c r="B86" s="19"/>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
         <v>85</v>
       </c>
-      <c r="B87" s="2"/>
+      <c r="B87" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
@@ -11778,6 +11937,12 @@
     <hyperlink ref="F55" r:id="rId40" xr:uid="{CF93A748-115E-4A48-ABCE-7B4D0955A1F8}"/>
     <hyperlink ref="F56" r:id="rId41" xr:uid="{5E24FF08-E138-4045-A9A3-5DCF4400154E}"/>
     <hyperlink ref="F57" r:id="rId42" xr:uid="{E81214BD-229B-3744-9EF2-421F7DC8E233}"/>
+    <hyperlink ref="F58" r:id="rId43" xr:uid="{C538A92A-E9D6-984A-827A-AD4EF135C8EE}"/>
+    <hyperlink ref="F59" r:id="rId44" xr:uid="{D3AD1513-DB83-3F45-A964-31A641CF5587}"/>
+    <hyperlink ref="F60" r:id="rId45" xr:uid="{56D73645-184A-EF46-8752-5909A6FF2D96}"/>
+    <hyperlink ref="F61" r:id="rId46" xr:uid="{9EB7CB74-E729-284D-9229-0AE1789F23B6}"/>
+    <hyperlink ref="F62" r:id="rId47" xr:uid="{3267F658-1948-C645-BEA2-B61F63545223}"/>
+    <hyperlink ref="F63" r:id="rId48" xr:uid="{55055917-67C5-A34D-A258-EE11EA6DB78C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240112] Google Interview (85) 58-60
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826E2A62-DD69-3A49-B6EC-0578C1567AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291EB192-7717-2F4D-9B87-B5B56587CC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="906">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3322,6 +3322,41 @@
   </si>
   <si>
     <t>Peak Index in a Mountain Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/63/sorting-and-searching-4/3084/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.12</t>
+  </si>
+  <si>
+    <t>Binary search if arr[mid] &lt; arr[mid + 1]: left = mid + 1, or, return arr.index(max(arr)), or, while arr[i] &lt; arr[i + 1]: i+= 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Longest Palindromic Substring</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/64/dynamic-programming-4/451/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/64/dynamic-programming-4/3085/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>check odd or even, for loop for par_twoSame, par_one = get_internal_pal(s, i, i+1), get_internal_pal(s, i, i), get_internal_pal is check left and right same, return max strings</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP or Kadane's Algorithm, for loop all num: sum_value = max(sum_value + nums[i], nums[i]), max_value = max(max_value, sum_value)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pal = max([pal, par_twoSame, par], key=len)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10081,16 +10116,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10120,8 +10155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11630,49 +11665,87 @@
         <v>894</v>
       </c>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1">
       <c r="A64" s="2">
         <v>62</v>
       </c>
       <c r="B64" s="19"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
+      <c r="C64" s="2">
+        <v>852</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E64" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="F64" s="6"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="1:8" ht="15" customHeight="1">
+      <c r="F64" s="6" t="s">
+        <v>897</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15" customHeight="1">
       <c r="A65" s="2">
         <v>63</v>
       </c>
       <c r="B65" s="31" t="s">
         <v>895</v>
       </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="6"/>
-      <c r="G65" s="2"/>
+      <c r="C65" s="2">
+        <v>5</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>901</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>903</v>
+      </c>
       <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1">
+      <c r="I65" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15" customHeight="1">
       <c r="A66" s="2">
         <v>64</v>
       </c>
       <c r="B66" s="19"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="6"/>
-      <c r="G66" s="2"/>
+      <c r="C66" s="2">
+        <v>53</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>902</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>904</v>
+      </c>
       <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1">
+      <c r="I66" s="2" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15" customHeight="1">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -11684,7 +11757,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15" customHeight="1">
+    <row r="68" spans="1:10" ht="15" customHeight="1">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -11696,7 +11769,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15" customHeight="1">
+    <row r="69" spans="1:10" ht="15" customHeight="1">
       <c r="A69" s="2">
         <v>67</v>
       </c>
@@ -11708,7 +11781,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15" customHeight="1">
+    <row r="70" spans="1:10" ht="15" customHeight="1">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -11720,7 +11793,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15" customHeight="1">
+    <row r="71" spans="1:10" ht="15" customHeight="1">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -11734,7 +11807,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15" customHeight="1">
+    <row r="72" spans="1:10" ht="15" customHeight="1">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -11746,7 +11819,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15" customHeight="1">
+    <row r="73" spans="1:10" ht="15" customHeight="1">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -11758,7 +11831,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15" customHeight="1">
+    <row r="74" spans="1:10" ht="15" customHeight="1">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -11770,7 +11843,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1">
+    <row r="75" spans="1:10" ht="15" customHeight="1">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -11782,7 +11855,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15" customHeight="1">
+    <row r="76" spans="1:10" ht="15" customHeight="1">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -11794,7 +11867,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1">
+    <row r="77" spans="1:10" ht="15" customHeight="1">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -11808,7 +11881,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1">
+    <row r="78" spans="1:10" ht="15" customHeight="1">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -11820,7 +11893,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15" customHeight="1">
+    <row r="79" spans="1:10" ht="15" customHeight="1">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -11832,7 +11905,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:10">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -11882,16 +11955,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="B65:B70"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B34"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -11943,6 +12016,9 @@
     <hyperlink ref="F61" r:id="rId46" xr:uid="{9EB7CB74-E729-284D-9229-0AE1789F23B6}"/>
     <hyperlink ref="F62" r:id="rId47" xr:uid="{3267F658-1948-C645-BEA2-B61F63545223}"/>
     <hyperlink ref="F63" r:id="rId48" xr:uid="{55055917-67C5-A34D-A258-EE11EA6DB78C}"/>
+    <hyperlink ref="F64" r:id="rId49" xr:uid="{1B85C16C-720E-0A4A-92B6-5A6EA2B5B713}"/>
+    <hyperlink ref="F65" r:id="rId50" xr:uid="{3EA4CFCA-87AA-4941-AA02-F2FECD9A30D5}"/>
+    <hyperlink ref="F66" r:id="rId51" xr:uid="{4392D927-9AD9-224E-9BA3-CC4EEE96C459}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240113] Google Interview (85) 61-64
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291EB192-7717-2F4D-9B87-B5B56587CC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9A6739-EB84-1841-81F1-BE09C2B2E7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="917">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3358,6 +3358,48 @@
   <si>
     <t>pal = max([pal, par_twoSame, par], key=len)</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/64/dynamic-programming-4/3086/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>one pass: min_val, max_val to save min and max(price-min, max), or, dp: [0] * len(prices), dp[i] = max(dp[i-1], prices[i] - min_val))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximum Product Subarray</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/64/dynamic-programming-4/3087/</t>
+  </si>
+  <si>
+    <t>max_num, min_num, for loop: if i &lt;0: max &lt;-&gt; min, and get max/min by max/min(nums[i], nums[i] * max/min), then answer = max(answer, max_num)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coin Change</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/64/dynamic-programming-4/3088/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>minCoin = [amount + 1] * (amount + 1), for loop in numCoin and for loop in coin: minCoin[curNum] = min(minCoin[curNum], minCoin[curNum - coin] + 1), minCoin[amount] != (amount + 1), return</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Split Array Largest Sum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/64/dynamic-programming-4/3089/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.13</t>
   </si>
 </sst>
 </file>
@@ -10155,8 +10197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11750,46 +11792,93 @@
         <v>65</v>
       </c>
       <c r="B67" s="19"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="2"/>
+      <c r="C67" s="2">
+        <v>121</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>906</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>907</v>
+      </c>
       <c r="H67" s="2"/>
+      <c r="I67" s="2" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="68" spans="1:10" ht="15" customHeight="1">
       <c r="A68" s="2">
         <v>66</v>
       </c>
       <c r="B68" s="19"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="2"/>
+      <c r="C68" s="2">
+        <v>152</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>909</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>910</v>
+      </c>
       <c r="H68" s="2"/>
+      <c r="I68" s="2" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="69" spans="1:10" ht="15" customHeight="1">
       <c r="A69" s="2">
         <v>67</v>
       </c>
       <c r="B69" s="19"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="2"/>
+      <c r="C69" s="2">
+        <v>322</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>912</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>913</v>
+      </c>
       <c r="H69" s="2"/>
+      <c r="I69" s="2" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1">
       <c r="A70" s="2">
         <v>68</v>
       </c>
       <c r="B70" s="19"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="6"/>
+      <c r="C70" s="2">
+        <v>410</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>915</v>
+      </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
@@ -12019,6 +12108,9 @@
     <hyperlink ref="F64" r:id="rId49" xr:uid="{1B85C16C-720E-0A4A-92B6-5A6EA2B5B713}"/>
     <hyperlink ref="F65" r:id="rId50" xr:uid="{3EA4CFCA-87AA-4941-AA02-F2FECD9A30D5}"/>
     <hyperlink ref="F66" r:id="rId51" xr:uid="{4392D927-9AD9-224E-9BA3-CC4EEE96C459}"/>
+    <hyperlink ref="F67" r:id="rId52" xr:uid="{1F2EB0A4-B5C3-734D-A1A5-D0606AAEF2A8}"/>
+    <hyperlink ref="F69" r:id="rId53" xr:uid="{9610342B-03E0-E047-ADA2-71A22DF74A15}"/>
+    <hyperlink ref="F70" r:id="rId54" xr:uid="{8F2EE085-81B9-4C49-8000-265D0B27DC74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240115] Google Interview (85) 65-67
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9A6739-EB84-1841-81F1-BE09C2B2E7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05BA060-20C0-2341-9B67-F6CDB8716561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="925">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3400,6 +3400,38 @@
   </si>
   <si>
     <t>2024.01.13</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/65/design-4/3090/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bidrectional-linkedlist or OrderDict, bi: class for Node creat, funcs to add node to last  and rm specific node, then get: return and rm/add node, put: check len and add. Or, OrderDict with move_to_end</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>in collections lib, OrderDict:  move_to_end, self.table.popitem(last = False)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/65/design-4/3091/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two list: stack and min_list, if smaller than min_lst[-1] then append val, pop mini: reutnr mini_lst[-1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/65/design-4/3092/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -10158,16 +10190,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10197,8 +10229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10210,7 +10242,7 @@
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="159.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
@@ -11870,7 +11902,7 @@
       <c r="C70" s="2">
         <v>410</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E70" s="2" t="s">
@@ -11889,36 +11921,73 @@
       <c r="B71" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
+      <c r="C71" s="2">
+        <v>146</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>917</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>921</v>
+      </c>
     </row>
     <row r="72" spans="1:10" ht="15" customHeight="1">
       <c r="A72" s="2">
         <v>70</v>
       </c>
       <c r="B72" s="19"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="2"/>
+      <c r="C72" s="2">
+        <v>155</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>923</v>
+      </c>
       <c r="H72" s="2"/>
+      <c r="I72" s="2" t="s">
+        <v>919</v>
+      </c>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1">
       <c r="A73" s="2">
         <v>71</v>
       </c>
       <c r="B73" s="19"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="6"/>
+      <c r="C73" s="2">
+        <v>297</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>924</v>
+      </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:10" ht="15" customHeight="1">
       <c r="A74" s="2">
@@ -12044,16 +12113,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B77:B87"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B51"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="B77:B87"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B52:B57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12111,6 +12180,9 @@
     <hyperlink ref="F67" r:id="rId52" xr:uid="{1F2EB0A4-B5C3-734D-A1A5-D0606AAEF2A8}"/>
     <hyperlink ref="F69" r:id="rId53" xr:uid="{9610342B-03E0-E047-ADA2-71A22DF74A15}"/>
     <hyperlink ref="F70" r:id="rId54" xr:uid="{8F2EE085-81B9-4C49-8000-265D0B27DC74}"/>
+    <hyperlink ref="F71" r:id="rId55" xr:uid="{2E55D4E7-4B36-7749-B6BA-8630A2517B19}"/>
+    <hyperlink ref="F72" r:id="rId56" xr:uid="{C7E6258D-5E6A-E249-B9EF-D8B6537907C6}"/>
+    <hyperlink ref="F73" r:id="rId57" xr:uid="{1DB18B2C-A1FB-DA4A-9F85-E9A5B9531018}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240116] Google Interview (85) 68-70
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05BA060-20C0-2341-9B67-F6CDB8716561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E730860-2222-1D42-A92F-E96FD65B7B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="935">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3431,6 +3431,45 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/interview/card/google/65/design-4/3092/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.16</t>
+  </si>
+  <si>
+    <t>Logger Rate Limiter</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/65/design-4/3093/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dict to save msg:time, if in table and &gt;=10: update and return True, or not in table: return true</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design Search Autocomplete System</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insert Delete GetRandom O(1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/65/design-4/3094/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/65/design-4/3095/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>set with add/remove is too slow, list with dict: list for val and dic for order idx, insert: append with len for idx, remote: switch the val posi and idx for will del value and last one, and del</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>random.choice(self.data), set() with add, remove</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4028,7 +4067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -5583,7 +5622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A3E788-79EF-43BB-839C-C5A19C7470CF}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
@@ -8111,7 +8150,7 @@
   <dimension ref="A1:K290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="C21" sqref="C21:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10190,16 +10229,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10229,8 +10268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11987,42 +12026,75 @@
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:10" ht="15" customHeight="1">
       <c r="A74" s="2">
         <v>72</v>
       </c>
       <c r="B74" s="19"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
+      <c r="C74" s="2">
+        <v>359</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>927</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>925</v>
+      </c>
     </row>
     <row r="75" spans="1:10" ht="15" customHeight="1">
       <c r="A75" s="2">
         <v>73</v>
       </c>
       <c r="B75" s="19"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
+      <c r="C75" s="2">
+        <v>380</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>931</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="76" spans="1:10" ht="15" customHeight="1">
       <c r="A76" s="2">
         <v>74</v>
       </c>
       <c r="B76" s="19"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="2"/>
+      <c r="C76" s="2">
+        <v>642</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>932</v>
+      </c>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1">
@@ -12113,16 +12185,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="B65:B70"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B34"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12183,6 +12255,9 @@
     <hyperlink ref="F71" r:id="rId55" xr:uid="{2E55D4E7-4B36-7749-B6BA-8630A2517B19}"/>
     <hyperlink ref="F72" r:id="rId56" xr:uid="{C7E6258D-5E6A-E249-B9EF-D8B6537907C6}"/>
     <hyperlink ref="F73" r:id="rId57" xr:uid="{1DB18B2C-A1FB-DA4A-9F85-E9A5B9531018}"/>
+    <hyperlink ref="F74" r:id="rId58" xr:uid="{B637672C-4A08-C649-B12A-5B64803C8114}"/>
+    <hyperlink ref="F75" r:id="rId59" xr:uid="{82D980EE-1B67-204C-BB65-128DE865CFC5}"/>
+    <hyperlink ref="F76" r:id="rId60" xr:uid="{C11A09BF-E1B6-254D-8EB8-DA021BE1CA4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240117] Google Interview (85) 71-74
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E730860-2222-1D42-A92F-E96FD65B7B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88801B3A-10A6-6A46-9C14-C24B310CE30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="947">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3470,6 +3470,54 @@
   </si>
   <si>
     <t>random.choice(self.data), set() with add, remove</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3096/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.18</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>x = int(str(x)[::-1]) if x &gt; 0 else int((str(x)[1:])[::-1]) * -1 and return x if (-(2**31) &lt;= x &lt;= (2**31-1)), or, recursion: answer+= digit (from  %10 or %-10) and math.trunc(x / 10)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>math.trunc(x / 10) 去小數</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Candy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3097/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3098/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Isomorphic (同構) Strings</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>len(set(s)) == len(set(t)) == len(set(zip(s, t))); or; two dict, for loop in zip(s,t): s[s1]=t1, t[t1]=s1, if (s1 in s_dict and s[s1] != t1) or (same to t) return False</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Strobogrammatic Number</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3099/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two ptr left and right to check left &lt;= right: if (num[left] not in table) or (table[num[left]] != num[right]): return False</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10229,16 +10277,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10268,8 +10316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12104,22 +12152,46 @@
       <c r="B77" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="2"/>
+      <c r="C77" s="2">
+        <v>7</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>937</v>
+      </c>
       <c r="H77" s="2"/>
+      <c r="I77" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>938</v>
+      </c>
     </row>
     <row r="78" spans="1:10" ht="15" customHeight="1">
       <c r="A78" s="2">
         <v>76</v>
       </c>
       <c r="B78" s="19"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="6"/>
+      <c r="C78" s="2">
+        <v>135</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>940</v>
+      </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
@@ -12128,18 +12200,48 @@
         <v>77</v>
       </c>
       <c r="B79" s="19"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
+      <c r="C79" s="2">
+        <v>205</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>941</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="2">
         <v>78</v>
       </c>
       <c r="B80" s="19"/>
+      <c r="C80" s="2">
+        <v>246</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>945</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
@@ -12185,16 +12287,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B77:B87"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B51"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="B77:B87"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B52:B57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12258,6 +12360,10 @@
     <hyperlink ref="F74" r:id="rId58" xr:uid="{B637672C-4A08-C649-B12A-5B64803C8114}"/>
     <hyperlink ref="F75" r:id="rId59" xr:uid="{82D980EE-1B67-204C-BB65-128DE865CFC5}"/>
     <hyperlink ref="F76" r:id="rId60" xr:uid="{C11A09BF-E1B6-254D-8EB8-DA021BE1CA4B}"/>
+    <hyperlink ref="F77" r:id="rId61" xr:uid="{EE7C809E-DB39-F143-9808-E1B9B233A448}"/>
+    <hyperlink ref="F78" r:id="rId62" xr:uid="{13E11C4D-C768-354B-B1D4-50C2141A27E1}"/>
+    <hyperlink ref="F79" r:id="rId63" xr:uid="{5911E4F0-7A34-BA44-AF21-77D577D681F2}"/>
+    <hyperlink ref="F80" r:id="rId64" xr:uid="{BD52BE01-6AD2-634C-97A7-411158AA3F75}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240119] Google Interview (85) 75-78
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88801B3A-10A6-6A46-9C14-C24B310CE30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DD7B7F-FE7F-9F42-8A64-79C39B9C1CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="959">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3518,6 +3518,53 @@
   </si>
   <si>
     <t>two ptr left and right to check left &lt;= right: if (num[left] not in table) or (table[num[left]] != num[right]): return False</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.19</t>
+  </si>
+  <si>
+    <t>Bulls and Cows</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3100/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range Sum Query 2D - Mutable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/477/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>My Calendar II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3101/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>set and for loop to check in set</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jewels and Stones</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stones.count(jewel)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3102/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two list for single and double booked, book func: first to check if overlap interval in double list (if start &lt; e and end &gt; s), then check in single list: if so append to double list, finally add to single list</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10277,16 +10324,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10316,8 +10363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12183,7 +12230,7 @@
       <c r="C78" s="2">
         <v>135</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="17" t="s">
         <v>87</v>
       </c>
       <c r="E78" s="2" t="s">
@@ -12243,43 +12290,109 @@
         <v>936</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:10">
       <c r="A81" s="2">
         <v>79</v>
       </c>
       <c r="B81" s="19"/>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81" s="2">
+        <v>299</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>949</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="2">
         <v>80</v>
       </c>
       <c r="B82" s="19"/>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82" s="2">
+        <v>308</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="2">
         <v>81</v>
       </c>
       <c r="B83" s="19"/>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83" s="2">
+        <v>731</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="2">
         <v>82</v>
       </c>
       <c r="B84" s="19"/>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84" s="2">
+        <v>771</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>957</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="2">
         <v>83</v>
       </c>
       <c r="B85" s="19"/>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="J85" s="2" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="2">
         <v>84</v>
       </c>
       <c r="B86" s="19"/>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:10">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -12287,16 +12400,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="B65:B70"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B34"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12364,6 +12477,10 @@
     <hyperlink ref="F78" r:id="rId62" xr:uid="{13E11C4D-C768-354B-B1D4-50C2141A27E1}"/>
     <hyperlink ref="F79" r:id="rId63" xr:uid="{5911E4F0-7A34-BA44-AF21-77D577D681F2}"/>
     <hyperlink ref="F80" r:id="rId64" xr:uid="{BD52BE01-6AD2-634C-97A7-411158AA3F75}"/>
+    <hyperlink ref="F81" r:id="rId65" xr:uid="{DBDCDF10-4451-AA4A-968B-27BA94872A95}"/>
+    <hyperlink ref="F82" r:id="rId66" xr:uid="{255C6FCC-14DF-B440-9D5E-2B9BF1EBA92C}"/>
+    <hyperlink ref="F83" r:id="rId67" xr:uid="{0BC80FE7-23DD-4C4E-B09D-C812D887B468}"/>
+    <hyperlink ref="F84" r:id="rId68" xr:uid="{85F0F672-A7BB-2642-9889-9A907F558958}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240120] Google Interview (85) reorder num
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DD7B7F-FE7F-9F42-8A64-79C39B9C1CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68722784-9980-8943-B960-B2678BCD5D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="969">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3565,6 +3565,46 @@
   </si>
   <si>
     <t>two list for single and double booked, book func: first to check if overlap interval in double list (if start &lt; e and end &gt; s), then check in single list: if so append to double list, finally add to single list</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Swap Adjacent in LR String</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3103/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guess the Word</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/swap-adjacent-in-lr-string/description/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum Area Rectangle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/66/others-4/3105/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/526/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/525/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/527/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/google/67/sql-2/528/</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10324,16 +10364,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10363,8 +10403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10539,7 +10579,9 @@
       <c r="E7" s="2" t="s">
         <v>717</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>966</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
@@ -10553,7 +10595,9 @@
       <c r="E8" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="15" t="s">
+        <v>965</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -10567,7 +10611,9 @@
       <c r="E9" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>967</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -10581,7 +10627,9 @@
       <c r="E10" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>968</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
@@ -12382,6 +12430,18 @@
         <v>83</v>
       </c>
       <c r="B85" s="19"/>
+      <c r="C85" s="2">
+        <v>777</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>960</v>
+      </c>
       <c r="J85" s="2" t="s">
         <v>956</v>
       </c>
@@ -12391,25 +12451,49 @@
         <v>84</v>
       </c>
       <c r="B86" s="19"/>
+      <c r="C86" s="2">
+        <v>843</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>962</v>
+      </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="2">
         <v>85</v>
       </c>
       <c r="B87" s="19"/>
+      <c r="C87" s="2">
+        <v>939</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>964</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B77:B87"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B51"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="B77:B87"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B52:B57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12481,6 +12565,13 @@
     <hyperlink ref="F82" r:id="rId66" xr:uid="{255C6FCC-14DF-B440-9D5E-2B9BF1EBA92C}"/>
     <hyperlink ref="F83" r:id="rId67" xr:uid="{0BC80FE7-23DD-4C4E-B09D-C812D887B468}"/>
     <hyperlink ref="F84" r:id="rId68" xr:uid="{85F0F672-A7BB-2642-9889-9A907F558958}"/>
+    <hyperlink ref="F85" r:id="rId69" xr:uid="{D4C8D07B-D6F6-E64E-B4C2-352D1B7BD207}"/>
+    <hyperlink ref="F86" r:id="rId70" xr:uid="{4166EB0F-C662-B84F-BA24-7C524274F6EC}"/>
+    <hyperlink ref="F87" r:id="rId71" xr:uid="{70CA95C6-1D8C-8E42-99B1-7AD1820B0453}"/>
+    <hyperlink ref="F8" r:id="rId72" xr:uid="{EDEDE48E-A820-5C40-899B-B2CD7B86FF65}"/>
+    <hyperlink ref="F7" r:id="rId73" xr:uid="{CF2EF0D8-4A3E-354F-8836-5A6D882E579E}"/>
+    <hyperlink ref="F9" r:id="rId74" xr:uid="{46956950-322A-4141-AB9C-F25ADE4ECC65}"/>
+    <hyperlink ref="F10" r:id="rId75" xr:uid="{351DA4DD-BBA3-5546-95F0-82093104C951}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240121] Google Interview (85) 83-85
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68722784-9980-8943-B960-B2678BCD5D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9310221-3D70-D045-9427-DD9B187052E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="974">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3605,6 +3605,25 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/interview/card/google/67/sql-2/528/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>check (1) len same,  (2) RL order same because order change is only for X with R/L, (3)  the order is right for L (end idx &lt;= start) and R (end idx &gt;= start)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.20</t>
+  </si>
+  <si>
+    <t>start.replace('X', '')</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mini_area = float('inf')</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bruce sol: set to save seen, two loop to check two points and calc to find mini area (abs(x2-x1)*(y2-y1)) then add x1y1 to seen, or, optmized: sort, add to tuple, and two loop to check x1,y1&lt;x2,y2 and in set</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10404,7 +10423,7 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12424,6 +12443,9 @@
       <c r="H84" s="2" t="s">
         <v>947</v>
       </c>
+      <c r="J84" s="2" t="s">
+        <v>956</v>
+      </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="2">
@@ -12442,8 +12464,14 @@
       <c r="F85" s="6" t="s">
         <v>960</v>
       </c>
+      <c r="G85" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>970</v>
+      </c>
       <c r="J85" s="2" t="s">
-        <v>956</v>
+        <v>971</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -12480,6 +12508,15 @@
       </c>
       <c r="F87" s="6" t="s">
         <v>964</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>972</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[20240121] Amazon Interview (68) 1-3
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9310221-3D70-D045-9427-DD9B187052E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24CF74A-A6CA-6842-AFF5-695844C63574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="984">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3624,6 +3624,47 @@
   </si>
   <si>
     <t>Bruce sol: set to save seen, two loop to check two points and calc to find mini area (abs(x2-x1)*(y2-y1)) then add x1y1 to seen, or, optmized: sort, add to tuple, and two loop to check x1,y1&lt;x2,y2 and in set</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trees
+and
+Graphs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/508/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.21</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dict to save, if (target - num) in table:  return [idx, table[target - num]], add to dict</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2961/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>left, dict, mva_val, for loop for right, if s[r] not in dict or dic[s[r]] &lt; left: check max, else left=dic[s[r]]+1, dic[s[r]]=right</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2962/</t>
+  </si>
+  <si>
+    <t>c.isdigit()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>while to three state, 0: check ' ' (j=keep 0), +-(state 1), or isdigit() (state 2 and ans*10 +int(c)), 1: isdigit() (state 2 and add), 2: isdigit() (state 2 and add), return sign and border</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3807,7 +3848,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3902,6 +3943,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4221,7 +4265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04A07DF-59CD-1C4D-A2B7-6251E393B23B}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -8303,7 +8347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K290"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:C25"/>
     </sheetView>
   </sheetViews>
@@ -10383,16 +10427,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10422,8 +10466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="F61" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12521,16 +12565,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="B65:B70"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B34"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12618,8 +12662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA7C0AF-7D3E-B64D-B4A5-6DFBB1424920}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F12"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12628,15 +12672,17 @@
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="130.33203125" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="21"/>
+      <c r="A1" s="21" t="s">
+        <v>974</v>
+      </c>
       <c r="B1" s="21"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -12676,50 +12722,91 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" ht="16">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="B3" s="32" t="s">
+        <v>707</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>976</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>978</v>
+      </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="I3" s="2" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="7"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>979</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>980</v>
+      </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="2" t="s">
+        <v>977</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>981</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>983</v>
+      </c>
       <c r="H5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>982</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -12732,7 +12819,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -12744,7 +12831,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -12756,7 +12843,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -12768,7 +12855,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -12780,7 +12867,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -12793,7 +12880,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -12806,7 +12893,7 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -12819,7 +12906,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -12832,7 +12919,7 @@
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -12845,7 +12932,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -12858,7 +12945,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -12871,7 +12958,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -12884,7 +12971,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -12896,7 +12983,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -12908,7 +12995,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -12921,7 +13008,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -12933,7 +13020,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -12945,7 +13032,9 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="31" t="s">
+        <v>802</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -12957,7 +13046,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -12972,7 +13061,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -12984,7 +13073,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -12997,7 +13086,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -13009,7 +13098,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -13021,7 +13110,9 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="31" t="s">
+        <v>975</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -13035,7 +13126,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -13049,7 +13140,7 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -13061,7 +13152,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -13072,7 +13163,7 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -13086,7 +13177,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="19"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -13099,7 +13190,7 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="19"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -13113,7 +13204,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="19"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -13126,7 +13217,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -13139,7 +13230,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -13150,7 +13241,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -13162,7 +13253,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -13175,7 +13266,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -13635,10 +13726,18 @@
       <c r="B87" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B3:B23"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="B30:B42"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{0CCF9E97-B4F9-3740-A6A0-40FFCDECB8E2}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{142AEA7F-0B26-AD46-BF0D-D2A4368318AE}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{085CA608-439A-F14E-A719-17A8A2BBCA48}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[20240122] Amazon Interview (68) 4-6
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24CF74A-A6CA-6842-AFF5-695844C63574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CEA7C0-BF77-8049-82F2-2F27ABB55CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="992">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3665,6 +3665,37 @@
   </si>
   <si>
     <t>while to three state, 0: check ' ' (j=keep 0), +-(state 1), or isdigit() (state 2 and ans*10 +int(c)), 1: isdigit() (state 2 and add), 2: isdigit() (state 2 and add), return sign and border</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2963/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integer to Roman</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2964/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2965/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.22</t>
+  </si>
+  <si>
+    <t>two ptr left, right, maxArea to save, while l &lt; r: get max area frist and then if l &lt; r: l++ else r --</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>table, if (i &lt; (len(s)-1)) and (table[s[i]] &lt; table[s[i+1]]) value - num[s[i]] else +</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>table for all values with 4,9 prefix, and for loop to check in order from biggest to smallest while n &lt; num: answer += table[n] num -= n</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10427,16 +10458,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12565,16 +12596,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B77:B87"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B51"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="B77:B87"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B52:B57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12663,7 +12694,7 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12807,12 +12838,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="2"/>
+      <c r="C6" s="2">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>984</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>989</v>
+      </c>
       <c r="H6" s="16"/>
+      <c r="I6" s="2" t="s">
+        <v>988</v>
+      </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10">
@@ -12820,24 +12864,49 @@
         <v>5</v>
       </c>
       <c r="B7" s="19"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="C7" s="2">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>986</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="19"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2"/>
+      <c r="C8" s="2">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>987</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>990</v>
+      </c>
       <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>988</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2">
@@ -13737,6 +13806,9 @@
     <hyperlink ref="A1" r:id="rId1" xr:uid="{0CCF9E97-B4F9-3740-A6A0-40FFCDECB8E2}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{142AEA7F-0B26-AD46-BF0D-D2A4368318AE}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{085CA608-439A-F14E-A719-17A8A2BBCA48}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{D12CEFE5-41A0-204C-8816-46ECE0109FA2}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{3A069412-4F3A-EF49-8C6E-05DFADCE553D}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{54E39176-3B8F-4843-9D05-2EB3FAA9F0D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240124] Amazon Interview (68) 7-8
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CEA7C0-BF77-8049-82F2-2F27ABB55CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E9F52-252C-5D4B-A42E-CB3D34301ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="998">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3696,6 +3696,30 @@
   </si>
   <si>
     <t>table for all values with 4,9 prefix, and for loop to check in order from biggest to smallest while n &lt; num: answer += table[n] num -= n</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2966/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.24</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>three answer: 1. set one num &lt;= 0 and call func to check the rest of two num (two sum), 2. two loop with set for ans, dup and dict for seen, similar to TwoSum, 3. list all status and count</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Sum Closest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2967/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two ptr: diff and sort nums, for loop with low, height, then while low &lt; height to check dif through (abs(target - summ) &lt; abs(diff)), and if summ &lt; target: l++ else: h--, if dif=0:break</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10458,16 +10482,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12596,16 +12620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="B65:B70"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B34"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12694,7 +12718,7 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12705,7 +12729,7 @@
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="67.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="130.33203125" customWidth="1"/>
+    <col min="7" max="7" width="160" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
   </cols>
@@ -12913,24 +12937,48 @@
         <v>7</v>
       </c>
       <c r="B9" s="19"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="C9" s="2">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>992</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>993</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="19"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="C10" s="2">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>993</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2">
@@ -13809,6 +13857,8 @@
     <hyperlink ref="F6" r:id="rId4" xr:uid="{D12CEFE5-41A0-204C-8816-46ECE0109FA2}"/>
     <hyperlink ref="F7" r:id="rId5" xr:uid="{3A069412-4F3A-EF49-8C6E-05DFADCE553D}"/>
     <hyperlink ref="F8" r:id="rId6" xr:uid="{54E39176-3B8F-4843-9D05-2EB3FAA9F0D9}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{A920BBF9-6D3F-2F4A-8990-BE4E46474204}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{3EDCF635-7852-3049-B6D4-6A76750BB3E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240126] Amazon Interview (68) 9-11
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E9F52-252C-5D4B-A42E-CB3D34301ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BB20BF-5C47-7449-8C87-6845B8175958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="1009">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3720,6 +3720,50 @@
   </si>
   <si>
     <t>two ptr: diff and sort nums, for loop with low, height, then while low &lt; height to check dif through (abs(target - summ) &lt; abs(diff)), and if summ &lt; target: l++ else: h--, if dif=0:break</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2968/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.26</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>find func or for loop to check [i: i+len(needle)]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>haystack.find(needle)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2969/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>col  &lt;-&gt; row and reverse, two for loop to w and I, switch by matrix[i][j], matrix[j][i] = matrix[j][i], matrix[i][j], for loop for h to reverse</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>matrix[i].reverse()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group Anagrams</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2970/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>defaultdict(list) for answer, for loop for strs: s_sort = ''.join(sorted(s)), dic[s_sort].append(s), return dic.values</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>'.join(sorted(s)), dic.values()</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3903,7 +3947,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4002,6 +4046,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10482,16 +10529,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12620,16 +12667,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B77:B87"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B51"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="B77:B87"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B52:B57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12718,7 +12765,7 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12731,7 +12778,8 @@
     <col min="6" max="6" width="67.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="160" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -12980,44 +13028,88 @@
         <v>993</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="16">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="2"/>
+      <c r="C11" s="2">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>998</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>1000</v>
+      </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>1001</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="19"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="2"/>
+      <c r="C12" s="2">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>1003</v>
+      </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="I12" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="19"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="C13" s="2">
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>1008</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2">
@@ -13859,6 +13951,9 @@
     <hyperlink ref="F8" r:id="rId6" xr:uid="{54E39176-3B8F-4843-9D05-2EB3FAA9F0D9}"/>
     <hyperlink ref="F9" r:id="rId7" xr:uid="{A920BBF9-6D3F-2F4A-8990-BE4E46474204}"/>
     <hyperlink ref="F10" r:id="rId8" xr:uid="{3EDCF635-7852-3049-B6D4-6A76750BB3E0}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{338E938B-A734-3748-A5D0-2DE9E50ACACD}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{D6BA41D1-98EC-AF4C-996B-E462E03744E0}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{B7AEBFFD-76EC-F24E-AB37-D58E07DCBC7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240127] Amazon Interview (68) 12-15
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BB20BF-5C47-7449-8C87-6845B8175958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BCCE74-F0E0-BE49-9A03-C59C2C985342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="1009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="1020">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3764,6 +3764,49 @@
   </si>
   <si>
     <t>'.join(sorted(s)), dic.values()</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/902/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compare Version Numbers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/502/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.27</t>
+  </si>
+  <si>
+    <t>split('.') first and len, for max(l1,l2) loop to get int(num[i]) if i&lt;l1 else 0, and compare l1,l2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>split('.')  will transfer to list</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/499/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list for L, R, Answer, skip i to product others for L, R, answer = L*R, or, pre, post = 1, 1, for loop to answer[i] *= pre, pre *= nums[i], answer[l-i-1] *= post, post *= nums[l-i-1]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2971/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1 + l) * l // 2 - sum, or, for loop to check I not in list</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4005,6 +4048,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4046,9 +4092,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4383,14 +4426,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -4432,7 +4475,7 @@
       <c r="B3" s="2">
         <v>26</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4465,7 +4508,7 @@
       <c r="B4" s="2">
         <v>122</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -4493,7 +4536,7 @@
       <c r="B5" s="2">
         <v>189</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -4520,7 +4563,7 @@
       <c r="B6" s="2">
         <v>217</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
@@ -4547,7 +4590,7 @@
       <c r="B7" s="2">
         <v>136</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4574,7 +4617,7 @@
       <c r="B8" s="2">
         <v>350</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
@@ -4604,7 +4647,7 @@
       <c r="B9" s="2">
         <v>66</v>
       </c>
-      <c r="C9" s="19"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -4631,7 +4674,7 @@
       <c r="B10" s="2">
         <v>283</v>
       </c>
-      <c r="C10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
@@ -4658,7 +4701,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -4685,7 +4728,7 @@
       <c r="B12" s="2">
         <v>36</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -4715,7 +4758,7 @@
       <c r="B13" s="2">
         <v>48</v>
       </c>
-      <c r="C13" s="19"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -4742,7 +4785,7 @@
       <c r="B14" s="2">
         <v>344</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="20" t="s">
         <v>123</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -4774,7 +4817,7 @@
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -4801,7 +4844,7 @@
       <c r="B16" s="2">
         <v>387</v>
       </c>
-      <c r="C16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
@@ -4828,7 +4871,7 @@
       <c r="B17" s="2">
         <v>242</v>
       </c>
-      <c r="C17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
@@ -4855,7 +4898,7 @@
       <c r="B18" s="2">
         <v>125</v>
       </c>
-      <c r="C18" s="19"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
@@ -4885,7 +4928,7 @@
       <c r="B19" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="19"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -4909,7 +4952,7 @@
       <c r="B20" s="2">
         <v>28</v>
       </c>
-      <c r="C20" s="19"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
@@ -4936,7 +4979,7 @@
       <c r="B21" s="2">
         <v>14</v>
       </c>
-      <c r="C21" s="19"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
@@ -4963,7 +5006,7 @@
       <c r="B22" s="2">
         <v>237</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="20" t="s">
         <v>124</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -4992,7 +5035,7 @@
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="19"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -5019,7 +5062,7 @@
       <c r="B24" s="2">
         <v>206</v>
       </c>
-      <c r="C24" s="19"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
@@ -5046,7 +5089,7 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="19"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
@@ -5073,7 +5116,7 @@
       <c r="B26" s="2">
         <v>234</v>
       </c>
-      <c r="C26" s="19"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
@@ -5100,7 +5143,7 @@
       <c r="B27" s="2">
         <v>141</v>
       </c>
-      <c r="C27" s="19"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="2" t="s">
         <v>21</v>
       </c>
@@ -5130,7 +5173,7 @@
       <c r="B28" s="2">
         <v>104</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="20" t="s">
         <v>125</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -5162,7 +5205,7 @@
       <c r="B29" s="2">
         <v>98</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -5186,7 +5229,7 @@
       <c r="B30" s="2">
         <v>101</v>
       </c>
-      <c r="C30" s="19"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
@@ -5216,7 +5259,7 @@
       <c r="B31" s="2">
         <v>102</v>
       </c>
-      <c r="C31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -5240,7 +5283,7 @@
       <c r="B32" s="2">
         <v>108</v>
       </c>
-      <c r="C32" s="19"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
@@ -5264,7 +5307,7 @@
       <c r="B33" s="2">
         <v>88</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="20" t="s">
         <v>126</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -5290,7 +5333,7 @@
       <c r="B34" s="2">
         <v>278</v>
       </c>
-      <c r="C34" s="19"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
@@ -5314,7 +5357,7 @@
       <c r="B35" s="2">
         <v>70</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -5340,7 +5383,7 @@
       <c r="B36" s="2">
         <v>121</v>
       </c>
-      <c r="C36" s="19"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
@@ -5364,7 +5407,7 @@
       <c r="B37" s="2">
         <v>53</v>
       </c>
-      <c r="C37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -5388,7 +5431,7 @@
       <c r="B38" s="2">
         <v>198</v>
       </c>
-      <c r="C38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -5412,7 +5455,7 @@
       <c r="B39" s="2">
         <v>384</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="20" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -5438,7 +5481,7 @@
       <c r="B40" s="2">
         <v>155</v>
       </c>
-      <c r="C40" s="19"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
@@ -5462,7 +5505,7 @@
       <c r="B41" s="2">
         <v>412</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="20" t="s">
         <v>129</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -5488,7 +5531,7 @@
       <c r="B42" s="2">
         <v>204</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -5512,7 +5555,7 @@
       <c r="B43" s="2">
         <v>326</v>
       </c>
-      <c r="C43" s="19"/>
+      <c r="C43" s="20"/>
       <c r="D43" s="2" t="s">
         <v>21</v>
       </c>
@@ -5536,7 +5579,7 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="19"/>
+      <c r="C44" s="20"/>
       <c r="D44" s="2" t="s">
         <v>21</v>
       </c>
@@ -5560,7 +5603,7 @@
       <c r="B45" s="2">
         <v>191</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="20" t="s">
         <v>130</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -5586,7 +5629,7 @@
       <c r="B46" s="2">
         <v>44</v>
       </c>
-      <c r="C46" s="19"/>
+      <c r="C46" s="20"/>
       <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
@@ -5610,7 +5653,7 @@
       <c r="B47" s="2">
         <v>190</v>
       </c>
-      <c r="C47" s="19"/>
+      <c r="C47" s="20"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -5634,7 +5677,7 @@
       <c r="B48" s="2">
         <v>118</v>
       </c>
-      <c r="C48" s="19"/>
+      <c r="C48" s="20"/>
       <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
@@ -5658,7 +5701,7 @@
       <c r="B49" s="2">
         <v>20</v>
       </c>
-      <c r="C49" s="19"/>
+      <c r="C49" s="20"/>
       <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
@@ -5682,7 +5725,7 @@
       <c r="B50" s="2">
         <v>268</v>
       </c>
-      <c r="C50" s="19"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
@@ -5943,15 +5986,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="5" t="s">
@@ -5995,7 +6038,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="31">
         <v>1</v>
       </c>
       <c r="C3" s="2">
@@ -6033,7 +6076,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="2">
         <v>20</v>
       </c>
@@ -6064,7 +6107,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="2">
         <v>21</v>
       </c>
@@ -6094,7 +6137,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="2">
         <v>121</v>
       </c>
@@ -6124,7 +6167,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="30"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="2">
         <v>125</v>
       </c>
@@ -6154,7 +6197,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="2">
         <v>226</v>
       </c>
@@ -6184,7 +6227,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="30"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="2">
         <v>242</v>
       </c>
@@ -6214,7 +6257,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="2">
         <v>704</v>
       </c>
@@ -6244,7 +6287,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="30"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="2">
         <v>733</v>
       </c>
@@ -6274,7 +6317,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="30"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="2">
         <v>235</v>
       </c>
@@ -6304,7 +6347,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="30"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="2">
         <v>110</v>
       </c>
@@ -6334,7 +6377,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="2">
         <v>141</v>
       </c>
@@ -6364,7 +6407,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="30"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="2">
         <v>232</v>
       </c>
@@ -6397,7 +6440,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="26">
         <v>2</v>
       </c>
       <c r="C16" s="2">
@@ -6429,7 +6472,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="25"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="2">
         <v>383</v>
       </c>
@@ -6459,7 +6502,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="2">
         <v>70</v>
       </c>
@@ -6489,7 +6532,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="25"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="2">
         <v>409</v>
       </c>
@@ -6519,7 +6562,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="25"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="2">
         <v>206</v>
       </c>
@@ -6549,7 +6592,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="25"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="2">
         <v>169</v>
       </c>
@@ -6579,7 +6622,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="25"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="2">
         <v>67</v>
       </c>
@@ -6609,7 +6652,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="25"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="2">
         <v>543</v>
       </c>
@@ -6639,7 +6682,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="25"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="2">
         <v>876</v>
       </c>
@@ -6669,7 +6712,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="25"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="2">
         <v>104</v>
       </c>
@@ -6699,7 +6742,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="25"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="2">
         <v>217</v>
       </c>
@@ -6729,7 +6772,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="25"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="2">
         <v>53</v>
       </c>
@@ -6759,7 +6802,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="26">
+      <c r="B28" s="27">
         <v>3</v>
       </c>
       <c r="C28" s="2">
@@ -6791,7 +6834,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="26"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="2">
         <v>542</v>
       </c>
@@ -6821,7 +6864,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="26"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="2">
         <v>973</v>
       </c>
@@ -6851,7 +6894,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="26"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="2">
         <v>3</v>
       </c>
@@ -6881,7 +6924,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="26"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="2">
         <v>15</v>
       </c>
@@ -6911,7 +6954,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="26"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="2">
         <v>102</v>
       </c>
@@ -6941,7 +6984,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="26"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="2">
         <v>133</v>
       </c>
@@ -6974,7 +7017,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="26"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="2">
         <v>150</v>
       </c>
@@ -7004,7 +7047,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B36" s="28">
         <v>4</v>
       </c>
       <c r="C36" s="2">
@@ -7039,7 +7082,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="27"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="2">
         <v>208</v>
       </c>
@@ -7069,7 +7112,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="2">
         <v>322</v>
       </c>
@@ -7099,7 +7142,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="27"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="2">
         <v>238</v>
       </c>
@@ -7129,7 +7172,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="27"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="2">
         <v>155</v>
       </c>
@@ -7159,7 +7202,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="27"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="2">
         <v>98</v>
       </c>
@@ -7189,7 +7232,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="27"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="2">
         <v>200</v>
       </c>
@@ -7219,7 +7262,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="27"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="2">
         <v>994</v>
       </c>
@@ -7249,7 +7292,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B44" s="29">
         <v>5</v>
       </c>
       <c r="C44" s="2">
@@ -7281,7 +7324,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="28"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="2">
         <v>39</v>
       </c>
@@ -7314,7 +7357,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="28"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="2">
         <v>46</v>
       </c>
@@ -7344,7 +7387,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="28"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="2">
         <v>56</v>
       </c>
@@ -7374,7 +7417,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="28"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="2">
         <v>236</v>
       </c>
@@ -7404,7 +7447,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="28"/>
+      <c r="B49" s="29"/>
       <c r="C49" s="2">
         <v>981</v>
       </c>
@@ -7434,7 +7477,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="28"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="2">
         <v>721</v>
       </c>
@@ -7467,7 +7510,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="28"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="2">
         <v>75</v>
       </c>
@@ -7497,7 +7540,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="29">
+      <c r="B52" s="30">
         <v>6</v>
       </c>
       <c r="C52" s="2">
@@ -7529,7 +7572,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="29"/>
+      <c r="B53" s="30"/>
       <c r="C53" s="2">
         <v>416</v>
       </c>
@@ -7559,7 +7602,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="29"/>
+      <c r="B54" s="30"/>
       <c r="C54" s="2">
         <v>8</v>
       </c>
@@ -7589,7 +7632,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="29"/>
+      <c r="B55" s="30"/>
       <c r="C55" s="2">
         <v>54</v>
       </c>
@@ -7619,7 +7662,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="2">
         <v>78</v>
       </c>
@@ -7649,7 +7692,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="29"/>
+      <c r="B57" s="30"/>
       <c r="C57" s="2">
         <v>199</v>
       </c>
@@ -7679,7 +7722,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="29"/>
+      <c r="B58" s="30"/>
       <c r="C58" s="2">
         <v>5</v>
       </c>
@@ -7709,7 +7752,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="29"/>
+      <c r="B59" s="30"/>
       <c r="C59" s="2">
         <v>62</v>
       </c>
@@ -7739,7 +7782,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="29"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="2">
         <v>105</v>
       </c>
@@ -7769,7 +7812,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="22">
+      <c r="B61" s="23">
         <v>7</v>
       </c>
       <c r="C61" s="2">
@@ -7801,7 +7844,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="22"/>
+      <c r="B62" s="23"/>
       <c r="C62" s="2">
         <v>17</v>
       </c>
@@ -7831,7 +7874,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="22"/>
+      <c r="B63" s="23"/>
       <c r="C63" s="2">
         <v>79</v>
       </c>
@@ -7861,7 +7904,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="22"/>
+      <c r="B64" s="23"/>
       <c r="C64" s="2">
         <v>438</v>
       </c>
@@ -7891,7 +7934,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="22"/>
+      <c r="B65" s="23"/>
       <c r="C65" s="2">
         <v>310</v>
       </c>
@@ -7921,7 +7964,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="22"/>
+      <c r="B66" s="23"/>
       <c r="C66" s="2">
         <v>621</v>
       </c>
@@ -7951,7 +7994,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="22"/>
+      <c r="B67" s="23"/>
       <c r="C67" s="2">
         <v>146</v>
       </c>
@@ -7981,7 +8024,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="23">
+      <c r="B68" s="24">
         <v>8</v>
       </c>
       <c r="C68" s="2">
@@ -8013,7 +8056,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="23"/>
+      <c r="B69" s="24"/>
       <c r="C69" s="2">
         <v>76</v>
       </c>
@@ -8043,7 +8086,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="23"/>
+      <c r="B70" s="24"/>
       <c r="C70" s="2">
         <v>297</v>
       </c>
@@ -8073,7 +8116,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="23"/>
+      <c r="B71" s="24"/>
       <c r="C71" s="2">
         <v>42</v>
       </c>
@@ -8103,7 +8146,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="23"/>
+      <c r="B72" s="24"/>
       <c r="C72" s="2">
         <v>295</v>
       </c>
@@ -8133,7 +8176,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="23"/>
+      <c r="B73" s="24"/>
       <c r="C73" s="2">
         <v>127</v>
       </c>
@@ -8163,7 +8206,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="23"/>
+      <c r="B74" s="24"/>
       <c r="C74" s="2">
         <v>224</v>
       </c>
@@ -8193,7 +8236,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="23"/>
+      <c r="B75" s="24"/>
       <c r="C75" s="2">
         <v>1235</v>
       </c>
@@ -8223,7 +8266,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="23"/>
+      <c r="B76" s="24"/>
       <c r="C76" s="2">
         <v>23</v>
       </c>
@@ -8253,7 +8296,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="23"/>
+      <c r="B77" s="24"/>
       <c r="C77" s="2">
         <v>84</v>
       </c>
@@ -8286,7 +8329,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="B78" s="20" t="s">
         <v>130</v>
       </c>
       <c r="C78" s="2">
@@ -8318,7 +8361,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="19"/>
+      <c r="B79" s="20"/>
       <c r="C79" s="2">
         <v>153</v>
       </c>
@@ -8354,15 +8397,15 @@
       <c r="A85" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B85" s="24" t="s">
+      <c r="B85" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
-      <c r="H85" s="24"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="25"/>
+      <c r="H85" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -8467,14 +8510,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>467</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
@@ -8518,7 +8561,7 @@
       <c r="B3" s="2">
         <v>15</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>480</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -8551,7 +8594,7 @@
       <c r="B4" s="2">
         <v>73</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
@@ -8577,7 +8620,7 @@
       <c r="B5" s="2">
         <v>49</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
@@ -8601,7 +8644,7 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
@@ -8625,7 +8668,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
@@ -8649,7 +8692,7 @@
       <c r="B8" s="2">
         <v>334</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
@@ -8673,7 +8716,7 @@
       <c r="B9" s="2">
         <v>163</v>
       </c>
-      <c r="C9" s="19"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -8697,7 +8740,7 @@
       <c r="B10" s="2">
         <v>38</v>
       </c>
-      <c r="C10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
@@ -8721,7 +8764,7 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="20" t="s">
         <v>481</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -8747,7 +8790,7 @@
       <c r="B12" s="2">
         <v>328</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
@@ -8771,7 +8814,7 @@
       <c r="B13" s="2">
         <v>160</v>
       </c>
-      <c r="C13" s="19"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
@@ -8795,7 +8838,7 @@
       <c r="B14" s="2">
         <v>94</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="20" t="s">
         <v>482</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -8821,7 +8864,7 @@
       <c r="B15" s="2">
         <v>103</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
@@ -8845,7 +8888,7 @@
       <c r="B16" s="2">
         <v>105</v>
       </c>
-      <c r="C16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
@@ -8872,7 +8915,7 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
@@ -8896,7 +8939,7 @@
       <c r="B18" s="2">
         <v>230</v>
       </c>
-      <c r="C18" s="19"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -8920,7 +8963,7 @@
       <c r="B19" s="2">
         <v>285</v>
       </c>
-      <c r="C19" s="19"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="2" t="s">
         <v>38</v>
       </c>
@@ -8947,7 +8990,7 @@
       <c r="B20" s="2">
         <v>200</v>
       </c>
-      <c r="C20" s="19"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
@@ -8971,7 +9014,7 @@
       <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="20" t="s">
         <v>483</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -8997,7 +9040,7 @@
       <c r="B22" s="2">
         <v>22</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
@@ -9021,7 +9064,7 @@
       <c r="B23" s="2">
         <v>46</v>
       </c>
-      <c r="C23" s="19"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
@@ -9045,7 +9088,7 @@
       <c r="B24" s="2">
         <v>78</v>
       </c>
-      <c r="C24" s="19"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
@@ -9069,7 +9112,7 @@
       <c r="B25" s="2">
         <v>79</v>
       </c>
-      <c r="C25" s="19"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
@@ -9096,7 +9139,7 @@
       <c r="B26" s="2">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="20" t="s">
         <v>126</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -9122,7 +9165,7 @@
       <c r="B27" s="2">
         <v>347</v>
       </c>
-      <c r="C27" s="19"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
@@ -9149,7 +9192,7 @@
       <c r="B28" s="2">
         <v>215</v>
       </c>
-      <c r="C28" s="19"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -9176,7 +9219,7 @@
       <c r="B29" s="2">
         <v>162</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
@@ -9200,7 +9243,7 @@
       <c r="B30" s="2">
         <v>34</v>
       </c>
-      <c r="C30" s="19"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="2" t="s">
         <v>38</v>
       </c>
@@ -9224,7 +9267,7 @@
       <c r="B31" s="2">
         <v>56</v>
       </c>
-      <c r="C31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="2" t="s">
         <v>38</v>
       </c>
@@ -9248,7 +9291,7 @@
       <c r="B32" s="2">
         <v>33</v>
       </c>
-      <c r="C32" s="19"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
@@ -9272,7 +9315,7 @@
       <c r="B33" s="2">
         <v>253</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
@@ -9296,7 +9339,7 @@
       <c r="B34" s="2">
         <v>240</v>
       </c>
-      <c r="C34" s="19"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
@@ -9320,7 +9363,7 @@
       <c r="B35" s="2">
         <v>55</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -9346,7 +9389,7 @@
       <c r="B36" s="2">
         <v>62</v>
       </c>
-      <c r="C36" s="19"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
@@ -9370,7 +9413,7 @@
       <c r="B37" s="2">
         <v>322</v>
       </c>
-      <c r="C37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
@@ -9394,7 +9437,7 @@
       <c r="B38" s="2">
         <v>300</v>
       </c>
-      <c r="C38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
@@ -9421,7 +9464,7 @@
       <c r="B39" s="2">
         <v>251</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="20" t="s">
         <v>128</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -9447,7 +9490,7 @@
       <c r="B40" s="2">
         <v>297</v>
       </c>
-      <c r="C40" s="19"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="2" t="s">
         <v>87</v>
       </c>
@@ -9471,7 +9514,7 @@
       <c r="B41" s="2">
         <v>380</v>
       </c>
-      <c r="C41" s="19"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
@@ -9498,7 +9541,7 @@
       <c r="B42" s="2">
         <v>348</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
@@ -9522,7 +9565,7 @@
       <c r="B43" s="2">
         <v>202</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="20" t="s">
         <v>129</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -9548,7 +9591,7 @@
       <c r="B44" s="2">
         <v>172</v>
       </c>
-      <c r="C44" s="19"/>
+      <c r="C44" s="20"/>
       <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
@@ -9572,7 +9615,7 @@
       <c r="B45" s="2">
         <v>171</v>
       </c>
-      <c r="C45" s="19"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
@@ -9599,7 +9642,7 @@
       <c r="B46" s="2">
         <v>50</v>
       </c>
-      <c r="C46" s="19"/>
+      <c r="C46" s="20"/>
       <c r="D46" s="2" t="s">
         <v>38</v>
       </c>
@@ -9626,7 +9669,7 @@
       <c r="B47" s="2">
         <v>69</v>
       </c>
-      <c r="C47" s="19"/>
+      <c r="C47" s="20"/>
       <c r="D47" s="2" t="s">
         <v>21</v>
       </c>
@@ -9653,7 +9696,7 @@
       <c r="B48" s="2">
         <v>29</v>
       </c>
-      <c r="C48" s="19"/>
+      <c r="C48" s="20"/>
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
@@ -9677,7 +9720,7 @@
       <c r="B49" s="2">
         <v>166</v>
       </c>
-      <c r="C49" s="19"/>
+      <c r="C49" s="20"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
       </c>
@@ -9701,7 +9744,7 @@
       <c r="B50" s="2">
         <v>371</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="20" t="s">
         <v>130</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -9727,7 +9770,7 @@
       <c r="B51" s="2">
         <v>150</v>
       </c>
-      <c r="C51" s="19"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
@@ -9751,7 +9794,7 @@
       <c r="B52" s="2">
         <v>169</v>
       </c>
-      <c r="C52" s="19"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="2" t="s">
         <v>21</v>
       </c>
@@ -9775,7 +9818,7 @@
       <c r="B53" s="2">
         <v>645</v>
       </c>
-      <c r="C53" s="19"/>
+      <c r="C53" s="20"/>
       <c r="D53" s="2" t="s">
         <v>38</v>
       </c>
@@ -9799,7 +9842,7 @@
       <c r="B54" s="2">
         <v>621</v>
       </c>
-      <c r="C54" s="19"/>
+      <c r="C54" s="20"/>
       <c r="D54" s="2" t="s">
         <v>38</v>
       </c>
@@ -10529,16 +10572,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10585,14 +10628,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>706</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
@@ -10631,7 +10674,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>702</v>
       </c>
       <c r="C3" s="2">
@@ -10663,7 +10706,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="2">
         <v>975</v>
       </c>
@@ -10684,7 +10727,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="2">
         <v>482</v>
       </c>
@@ -10711,7 +10754,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="2">
         <v>904</v>
       </c>
@@ -10738,7 +10781,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
@@ -10754,7 +10797,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
@@ -10770,7 +10813,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
@@ -10786,7 +10829,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
@@ -10802,7 +10845,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="32" t="s">
         <v>707</v>
       </c>
       <c r="C11" s="2">
@@ -10829,7 +10872,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="2">
         <v>11</v>
       </c>
@@ -10854,7 +10897,7 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="2">
         <v>15</v>
       </c>
@@ -10881,7 +10924,7 @@
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="2">
         <v>31</v>
       </c>
@@ -10908,7 +10951,7 @@
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="2">
         <v>43</v>
       </c>
@@ -10935,7 +10978,7 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="2">
         <v>48</v>
       </c>
@@ -10960,7 +11003,7 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="2">
         <v>55</v>
       </c>
@@ -10985,7 +11028,7 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="2">
         <v>66</v>
       </c>
@@ -11010,7 +11053,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="2">
         <v>76</v>
       </c>
@@ -11030,7 +11073,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="2">
         <v>158</v>
       </c>
@@ -11050,7 +11093,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="2">
         <v>159</v>
       </c>
@@ -11077,7 +11120,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="19"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="2">
         <v>163</v>
       </c>
@@ -11101,7 +11144,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="19"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="2">
         <v>681</v>
       </c>
@@ -11125,7 +11168,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="19"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="2">
         <v>809</v>
       </c>
@@ -11149,7 +11192,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="19"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="2">
         <v>833</v>
       </c>
@@ -11182,7 +11225,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="2">
         <v>849</v>
       </c>
@@ -11206,7 +11249,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="19"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="2">
         <v>20</v>
       </c>
@@ -11231,7 +11274,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="2">
         <v>23</v>
       </c>
@@ -11251,7 +11294,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="19"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="2">
         <v>42</v>
       </c>
@@ -11271,7 +11314,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="19"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="2">
         <v>215</v>
       </c>
@@ -11299,7 +11342,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="19"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="2">
         <v>253</v>
       </c>
@@ -11327,7 +11370,7 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="2">
         <v>844</v>
       </c>
@@ -11351,7 +11394,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="19"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="2">
         <v>857</v>
       </c>
@@ -11370,7 +11413,7 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="2">
         <v>973</v>
       </c>
@@ -11398,7 +11441,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="32" t="s">
         <v>802</v>
       </c>
       <c r="C35" s="2">
@@ -11425,7 +11468,7 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="19"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="2">
         <v>19</v>
       </c>
@@ -11450,7 +11493,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="2">
         <v>21</v>
       </c>
@@ -11475,7 +11518,7 @@
       <c r="A38" s="9">
         <v>36</v>
       </c>
-      <c r="B38" s="19"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="2">
         <v>138</v>
       </c>
@@ -11502,7 +11545,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="32" t="s">
         <v>814</v>
       </c>
       <c r="C39" s="2">
@@ -11523,7 +11566,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="19"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="2">
         <v>127</v>
       </c>
@@ -11543,7 +11586,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="19"/>
+      <c r="B41" s="20"/>
       <c r="C41" s="2">
         <v>200</v>
       </c>
@@ -11568,7 +11611,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="2">
         <v>210</v>
       </c>
@@ -11592,7 +11635,7 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="19"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="2">
         <v>222</v>
       </c>
@@ -11616,7 +11659,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="2">
         <v>329</v>
       </c>
@@ -11635,7 +11678,7 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="19"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="2">
         <v>394</v>
       </c>
@@ -11659,7 +11702,7 @@
       <c r="A46" s="9">
         <v>44</v>
       </c>
-      <c r="B46" s="19"/>
+      <c r="B46" s="20"/>
       <c r="C46" s="2">
         <v>399</v>
       </c>
@@ -11683,7 +11726,7 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="19"/>
+      <c r="B47" s="20"/>
       <c r="C47" s="2">
         <v>543</v>
       </c>
@@ -11707,7 +11750,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="19"/>
+      <c r="B48" s="20"/>
       <c r="C48" s="2">
         <v>753</v>
       </c>
@@ -11726,7 +11769,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="19"/>
+      <c r="B49" s="20"/>
       <c r="C49" s="2">
         <v>489</v>
       </c>
@@ -11746,7 +11789,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="19"/>
+      <c r="B50" s="20"/>
       <c r="C50" s="2">
         <v>947</v>
       </c>
@@ -11773,7 +11816,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="19"/>
+      <c r="B51" s="20"/>
       <c r="C51" s="2">
         <v>951</v>
       </c>
@@ -11797,7 +11840,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="20" t="s">
         <v>858</v>
       </c>
       <c r="C52" s="2">
@@ -11818,7 +11861,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="19"/>
+      <c r="B53" s="20"/>
       <c r="C53" s="2">
         <v>247</v>
       </c>
@@ -11845,7 +11888,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="19"/>
+      <c r="B54" s="20"/>
       <c r="C54" s="2">
         <v>212</v>
       </c>
@@ -11864,7 +11907,7 @@
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="19"/>
+      <c r="B55" s="20"/>
       <c r="C55" s="2">
         <v>351</v>
       </c>
@@ -11891,7 +11934,7 @@
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="19"/>
+      <c r="B56" s="20"/>
       <c r="C56" s="2">
         <v>17</v>
       </c>
@@ -11919,7 +11962,7 @@
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="19"/>
+      <c r="B57" s="20"/>
       <c r="C57" s="2">
         <v>22</v>
       </c>
@@ -11947,7 +11990,7 @@
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="32" t="s">
         <v>877</v>
       </c>
       <c r="C58" s="2">
@@ -11969,7 +12012,7 @@
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="19"/>
+      <c r="B59" s="20"/>
       <c r="C59" s="2">
         <v>34</v>
       </c>
@@ -11994,7 +12037,7 @@
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="19"/>
+      <c r="B60" s="20"/>
       <c r="C60" s="2">
         <v>56</v>
       </c>
@@ -12022,7 +12065,7 @@
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="19"/>
+      <c r="B61" s="20"/>
       <c r="C61" s="2">
         <v>57</v>
       </c>
@@ -12047,7 +12090,7 @@
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="19"/>
+      <c r="B62" s="20"/>
       <c r="C62" s="2">
         <v>242</v>
       </c>
@@ -12072,7 +12115,7 @@
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="19"/>
+      <c r="B63" s="20"/>
       <c r="C63" s="2">
         <v>315</v>
       </c>
@@ -12091,7 +12134,7 @@
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="19"/>
+      <c r="B64" s="20"/>
       <c r="C64" s="2">
         <v>852</v>
       </c>
@@ -12115,7 +12158,7 @@
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B65" s="32" t="s">
         <v>895</v>
       </c>
       <c r="C65" s="2">
@@ -12145,7 +12188,7 @@
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="19"/>
+      <c r="B66" s="20"/>
       <c r="C66" s="2">
         <v>53</v>
       </c>
@@ -12170,7 +12213,7 @@
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="19"/>
+      <c r="B67" s="20"/>
       <c r="C67" s="2">
         <v>121</v>
       </c>
@@ -12195,7 +12238,7 @@
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="19"/>
+      <c r="B68" s="20"/>
       <c r="C68" s="2">
         <v>152</v>
       </c>
@@ -12220,7 +12263,7 @@
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="19"/>
+      <c r="B69" s="20"/>
       <c r="C69" s="2">
         <v>322</v>
       </c>
@@ -12245,7 +12288,7 @@
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="19"/>
+      <c r="B70" s="20"/>
       <c r="C70" s="2">
         <v>410</v>
       </c>
@@ -12265,7 +12308,7 @@
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="19" t="s">
+      <c r="B71" s="20" t="s">
         <v>128</v>
       </c>
       <c r="C71" s="2">
@@ -12294,7 +12337,7 @@
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="19"/>
+      <c r="B72" s="20"/>
       <c r="C72" s="2">
         <v>155</v>
       </c>
@@ -12319,7 +12362,7 @@
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="19"/>
+      <c r="B73" s="20"/>
       <c r="C73" s="2">
         <v>297</v>
       </c>
@@ -12339,7 +12382,7 @@
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="19"/>
+      <c r="B74" s="20"/>
       <c r="C74" s="2">
         <v>359</v>
       </c>
@@ -12363,7 +12406,7 @@
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="19"/>
+      <c r="B75" s="20"/>
       <c r="C75" s="2">
         <v>380</v>
       </c>
@@ -12390,7 +12433,7 @@
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="19"/>
+      <c r="B76" s="20"/>
       <c r="C76" s="2">
         <v>642</v>
       </c>
@@ -12409,7 +12452,7 @@
       <c r="A77" s="2">
         <v>75</v>
       </c>
-      <c r="B77" s="19" t="s">
+      <c r="B77" s="20" t="s">
         <v>130</v>
       </c>
       <c r="C77" s="2">
@@ -12439,7 +12482,7 @@
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="19"/>
+      <c r="B78" s="20"/>
       <c r="C78" s="2">
         <v>135</v>
       </c>
@@ -12459,7 +12502,7 @@
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="19"/>
+      <c r="B79" s="20"/>
       <c r="C79" s="2">
         <v>205</v>
       </c>
@@ -12483,7 +12526,7 @@
       <c r="A80" s="2">
         <v>78</v>
       </c>
-      <c r="B80" s="19"/>
+      <c r="B80" s="20"/>
       <c r="C80" s="2">
         <v>246</v>
       </c>
@@ -12507,7 +12550,7 @@
       <c r="A81" s="2">
         <v>79</v>
       </c>
-      <c r="B81" s="19"/>
+      <c r="B81" s="20"/>
       <c r="C81" s="2">
         <v>299</v>
       </c>
@@ -12528,7 +12571,7 @@
       <c r="A82" s="2">
         <v>80</v>
       </c>
-      <c r="B82" s="19"/>
+      <c r="B82" s="20"/>
       <c r="C82" s="2">
         <v>308</v>
       </c>
@@ -12546,7 +12589,7 @@
       <c r="A83" s="2">
         <v>81</v>
       </c>
-      <c r="B83" s="19"/>
+      <c r="B83" s="20"/>
       <c r="C83" s="2">
         <v>731</v>
       </c>
@@ -12570,7 +12613,7 @@
       <c r="A84" s="2">
         <v>82</v>
       </c>
-      <c r="B84" s="19"/>
+      <c r="B84" s="20"/>
       <c r="C84" s="2">
         <v>771</v>
       </c>
@@ -12597,7 +12640,7 @@
       <c r="A85" s="2">
         <v>83</v>
       </c>
-      <c r="B85" s="19"/>
+      <c r="B85" s="20"/>
       <c r="C85" s="2">
         <v>777</v>
       </c>
@@ -12624,7 +12667,7 @@
       <c r="A86" s="2">
         <v>84</v>
       </c>
-      <c r="B86" s="19"/>
+      <c r="B86" s="20"/>
       <c r="C86" s="2">
         <v>843</v>
       </c>
@@ -12642,7 +12685,7 @@
       <c r="A87" s="2">
         <v>85</v>
       </c>
-      <c r="B87" s="19"/>
+      <c r="B87" s="20"/>
       <c r="C87" s="2">
         <v>939</v>
       </c>
@@ -12667,16 +12710,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="B65:B70"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B34"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12764,8 +12807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA7C0AF-7D3E-B64D-B4A5-6DFBB1424920}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12783,14 +12826,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>974</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10">
@@ -12829,7 +12872,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>707</v>
       </c>
       <c r="C3" s="2">
@@ -12856,7 +12899,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="2">
         <v>3</v>
       </c>
@@ -12881,7 +12924,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="2">
         <v>8</v>
       </c>
@@ -12909,7 +12952,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="2">
         <v>11</v>
       </c>
@@ -12935,7 +12978,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="2">
         <v>12</v>
       </c>
@@ -12959,7 +13002,7 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="2">
         <v>13</v>
       </c>
@@ -12984,7 +13027,7 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="2">
         <v>15</v>
       </c>
@@ -13008,7 +13051,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="2">
         <v>16</v>
       </c>
@@ -13032,7 +13075,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="2">
         <v>28</v>
       </c>
@@ -13060,7 +13103,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="2">
         <v>48</v>
       </c>
@@ -13088,7 +13131,7 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="2">
         <v>49</v>
       </c>
@@ -13107,7 +13150,7 @@
       <c r="I13" s="2" t="s">
         <v>999</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="19" t="s">
         <v>1008</v>
       </c>
     </row>
@@ -13115,59 +13158,105 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="6"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="2">
+        <v>76</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>1009</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="16">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="2">
+        <v>165</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>1014</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="2"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="2">
+        <v>238</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>1016</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>1017</v>
+      </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="I16" s="2" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="2"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="2">
+        <v>268</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>1019</v>
+      </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>1012</v>
+      </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -13180,7 +13269,7 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -13192,7 +13281,7 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -13204,7 +13293,7 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -13217,7 +13306,7 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="19"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -13229,7 +13318,7 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="19"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -13241,7 +13330,7 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="32" t="s">
         <v>802</v>
       </c>
       <c r="C24" s="2"/>
@@ -13255,7 +13344,7 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="19"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -13270,7 +13359,7 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -13282,7 +13371,7 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="19"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -13295,7 +13384,7 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -13307,7 +13396,7 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="19"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -13319,7 +13408,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="32" t="s">
         <v>975</v>
       </c>
       <c r="C30" s="2"/>
@@ -13335,7 +13424,7 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="19"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -13349,7 +13438,7 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -13361,7 +13450,7 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="19"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -13372,7 +13461,7 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -13386,7 +13475,7 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="20"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -13399,7 +13488,7 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="19"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -13413,7 +13502,7 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -13426,7 +13515,7 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="19"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -13439,7 +13528,7 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="19"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -13450,7 +13539,7 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="19"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -13462,7 +13551,7 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="19"/>
+      <c r="B41" s="20"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -13475,7 +13564,7 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -13954,6 +14043,10 @@
     <hyperlink ref="F11" r:id="rId9" xr:uid="{338E938B-A734-3748-A5D0-2DE9E50ACACD}"/>
     <hyperlink ref="F12" r:id="rId10" xr:uid="{D6BA41D1-98EC-AF4C-996B-E462E03744E0}"/>
     <hyperlink ref="F13" r:id="rId11" xr:uid="{B7AEBFFD-76EC-F24E-AB37-D58E07DCBC7B}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{2E5A9081-09E0-6C4A-BF9C-7DB717EF5A45}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{26282DA2-504F-F243-B1D9-C9E7A5FE8C70}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{0FF0F503-C32A-D448-BAAE-F65DBC1933CC}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{F114A172-484B-A447-9655-8BCB252A33F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13970,14 +14063,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>643</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="J1" s="2"/>

</xml_diff>

<commit_message>
[20240128] Amazon Interview (68) 16-18
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BCCE74-F0E0-BE49-9A03-C59C2C985342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F897FD-BD7E-5045-85F7-C453849397B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="1027">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3807,6 +3807,33 @@
   </si>
   <si>
     <t>(1 + l) * l // 2 - sum, or, for loop to check I not in list</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integer to English Words</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/481/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/480/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.28</t>
+  </si>
+  <si>
+    <t>Counter and for loop in s: check which dict is 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2972/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dict to {([ to ])}, for loop with if not in table: append elif stack[-1]!=table[s[i]] return False else pop(),  else: False, finally, return len(stack)==0</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10572,16 +10599,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12710,16 +12737,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B77:B87"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B51"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="B77:B87"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B52:B57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12808,7 +12835,7 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12818,7 +12845,7 @@
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" customWidth="1"/>
     <col min="7" max="7" width="160" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
@@ -13227,7 +13254,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16">
+    <row r="17" spans="1:12" ht="15" customHeight="1">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -13252,44 +13279,77 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="15" customHeight="1">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="20"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="4"/>
+      <c r="C18" s="2">
+        <v>273</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>1021</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:12">
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1">
       <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" s="20"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="2"/>
+      <c r="C19" s="2">
+        <v>387</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>1024</v>
+      </c>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="I19" s="2" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" s="20"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="2"/>
+      <c r="C20" s="2">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>1025</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>1026</v>
+      </c>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="I20" s="2" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15" customHeight="1">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -13302,7 +13362,7 @@
       <c r="H21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -14047,6 +14107,9 @@
     <hyperlink ref="F15" r:id="rId13" xr:uid="{26282DA2-504F-F243-B1D9-C9E7A5FE8C70}"/>
     <hyperlink ref="F16" r:id="rId14" xr:uid="{0FF0F503-C32A-D448-BAAE-F65DBC1933CC}"/>
     <hyperlink ref="F17" r:id="rId15" xr:uid="{F114A172-484B-A447-9655-8BCB252A33F0}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{60706D53-194F-5441-A6A7-01DC1A7688BE}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{02E21FD2-350E-0D49-8CA3-9F3D25712B49}"/>
+    <hyperlink ref="F20" r:id="rId18" xr:uid="{AC39263B-902D-C44A-B322-DA507795283C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240130] Amazon Interview (68) 19-20
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F897FD-BD7E-5045-85F7-C453849397B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61107E0A-CFDA-C04E-995C-64DCDD75EEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Interview Q - Easy 48" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="1036">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3834,6 +3834,42 @@
   </si>
   <si>
     <t>dict to {([ to ])}, for loop with if not in table: append elif stack[-1]!=table[s[i]] return False else pop(),  else: False, finally, return len(stack)==0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.01.30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Most Common Word</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>return dict key with max v: max(table, key=table.get)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>lower, seet symbol and for loop to replace to " ", split and Counter, for loop to del ban value in table, return key with max value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2973/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reorder Log Files</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2974/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>two list: letter and digits, for loop to append to each lists, then letter.sort(key=lambda x: (x.split()[1:], x.split()[0])), return letter + digits</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>.isdigit() or .isalpha(), .sort(key=lambda x: (x.split()[1:], x.split()[0]))</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10599,16 +10635,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10638,7 +10674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView topLeftCell="F61" workbookViewId="0">
+    <sheetView topLeftCell="G13" workbookViewId="0">
       <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
@@ -12737,16 +12773,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="B65:B70"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B34"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12834,8 +12870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA7C0AF-7D3E-B64D-B4A5-6DFBB1424920}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12849,7 +12885,7 @@
     <col min="7" max="7" width="160" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="60.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -12895,7 +12931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16">
+    <row r="3" spans="1:10" ht="15" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -12922,7 +12958,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16">
+    <row r="4" spans="1:10" ht="15" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -12947,7 +12983,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="15" customHeight="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -12975,7 +13011,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="15" customHeight="1">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -13001,7 +13037,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" ht="15" customHeight="1">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -13025,7 +13061,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16">
+    <row r="8" spans="1:10" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -13050,7 +13086,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="15" customHeight="1">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -13074,7 +13110,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="15" customHeight="1">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -13098,7 +13134,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16">
+    <row r="11" spans="1:10" ht="15" customHeight="1">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -13126,7 +13162,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="15" customHeight="1">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -13154,7 +13190,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="16">
+    <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -13181,7 +13217,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="15" customHeight="1">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -13202,7 +13238,7 @@
       <c r="H14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="16">
+    <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -13229,7 +13265,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -13354,25 +13390,55 @@
         <v>19</v>
       </c>
       <c r="B21" s="20"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="C21" s="2">
+        <v>819</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>1029</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22" s="20"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="2"/>
+      <c r="C22" s="2">
+        <v>937</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>1027</v>
+      </c>
       <c r="I22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>1035</v>
+      </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2">
@@ -14110,6 +14176,8 @@
     <hyperlink ref="F18" r:id="rId16" xr:uid="{60706D53-194F-5441-A6A7-01DC1A7688BE}"/>
     <hyperlink ref="F19" r:id="rId17" xr:uid="{02E21FD2-350E-0D49-8CA3-9F3D25712B49}"/>
     <hyperlink ref="F20" r:id="rId18" xr:uid="{AC39263B-902D-C44A-B322-DA507795283C}"/>
+    <hyperlink ref="F21" r:id="rId19" xr:uid="{875A45D7-8189-8D43-A743-F36795D789C9}"/>
+    <hyperlink ref="F22" r:id="rId20" xr:uid="{C7763638-9ED7-7646-910E-12AE3CB47DA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240208] Amazon Interview (68) 21-24
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61107E0A-CFDA-C04E-995C-64DCDD75EEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D21BF4C-28A1-A541-A445-D897079E872F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="1043">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3870,6 +3870,34 @@
   </si>
   <si>
     <t>.isdigit() or .isalpha(), .sort(key=lambda x: (x.split()[1:], x.split()[0]))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/76/array-and-strings/2975/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/77/linked-list/513/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.02.08</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reverse Nodes in k-Group</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/77/linked-list/2976/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_list=pre=ListNode(0), while l1 or l2 or add: add for carry, v1=l1.val if l1 else 0, l2 same, sum=v1+v2+add, new_list.next=ListNode(sum%10), add=sum//10, new_list.next, l1.next if l1 else None, l2 same</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>new_list=pre=ListNode(0), while l1 and l2: if v1&lt;v2: new_list.next=l1 l1.next else l2, new_list.next,, new_list.next=(l1 or l2), return pre.next</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -10635,16 +10663,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C25"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C43:C49"/>
     <mergeCell ref="C50:C54"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12773,16 +12801,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B77:B87"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="B52:B57"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B34"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B51"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="B77:B87"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="B52:B57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12870,8 +12898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA7C0AF-7D3E-B64D-B4A5-6DFBB1424920}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -13440,60 +13468,102 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="15" customHeight="1">
       <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" s="20"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="15"/>
+      <c r="C23" s="2">
+        <v>42</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>1036</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="15" customHeight="1">
       <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24" s="32" t="s">
         <v>802</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="2"/>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>1041</v>
+      </c>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="I24" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" customHeight="1">
       <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" s="20"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="2"/>
+      <c r="C25" s="2">
+        <v>21</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>1042</v>
+      </c>
       <c r="H25" s="2"/>
+      <c r="I25" s="2" t="s">
+        <v>1038</v>
+      </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" ht="15" customHeight="1">
       <c r="A26" s="2">
         <v>24</v>
       </c>
       <c r="B26" s="20"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="6"/>
+      <c r="C26" s="2">
+        <v>25</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>1040</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" ht="15" customHeight="1">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -13506,7 +13576,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" ht="15" customHeight="1">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -13518,7 +13588,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -13530,7 +13600,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" ht="15" customHeight="1">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -13546,7 +13616,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" ht="15" customHeight="1">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -13560,7 +13630,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" ht="15" customHeight="1">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -13572,7 +13642,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" ht="15" customHeight="1">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -13583,7 +13653,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" ht="15" customHeight="1">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -13597,7 +13667,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" ht="15" customHeight="1">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -13610,7 +13680,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" ht="15" customHeight="1">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -13624,7 +13694,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" ht="15" customHeight="1">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -13637,7 +13707,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" ht="15" customHeight="1">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -13650,7 +13720,7 @@
       <c r="H38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" ht="15" customHeight="1">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -13661,7 +13731,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" ht="15" customHeight="1">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -13673,7 +13743,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" ht="15" customHeight="1">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -13686,7 +13756,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" ht="15" customHeight="1">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -13697,7 +13767,7 @@
       <c r="F42" s="6"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" ht="15" customHeight="1">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -13709,7 +13779,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" ht="15" customHeight="1">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -13721,7 +13791,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" ht="15" customHeight="1">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -13733,7 +13803,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" ht="15" customHeight="1">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -13745,7 +13815,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" ht="15" customHeight="1">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -13757,7 +13827,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" ht="15" customHeight="1">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -13769,7 +13839,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" ht="15" customHeight="1">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -13781,7 +13851,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" ht="15" customHeight="1">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -13793,7 +13863,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" ht="15" customHeight="1">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -13805,7 +13875,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" ht="15" customHeight="1">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -13817,7 +13887,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" ht="15" customHeight="1">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -13829,7 +13899,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" ht="15" customHeight="1">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -13841,7 +13911,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" ht="15" customHeight="1">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -13853,7 +13923,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" ht="15" customHeight="1">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -13865,7 +13935,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" ht="15" customHeight="1">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -13877,7 +13947,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" ht="15" customHeight="1">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -13889,7 +13959,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" ht="15" customHeight="1">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -13901,7 +13971,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" ht="15" customHeight="1">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -13913,7 +13983,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" ht="15" customHeight="1">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -13925,7 +13995,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" ht="15" customHeight="1">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -13937,7 +14007,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" ht="15" customHeight="1">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -13949,7 +14019,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" ht="15" customHeight="1">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -13961,7 +14031,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" ht="15" customHeight="1">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -13973,7 +14043,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" ht="15" customHeight="1">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -13985,7 +14055,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" ht="15" customHeight="1">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -13997,7 +14067,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" ht="15" customHeight="1">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -14178,6 +14248,10 @@
     <hyperlink ref="F20" r:id="rId18" xr:uid="{AC39263B-902D-C44A-B322-DA507795283C}"/>
     <hyperlink ref="F21" r:id="rId19" xr:uid="{875A45D7-8189-8D43-A743-F36795D789C9}"/>
     <hyperlink ref="F22" r:id="rId20" xr:uid="{C7763638-9ED7-7646-910E-12AE3CB47DA2}"/>
+    <hyperlink ref="F23" r:id="rId21" xr:uid="{D3AB970F-4174-6444-ABE0-F19BFDFEE429}"/>
+    <hyperlink ref="F24" r:id="rId22" xr:uid="{AD3378F5-B972-FF40-BC9E-3063DB7B43BB}"/>
+    <hyperlink ref="F26" r:id="rId23" xr:uid="{076F7594-0F56-D946-A61F-097EF244D270}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{04DA801A-9CF8-594E-9F45-EDBFA6D9D09D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[20240212] Amazon Interview (68) 25-27
</commit_message>
<xml_diff>
--- a/LC Practice Progress.xlsx
+++ b/LC Practice Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoyao/Documents/Application/z_Leetcode/Learning-Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D21BF4C-28A1-A541-A445-D897079E872F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8EFE7B-54D1-D148-9E30-D918B65E876E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{9DA65407-6F32-4AE3-B903-FBFCBBE367E6}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="1050">
   <si>
     <t xml:space="preserve">
 </t>
@@ -3898,6 +3898,36 @@
   </si>
   <si>
     <t>new_list=pre=ListNode(0), while l1 and l2: if v1&lt;v2: new_list.next=l1 l1.next else l2, new_list.next,, new_list.next=(l1 or l2), return pre.next</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/77/linked-list/2978/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.02.12</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dict visited for copy, if not head return None, if head in visited: return visit[head], node=Node(val, none,none), node.next=copyfunc(head.next) node.ram=copyfunc(head.ram), return node, or, interweaving</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loop with Interweaving Nodes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/77/linked-list/2979/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/amazon/77/linked-list/512/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sorting
+and
+Searching</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -8583,7 +8613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAAD5F4-4B5F-431B-90FB-AD70DDF91B93}">
   <dimension ref="A1:K290"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21:C25"/>
     </sheetView>
   </sheetViews>
@@ -10663,16 +10693,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="C50:C54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -10702,7 +10732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64785B82-5922-EF42-A11A-F5E7D76479AD}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView topLeftCell="G13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
@@ -12801,16 +12831,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B34"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B51"/>
     <mergeCell ref="B65:B70"/>
     <mergeCell ref="B71:B76"/>
     <mergeCell ref="B77:B87"/>
     <mergeCell ref="B58:B64"/>
     <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B34"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B51"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -12899,13 +12929,13 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
@@ -13564,39 +13594,75 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1">
-      <c r="A27" s="2">
+      <c r="A27" s="9">
         <v>25</v>
       </c>
       <c r="B27" s="20"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="2"/>
+      <c r="C27" s="2">
+        <v>138</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>1043</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>1045</v>
+      </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="I27" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>1046</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1">
       <c r="A28" s="2">
         <v>26</v>
       </c>
       <c r="B28" s="20"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="2"/>
+      <c r="C28" s="2">
+        <v>206</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>1047</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>316</v>
+      </c>
       <c r="H28" s="2"/>
+      <c r="I28" s="2" t="s">
+        <v>1044</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="A29" s="2">
         <v>27</v>
       </c>
       <c r="B29" s="20"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="6"/>
+      <c r="C29" s="2">
+        <v>23</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>1048</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
@@ -13771,7 +13837,9 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="20" t="s">
+        <v>858</v>
+      </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -13783,7 +13851,7 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -13795,7 +13863,7 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -13807,7 +13875,7 @@
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="20"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -13819,7 +13887,9 @@
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="32" t="s">
+        <v>1049</v>
+      </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -13831,7 +13901,7 @@
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="20"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -13843,7 +13913,7 @@
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="20"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -13855,7 +13925,7 @@
       <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="20"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -13867,7 +13937,7 @@
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="20"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -13879,7 +13949,7 @@
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="20"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -13891,7 +13961,7 @@
       <c r="A53" s="2">
         <v>51</v>
       </c>
-      <c r="B53" s="2"/>
+      <c r="B53" s="20"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -13903,7 +13973,7 @@
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="20"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -14220,11 +14290,13 @@
       <c r="B87" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="B47:B54"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B3:B23"/>
     <mergeCell ref="B24:B29"/>
     <mergeCell ref="B30:B42"/>
+    <mergeCell ref="B43:B46"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -14252,6 +14324,9 @@
     <hyperlink ref="F24" r:id="rId22" xr:uid="{AD3378F5-B972-FF40-BC9E-3063DB7B43BB}"/>
     <hyperlink ref="F26" r:id="rId23" xr:uid="{076F7594-0F56-D946-A61F-097EF244D270}"/>
     <hyperlink ref="F25" r:id="rId24" xr:uid="{04DA801A-9CF8-594E-9F45-EDBFA6D9D09D}"/>
+    <hyperlink ref="F27" r:id="rId25" xr:uid="{FFBBE5D5-0CE2-1844-BEB6-35BFB5E6C5F6}"/>
+    <hyperlink ref="F28" r:id="rId26" xr:uid="{D516646C-353F-7F44-AFA7-3C5807B6A834}"/>
+    <hyperlink ref="F29" r:id="rId27" xr:uid="{30FAB00F-2C3B-394F-BA35-19B251EFDCA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>